<commit_message>
[Fonds de solidarite] Add 2020-07-16 data
</commit_message>
<xml_diff>
--- a/published-data/fonds-solidarite-volet-1-departemental-classe-effectif-latest.xlsx
+++ b/published-data/fonds-solidarite-volet-1-departemental-classe-effectif-latest.xlsx
@@ -478,10 +478,10 @@
         </is>
       </c>
       <c r="C3" t="n">
-        <v>5393</v>
+        <v>5397</v>
       </c>
       <c r="D3" t="n">
-        <v>7927163</v>
+        <v>7933163</v>
       </c>
       <c r="E3" t="inlineStr">
         <is>
@@ -526,10 +526,10 @@
         </is>
       </c>
       <c r="C4" t="n">
-        <v>1923</v>
+        <v>1929</v>
       </c>
       <c r="D4" t="n">
-        <v>2857563</v>
+        <v>2866563</v>
       </c>
       <c r="E4" t="inlineStr">
         <is>
@@ -574,10 +574,10 @@
         </is>
       </c>
       <c r="C5" t="n">
-        <v>486</v>
+        <v>489</v>
       </c>
       <c r="D5" t="n">
-        <v>724722</v>
+        <v>729222</v>
       </c>
       <c r="E5" t="inlineStr">
         <is>
@@ -718,10 +718,10 @@
         </is>
       </c>
       <c r="C8" t="n">
-        <v>518</v>
+        <v>520</v>
       </c>
       <c r="D8" t="n">
-        <v>685556</v>
+        <v>688556</v>
       </c>
       <c r="E8" t="inlineStr">
         <is>
@@ -814,10 +814,10 @@
         </is>
       </c>
       <c r="C10" t="n">
-        <v>3319</v>
+        <v>3321</v>
       </c>
       <c r="D10" t="n">
-        <v>4861428</v>
+        <v>4863758</v>
       </c>
       <c r="E10" t="inlineStr">
         <is>
@@ -862,10 +862,10 @@
         </is>
       </c>
       <c r="C11" t="n">
-        <v>873</v>
+        <v>874</v>
       </c>
       <c r="D11" t="n">
-        <v>1289379</v>
+        <v>1290879</v>
       </c>
       <c r="E11" t="inlineStr">
         <is>
@@ -1006,10 +1006,10 @@
         </is>
       </c>
       <c r="C14" t="n">
-        <v>1732</v>
+        <v>1742</v>
       </c>
       <c r="D14" t="n">
-        <v>2280151</v>
+        <v>2289992</v>
       </c>
       <c r="E14" t="inlineStr">
         <is>
@@ -1054,10 +1054,10 @@
         </is>
       </c>
       <c r="C15" t="n">
-        <v>2322</v>
+        <v>2324</v>
       </c>
       <c r="D15" t="n">
-        <v>3363270</v>
+        <v>3366270</v>
       </c>
       <c r="E15" t="inlineStr">
         <is>
@@ -1102,10 +1102,10 @@
         </is>
       </c>
       <c r="C16" t="n">
-        <v>3928</v>
+        <v>3931</v>
       </c>
       <c r="D16" t="n">
-        <v>5743950</v>
+        <v>5748450</v>
       </c>
       <c r="E16" t="inlineStr">
         <is>
@@ -1150,10 +1150,10 @@
         </is>
       </c>
       <c r="C17" t="n">
-        <v>1083</v>
+        <v>1085</v>
       </c>
       <c r="D17" t="n">
-        <v>1607878</v>
+        <v>1610878</v>
       </c>
       <c r="E17" t="inlineStr">
         <is>
@@ -1390,10 +1390,10 @@
         </is>
       </c>
       <c r="C22" t="n">
-        <v>1820</v>
+        <v>1822</v>
       </c>
       <c r="D22" t="n">
-        <v>2643226</v>
+        <v>2645733</v>
       </c>
       <c r="E22" t="inlineStr">
         <is>
@@ -1678,10 +1678,10 @@
         </is>
       </c>
       <c r="C28" t="n">
-        <v>2960</v>
+        <v>2961</v>
       </c>
       <c r="D28" t="n">
-        <v>4278498</v>
+        <v>4279998</v>
       </c>
       <c r="E28" t="inlineStr">
         <is>
@@ -1726,10 +1726,10 @@
         </is>
       </c>
       <c r="C29" t="n">
-        <v>6042</v>
+        <v>6043</v>
       </c>
       <c r="D29" t="n">
-        <v>8859775</v>
+        <v>8861275</v>
       </c>
       <c r="E29" t="inlineStr">
         <is>
@@ -1774,10 +1774,10 @@
         </is>
       </c>
       <c r="C30" t="n">
-        <v>1878</v>
+        <v>1881</v>
       </c>
       <c r="D30" t="n">
-        <v>2784329</v>
+        <v>2788829</v>
       </c>
       <c r="E30" t="inlineStr">
         <is>
@@ -1966,10 +1966,10 @@
         </is>
       </c>
       <c r="C34" t="n">
-        <v>2334</v>
+        <v>2335</v>
       </c>
       <c r="D34" t="n">
-        <v>2994499</v>
+        <v>2995999</v>
       </c>
       <c r="E34" t="inlineStr">
         <is>
@@ -2062,10 +2062,10 @@
         </is>
       </c>
       <c r="C36" t="n">
-        <v>2643</v>
+        <v>2644</v>
       </c>
       <c r="D36" t="n">
-        <v>3854239</v>
+        <v>3855739</v>
       </c>
       <c r="E36" t="inlineStr">
         <is>
@@ -2350,10 +2350,10 @@
         </is>
       </c>
       <c r="C42" t="n">
-        <v>3659</v>
+        <v>3663</v>
       </c>
       <c r="D42" t="n">
-        <v>5326260</v>
+        <v>5332260</v>
       </c>
       <c r="E42" t="inlineStr">
         <is>
@@ -2398,10 +2398,10 @@
         </is>
       </c>
       <c r="C43" t="n">
-        <v>8338</v>
+        <v>8340</v>
       </c>
       <c r="D43" t="n">
-        <v>12242620</v>
+        <v>12245418</v>
       </c>
       <c r="E43" t="inlineStr">
         <is>
@@ -2446,10 +2446,10 @@
         </is>
       </c>
       <c r="C44" t="n">
-        <v>3375</v>
+        <v>3381</v>
       </c>
       <c r="D44" t="n">
-        <v>5002133</v>
+        <v>5009883</v>
       </c>
       <c r="E44" t="inlineStr">
         <is>
@@ -2542,10 +2542,10 @@
         </is>
       </c>
       <c r="C46" t="n">
-        <v>274</v>
+        <v>275</v>
       </c>
       <c r="D46" t="n">
-        <v>408037</v>
+        <v>409537</v>
       </c>
       <c r="E46" t="inlineStr">
         <is>
@@ -2638,10 +2638,10 @@
         </is>
       </c>
       <c r="C48" t="n">
-        <v>4625</v>
+        <v>4629</v>
       </c>
       <c r="D48" t="n">
-        <v>6338856</v>
+        <v>6342846</v>
       </c>
       <c r="E48" t="inlineStr">
         <is>
@@ -2686,10 +2686,10 @@
         </is>
       </c>
       <c r="C49" t="n">
-        <v>5435</v>
+        <v>5439</v>
       </c>
       <c r="D49" t="n">
-        <v>7878627</v>
+        <v>7882406</v>
       </c>
       <c r="E49" t="inlineStr">
         <is>
@@ -2734,10 +2734,10 @@
         </is>
       </c>
       <c r="C50" t="n">
-        <v>12852</v>
+        <v>12864</v>
       </c>
       <c r="D50" t="n">
-        <v>18920333</v>
+        <v>18936821</v>
       </c>
       <c r="E50" t="inlineStr">
         <is>
@@ -2782,10 +2782,10 @@
         </is>
       </c>
       <c r="C51" t="n">
-        <v>4361</v>
+        <v>4363</v>
       </c>
       <c r="D51" t="n">
-        <v>6467213</v>
+        <v>6470213</v>
       </c>
       <c r="E51" t="inlineStr">
         <is>
@@ -2830,10 +2830,10 @@
         </is>
       </c>
       <c r="C52" t="n">
-        <v>1155</v>
+        <v>1156</v>
       </c>
       <c r="D52" t="n">
-        <v>1715623</v>
+        <v>1717123</v>
       </c>
       <c r="E52" t="inlineStr">
         <is>
@@ -2878,10 +2878,10 @@
         </is>
       </c>
       <c r="C53" t="n">
-        <v>231</v>
+        <v>233</v>
       </c>
       <c r="D53" t="n">
-        <v>344403</v>
+        <v>347403</v>
       </c>
       <c r="E53" t="inlineStr">
         <is>
@@ -3022,10 +3022,10 @@
         </is>
       </c>
       <c r="C56" t="n">
-        <v>5234</v>
+        <v>5238</v>
       </c>
       <c r="D56" t="n">
-        <v>7191551</v>
+        <v>7197146</v>
       </c>
       <c r="E56" t="inlineStr">
         <is>
@@ -3118,10 +3118,10 @@
         </is>
       </c>
       <c r="C58" t="n">
-        <v>7393</v>
+        <v>7396</v>
       </c>
       <c r="D58" t="n">
-        <v>10848770</v>
+        <v>10853270</v>
       </c>
       <c r="E58" t="inlineStr">
         <is>
@@ -3166,10 +3166,10 @@
         </is>
       </c>
       <c r="C59" t="n">
-        <v>2346</v>
+        <v>2347</v>
       </c>
       <c r="D59" t="n">
-        <v>3465995</v>
+        <v>3467495</v>
       </c>
       <c r="E59" t="inlineStr">
         <is>
@@ -3214,10 +3214,10 @@
         </is>
       </c>
       <c r="C60" t="n">
-        <v>586</v>
+        <v>591</v>
       </c>
       <c r="D60" t="n">
-        <v>872075</v>
+        <v>877979</v>
       </c>
       <c r="E60" t="inlineStr">
         <is>
@@ -3262,10 +3262,10 @@
         </is>
       </c>
       <c r="C61" t="n">
-        <v>135</v>
+        <v>138</v>
       </c>
       <c r="D61" t="n">
-        <v>201019</v>
+        <v>205207</v>
       </c>
       <c r="E61" t="inlineStr">
         <is>
@@ -3358,10 +3358,10 @@
         </is>
       </c>
       <c r="C63" t="n">
-        <v>3171</v>
+        <v>3172</v>
       </c>
       <c r="D63" t="n">
-        <v>4151557</v>
+        <v>4153007</v>
       </c>
       <c r="E63" t="inlineStr">
         <is>
@@ -3406,10 +3406,10 @@
         </is>
       </c>
       <c r="C64" t="n">
-        <v>2462</v>
+        <v>2465</v>
       </c>
       <c r="D64" t="n">
-        <v>3548080</v>
+        <v>3551398</v>
       </c>
       <c r="E64" t="inlineStr">
         <is>
@@ -3454,10 +3454,10 @@
         </is>
       </c>
       <c r="C65" t="n">
-        <v>6582</v>
+        <v>6592</v>
       </c>
       <c r="D65" t="n">
-        <v>9636303</v>
+        <v>9649984</v>
       </c>
       <c r="E65" t="inlineStr">
         <is>
@@ -3502,10 +3502,10 @@
         </is>
       </c>
       <c r="C66" t="n">
-        <v>2217</v>
+        <v>2219</v>
       </c>
       <c r="D66" t="n">
-        <v>3282733</v>
+        <v>3285733</v>
       </c>
       <c r="E66" t="inlineStr">
         <is>
@@ -3694,10 +3694,10 @@
         </is>
       </c>
       <c r="C70" t="n">
-        <v>2779</v>
+        <v>2781</v>
       </c>
       <c r="D70" t="n">
-        <v>3683708</v>
+        <v>3684501</v>
       </c>
       <c r="E70" t="inlineStr">
         <is>
@@ -3742,10 +3742,10 @@
         </is>
       </c>
       <c r="C71" t="n">
-        <v>8379</v>
+        <v>8391</v>
       </c>
       <c r="D71" t="n">
-        <v>12171153</v>
+        <v>12187036</v>
       </c>
       <c r="E71" t="inlineStr">
         <is>
@@ -3790,10 +3790,10 @@
         </is>
       </c>
       <c r="C72" t="n">
-        <v>20925</v>
+        <v>20956</v>
       </c>
       <c r="D72" t="n">
-        <v>30774554</v>
+        <v>30819626</v>
       </c>
       <c r="E72" t="inlineStr">
         <is>
@@ -3838,10 +3838,10 @@
         </is>
       </c>
       <c r="C73" t="n">
-        <v>7276</v>
+        <v>7281</v>
       </c>
       <c r="D73" t="n">
-        <v>10808203</v>
+        <v>10815703</v>
       </c>
       <c r="E73" t="inlineStr">
         <is>
@@ -3886,10 +3886,10 @@
         </is>
       </c>
       <c r="C74" t="n">
-        <v>2004</v>
+        <v>2009</v>
       </c>
       <c r="D74" t="n">
-        <v>2984225</v>
+        <v>2990585</v>
       </c>
       <c r="E74" t="inlineStr">
         <is>
@@ -4126,10 +4126,10 @@
         </is>
       </c>
       <c r="C79" t="n">
-        <v>6894</v>
+        <v>6896</v>
       </c>
       <c r="D79" t="n">
-        <v>9514789</v>
+        <v>9517789</v>
       </c>
       <c r="E79" t="inlineStr">
         <is>
@@ -4174,10 +4174,10 @@
         </is>
       </c>
       <c r="C80" t="n">
-        <v>2521</v>
+        <v>2522</v>
       </c>
       <c r="D80" t="n">
-        <v>3662752</v>
+        <v>3664252</v>
       </c>
       <c r="E80" t="inlineStr">
         <is>
@@ -4222,10 +4222,10 @@
         </is>
       </c>
       <c r="C81" t="n">
-        <v>5984</v>
+        <v>5985</v>
       </c>
       <c r="D81" t="n">
-        <v>8779845</v>
+        <v>8781345</v>
       </c>
       <c r="E81" t="inlineStr">
         <is>
@@ -4270,10 +4270,10 @@
         </is>
       </c>
       <c r="C82" t="n">
-        <v>2649</v>
+        <v>2654</v>
       </c>
       <c r="D82" t="n">
-        <v>3926313</v>
+        <v>3933813</v>
       </c>
       <c r="E82" t="inlineStr">
         <is>
@@ -4318,10 +4318,10 @@
         </is>
       </c>
       <c r="C83" t="n">
-        <v>932</v>
+        <v>936</v>
       </c>
       <c r="D83" t="n">
-        <v>1381497</v>
+        <v>1387497</v>
       </c>
       <c r="E83" t="inlineStr">
         <is>
@@ -4462,10 +4462,10 @@
         </is>
       </c>
       <c r="C86" t="n">
-        <v>6082</v>
+        <v>6085</v>
       </c>
       <c r="D86" t="n">
-        <v>8569693</v>
+        <v>8572953</v>
       </c>
       <c r="E86" t="inlineStr">
         <is>
@@ -4558,10 +4558,10 @@
         </is>
       </c>
       <c r="C88" t="n">
-        <v>4625</v>
+        <v>4632</v>
       </c>
       <c r="D88" t="n">
-        <v>6798478</v>
+        <v>6808978</v>
       </c>
       <c r="E88" t="inlineStr">
         <is>
@@ -4654,10 +4654,10 @@
         </is>
       </c>
       <c r="C90" t="n">
-        <v>443</v>
+        <v>446</v>
       </c>
       <c r="D90" t="n">
-        <v>659075</v>
+        <v>663575</v>
       </c>
       <c r="E90" t="inlineStr">
         <is>
@@ -4894,10 +4894,10 @@
         </is>
       </c>
       <c r="C95" t="n">
-        <v>4290</v>
+        <v>4297</v>
       </c>
       <c r="D95" t="n">
-        <v>6303049</v>
+        <v>6313249</v>
       </c>
       <c r="E95" t="inlineStr">
         <is>
@@ -5182,10 +5182,10 @@
         </is>
       </c>
       <c r="C101" t="n">
-        <v>1454</v>
+        <v>1455</v>
       </c>
       <c r="D101" t="n">
-        <v>1969969</v>
+        <v>1971469</v>
       </c>
       <c r="E101" t="inlineStr">
         <is>
@@ -5230,10 +5230,10 @@
         </is>
       </c>
       <c r="C102" t="n">
-        <v>653</v>
+        <v>654</v>
       </c>
       <c r="D102" t="n">
-        <v>947306</v>
+        <v>948806</v>
       </c>
       <c r="E102" t="inlineStr">
         <is>
@@ -5278,10 +5278,10 @@
         </is>
       </c>
       <c r="C103" t="n">
-        <v>1676</v>
+        <v>1677</v>
       </c>
       <c r="D103" t="n">
-        <v>2466623</v>
+        <v>2468123</v>
       </c>
       <c r="E103" t="inlineStr">
         <is>
@@ -5518,10 +5518,10 @@
         </is>
       </c>
       <c r="C108" t="n">
-        <v>1036</v>
+        <v>1037</v>
       </c>
       <c r="D108" t="n">
-        <v>1498103</v>
+        <v>1499603</v>
       </c>
       <c r="E108" t="inlineStr">
         <is>
@@ -5566,10 +5566,10 @@
         </is>
       </c>
       <c r="C109" t="n">
-        <v>2549</v>
+        <v>2550</v>
       </c>
       <c r="D109" t="n">
-        <v>3736130</v>
+        <v>3737630</v>
       </c>
       <c r="E109" t="inlineStr">
         <is>
@@ -5614,10 +5614,10 @@
         </is>
       </c>
       <c r="C110" t="n">
-        <v>754</v>
+        <v>757</v>
       </c>
       <c r="D110" t="n">
-        <v>1115101</v>
+        <v>1118557</v>
       </c>
       <c r="E110" t="inlineStr">
         <is>
@@ -5854,10 +5854,10 @@
         </is>
       </c>
       <c r="C115" t="n">
-        <v>675</v>
+        <v>676</v>
       </c>
       <c r="D115" t="n">
-        <v>965420</v>
+        <v>966920</v>
       </c>
       <c r="E115" t="inlineStr">
         <is>
@@ -5902,10 +5902,10 @@
         </is>
       </c>
       <c r="C116" t="n">
-        <v>1833</v>
+        <v>1834</v>
       </c>
       <c r="D116" t="n">
-        <v>2673023</v>
+        <v>2674523</v>
       </c>
       <c r="E116" t="inlineStr">
         <is>
@@ -6142,10 +6142,10 @@
         </is>
       </c>
       <c r="C121" t="n">
-        <v>1818</v>
+        <v>1819</v>
       </c>
       <c r="D121" t="n">
-        <v>2632413</v>
+        <v>2633913</v>
       </c>
       <c r="E121" t="inlineStr">
         <is>
@@ -6190,10 +6190,10 @@
         </is>
       </c>
       <c r="C122" t="n">
-        <v>5429</v>
+        <v>5433</v>
       </c>
       <c r="D122" t="n">
-        <v>7960626</v>
+        <v>7966179</v>
       </c>
       <c r="E122" t="inlineStr">
         <is>
@@ -6238,10 +6238,10 @@
         </is>
       </c>
       <c r="C123" t="n">
-        <v>1628</v>
+        <v>1629</v>
       </c>
       <c r="D123" t="n">
-        <v>2425884</v>
+        <v>2427384</v>
       </c>
       <c r="E123" t="inlineStr">
         <is>
@@ -6286,10 +6286,10 @@
         </is>
       </c>
       <c r="C124" t="n">
-        <v>338</v>
+        <v>341</v>
       </c>
       <c r="D124" t="n">
-        <v>503965</v>
+        <v>508465</v>
       </c>
       <c r="E124" t="inlineStr">
         <is>
@@ -6382,10 +6382,10 @@
         </is>
       </c>
       <c r="C126" t="n">
-        <v>2266</v>
+        <v>2269</v>
       </c>
       <c r="D126" t="n">
-        <v>3058517</v>
+        <v>3063017</v>
       </c>
       <c r="E126" t="inlineStr">
         <is>
@@ -6526,10 +6526,10 @@
         </is>
       </c>
       <c r="C129" t="n">
-        <v>386</v>
+        <v>388</v>
       </c>
       <c r="D129" t="n">
-        <v>572627</v>
+        <v>575627</v>
       </c>
       <c r="E129" t="inlineStr">
         <is>
@@ -7102,10 +7102,10 @@
         </is>
       </c>
       <c r="C141" t="n">
-        <v>5742</v>
+        <v>5747</v>
       </c>
       <c r="D141" t="n">
-        <v>8414151</v>
+        <v>8421651</v>
       </c>
       <c r="E141" t="inlineStr">
         <is>
@@ -7150,10 +7150,10 @@
         </is>
       </c>
       <c r="C142" t="n">
-        <v>1597</v>
+        <v>1598</v>
       </c>
       <c r="D142" t="n">
-        <v>2375109</v>
+        <v>2376609</v>
       </c>
       <c r="E142" t="inlineStr">
         <is>
@@ -7342,10 +7342,10 @@
         </is>
       </c>
       <c r="C146" t="n">
-        <v>2228</v>
+        <v>2229</v>
       </c>
       <c r="D146" t="n">
-        <v>2939188</v>
+        <v>2940688</v>
       </c>
       <c r="E146" t="inlineStr">
         <is>
@@ -7390,10 +7390,10 @@
         </is>
       </c>
       <c r="C147" t="n">
-        <v>3395</v>
+        <v>3397</v>
       </c>
       <c r="D147" t="n">
-        <v>4898508</v>
+        <v>4901508</v>
       </c>
       <c r="E147" t="inlineStr">
         <is>
@@ -7438,10 +7438,10 @@
         </is>
       </c>
       <c r="C148" t="n">
-        <v>7791</v>
+        <v>7800</v>
       </c>
       <c r="D148" t="n">
-        <v>11420099</v>
+        <v>11433599</v>
       </c>
       <c r="E148" t="inlineStr">
         <is>
@@ -7486,10 +7486,10 @@
         </is>
       </c>
       <c r="C149" t="n">
-        <v>2746</v>
+        <v>2750</v>
       </c>
       <c r="D149" t="n">
-        <v>4076170</v>
+        <v>4082170</v>
       </c>
       <c r="E149" t="inlineStr">
         <is>
@@ -7534,10 +7534,10 @@
         </is>
       </c>
       <c r="C150" t="n">
-        <v>647</v>
+        <v>649</v>
       </c>
       <c r="D150" t="n">
-        <v>959826</v>
+        <v>962826</v>
       </c>
       <c r="E150" t="inlineStr">
         <is>
@@ -7678,10 +7678,10 @@
         </is>
       </c>
       <c r="C153" t="n">
-        <v>2962</v>
+        <v>2965</v>
       </c>
       <c r="D153" t="n">
-        <v>3969138</v>
+        <v>3971546</v>
       </c>
       <c r="E153" t="inlineStr">
         <is>
@@ -7774,10 +7774,10 @@
         </is>
       </c>
       <c r="C155" t="n">
-        <v>8954</v>
+        <v>8960</v>
       </c>
       <c r="D155" t="n">
-        <v>13218526</v>
+        <v>13226626</v>
       </c>
       <c r="E155" t="inlineStr">
         <is>
@@ -7822,10 +7822,10 @@
         </is>
       </c>
       <c r="C156" t="n">
-        <v>2949</v>
+        <v>2950</v>
       </c>
       <c r="D156" t="n">
-        <v>4391412</v>
+        <v>4392912</v>
       </c>
       <c r="E156" t="inlineStr">
         <is>
@@ -7870,10 +7870,10 @@
         </is>
       </c>
       <c r="C157" t="n">
-        <v>862</v>
+        <v>863</v>
       </c>
       <c r="D157" t="n">
-        <v>1288475</v>
+        <v>1289975</v>
       </c>
       <c r="E157" t="inlineStr">
         <is>
@@ -8014,10 +8014,10 @@
         </is>
       </c>
       <c r="C160" t="n">
-        <v>2946</v>
+        <v>2952</v>
       </c>
       <c r="D160" t="n">
-        <v>4003143</v>
+        <v>4005401</v>
       </c>
       <c r="E160" t="inlineStr">
         <is>
@@ -8062,10 +8062,10 @@
         </is>
       </c>
       <c r="C161" t="n">
-        <v>3481</v>
+        <v>3482</v>
       </c>
       <c r="D161" t="n">
-        <v>5014449</v>
+        <v>5015949</v>
       </c>
       <c r="E161" t="inlineStr">
         <is>
@@ -8110,10 +8110,10 @@
         </is>
       </c>
       <c r="C162" t="n">
-        <v>7475</v>
+        <v>7479</v>
       </c>
       <c r="D162" t="n">
-        <v>10973720</v>
+        <v>10979720</v>
       </c>
       <c r="E162" t="inlineStr">
         <is>
@@ -8158,10 +8158,10 @@
         </is>
       </c>
       <c r="C163" t="n">
-        <v>2436</v>
+        <v>2441</v>
       </c>
       <c r="D163" t="n">
-        <v>3626731</v>
+        <v>3634231</v>
       </c>
       <c r="E163" t="inlineStr">
         <is>
@@ -8398,10 +8398,10 @@
         </is>
       </c>
       <c r="C168" t="n">
-        <v>781</v>
+        <v>783</v>
       </c>
       <c r="D168" t="n">
-        <v>1134506</v>
+        <v>1137090</v>
       </c>
       <c r="E168" t="inlineStr">
         <is>
@@ -8446,10 +8446,10 @@
         </is>
       </c>
       <c r="C169" t="n">
-        <v>2365</v>
+        <v>2369</v>
       </c>
       <c r="D169" t="n">
-        <v>3468331</v>
+        <v>3473653</v>
       </c>
       <c r="E169" t="inlineStr">
         <is>
@@ -8686,10 +8686,10 @@
         </is>
       </c>
       <c r="C174" t="n">
-        <v>1123</v>
+        <v>1124</v>
       </c>
       <c r="D174" t="n">
-        <v>1461939</v>
+        <v>1463439</v>
       </c>
       <c r="E174" t="inlineStr">
         <is>
@@ -8782,10 +8782,10 @@
         </is>
       </c>
       <c r="C176" t="n">
-        <v>3314</v>
+        <v>3316</v>
       </c>
       <c r="D176" t="n">
-        <v>4891166</v>
+        <v>4894166</v>
       </c>
       <c r="E176" t="inlineStr">
         <is>
@@ -9022,10 +9022,10 @@
         </is>
       </c>
       <c r="C181" t="n">
-        <v>1051</v>
+        <v>1056</v>
       </c>
       <c r="D181" t="n">
-        <v>1414712</v>
+        <v>1419998</v>
       </c>
       <c r="E181" t="inlineStr">
         <is>
@@ -9118,10 +9118,10 @@
         </is>
       </c>
       <c r="C183" t="n">
-        <v>1805</v>
+        <v>1806</v>
       </c>
       <c r="D183" t="n">
-        <v>2636061</v>
+        <v>2637561</v>
       </c>
       <c r="E183" t="inlineStr">
         <is>
@@ -9166,10 +9166,10 @@
         </is>
       </c>
       <c r="C184" t="n">
-        <v>630</v>
+        <v>631</v>
       </c>
       <c r="D184" t="n">
-        <v>933638</v>
+        <v>935138</v>
       </c>
       <c r="E184" t="inlineStr">
         <is>
@@ -9406,10 +9406,10 @@
         </is>
       </c>
       <c r="C189" t="n">
-        <v>5419</v>
+        <v>5423</v>
       </c>
       <c r="D189" t="n">
-        <v>7940823</v>
+        <v>7946293</v>
       </c>
       <c r="E189" t="inlineStr">
         <is>
@@ -9454,10 +9454,10 @@
         </is>
       </c>
       <c r="C190" t="n">
-        <v>1891</v>
+        <v>1892</v>
       </c>
       <c r="D190" t="n">
-        <v>2817933</v>
+        <v>2819433</v>
       </c>
       <c r="E190" t="inlineStr">
         <is>
@@ -9502,10 +9502,10 @@
         </is>
       </c>
       <c r="C191" t="n">
-        <v>490</v>
+        <v>491</v>
       </c>
       <c r="D191" t="n">
-        <v>734124</v>
+        <v>735624</v>
       </c>
       <c r="E191" t="inlineStr">
         <is>
@@ -9646,10 +9646,10 @@
         </is>
       </c>
       <c r="C194" t="n">
-        <v>1964</v>
+        <v>1967</v>
       </c>
       <c r="D194" t="n">
-        <v>2645260</v>
+        <v>2648760</v>
       </c>
       <c r="E194" t="inlineStr">
         <is>
@@ -9694,10 +9694,10 @@
         </is>
       </c>
       <c r="C195" t="n">
-        <v>1751</v>
+        <v>1752</v>
       </c>
       <c r="D195" t="n">
-        <v>2553775</v>
+        <v>2555275</v>
       </c>
       <c r="E195" t="inlineStr">
         <is>
@@ -9742,10 +9742,10 @@
         </is>
       </c>
       <c r="C196" t="n">
-        <v>5317</v>
+        <v>5322</v>
       </c>
       <c r="D196" t="n">
-        <v>7828448</v>
+        <v>7834768</v>
       </c>
       <c r="E196" t="inlineStr">
         <is>
@@ -9790,10 +9790,10 @@
         </is>
       </c>
       <c r="C197" t="n">
-        <v>1970</v>
+        <v>1971</v>
       </c>
       <c r="D197" t="n">
-        <v>2933430</v>
+        <v>2934930</v>
       </c>
       <c r="E197" t="inlineStr">
         <is>
@@ -9838,10 +9838,10 @@
         </is>
       </c>
       <c r="C198" t="n">
-        <v>460</v>
+        <v>462</v>
       </c>
       <c r="D198" t="n">
-        <v>685675</v>
+        <v>685875</v>
       </c>
       <c r="E198" t="inlineStr">
         <is>
@@ -9982,10 +9982,10 @@
         </is>
       </c>
       <c r="C201" t="n">
-        <v>1757</v>
+        <v>1761</v>
       </c>
       <c r="D201" t="n">
-        <v>2315245</v>
+        <v>2320398</v>
       </c>
       <c r="E201" t="inlineStr">
         <is>
@@ -10078,10 +10078,10 @@
         </is>
       </c>
       <c r="C203" t="n">
-        <v>2997</v>
+        <v>2999</v>
       </c>
       <c r="D203" t="n">
-        <v>4411074</v>
+        <v>4414074</v>
       </c>
       <c r="E203" t="inlineStr">
         <is>
@@ -10270,10 +10270,10 @@
         </is>
       </c>
       <c r="C207" t="n">
-        <v>1044</v>
+        <v>1045</v>
       </c>
       <c r="D207" t="n">
-        <v>1411495</v>
+        <v>1412995</v>
       </c>
       <c r="E207" t="inlineStr">
         <is>
@@ -10366,10 +10366,10 @@
         </is>
       </c>
       <c r="C209" t="n">
-        <v>3273</v>
+        <v>3275</v>
       </c>
       <c r="D209" t="n">
-        <v>4785042</v>
+        <v>4788042</v>
       </c>
       <c r="E209" t="inlineStr">
         <is>
@@ -10558,10 +10558,10 @@
         </is>
       </c>
       <c r="C213" t="n">
-        <v>638</v>
+        <v>642</v>
       </c>
       <c r="D213" t="n">
-        <v>850360</v>
+        <v>855664</v>
       </c>
       <c r="E213" t="inlineStr">
         <is>
@@ -10606,10 +10606,10 @@
         </is>
       </c>
       <c r="C214" t="n">
-        <v>1946</v>
+        <v>1949</v>
       </c>
       <c r="D214" t="n">
-        <v>2814310</v>
+        <v>2818810</v>
       </c>
       <c r="E214" t="inlineStr">
         <is>
@@ -10654,10 +10654,10 @@
         </is>
       </c>
       <c r="C215" t="n">
-        <v>3712</v>
+        <v>3714</v>
       </c>
       <c r="D215" t="n">
-        <v>5422805</v>
+        <v>5425805</v>
       </c>
       <c r="E215" t="inlineStr">
         <is>
@@ -10702,10 +10702,10 @@
         </is>
       </c>
       <c r="C216" t="n">
-        <v>1158</v>
+        <v>1160</v>
       </c>
       <c r="D216" t="n">
-        <v>1716542</v>
+        <v>1719542</v>
       </c>
       <c r="E216" t="inlineStr">
         <is>
@@ -10846,10 +10846,10 @@
         </is>
       </c>
       <c r="C219" t="n">
-        <v>1509</v>
+        <v>1510</v>
       </c>
       <c r="D219" t="n">
-        <v>2045164</v>
+        <v>2046664</v>
       </c>
       <c r="E219" t="inlineStr">
         <is>
@@ -10942,10 +10942,10 @@
         </is>
       </c>
       <c r="C221" t="n">
-        <v>2122</v>
+        <v>2124</v>
       </c>
       <c r="D221" t="n">
-        <v>3089471</v>
+        <v>3092471</v>
       </c>
       <c r="E221" t="inlineStr">
         <is>
@@ -10990,10 +10990,10 @@
         </is>
       </c>
       <c r="C222" t="n">
-        <v>690</v>
+        <v>691</v>
       </c>
       <c r="D222" t="n">
-        <v>1024630</v>
+        <v>1026130</v>
       </c>
       <c r="E222" t="inlineStr">
         <is>
@@ -11038,10 +11038,10 @@
         </is>
       </c>
       <c r="C223" t="n">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="D223" t="n">
-        <v>307928</v>
+        <v>309428</v>
       </c>
       <c r="E223" t="inlineStr">
         <is>
@@ -11134,10 +11134,10 @@
         </is>
       </c>
       <c r="C225" t="n">
-        <v>879</v>
+        <v>880</v>
       </c>
       <c r="D225" t="n">
-        <v>1135398</v>
+        <v>1136898</v>
       </c>
       <c r="E225" t="inlineStr">
         <is>
@@ -11278,10 +11278,10 @@
         </is>
       </c>
       <c r="C228" t="n">
-        <v>781</v>
+        <v>784</v>
       </c>
       <c r="D228" t="n">
-        <v>1162340</v>
+        <v>1166840</v>
       </c>
       <c r="E228" t="inlineStr">
         <is>
@@ -11422,10 +11422,10 @@
         </is>
       </c>
       <c r="C231" t="n">
-        <v>869</v>
+        <v>871</v>
       </c>
       <c r="D231" t="n">
-        <v>1164674</v>
+        <v>1165546</v>
       </c>
       <c r="E231" t="inlineStr">
         <is>
@@ -11470,10 +11470,10 @@
         </is>
       </c>
       <c r="C232" t="n">
-        <v>3622</v>
+        <v>3629</v>
       </c>
       <c r="D232" t="n">
-        <v>5252214</v>
+        <v>5258626</v>
       </c>
       <c r="E232" t="inlineStr">
         <is>
@@ -11518,10 +11518,10 @@
         </is>
       </c>
       <c r="C233" t="n">
-        <v>11650</v>
+        <v>11661</v>
       </c>
       <c r="D233" t="n">
-        <v>17105910</v>
+        <v>17121606</v>
       </c>
       <c r="E233" t="inlineStr">
         <is>
@@ -11614,10 +11614,10 @@
         </is>
       </c>
       <c r="C235" t="n">
-        <v>1376</v>
+        <v>1379</v>
       </c>
       <c r="D235" t="n">
-        <v>2047290</v>
+        <v>2051790</v>
       </c>
       <c r="E235" t="inlineStr">
         <is>
@@ -11998,10 +11998,10 @@
         </is>
       </c>
       <c r="C243" t="n">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="D243" t="n">
-        <v>60017</v>
+        <v>61517</v>
       </c>
       <c r="E243" t="inlineStr">
         <is>
@@ -12142,10 +12142,10 @@
         </is>
       </c>
       <c r="C246" t="n">
-        <v>2490</v>
+        <v>2492</v>
       </c>
       <c r="D246" t="n">
-        <v>3601530</v>
+        <v>3604530</v>
       </c>
       <c r="E246" t="inlineStr">
         <is>
@@ -12190,10 +12190,10 @@
         </is>
       </c>
       <c r="C247" t="n">
-        <v>7417</v>
+        <v>7426</v>
       </c>
       <c r="D247" t="n">
-        <v>10895054</v>
+        <v>10906651</v>
       </c>
       <c r="E247" t="inlineStr">
         <is>
@@ -12334,10 +12334,10 @@
         </is>
       </c>
       <c r="C250" t="n">
-        <v>183</v>
+        <v>185</v>
       </c>
       <c r="D250" t="n">
-        <v>274230</v>
+        <v>277230</v>
       </c>
       <c r="E250" t="inlineStr">
         <is>
@@ -12526,10 +12526,10 @@
         </is>
       </c>
       <c r="C254" t="n">
-        <v>1921</v>
+        <v>1922</v>
       </c>
       <c r="D254" t="n">
-        <v>2539759</v>
+        <v>2541259</v>
       </c>
       <c r="E254" t="inlineStr">
         <is>
@@ -12574,10 +12574,10 @@
         </is>
       </c>
       <c r="C255" t="n">
-        <v>1657</v>
+        <v>1658</v>
       </c>
       <c r="D255" t="n">
-        <v>2407409</v>
+        <v>2408909</v>
       </c>
       <c r="E255" t="inlineStr">
         <is>
@@ -12622,10 +12622,10 @@
         </is>
       </c>
       <c r="C256" t="n">
-        <v>4676</v>
+        <v>4678</v>
       </c>
       <c r="D256" t="n">
-        <v>6887086</v>
+        <v>6890086</v>
       </c>
       <c r="E256" t="inlineStr">
         <is>
@@ -12910,10 +12910,10 @@
         </is>
       </c>
       <c r="C262" t="n">
-        <v>1734</v>
+        <v>1736</v>
       </c>
       <c r="D262" t="n">
-        <v>2538979</v>
+        <v>2541088</v>
       </c>
       <c r="E262" t="inlineStr">
         <is>
@@ -12958,10 +12958,10 @@
         </is>
       </c>
       <c r="C263" t="n">
-        <v>5259</v>
+        <v>5261</v>
       </c>
       <c r="D263" t="n">
-        <v>7738587</v>
+        <v>7740742</v>
       </c>
       <c r="E263" t="inlineStr">
         <is>
@@ -13006,10 +13006,10 @@
         </is>
       </c>
       <c r="C264" t="n">
-        <v>1837</v>
+        <v>1840</v>
       </c>
       <c r="D264" t="n">
-        <v>2727653</v>
+        <v>2732153</v>
       </c>
       <c r="E264" t="inlineStr">
         <is>
@@ -13198,10 +13198,10 @@
         </is>
       </c>
       <c r="C268" t="n">
-        <v>2030</v>
+        <v>2032</v>
       </c>
       <c r="D268" t="n">
-        <v>2748399</v>
+        <v>2751399</v>
       </c>
       <c r="E268" t="inlineStr">
         <is>
@@ -13294,10 +13294,10 @@
         </is>
       </c>
       <c r="C270" t="n">
-        <v>1337</v>
+        <v>1338</v>
       </c>
       <c r="D270" t="n">
-        <v>1946311</v>
+        <v>1947811</v>
       </c>
       <c r="E270" t="inlineStr">
         <is>
@@ -13534,10 +13534,10 @@
         </is>
       </c>
       <c r="C275" t="n">
-        <v>2471</v>
+        <v>2473</v>
       </c>
       <c r="D275" t="n">
-        <v>3578799</v>
+        <v>3581799</v>
       </c>
       <c r="E275" t="inlineStr">
         <is>
@@ -13582,10 +13582,10 @@
         </is>
       </c>
       <c r="C276" t="n">
-        <v>8153</v>
+        <v>8156</v>
       </c>
       <c r="D276" t="n">
-        <v>11953722</v>
+        <v>11958222</v>
       </c>
       <c r="E276" t="inlineStr">
         <is>
@@ -13630,10 +13630,10 @@
         </is>
       </c>
       <c r="C277" t="n">
-        <v>3400</v>
+        <v>3402</v>
       </c>
       <c r="D277" t="n">
-        <v>5058914</v>
+        <v>5061914</v>
       </c>
       <c r="E277" t="inlineStr">
         <is>
@@ -13726,10 +13726,10 @@
         </is>
       </c>
       <c r="C279" t="n">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="D279" t="n">
-        <v>217656</v>
+        <v>219156</v>
       </c>
       <c r="E279" t="inlineStr">
         <is>
@@ -13822,10 +13822,10 @@
         </is>
       </c>
       <c r="C281" t="n">
-        <v>2236</v>
+        <v>2240</v>
       </c>
       <c r="D281" t="n">
-        <v>2993986</v>
+        <v>2999986</v>
       </c>
       <c r="E281" t="inlineStr">
         <is>
@@ -13918,10 +13918,10 @@
         </is>
       </c>
       <c r="C283" t="n">
-        <v>3718</v>
+        <v>3721</v>
       </c>
       <c r="D283" t="n">
-        <v>5466462</v>
+        <v>5470962</v>
       </c>
       <c r="E283" t="inlineStr">
         <is>
@@ -13966,10 +13966,10 @@
         </is>
       </c>
       <c r="C284" t="n">
-        <v>1231</v>
+        <v>1232</v>
       </c>
       <c r="D284" t="n">
-        <v>1829289</v>
+        <v>1830789</v>
       </c>
       <c r="E284" t="inlineStr">
         <is>
@@ -14158,10 +14158,10 @@
         </is>
       </c>
       <c r="C288" t="n">
-        <v>1520</v>
+        <v>1527</v>
       </c>
       <c r="D288" t="n">
-        <v>2006543</v>
+        <v>2017043</v>
       </c>
       <c r="E288" t="inlineStr">
         <is>
@@ -14206,10 +14206,10 @@
         </is>
       </c>
       <c r="C289" t="n">
-        <v>1671</v>
+        <v>1675</v>
       </c>
       <c r="D289" t="n">
-        <v>2425133</v>
+        <v>2431133</v>
       </c>
       <c r="E289" t="inlineStr">
         <is>
@@ -14254,10 +14254,10 @@
         </is>
       </c>
       <c r="C290" t="n">
-        <v>5933</v>
+        <v>5947</v>
       </c>
       <c r="D290" t="n">
-        <v>8735326</v>
+        <v>8756326</v>
       </c>
       <c r="E290" t="inlineStr">
         <is>
@@ -14302,10 +14302,10 @@
         </is>
       </c>
       <c r="C291" t="n">
-        <v>2081</v>
+        <v>2083</v>
       </c>
       <c r="D291" t="n">
-        <v>3108370</v>
+        <v>3111370</v>
       </c>
       <c r="E291" t="inlineStr">
         <is>
@@ -14350,10 +14350,10 @@
         </is>
       </c>
       <c r="C292" t="n">
-        <v>677</v>
+        <v>678</v>
       </c>
       <c r="D292" t="n">
-        <v>1010805</v>
+        <v>1012305</v>
       </c>
       <c r="E292" t="inlineStr">
         <is>
@@ -14494,10 +14494,10 @@
         </is>
       </c>
       <c r="C295" t="n">
-        <v>5376</v>
+        <v>5408</v>
       </c>
       <c r="D295" t="n">
-        <v>7428230</v>
+        <v>7473915</v>
       </c>
       <c r="E295" t="inlineStr">
         <is>
@@ -14542,10 +14542,10 @@
         </is>
       </c>
       <c r="C296" t="n">
-        <v>678</v>
+        <v>679</v>
       </c>
       <c r="D296" t="n">
-        <v>993340</v>
+        <v>994840</v>
       </c>
       <c r="E296" t="inlineStr">
         <is>
@@ -14590,10 +14590,10 @@
         </is>
       </c>
       <c r="C297" t="n">
-        <v>1706</v>
+        <v>1722</v>
       </c>
       <c r="D297" t="n">
-        <v>2527414</v>
+        <v>2551414</v>
       </c>
       <c r="E297" t="inlineStr">
         <is>
@@ -14638,10 +14638,10 @@
         </is>
       </c>
       <c r="C298" t="n">
-        <v>686</v>
+        <v>692</v>
       </c>
       <c r="D298" t="n">
-        <v>1023219</v>
+        <v>1032219</v>
       </c>
       <c r="E298" t="inlineStr">
         <is>
@@ -14782,10 +14782,10 @@
         </is>
       </c>
       <c r="C301" t="n">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="D301" t="n">
-        <v>13500</v>
+        <v>18000</v>
       </c>
       <c r="E301" t="inlineStr">
         <is>
@@ -14830,10 +14830,10 @@
         </is>
       </c>
       <c r="C302" t="n">
-        <v>996</v>
+        <v>1001</v>
       </c>
       <c r="D302" t="n">
-        <v>1412214</v>
+        <v>1419265</v>
       </c>
       <c r="E302" t="inlineStr">
         <is>
@@ -14878,10 +14878,10 @@
         </is>
       </c>
       <c r="C303" t="n">
-        <v>1086</v>
+        <v>1087</v>
       </c>
       <c r="D303" t="n">
-        <v>1559184</v>
+        <v>1560684</v>
       </c>
       <c r="E303" t="inlineStr">
         <is>
@@ -14926,10 +14926,10 @@
         </is>
       </c>
       <c r="C304" t="n">
-        <v>3403</v>
+        <v>3408</v>
       </c>
       <c r="D304" t="n">
-        <v>4992428</v>
+        <v>4999928</v>
       </c>
       <c r="E304" t="inlineStr">
         <is>
@@ -14974,10 +14974,10 @@
         </is>
       </c>
       <c r="C305" t="n">
-        <v>1274</v>
+        <v>1275</v>
       </c>
       <c r="D305" t="n">
-        <v>1889919</v>
+        <v>1891419</v>
       </c>
       <c r="E305" t="inlineStr">
         <is>
@@ -15214,10 +15214,10 @@
         </is>
       </c>
       <c r="C310" t="n">
-        <v>6459</v>
+        <v>6467</v>
       </c>
       <c r="D310" t="n">
-        <v>9324163</v>
+        <v>9336163</v>
       </c>
       <c r="E310" t="inlineStr">
         <is>
@@ -15262,10 +15262,10 @@
         </is>
       </c>
       <c r="C311" t="n">
-        <v>18511</v>
+        <v>18522</v>
       </c>
       <c r="D311" t="n">
-        <v>27104234</v>
+        <v>27120734</v>
       </c>
       <c r="E311" t="inlineStr">
         <is>
@@ -15310,10 +15310,10 @@
         </is>
       </c>
       <c r="C312" t="n">
-        <v>6596</v>
+        <v>6603</v>
       </c>
       <c r="D312" t="n">
-        <v>9820207</v>
+        <v>9830707</v>
       </c>
       <c r="E312" t="inlineStr">
         <is>
@@ -15358,10 +15358,10 @@
         </is>
       </c>
       <c r="C313" t="n">
-        <v>1980</v>
+        <v>1986</v>
       </c>
       <c r="D313" t="n">
-        <v>2955752</v>
+        <v>2964752</v>
       </c>
       <c r="E313" t="inlineStr">
         <is>
@@ -15406,10 +15406,10 @@
         </is>
       </c>
       <c r="C314" t="n">
-        <v>410</v>
+        <v>412</v>
       </c>
       <c r="D314" t="n">
-        <v>611470</v>
+        <v>614470</v>
       </c>
       <c r="E314" t="inlineStr">
         <is>
@@ -15502,10 +15502,10 @@
         </is>
       </c>
       <c r="C316" t="n">
-        <v>5789</v>
+        <v>5792</v>
       </c>
       <c r="D316" t="n">
-        <v>7657551</v>
+        <v>7662051</v>
       </c>
       <c r="E316" t="inlineStr">
         <is>
@@ -15598,10 +15598,10 @@
         </is>
       </c>
       <c r="C318" t="n">
-        <v>6085</v>
+        <v>6089</v>
       </c>
       <c r="D318" t="n">
-        <v>8941729</v>
+        <v>8947729</v>
       </c>
       <c r="E318" t="inlineStr">
         <is>
@@ -15646,10 +15646,10 @@
         </is>
       </c>
       <c r="C319" t="n">
-        <v>2166</v>
+        <v>2170</v>
       </c>
       <c r="D319" t="n">
-        <v>3224670</v>
+        <v>3230670</v>
       </c>
       <c r="E319" t="inlineStr">
         <is>
@@ -15694,10 +15694,10 @@
         </is>
       </c>
       <c r="C320" t="n">
-        <v>573</v>
+        <v>576</v>
       </c>
       <c r="D320" t="n">
-        <v>857699</v>
+        <v>862199</v>
       </c>
       <c r="E320" t="inlineStr">
         <is>
@@ -15886,10 +15886,10 @@
         </is>
       </c>
       <c r="C324" t="n">
-        <v>3365</v>
+        <v>3369</v>
       </c>
       <c r="D324" t="n">
-        <v>4846735</v>
+        <v>4851603</v>
       </c>
       <c r="E324" t="inlineStr">
         <is>
@@ -15934,10 +15934,10 @@
         </is>
       </c>
       <c r="C325" t="n">
-        <v>10266</v>
+        <v>10270</v>
       </c>
       <c r="D325" t="n">
-        <v>15017413</v>
+        <v>15022045</v>
       </c>
       <c r="E325" t="inlineStr">
         <is>
@@ -15982,10 +15982,10 @@
         </is>
       </c>
       <c r="C326" t="n">
-        <v>3358</v>
+        <v>3359</v>
       </c>
       <c r="D326" t="n">
-        <v>4981201</v>
+        <v>4982701</v>
       </c>
       <c r="E326" t="inlineStr">
         <is>
@@ -16030,10 +16030,10 @@
         </is>
       </c>
       <c r="C327" t="n">
-        <v>1027</v>
+        <v>1028</v>
       </c>
       <c r="D327" t="n">
-        <v>1527373</v>
+        <v>1528873</v>
       </c>
       <c r="E327" t="inlineStr">
         <is>
@@ -16222,10 +16222,10 @@
         </is>
       </c>
       <c r="C331" t="n">
-        <v>3586</v>
+        <v>3588</v>
       </c>
       <c r="D331" t="n">
-        <v>4695205</v>
+        <v>4695907</v>
       </c>
       <c r="E331" t="inlineStr">
         <is>
@@ -16270,10 +16270,10 @@
         </is>
       </c>
       <c r="C332" t="n">
-        <v>1412</v>
+        <v>1413</v>
       </c>
       <c r="D332" t="n">
-        <v>2051014</v>
+        <v>2051944</v>
       </c>
       <c r="E332" t="inlineStr">
         <is>
@@ -16318,10 +16318,10 @@
         </is>
       </c>
       <c r="C333" t="n">
-        <v>4018</v>
+        <v>4032</v>
       </c>
       <c r="D333" t="n">
-        <v>5876785</v>
+        <v>5892216</v>
       </c>
       <c r="E333" t="inlineStr">
         <is>
@@ -16606,10 +16606,10 @@
         </is>
       </c>
       <c r="C339" t="n">
-        <v>3257</v>
+        <v>3264</v>
       </c>
       <c r="D339" t="n">
-        <v>4755476</v>
+        <v>4765976</v>
       </c>
       <c r="E339" t="inlineStr">
         <is>
@@ -16654,10 +16654,10 @@
         </is>
       </c>
       <c r="C340" t="n">
-        <v>9574</v>
+        <v>9586</v>
       </c>
       <c r="D340" t="n">
-        <v>14135639</v>
+        <v>14153539</v>
       </c>
       <c r="E340" t="inlineStr">
         <is>
@@ -16702,10 +16702,10 @@
         </is>
       </c>
       <c r="C341" t="n">
-        <v>3734</v>
+        <v>3738</v>
       </c>
       <c r="D341" t="n">
-        <v>5560427</v>
+        <v>5566427</v>
       </c>
       <c r="E341" t="inlineStr">
         <is>
@@ -16750,10 +16750,10 @@
         </is>
       </c>
       <c r="C342" t="n">
-        <v>1096</v>
+        <v>1101</v>
       </c>
       <c r="D342" t="n">
-        <v>1635679</v>
+        <v>1643179</v>
       </c>
       <c r="E342" t="inlineStr">
         <is>
@@ -16894,10 +16894,10 @@
         </is>
       </c>
       <c r="C345" t="n">
-        <v>3159</v>
+        <v>3163</v>
       </c>
       <c r="D345" t="n">
-        <v>4393370</v>
+        <v>4398080</v>
       </c>
       <c r="E345" t="inlineStr">
         <is>
@@ -16942,10 +16942,10 @@
         </is>
       </c>
       <c r="C346" t="n">
-        <v>5644</v>
+        <v>5650</v>
       </c>
       <c r="D346" t="n">
-        <v>8236184</v>
+        <v>8245184</v>
       </c>
       <c r="E346" t="inlineStr">
         <is>
@@ -16990,10 +16990,10 @@
         </is>
       </c>
       <c r="C347" t="n">
-        <v>14069</v>
+        <v>14086</v>
       </c>
       <c r="D347" t="n">
-        <v>20731229</v>
+        <v>20756729</v>
       </c>
       <c r="E347" t="inlineStr">
         <is>
@@ -17038,10 +17038,10 @@
         </is>
       </c>
       <c r="C348" t="n">
-        <v>6379</v>
+        <v>6381</v>
       </c>
       <c r="D348" t="n">
-        <v>9517284</v>
+        <v>9520040</v>
       </c>
       <c r="E348" t="inlineStr">
         <is>
@@ -17086,10 +17086,10 @@
         </is>
       </c>
       <c r="C349" t="n">
-        <v>1944</v>
+        <v>1946</v>
       </c>
       <c r="D349" t="n">
-        <v>2901872</v>
+        <v>2904872</v>
       </c>
       <c r="E349" t="inlineStr">
         <is>
@@ -17230,10 +17230,10 @@
         </is>
       </c>
       <c r="C352" t="n">
-        <v>5092</v>
+        <v>5099</v>
       </c>
       <c r="D352" t="n">
-        <v>6989017</v>
+        <v>6997881</v>
       </c>
       <c r="E352" t="inlineStr">
         <is>
@@ -17278,10 +17278,10 @@
         </is>
       </c>
       <c r="C353" t="n">
-        <v>16572</v>
+        <v>16589</v>
       </c>
       <c r="D353" t="n">
-        <v>24074669</v>
+        <v>24095916</v>
       </c>
       <c r="E353" t="inlineStr">
         <is>
@@ -17326,10 +17326,10 @@
         </is>
       </c>
       <c r="C354" t="n">
-        <v>46192</v>
+        <v>46251</v>
       </c>
       <c r="D354" t="n">
-        <v>68132097</v>
+        <v>68219834</v>
       </c>
       <c r="E354" t="inlineStr">
         <is>
@@ -17374,10 +17374,10 @@
         </is>
       </c>
       <c r="C355" t="n">
-        <v>21571</v>
+        <v>21598</v>
       </c>
       <c r="D355" t="n">
-        <v>32198919</v>
+        <v>32237016</v>
       </c>
       <c r="E355" t="inlineStr">
         <is>
@@ -17422,10 +17422,10 @@
         </is>
       </c>
       <c r="C356" t="n">
-        <v>7659</v>
+        <v>7681</v>
       </c>
       <c r="D356" t="n">
-        <v>11455277</v>
+        <v>11486983</v>
       </c>
       <c r="E356" t="inlineStr">
         <is>
@@ -17470,10 +17470,10 @@
         </is>
       </c>
       <c r="C357" t="n">
-        <v>1801</v>
+        <v>1809</v>
       </c>
       <c r="D357" t="n">
-        <v>2693416</v>
+        <v>2705416</v>
       </c>
       <c r="E357" t="inlineStr">
         <is>
@@ -17710,10 +17710,10 @@
         </is>
       </c>
       <c r="C362" t="n">
-        <v>16276</v>
+        <v>16298</v>
       </c>
       <c r="D362" t="n">
-        <v>22220258</v>
+        <v>22244837</v>
       </c>
       <c r="E362" t="inlineStr">
         <is>
@@ -17758,10 +17758,10 @@
         </is>
       </c>
       <c r="C363" t="n">
-        <v>3941</v>
+        <v>3945</v>
       </c>
       <c r="D363" t="n">
-        <v>5742240</v>
+        <v>5748240</v>
       </c>
       <c r="E363" t="inlineStr">
         <is>
@@ -17806,10 +17806,10 @@
         </is>
       </c>
       <c r="C364" t="n">
-        <v>11442</v>
+        <v>11447</v>
       </c>
       <c r="D364" t="n">
-        <v>16839819</v>
+        <v>16847319</v>
       </c>
       <c r="E364" t="inlineStr">
         <is>
@@ -17854,10 +17854,10 @@
         </is>
       </c>
       <c r="C365" t="n">
-        <v>4363</v>
+        <v>4368</v>
       </c>
       <c r="D365" t="n">
-        <v>6480544</v>
+        <v>6488044</v>
       </c>
       <c r="E365" t="inlineStr">
         <is>
@@ -18046,10 +18046,10 @@
         </is>
       </c>
       <c r="C369" t="n">
-        <v>3889</v>
+        <v>3897</v>
       </c>
       <c r="D369" t="n">
-        <v>5331821</v>
+        <v>5341764</v>
       </c>
       <c r="E369" t="inlineStr">
         <is>
@@ -18094,10 +18094,10 @@
         </is>
       </c>
       <c r="C370" t="n">
-        <v>4696</v>
+        <v>4700</v>
       </c>
       <c r="D370" t="n">
-        <v>6834129</v>
+        <v>6840129</v>
       </c>
       <c r="E370" t="inlineStr">
         <is>
@@ -18142,10 +18142,10 @@
         </is>
       </c>
       <c r="C371" t="n">
-        <v>17137</v>
+        <v>17157</v>
       </c>
       <c r="D371" t="n">
-        <v>25259571</v>
+        <v>25289413</v>
       </c>
       <c r="E371" t="inlineStr">
         <is>
@@ -18190,10 +18190,10 @@
         </is>
       </c>
       <c r="C372" t="n">
-        <v>8226</v>
+        <v>8238</v>
       </c>
       <c r="D372" t="n">
-        <v>12267894</v>
+        <v>12285625</v>
       </c>
       <c r="E372" t="inlineStr">
         <is>
@@ -18238,10 +18238,10 @@
         </is>
       </c>
       <c r="C373" t="n">
-        <v>2311</v>
+        <v>2313</v>
       </c>
       <c r="D373" t="n">
-        <v>3455388</v>
+        <v>3458388</v>
       </c>
       <c r="E373" t="inlineStr">
         <is>
@@ -18286,10 +18286,10 @@
         </is>
       </c>
       <c r="C374" t="n">
-        <v>559</v>
+        <v>561</v>
       </c>
       <c r="D374" t="n">
-        <v>835595</v>
+        <v>838595</v>
       </c>
       <c r="E374" t="inlineStr">
         <is>
@@ -18382,10 +18382,10 @@
         </is>
       </c>
       <c r="C376" t="n">
-        <v>4818</v>
+        <v>4822</v>
       </c>
       <c r="D376" t="n">
-        <v>6541263</v>
+        <v>6546794</v>
       </c>
       <c r="E376" t="inlineStr">
         <is>
@@ -18430,10 +18430,10 @@
         </is>
       </c>
       <c r="C377" t="n">
-        <v>4279</v>
+        <v>4293</v>
       </c>
       <c r="D377" t="n">
-        <v>6238536</v>
+        <v>6259276</v>
       </c>
       <c r="E377" t="inlineStr">
         <is>
@@ -18478,10 +18478,10 @@
         </is>
       </c>
       <c r="C378" t="n">
-        <v>12575</v>
+        <v>12596</v>
       </c>
       <c r="D378" t="n">
-        <v>18525957</v>
+        <v>18556757</v>
       </c>
       <c r="E378" t="inlineStr">
         <is>
@@ -18526,10 +18526,10 @@
         </is>
       </c>
       <c r="C379" t="n">
-        <v>5267</v>
+        <v>5278</v>
       </c>
       <c r="D379" t="n">
-        <v>7852744</v>
+        <v>7868529</v>
       </c>
       <c r="E379" t="inlineStr">
         <is>
@@ -18574,10 +18574,10 @@
         </is>
       </c>
       <c r="C380" t="n">
-        <v>1510</v>
+        <v>1513</v>
       </c>
       <c r="D380" t="n">
-        <v>2254742</v>
+        <v>2259242</v>
       </c>
       <c r="E380" t="inlineStr">
         <is>
@@ -18622,10 +18622,10 @@
         </is>
       </c>
       <c r="C381" t="n">
-        <v>349</v>
+        <v>353</v>
       </c>
       <c r="D381" t="n">
-        <v>520606</v>
+        <v>526606</v>
       </c>
       <c r="E381" t="inlineStr">
         <is>
@@ -18718,10 +18718,10 @@
         </is>
       </c>
       <c r="C383" t="n">
-        <v>4410</v>
+        <v>4414</v>
       </c>
       <c r="D383" t="n">
-        <v>6060733</v>
+        <v>6064408</v>
       </c>
       <c r="E383" t="inlineStr">
         <is>
@@ -18814,10 +18814,10 @@
         </is>
       </c>
       <c r="C385" t="n">
-        <v>10524</v>
+        <v>10540</v>
       </c>
       <c r="D385" t="n">
-        <v>15530123</v>
+        <v>15554123</v>
       </c>
       <c r="E385" t="inlineStr">
         <is>
@@ -18862,10 +18862,10 @@
         </is>
       </c>
       <c r="C386" t="n">
-        <v>4488</v>
+        <v>4497</v>
       </c>
       <c r="D386" t="n">
-        <v>6675272</v>
+        <v>6688772</v>
       </c>
       <c r="E386" t="inlineStr">
         <is>
@@ -18910,10 +18910,10 @@
         </is>
       </c>
       <c r="C387" t="n">
-        <v>1278</v>
+        <v>1279</v>
       </c>
       <c r="D387" t="n">
-        <v>1908116</v>
+        <v>1909616</v>
       </c>
       <c r="E387" t="inlineStr">
         <is>
@@ -19054,10 +19054,10 @@
         </is>
       </c>
       <c r="C390" t="n">
-        <v>3469</v>
+        <v>3473</v>
       </c>
       <c r="D390" t="n">
-        <v>4711422</v>
+        <v>4714324</v>
       </c>
       <c r="E390" t="inlineStr">
         <is>
@@ -19102,10 +19102,10 @@
         </is>
       </c>
       <c r="C391" t="n">
-        <v>3791</v>
+        <v>3792</v>
       </c>
       <c r="D391" t="n">
-        <v>5529840</v>
+        <v>5531340</v>
       </c>
       <c r="E391" t="inlineStr">
         <is>
@@ -19150,10 +19150,10 @@
         </is>
       </c>
       <c r="C392" t="n">
-        <v>10417</v>
+        <v>10433</v>
       </c>
       <c r="D392" t="n">
-        <v>15356336</v>
+        <v>15380336</v>
       </c>
       <c r="E392" t="inlineStr">
         <is>
@@ -19198,10 +19198,10 @@
         </is>
       </c>
       <c r="C393" t="n">
-        <v>4026</v>
+        <v>4029</v>
       </c>
       <c r="D393" t="n">
-        <v>5992762</v>
+        <v>5997262</v>
       </c>
       <c r="E393" t="inlineStr">
         <is>
@@ -19294,10 +19294,10 @@
         </is>
       </c>
       <c r="C395" t="n">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="D395" t="n">
-        <v>375560</v>
+        <v>377060</v>
       </c>
       <c r="E395" t="inlineStr">
         <is>
@@ -19390,10 +19390,10 @@
         </is>
       </c>
       <c r="C397" t="n">
-        <v>3788</v>
+        <v>3790</v>
       </c>
       <c r="D397" t="n">
-        <v>5208068</v>
+        <v>5211068</v>
       </c>
       <c r="E397" t="inlineStr">
         <is>
@@ -19438,10 +19438,10 @@
         </is>
       </c>
       <c r="C398" t="n">
-        <v>4073</v>
+        <v>4077</v>
       </c>
       <c r="D398" t="n">
-        <v>5908860</v>
+        <v>5913759</v>
       </c>
       <c r="E398" t="inlineStr">
         <is>
@@ -19486,10 +19486,10 @@
         </is>
       </c>
       <c r="C399" t="n">
-        <v>10560</v>
+        <v>10570</v>
       </c>
       <c r="D399" t="n">
-        <v>15522740</v>
+        <v>15537460</v>
       </c>
       <c r="E399" t="inlineStr">
         <is>
@@ -19534,10 +19534,10 @@
         </is>
       </c>
       <c r="C400" t="n">
-        <v>3616</v>
+        <v>3622</v>
       </c>
       <c r="D400" t="n">
-        <v>5391196</v>
+        <v>5399081</v>
       </c>
       <c r="E400" t="inlineStr">
         <is>
@@ -19582,10 +19582,10 @@
         </is>
       </c>
       <c r="C401" t="n">
-        <v>1255</v>
+        <v>1261</v>
       </c>
       <c r="D401" t="n">
-        <v>1877091</v>
+        <v>1886091</v>
       </c>
       <c r="E401" t="inlineStr">
         <is>
@@ -19630,10 +19630,10 @@
         </is>
       </c>
       <c r="C402" t="n">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="D402" t="n">
-        <v>382112</v>
+        <v>383612</v>
       </c>
       <c r="E402" t="inlineStr">
         <is>
@@ -19774,10 +19774,10 @@
         </is>
       </c>
       <c r="C405" t="n">
-        <v>4736</v>
+        <v>4742</v>
       </c>
       <c r="D405" t="n">
-        <v>6389537</v>
+        <v>6398037</v>
       </c>
       <c r="E405" t="inlineStr">
         <is>
@@ -19822,10 +19822,10 @@
         </is>
       </c>
       <c r="C406" t="n">
-        <v>1376</v>
+        <v>1378</v>
       </c>
       <c r="D406" t="n">
-        <v>1988490</v>
+        <v>1991490</v>
       </c>
       <c r="E406" t="inlineStr">
         <is>
@@ -19870,10 +19870,10 @@
         </is>
       </c>
       <c r="C407" t="n">
-        <v>4568</v>
+        <v>4571</v>
       </c>
       <c r="D407" t="n">
-        <v>6731495</v>
+        <v>6735995</v>
       </c>
       <c r="E407" t="inlineStr">
         <is>
@@ -19918,10 +19918,10 @@
         </is>
       </c>
       <c r="C408" t="n">
-        <v>1772</v>
+        <v>1775</v>
       </c>
       <c r="D408" t="n">
-        <v>2642616</v>
+        <v>2647116</v>
       </c>
       <c r="E408" t="inlineStr">
         <is>
@@ -19966,10 +19966,10 @@
         </is>
       </c>
       <c r="C409" t="n">
-        <v>619</v>
+        <v>622</v>
       </c>
       <c r="D409" t="n">
-        <v>927641</v>
+        <v>932141</v>
       </c>
       <c r="E409" t="inlineStr">
         <is>
@@ -20158,10 +20158,10 @@
         </is>
       </c>
       <c r="C413" t="n">
-        <v>3021</v>
+        <v>3028</v>
       </c>
       <c r="D413" t="n">
-        <v>4010297</v>
+        <v>4020458</v>
       </c>
       <c r="E413" t="inlineStr">
         <is>
@@ -20254,10 +20254,10 @@
         </is>
       </c>
       <c r="C415" t="n">
-        <v>261</v>
+        <v>263</v>
       </c>
       <c r="D415" t="n">
-        <v>389765</v>
+        <v>392765</v>
       </c>
       <c r="E415" t="inlineStr">
         <is>
@@ -20302,10 +20302,10 @@
         </is>
       </c>
       <c r="C416" t="n">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="D416" t="n">
-        <v>135000</v>
+        <v>138000</v>
       </c>
       <c r="E416" t="inlineStr">
         <is>
@@ -20446,10 +20446,10 @@
         </is>
       </c>
       <c r="C419" t="n">
-        <v>2876</v>
+        <v>2880</v>
       </c>
       <c r="D419" t="n">
-        <v>4177184</v>
+        <v>4183184</v>
       </c>
       <c r="E419" t="inlineStr">
         <is>
@@ -20494,10 +20494,10 @@
         </is>
       </c>
       <c r="C420" t="n">
-        <v>6970</v>
+        <v>6975</v>
       </c>
       <c r="D420" t="n">
-        <v>10236232</v>
+        <v>10243732</v>
       </c>
       <c r="E420" t="inlineStr">
         <is>
@@ -20542,10 +20542,10 @@
         </is>
       </c>
       <c r="C421" t="n">
-        <v>2302</v>
+        <v>2303</v>
       </c>
       <c r="D421" t="n">
-        <v>3430795</v>
+        <v>3432295</v>
       </c>
       <c r="E421" t="inlineStr">
         <is>
@@ -20590,10 +20590,10 @@
         </is>
       </c>
       <c r="C422" t="n">
-        <v>672</v>
+        <v>673</v>
       </c>
       <c r="D422" t="n">
-        <v>1003142</v>
+        <v>1004642</v>
       </c>
       <c r="E422" t="inlineStr">
         <is>
@@ -20734,10 +20734,10 @@
         </is>
       </c>
       <c r="C425" t="n">
-        <v>2237</v>
+        <v>2238</v>
       </c>
       <c r="D425" t="n">
-        <v>2990632</v>
+        <v>2992132</v>
       </c>
       <c r="E425" t="inlineStr">
         <is>
@@ -20782,10 +20782,10 @@
         </is>
       </c>
       <c r="C426" t="n">
-        <v>1614</v>
+        <v>1616</v>
       </c>
       <c r="D426" t="n">
-        <v>2345314</v>
+        <v>2348314</v>
       </c>
       <c r="E426" t="inlineStr">
         <is>
@@ -20830,10 +20830,10 @@
         </is>
       </c>
       <c r="C427" t="n">
-        <v>4691</v>
+        <v>4692</v>
       </c>
       <c r="D427" t="n">
-        <v>6886253</v>
+        <v>6887160</v>
       </c>
       <c r="E427" t="inlineStr">
         <is>
@@ -21070,10 +21070,10 @@
         </is>
       </c>
       <c r="C432" t="n">
-        <v>1583</v>
+        <v>1585</v>
       </c>
       <c r="D432" t="n">
-        <v>2084116</v>
+        <v>2087116</v>
       </c>
       <c r="E432" t="inlineStr">
         <is>
@@ -21118,10 +21118,10 @@
         </is>
       </c>
       <c r="C433" t="n">
-        <v>1819</v>
+        <v>1820</v>
       </c>
       <c r="D433" t="n">
-        <v>2637479</v>
+        <v>2637850</v>
       </c>
       <c r="E433" t="inlineStr">
         <is>
@@ -21166,10 +21166,10 @@
         </is>
       </c>
       <c r="C434" t="n">
-        <v>4607</v>
+        <v>4610</v>
       </c>
       <c r="D434" t="n">
-        <v>6773691</v>
+        <v>6778191</v>
       </c>
       <c r="E434" t="inlineStr">
         <is>
@@ -21214,10 +21214,10 @@
         </is>
       </c>
       <c r="C435" t="n">
-        <v>1467</v>
+        <v>1468</v>
       </c>
       <c r="D435" t="n">
-        <v>2176161</v>
+        <v>2177661</v>
       </c>
       <c r="E435" t="inlineStr">
         <is>
@@ -21262,10 +21262,10 @@
         </is>
       </c>
       <c r="C436" t="n">
-        <v>399</v>
+        <v>400</v>
       </c>
       <c r="D436" t="n">
-        <v>593663</v>
+        <v>595163</v>
       </c>
       <c r="E436" t="inlineStr">
         <is>
@@ -21454,10 +21454,10 @@
         </is>
       </c>
       <c r="C440" t="n">
-        <v>2529</v>
+        <v>2532</v>
       </c>
       <c r="D440" t="n">
-        <v>3713457</v>
+        <v>3717957</v>
       </c>
       <c r="E440" t="inlineStr">
         <is>
@@ -21694,10 +21694,10 @@
         </is>
       </c>
       <c r="C445" t="n">
-        <v>2836</v>
+        <v>2838</v>
       </c>
       <c r="D445" t="n">
-        <v>4126927</v>
+        <v>4129927</v>
       </c>
       <c r="E445" t="inlineStr">
         <is>
@@ -21742,10 +21742,10 @@
         </is>
       </c>
       <c r="C446" t="n">
-        <v>8897</v>
+        <v>8909</v>
       </c>
       <c r="D446" t="n">
-        <v>13108445</v>
+        <v>13126328</v>
       </c>
       <c r="E446" t="inlineStr">
         <is>
@@ -21790,10 +21790,10 @@
         </is>
       </c>
       <c r="C447" t="n">
-        <v>3237</v>
+        <v>3241</v>
       </c>
       <c r="D447" t="n">
-        <v>4812008</v>
+        <v>4818008</v>
       </c>
       <c r="E447" t="inlineStr">
         <is>
@@ -21982,10 +21982,10 @@
         </is>
       </c>
       <c r="C451" t="n">
-        <v>2786</v>
+        <v>2789</v>
       </c>
       <c r="D451" t="n">
-        <v>3657044</v>
+        <v>3661544</v>
       </c>
       <c r="E451" t="inlineStr">
         <is>
@@ -22078,10 +22078,10 @@
         </is>
       </c>
       <c r="C453" t="n">
-        <v>3083</v>
+        <v>3089</v>
       </c>
       <c r="D453" t="n">
-        <v>4513715</v>
+        <v>4521546</v>
       </c>
       <c r="E453" t="inlineStr">
         <is>
@@ -22174,10 +22174,10 @@
         </is>
       </c>
       <c r="C455" t="n">
-        <v>298</v>
+        <v>299</v>
       </c>
       <c r="D455" t="n">
-        <v>444911</v>
+        <v>446411</v>
       </c>
       <c r="E455" t="inlineStr">
         <is>
@@ -22318,10 +22318,10 @@
         </is>
       </c>
       <c r="C458" t="n">
-        <v>1277</v>
+        <v>1278</v>
       </c>
       <c r="D458" t="n">
-        <v>1633932</v>
+        <v>1634612</v>
       </c>
       <c r="E458" t="inlineStr">
         <is>
@@ -22366,10 +22366,10 @@
         </is>
       </c>
       <c r="C459" t="n">
-        <v>4113</v>
+        <v>4115</v>
       </c>
       <c r="D459" t="n">
-        <v>5965873</v>
+        <v>5967513</v>
       </c>
       <c r="E459" t="inlineStr">
         <is>
@@ -22414,10 +22414,10 @@
         </is>
       </c>
       <c r="C460" t="n">
-        <v>7854</v>
+        <v>7858</v>
       </c>
       <c r="D460" t="n">
-        <v>11531162</v>
+        <v>11534822</v>
       </c>
       <c r="E460" t="inlineStr">
         <is>
@@ -22510,10 +22510,10 @@
         </is>
       </c>
       <c r="C462" t="n">
-        <v>574</v>
+        <v>575</v>
       </c>
       <c r="D462" t="n">
-        <v>855155</v>
+        <v>856655</v>
       </c>
       <c r="E462" t="inlineStr">
         <is>
@@ -22654,10 +22654,10 @@
         </is>
       </c>
       <c r="C465" t="n">
-        <v>2599</v>
+        <v>2600</v>
       </c>
       <c r="D465" t="n">
-        <v>3481390</v>
+        <v>3482890</v>
       </c>
       <c r="E465" t="inlineStr">
         <is>
@@ -22702,10 +22702,10 @@
         </is>
       </c>
       <c r="C466" t="n">
-        <v>984</v>
+        <v>986</v>
       </c>
       <c r="D466" t="n">
-        <v>1421317</v>
+        <v>1424317</v>
       </c>
       <c r="E466" t="inlineStr">
         <is>
@@ -22750,10 +22750,10 @@
         </is>
       </c>
       <c r="C467" t="n">
-        <v>2491</v>
+        <v>2494</v>
       </c>
       <c r="D467" t="n">
-        <v>3645714</v>
+        <v>3650214</v>
       </c>
       <c r="E467" t="inlineStr">
         <is>
@@ -22798,10 +22798,10 @@
         </is>
       </c>
       <c r="C468" t="n">
-        <v>745</v>
+        <v>746</v>
       </c>
       <c r="D468" t="n">
-        <v>1105755</v>
+        <v>1106257</v>
       </c>
       <c r="E468" t="inlineStr">
         <is>
@@ -22942,10 +22942,10 @@
         </is>
       </c>
       <c r="C471" t="n">
-        <v>1267</v>
+        <v>1271</v>
       </c>
       <c r="D471" t="n">
-        <v>1694594</v>
+        <v>1699297</v>
       </c>
       <c r="E471" t="inlineStr">
         <is>
@@ -23038,10 +23038,10 @@
         </is>
       </c>
       <c r="C473" t="n">
-        <v>1005</v>
+        <v>1008</v>
       </c>
       <c r="D473" t="n">
-        <v>1449489</v>
+        <v>1453989</v>
       </c>
       <c r="E473" t="inlineStr">
         <is>
@@ -23230,10 +23230,10 @@
         </is>
       </c>
       <c r="C477" t="n">
-        <v>554</v>
+        <v>555</v>
       </c>
       <c r="D477" t="n">
-        <v>717074</v>
+        <v>718574</v>
       </c>
       <c r="E477" t="inlineStr">
         <is>
@@ -23326,10 +23326,10 @@
         </is>
       </c>
       <c r="C479" t="n">
-        <v>2727</v>
+        <v>2729</v>
       </c>
       <c r="D479" t="n">
-        <v>4019945</v>
+        <v>4022945</v>
       </c>
       <c r="E479" t="inlineStr">
         <is>
@@ -23518,10 +23518,10 @@
         </is>
       </c>
       <c r="C483" t="n">
-        <v>939</v>
+        <v>940</v>
       </c>
       <c r="D483" t="n">
-        <v>1288819</v>
+        <v>1290319</v>
       </c>
       <c r="E483" t="inlineStr">
         <is>
@@ -23566,10 +23566,10 @@
         </is>
       </c>
       <c r="C484" t="n">
-        <v>2546</v>
+        <v>2550</v>
       </c>
       <c r="D484" t="n">
-        <v>3649969</v>
+        <v>3655969</v>
       </c>
       <c r="E484" t="inlineStr">
         <is>
@@ -23614,10 +23614,10 @@
         </is>
       </c>
       <c r="C485" t="n">
-        <v>5018</v>
+        <v>5022</v>
       </c>
       <c r="D485" t="n">
-        <v>7353845</v>
+        <v>7358865</v>
       </c>
       <c r="E485" t="inlineStr">
         <is>
@@ -23662,10 +23662,10 @@
         </is>
       </c>
       <c r="C486" t="n">
-        <v>1428</v>
+        <v>1429</v>
       </c>
       <c r="D486" t="n">
-        <v>2119741</v>
+        <v>2121241</v>
       </c>
       <c r="E486" t="inlineStr">
         <is>
@@ -23854,10 +23854,10 @@
         </is>
       </c>
       <c r="C490" t="n">
-        <v>2234</v>
+        <v>2236</v>
       </c>
       <c r="D490" t="n">
-        <v>2934875</v>
+        <v>2937106</v>
       </c>
       <c r="E490" t="inlineStr">
         <is>
@@ -23902,10 +23902,10 @@
         </is>
       </c>
       <c r="C491" t="n">
-        <v>8193</v>
+        <v>8198</v>
       </c>
       <c r="D491" t="n">
-        <v>11880048</v>
+        <v>11886781</v>
       </c>
       <c r="E491" t="inlineStr">
         <is>
@@ -23950,10 +23950,10 @@
         </is>
       </c>
       <c r="C492" t="n">
-        <v>17293</v>
+        <v>17301</v>
       </c>
       <c r="D492" t="n">
-        <v>25340041</v>
+        <v>25350484</v>
       </c>
       <c r="E492" t="inlineStr">
         <is>
@@ -23998,10 +23998,10 @@
         </is>
       </c>
       <c r="C493" t="n">
-        <v>5901</v>
+        <v>5907</v>
       </c>
       <c r="D493" t="n">
-        <v>8783861</v>
+        <v>8792861</v>
       </c>
       <c r="E493" t="inlineStr">
         <is>
@@ -24094,10 +24094,10 @@
         </is>
       </c>
       <c r="C495" t="n">
-        <v>357</v>
+        <v>358</v>
       </c>
       <c r="D495" t="n">
-        <v>535115</v>
+        <v>536615</v>
       </c>
       <c r="E495" t="inlineStr">
         <is>
@@ -24286,10 +24286,10 @@
         </is>
       </c>
       <c r="C499" t="n">
-        <v>6176</v>
+        <v>6182</v>
       </c>
       <c r="D499" t="n">
-        <v>8390284</v>
+        <v>8399044</v>
       </c>
       <c r="E499" t="inlineStr">
         <is>
@@ -24334,10 +24334,10 @@
         </is>
       </c>
       <c r="C500" t="n">
-        <v>1212</v>
+        <v>1214</v>
       </c>
       <c r="D500" t="n">
-        <v>1746256</v>
+        <v>1749256</v>
       </c>
       <c r="E500" t="inlineStr">
         <is>
@@ -24430,10 +24430,10 @@
         </is>
       </c>
       <c r="C502" t="n">
-        <v>1004</v>
+        <v>1006</v>
       </c>
       <c r="D502" t="n">
-        <v>1495241</v>
+        <v>1498241</v>
       </c>
       <c r="E502" t="inlineStr">
         <is>
@@ -24478,10 +24478,10 @@
         </is>
       </c>
       <c r="C503" t="n">
-        <v>329</v>
+        <v>330</v>
       </c>
       <c r="D503" t="n">
-        <v>490432</v>
+        <v>491932</v>
       </c>
       <c r="E503" t="inlineStr">
         <is>
@@ -24622,10 +24622,10 @@
         </is>
       </c>
       <c r="C506" t="n">
-        <v>1472</v>
+        <v>1473</v>
       </c>
       <c r="D506" t="n">
-        <v>1952892</v>
+        <v>1954392</v>
       </c>
       <c r="E506" t="inlineStr">
         <is>
@@ -24670,10 +24670,10 @@
         </is>
       </c>
       <c r="C507" t="n">
-        <v>2707</v>
+        <v>2708</v>
       </c>
       <c r="D507" t="n">
-        <v>3890233</v>
+        <v>3891139</v>
       </c>
       <c r="E507" t="inlineStr">
         <is>
@@ -24718,10 +24718,10 @@
         </is>
       </c>
       <c r="C508" t="n">
-        <v>4713</v>
+        <v>4716</v>
       </c>
       <c r="D508" t="n">
-        <v>6902103</v>
+        <v>6906603</v>
       </c>
       <c r="E508" t="inlineStr">
         <is>
@@ -24814,10 +24814,10 @@
         </is>
       </c>
       <c r="C510" t="n">
-        <v>365</v>
+        <v>366</v>
       </c>
       <c r="D510" t="n">
-        <v>544628</v>
+        <v>545373</v>
       </c>
       <c r="E510" t="inlineStr">
         <is>
@@ -24958,10 +24958,10 @@
         </is>
       </c>
       <c r="C513" t="n">
-        <v>1508</v>
+        <v>1512</v>
       </c>
       <c r="D513" t="n">
-        <v>2003257</v>
+        <v>2008357</v>
       </c>
       <c r="E513" t="inlineStr">
         <is>
@@ -25006,10 +25006,10 @@
         </is>
       </c>
       <c r="C514" t="n">
-        <v>1495</v>
+        <v>1497</v>
       </c>
       <c r="D514" t="n">
-        <v>2156168</v>
+        <v>2159168</v>
       </c>
       <c r="E514" t="inlineStr">
         <is>
@@ -25054,10 +25054,10 @@
         </is>
       </c>
       <c r="C515" t="n">
-        <v>3256</v>
+        <v>3258</v>
       </c>
       <c r="D515" t="n">
-        <v>4761378</v>
+        <v>4764378</v>
       </c>
       <c r="E515" t="inlineStr">
         <is>
@@ -25246,10 +25246,10 @@
         </is>
       </c>
       <c r="C519" t="n">
-        <v>1380</v>
+        <v>1382</v>
       </c>
       <c r="D519" t="n">
-        <v>1869166</v>
+        <v>1872166</v>
       </c>
       <c r="E519" t="inlineStr">
         <is>
@@ -25294,10 +25294,10 @@
         </is>
       </c>
       <c r="C520" t="n">
-        <v>3469</v>
+        <v>3471</v>
       </c>
       <c r="D520" t="n">
-        <v>4992294</v>
+        <v>4994334</v>
       </c>
       <c r="E520" t="inlineStr">
         <is>
@@ -25342,10 +25342,10 @@
         </is>
       </c>
       <c r="C521" t="n">
-        <v>8693</v>
+        <v>8699</v>
       </c>
       <c r="D521" t="n">
-        <v>12714592</v>
+        <v>12723592</v>
       </c>
       <c r="E521" t="inlineStr">
         <is>
@@ -25390,10 +25390,10 @@
         </is>
       </c>
       <c r="C522" t="n">
-        <v>2924</v>
+        <v>2927</v>
       </c>
       <c r="D522" t="n">
-        <v>4342240</v>
+        <v>4346740</v>
       </c>
       <c r="E522" t="inlineStr">
         <is>
@@ -25678,10 +25678,10 @@
         </is>
       </c>
       <c r="C528" t="n">
-        <v>1082</v>
+        <v>1085</v>
       </c>
       <c r="D528" t="n">
-        <v>1553097</v>
+        <v>1557597</v>
       </c>
       <c r="E528" t="inlineStr">
         <is>
@@ -25726,10 +25726,10 @@
         </is>
       </c>
       <c r="C529" t="n">
-        <v>3203</v>
+        <v>3207</v>
       </c>
       <c r="D529" t="n">
-        <v>4683196</v>
+        <v>4689196</v>
       </c>
       <c r="E529" t="inlineStr">
         <is>
@@ -25774,10 +25774,10 @@
         </is>
       </c>
       <c r="C530" t="n">
-        <v>1073</v>
+        <v>1074</v>
       </c>
       <c r="D530" t="n">
-        <v>1596578</v>
+        <v>1598078</v>
       </c>
       <c r="E530" t="inlineStr">
         <is>
@@ -25966,10 +25966,10 @@
         </is>
       </c>
       <c r="C534" t="n">
-        <v>1162</v>
+        <v>1164</v>
       </c>
       <c r="D534" t="n">
-        <v>1567948</v>
+        <v>1569838</v>
       </c>
       <c r="E534" t="inlineStr">
         <is>
@@ -26014,10 +26014,10 @@
         </is>
       </c>
       <c r="C535" t="n">
-        <v>465</v>
+        <v>468</v>
       </c>
       <c r="D535" t="n">
-        <v>667918</v>
+        <v>669467</v>
       </c>
       <c r="E535" t="inlineStr">
         <is>
@@ -26062,10 +26062,10 @@
         </is>
       </c>
       <c r="C536" t="n">
-        <v>1668</v>
+        <v>1671</v>
       </c>
       <c r="D536" t="n">
-        <v>2432647</v>
+        <v>2437147</v>
       </c>
       <c r="E536" t="inlineStr">
         <is>
@@ -26302,10 +26302,10 @@
         </is>
       </c>
       <c r="C541" t="n">
-        <v>797</v>
+        <v>799</v>
       </c>
       <c r="D541" t="n">
-        <v>1007713</v>
+        <v>1009658</v>
       </c>
       <c r="E541" t="inlineStr">
         <is>
@@ -26350,10 +26350,10 @@
         </is>
       </c>
       <c r="C542" t="n">
-        <v>2570</v>
+        <v>2572</v>
       </c>
       <c r="D542" t="n">
-        <v>3693025</v>
+        <v>3694837</v>
       </c>
       <c r="E542" t="inlineStr">
         <is>
@@ -26398,10 +26398,10 @@
         </is>
       </c>
       <c r="C543" t="n">
-        <v>4728</v>
+        <v>4734</v>
       </c>
       <c r="D543" t="n">
-        <v>6926112</v>
+        <v>6933930</v>
       </c>
       <c r="E543" t="inlineStr">
         <is>
@@ -26446,10 +26446,10 @@
         </is>
       </c>
       <c r="C544" t="n">
-        <v>1450</v>
+        <v>1451</v>
       </c>
       <c r="D544" t="n">
-        <v>2157609</v>
+        <v>2159109</v>
       </c>
       <c r="E544" t="inlineStr">
         <is>
@@ -26494,10 +26494,10 @@
         </is>
       </c>
       <c r="C545" t="n">
-        <v>394</v>
+        <v>396</v>
       </c>
       <c r="D545" t="n">
-        <v>584278</v>
+        <v>587278</v>
       </c>
       <c r="E545" t="inlineStr">
         <is>
@@ -26638,10 +26638,10 @@
         </is>
       </c>
       <c r="C548" t="n">
-        <v>1716</v>
+        <v>1717</v>
       </c>
       <c r="D548" t="n">
-        <v>2263075</v>
+        <v>2264575</v>
       </c>
       <c r="E548" t="inlineStr">
         <is>
@@ -26686,10 +26686,10 @@
         </is>
       </c>
       <c r="C549" t="n">
-        <v>1628</v>
+        <v>1629</v>
       </c>
       <c r="D549" t="n">
-        <v>2333259</v>
+        <v>2334759</v>
       </c>
       <c r="E549" t="inlineStr">
         <is>
@@ -26734,10 +26734,10 @@
         </is>
       </c>
       <c r="C550" t="n">
-        <v>3446</v>
+        <v>3447</v>
       </c>
       <c r="D550" t="n">
-        <v>5044344</v>
+        <v>5045844</v>
       </c>
       <c r="E550" t="inlineStr">
         <is>
@@ -26974,10 +26974,10 @@
         </is>
       </c>
       <c r="C555" t="n">
-        <v>1843</v>
+        <v>1844</v>
       </c>
       <c r="D555" t="n">
-        <v>2463219</v>
+        <v>2464719</v>
       </c>
       <c r="E555" t="inlineStr">
         <is>
@@ -27022,10 +27022,10 @@
         </is>
       </c>
       <c r="C556" t="n">
-        <v>4085</v>
+        <v>4086</v>
       </c>
       <c r="D556" t="n">
-        <v>5920387</v>
+        <v>5921887</v>
       </c>
       <c r="E556" t="inlineStr">
         <is>
@@ -27070,10 +27070,10 @@
         </is>
       </c>
       <c r="C557" t="n">
-        <v>9666</v>
+        <v>9675</v>
       </c>
       <c r="D557" t="n">
-        <v>14143654</v>
+        <v>14156142</v>
       </c>
       <c r="E557" t="inlineStr">
         <is>
@@ -27214,10 +27214,10 @@
         </is>
       </c>
       <c r="C560" t="n">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="D560" t="n">
-        <v>150740</v>
+        <v>152240</v>
       </c>
       <c r="E560" t="inlineStr">
         <is>
@@ -27262,10 +27262,10 @@
         </is>
       </c>
       <c r="C561" t="n">
-        <v>3739</v>
+        <v>3740</v>
       </c>
       <c r="D561" t="n">
-        <v>4982011</v>
+        <v>4983511</v>
       </c>
       <c r="E561" t="inlineStr">
         <is>
@@ -27358,10 +27358,10 @@
         </is>
       </c>
       <c r="C563" t="n">
-        <v>2125</v>
+        <v>2129</v>
       </c>
       <c r="D563" t="n">
-        <v>3101533</v>
+        <v>3107533</v>
       </c>
       <c r="E563" t="inlineStr">
         <is>
@@ -27406,10 +27406,10 @@
         </is>
       </c>
       <c r="C564" t="n">
-        <v>646</v>
+        <v>648</v>
       </c>
       <c r="D564" t="n">
-        <v>950513</v>
+        <v>953513</v>
       </c>
       <c r="E564" t="inlineStr">
         <is>
@@ -27598,10 +27598,10 @@
         </is>
       </c>
       <c r="C568" t="n">
-        <v>5770</v>
+        <v>5774</v>
       </c>
       <c r="D568" t="n">
-        <v>8346321</v>
+        <v>8351438</v>
       </c>
       <c r="E568" t="inlineStr">
         <is>
@@ -27646,10 +27646,10 @@
         </is>
       </c>
       <c r="C569" t="n">
-        <v>14028</v>
+        <v>14039</v>
       </c>
       <c r="D569" t="n">
-        <v>20583068</v>
+        <v>20598818</v>
       </c>
       <c r="E569" t="inlineStr">
         <is>
@@ -27694,10 +27694,10 @@
         </is>
       </c>
       <c r="C570" t="n">
-        <v>4970</v>
+        <v>4971</v>
       </c>
       <c r="D570" t="n">
-        <v>7385973</v>
+        <v>7387473</v>
       </c>
       <c r="E570" t="inlineStr">
         <is>
@@ -27742,10 +27742,10 @@
         </is>
       </c>
       <c r="C571" t="n">
-        <v>1506</v>
+        <v>1507</v>
       </c>
       <c r="D571" t="n">
-        <v>2245328</v>
+        <v>2246828</v>
       </c>
       <c r="E571" t="inlineStr">
         <is>
@@ -27790,10 +27790,10 @@
         </is>
       </c>
       <c r="C572" t="n">
-        <v>280</v>
+        <v>283</v>
       </c>
       <c r="D572" t="n">
-        <v>418585</v>
+        <v>423085</v>
       </c>
       <c r="E572" t="inlineStr">
         <is>
@@ -27934,10 +27934,10 @@
         </is>
       </c>
       <c r="C575" t="n">
-        <v>5641</v>
+        <v>5646</v>
       </c>
       <c r="D575" t="n">
-        <v>7561706</v>
+        <v>7568845</v>
       </c>
       <c r="E575" t="inlineStr">
         <is>
@@ -28030,10 +28030,10 @@
         </is>
       </c>
       <c r="C577" t="n">
-        <v>2971</v>
+        <v>2976</v>
       </c>
       <c r="D577" t="n">
-        <v>4314292</v>
+        <v>4321792</v>
       </c>
       <c r="E577" t="inlineStr">
         <is>
@@ -28078,10 +28078,10 @@
         </is>
       </c>
       <c r="C578" t="n">
-        <v>980</v>
+        <v>981</v>
       </c>
       <c r="D578" t="n">
-        <v>1452080</v>
+        <v>1453580</v>
       </c>
       <c r="E578" t="inlineStr">
         <is>
@@ -28270,10 +28270,10 @@
         </is>
       </c>
       <c r="C582" t="n">
-        <v>7940</v>
+        <v>7945</v>
       </c>
       <c r="D582" t="n">
-        <v>11516554</v>
+        <v>11524054</v>
       </c>
       <c r="E582" t="inlineStr">
         <is>
@@ -28318,10 +28318,10 @@
         </is>
       </c>
       <c r="C583" t="n">
-        <v>17043</v>
+        <v>17059</v>
       </c>
       <c r="D583" t="n">
-        <v>24995563</v>
+        <v>25019563</v>
       </c>
       <c r="E583" t="inlineStr">
         <is>
@@ -28366,10 +28366,10 @@
         </is>
       </c>
       <c r="C584" t="n">
-        <v>5195</v>
+        <v>5198</v>
       </c>
       <c r="D584" t="n">
-        <v>7726982</v>
+        <v>7731482</v>
       </c>
       <c r="E584" t="inlineStr">
         <is>
@@ -28462,10 +28462,10 @@
         </is>
       </c>
       <c r="C586" t="n">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="D586" t="n">
-        <v>352043</v>
+        <v>353543</v>
       </c>
       <c r="E586" t="inlineStr">
         <is>
@@ -28558,10 +28558,10 @@
         </is>
       </c>
       <c r="C588" t="n">
-        <v>5577</v>
+        <v>5582</v>
       </c>
       <c r="D588" t="n">
-        <v>7478066</v>
+        <v>7485566</v>
       </c>
       <c r="E588" t="inlineStr">
         <is>
@@ -28606,10 +28606,10 @@
         </is>
       </c>
       <c r="C589" t="n">
-        <v>1190</v>
+        <v>1192</v>
       </c>
       <c r="D589" t="n">
-        <v>1716528</v>
+        <v>1718441</v>
       </c>
       <c r="E589" t="inlineStr">
         <is>
@@ -28894,10 +28894,10 @@
         </is>
       </c>
       <c r="C595" t="n">
-        <v>1135</v>
+        <v>1137</v>
       </c>
       <c r="D595" t="n">
-        <v>1498572</v>
+        <v>1500384</v>
       </c>
       <c r="E595" t="inlineStr">
         <is>
@@ -28990,10 +28990,10 @@
         </is>
       </c>
       <c r="C597" t="n">
-        <v>995</v>
+        <v>997</v>
       </c>
       <c r="D597" t="n">
-        <v>1441555</v>
+        <v>1443215</v>
       </c>
       <c r="E597" t="inlineStr">
         <is>
@@ -29182,10 +29182,10 @@
         </is>
       </c>
       <c r="C601" t="n">
-        <v>618</v>
+        <v>625</v>
       </c>
       <c r="D601" t="n">
-        <v>852611</v>
+        <v>863111</v>
       </c>
       <c r="E601" t="inlineStr">
         <is>
@@ -29230,10 +29230,10 @@
         </is>
       </c>
       <c r="C602" t="n">
-        <v>3694</v>
+        <v>3698</v>
       </c>
       <c r="D602" t="n">
-        <v>5360714</v>
+        <v>5366214</v>
       </c>
       <c r="E602" t="inlineStr">
         <is>
@@ -29278,10 +29278,10 @@
         </is>
       </c>
       <c r="C603" t="n">
-        <v>6263</v>
+        <v>6267</v>
       </c>
       <c r="D603" t="n">
-        <v>9123613</v>
+        <v>9128533</v>
       </c>
       <c r="E603" t="inlineStr">
         <is>
@@ -29326,10 +29326,10 @@
         </is>
       </c>
       <c r="C604" t="n">
-        <v>1949</v>
+        <v>1950</v>
       </c>
       <c r="D604" t="n">
-        <v>2898850</v>
+        <v>2900350</v>
       </c>
       <c r="E604" t="inlineStr">
         <is>
@@ -29374,10 +29374,10 @@
         </is>
       </c>
       <c r="C605" t="n">
-        <v>531</v>
+        <v>532</v>
       </c>
       <c r="D605" t="n">
-        <v>790092</v>
+        <v>791592</v>
       </c>
       <c r="E605" t="inlineStr">
         <is>
@@ -29518,10 +29518,10 @@
         </is>
       </c>
       <c r="C608" t="n">
-        <v>2408</v>
+        <v>2409</v>
       </c>
       <c r="D608" t="n">
-        <v>3210007</v>
+        <v>3211507</v>
       </c>
       <c r="E608" t="inlineStr">
         <is>
@@ -29566,10 +29566,10 @@
         </is>
       </c>
       <c r="C609" t="n">
-        <v>1574</v>
+        <v>1575</v>
       </c>
       <c r="D609" t="n">
-        <v>2278794</v>
+        <v>2280294</v>
       </c>
       <c r="E609" t="inlineStr">
         <is>
@@ -29614,10 +29614,10 @@
         </is>
       </c>
       <c r="C610" t="n">
-        <v>3935</v>
+        <v>3937</v>
       </c>
       <c r="D610" t="n">
-        <v>5779762</v>
+        <v>5782762</v>
       </c>
       <c r="E610" t="inlineStr">
         <is>
@@ -29662,10 +29662,10 @@
         </is>
       </c>
       <c r="C611" t="n">
-        <v>1178</v>
+        <v>1180</v>
       </c>
       <c r="D611" t="n">
-        <v>1740511</v>
+        <v>1743511</v>
       </c>
       <c r="E611" t="inlineStr">
         <is>
@@ -29806,10 +29806,10 @@
         </is>
       </c>
       <c r="C614" t="n">
-        <v>1665</v>
+        <v>1666</v>
       </c>
       <c r="D614" t="n">
-        <v>2206852</v>
+        <v>2208352</v>
       </c>
       <c r="E614" t="inlineStr">
         <is>
@@ -29854,10 +29854,10 @@
         </is>
       </c>
       <c r="C615" t="n">
-        <v>1058</v>
+        <v>1059</v>
       </c>
       <c r="D615" t="n">
-        <v>1524730</v>
+        <v>1526230</v>
       </c>
       <c r="E615" t="inlineStr">
         <is>
@@ -29902,10 +29902,10 @@
         </is>
       </c>
       <c r="C616" t="n">
-        <v>2552</v>
+        <v>2557</v>
       </c>
       <c r="D616" t="n">
-        <v>3740339</v>
+        <v>3745525</v>
       </c>
       <c r="E616" t="inlineStr">
         <is>
@@ -30142,10 +30142,10 @@
         </is>
       </c>
       <c r="C621" t="n">
-        <v>1154</v>
+        <v>1155</v>
       </c>
       <c r="D621" t="n">
-        <v>1515456</v>
+        <v>1516956</v>
       </c>
       <c r="E621" t="inlineStr">
         <is>
@@ -30190,10 +30190,10 @@
         </is>
       </c>
       <c r="C622" t="n">
-        <v>4824</v>
+        <v>4826</v>
       </c>
       <c r="D622" t="n">
-        <v>6989745</v>
+        <v>6992340</v>
       </c>
       <c r="E622" t="inlineStr">
         <is>
@@ -30238,10 +30238,10 @@
         </is>
       </c>
       <c r="C623" t="n">
-        <v>11667</v>
+        <v>11673</v>
       </c>
       <c r="D623" t="n">
-        <v>17186655</v>
+        <v>17195655</v>
       </c>
       <c r="E623" t="inlineStr">
         <is>
@@ -30286,10 +30286,10 @@
         </is>
       </c>
       <c r="C624" t="n">
-        <v>4402</v>
+        <v>4407</v>
       </c>
       <c r="D624" t="n">
-        <v>6534953</v>
+        <v>6542453</v>
       </c>
       <c r="E624" t="inlineStr">
         <is>
@@ -30334,10 +30334,10 @@
         </is>
       </c>
       <c r="C625" t="n">
-        <v>1153</v>
+        <v>1154</v>
       </c>
       <c r="D625" t="n">
-        <v>1720857</v>
+        <v>1722357</v>
       </c>
       <c r="E625" t="inlineStr">
         <is>
@@ -30382,10 +30382,10 @@
         </is>
       </c>
       <c r="C626" t="n">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="D626" t="n">
-        <v>303262</v>
+        <v>304762</v>
       </c>
       <c r="E626" t="inlineStr">
         <is>
@@ -30478,10 +30478,10 @@
         </is>
       </c>
       <c r="C628" t="n">
-        <v>3976</v>
+        <v>3980</v>
       </c>
       <c r="D628" t="n">
-        <v>5338315</v>
+        <v>5343143</v>
       </c>
       <c r="E628" t="inlineStr">
         <is>
@@ -30526,10 +30526,10 @@
         </is>
       </c>
       <c r="C629" t="n">
-        <v>2144</v>
+        <v>2145</v>
       </c>
       <c r="D629" t="n">
-        <v>3094953</v>
+        <v>3096453</v>
       </c>
       <c r="E629" t="inlineStr">
         <is>
@@ -30670,10 +30670,10 @@
         </is>
       </c>
       <c r="C632" t="n">
-        <v>585</v>
+        <v>586</v>
       </c>
       <c r="D632" t="n">
-        <v>872060</v>
+        <v>873560</v>
       </c>
       <c r="E632" t="inlineStr">
         <is>
@@ -30718,10 +30718,10 @@
         </is>
       </c>
       <c r="C633" t="n">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="D633" t="n">
-        <v>129274</v>
+        <v>130774</v>
       </c>
       <c r="E633" t="inlineStr">
         <is>
@@ -30862,10 +30862,10 @@
         </is>
       </c>
       <c r="C636" t="n">
-        <v>2143</v>
+        <v>2144</v>
       </c>
       <c r="D636" t="n">
-        <v>2903121</v>
+        <v>2904621</v>
       </c>
       <c r="E636" t="inlineStr">
         <is>
@@ -31198,10 +31198,10 @@
         </is>
       </c>
       <c r="C643" t="n">
-        <v>788</v>
+        <v>789</v>
       </c>
       <c r="D643" t="n">
-        <v>1045899</v>
+        <v>1046164</v>
       </c>
       <c r="E643" t="inlineStr">
         <is>
@@ -31294,10 +31294,10 @@
         </is>
       </c>
       <c r="C645" t="n">
-        <v>3914</v>
+        <v>3917</v>
       </c>
       <c r="D645" t="n">
-        <v>5757160</v>
+        <v>5761002</v>
       </c>
       <c r="E645" t="inlineStr">
         <is>
@@ -31534,10 +31534,10 @@
         </is>
       </c>
       <c r="C650" t="n">
-        <v>1284</v>
+        <v>1285</v>
       </c>
       <c r="D650" t="n">
-        <v>1677096</v>
+        <v>1678596</v>
       </c>
       <c r="E650" t="inlineStr">
         <is>
@@ -31582,10 +31582,10 @@
         </is>
       </c>
       <c r="C651" t="n">
-        <v>3019</v>
+        <v>3020</v>
       </c>
       <c r="D651" t="n">
-        <v>4386740</v>
+        <v>4388240</v>
       </c>
       <c r="E651" t="inlineStr">
         <is>
@@ -31630,10 +31630,10 @@
         </is>
       </c>
       <c r="C652" t="n">
-        <v>6085</v>
+        <v>6090</v>
       </c>
       <c r="D652" t="n">
-        <v>8917583</v>
+        <v>8923038</v>
       </c>
       <c r="E652" t="inlineStr">
         <is>
@@ -31678,10 +31678,10 @@
         </is>
       </c>
       <c r="C653" t="n">
-        <v>2241</v>
+        <v>2242</v>
       </c>
       <c r="D653" t="n">
-        <v>3335689</v>
+        <v>3337189</v>
       </c>
       <c r="E653" t="inlineStr">
         <is>
@@ -31918,10 +31918,10 @@
         </is>
       </c>
       <c r="C658" t="n">
-        <v>1919</v>
+        <v>1922</v>
       </c>
       <c r="D658" t="n">
-        <v>2588148</v>
+        <v>2590173</v>
       </c>
       <c r="E658" t="inlineStr">
         <is>
@@ -32014,10 +32014,10 @@
         </is>
       </c>
       <c r="C660" t="n">
-        <v>2672</v>
+        <v>2674</v>
       </c>
       <c r="D660" t="n">
-        <v>3903380</v>
+        <v>3906380</v>
       </c>
       <c r="E660" t="inlineStr">
         <is>
@@ -32254,10 +32254,10 @@
         </is>
       </c>
       <c r="C665" t="n">
-        <v>1123</v>
+        <v>1124</v>
       </c>
       <c r="D665" t="n">
-        <v>1490498</v>
+        <v>1490948</v>
       </c>
       <c r="E665" t="inlineStr">
         <is>
@@ -32302,10 +32302,10 @@
         </is>
       </c>
       <c r="C666" t="n">
-        <v>7822</v>
+        <v>7824</v>
       </c>
       <c r="D666" t="n">
-        <v>11335503</v>
+        <v>11338503</v>
       </c>
       <c r="E666" t="inlineStr">
         <is>
@@ -32350,10 +32350,10 @@
         </is>
       </c>
       <c r="C667" t="n">
-        <v>18993</v>
+        <v>19006</v>
       </c>
       <c r="D667" t="n">
-        <v>27898879</v>
+        <v>27918379</v>
       </c>
       <c r="E667" t="inlineStr">
         <is>
@@ -32398,10 +32398,10 @@
         </is>
       </c>
       <c r="C668" t="n">
-        <v>5743</v>
+        <v>5747</v>
       </c>
       <c r="D668" t="n">
-        <v>8548311</v>
+        <v>8554311</v>
       </c>
       <c r="E668" t="inlineStr">
         <is>
@@ -32446,10 +32446,10 @@
         </is>
       </c>
       <c r="C669" t="n">
-        <v>1615</v>
+        <v>1618</v>
       </c>
       <c r="D669" t="n">
-        <v>2411287</v>
+        <v>2415787</v>
       </c>
       <c r="E669" t="inlineStr">
         <is>
@@ -32494,10 +32494,10 @@
         </is>
       </c>
       <c r="C670" t="n">
-        <v>357</v>
+        <v>359</v>
       </c>
       <c r="D670" t="n">
-        <v>530606</v>
+        <v>533606</v>
       </c>
       <c r="E670" t="inlineStr">
         <is>
@@ -32590,10 +32590,10 @@
         </is>
       </c>
       <c r="C672" t="n">
-        <v>6849</v>
+        <v>6857</v>
       </c>
       <c r="D672" t="n">
-        <v>9342875</v>
+        <v>9354656</v>
       </c>
       <c r="E672" t="inlineStr">
         <is>
@@ -32638,10 +32638,10 @@
         </is>
       </c>
       <c r="C673" t="n">
-        <v>9743</v>
+        <v>9751</v>
       </c>
       <c r="D673" t="n">
-        <v>14153123</v>
+        <v>14165123</v>
       </c>
       <c r="E673" t="inlineStr">
         <is>
@@ -32686,10 +32686,10 @@
         </is>
       </c>
       <c r="C674" t="n">
-        <v>26501</v>
+        <v>26533</v>
       </c>
       <c r="D674" t="n">
-        <v>38933542</v>
+        <v>38981542</v>
       </c>
       <c r="E674" t="inlineStr">
         <is>
@@ -32734,10 +32734,10 @@
         </is>
       </c>
       <c r="C675" t="n">
-        <v>8407</v>
+        <v>8413</v>
       </c>
       <c r="D675" t="n">
-        <v>12523657</v>
+        <v>12532655</v>
       </c>
       <c r="E675" t="inlineStr">
         <is>
@@ -32782,10 +32782,10 @@
         </is>
       </c>
       <c r="C676" t="n">
-        <v>2222</v>
+        <v>2223</v>
       </c>
       <c r="D676" t="n">
-        <v>3316602</v>
+        <v>3318102</v>
       </c>
       <c r="E676" t="inlineStr">
         <is>
@@ -32974,10 +32974,10 @@
         </is>
       </c>
       <c r="C680" t="n">
-        <v>8794</v>
+        <v>8796</v>
       </c>
       <c r="D680" t="n">
-        <v>11929564</v>
+        <v>11932307</v>
       </c>
       <c r="E680" t="inlineStr">
         <is>
@@ -33070,10 +33070,10 @@
         </is>
       </c>
       <c r="C682" t="n">
-        <v>2522</v>
+        <v>2530</v>
       </c>
       <c r="D682" t="n">
-        <v>3680090</v>
+        <v>3692060</v>
       </c>
       <c r="E682" t="inlineStr">
         <is>
@@ -33118,10 +33118,10 @@
         </is>
       </c>
       <c r="C683" t="n">
-        <v>961</v>
+        <v>962</v>
       </c>
       <c r="D683" t="n">
-        <v>1417669</v>
+        <v>1419169</v>
       </c>
       <c r="E683" t="inlineStr">
         <is>
@@ -33166,10 +33166,10 @@
         </is>
       </c>
       <c r="C684" t="n">
-        <v>273</v>
+        <v>274</v>
       </c>
       <c r="D684" t="n">
-        <v>409061</v>
+        <v>410561</v>
       </c>
       <c r="E684" t="inlineStr">
         <is>
@@ -33358,10 +33358,10 @@
         </is>
       </c>
       <c r="C688" t="n">
-        <v>8359</v>
+        <v>8368</v>
       </c>
       <c r="D688" t="n">
-        <v>11991433</v>
+        <v>12001823</v>
       </c>
       <c r="E688" t="inlineStr">
         <is>
@@ -33406,10 +33406,10 @@
         </is>
       </c>
       <c r="C689" t="n">
-        <v>16077</v>
+        <v>16088</v>
       </c>
       <c r="D689" t="n">
-        <v>23470932</v>
+        <v>23487432</v>
       </c>
       <c r="E689" t="inlineStr">
         <is>
@@ -33502,10 +33502,10 @@
         </is>
       </c>
       <c r="C691" t="n">
-        <v>1066</v>
+        <v>1067</v>
       </c>
       <c r="D691" t="n">
-        <v>1591876</v>
+        <v>1593376</v>
       </c>
       <c r="E691" t="inlineStr">
         <is>
@@ -33694,10 +33694,10 @@
         </is>
       </c>
       <c r="C695" t="n">
-        <v>5340</v>
+        <v>5350</v>
       </c>
       <c r="D695" t="n">
-        <v>7238415</v>
+        <v>7250442</v>
       </c>
       <c r="E695" t="inlineStr">
         <is>
@@ -33742,10 +33742,10 @@
         </is>
       </c>
       <c r="C696" t="n">
-        <v>3494</v>
+        <v>3496</v>
       </c>
       <c r="D696" t="n">
-        <v>5047656</v>
+        <v>5050656</v>
       </c>
       <c r="E696" t="inlineStr">
         <is>
@@ -33790,10 +33790,10 @@
         </is>
       </c>
       <c r="C697" t="n">
-        <v>8976</v>
+        <v>8986</v>
       </c>
       <c r="D697" t="n">
-        <v>13160671</v>
+        <v>13173231</v>
       </c>
       <c r="E697" t="inlineStr">
         <is>
@@ -33838,10 +33838,10 @@
         </is>
       </c>
       <c r="C698" t="n">
-        <v>2467</v>
+        <v>2470</v>
       </c>
       <c r="D698" t="n">
-        <v>3669299</v>
+        <v>3670931</v>
       </c>
       <c r="E698" t="inlineStr">
         <is>
@@ -33886,10 +33886,10 @@
         </is>
       </c>
       <c r="C699" t="n">
-        <v>544</v>
+        <v>545</v>
       </c>
       <c r="D699" t="n">
-        <v>809277</v>
+        <v>810777</v>
       </c>
       <c r="E699" t="inlineStr">
         <is>
@@ -34030,10 +34030,10 @@
         </is>
       </c>
       <c r="C702" t="n">
-        <v>2985</v>
+        <v>2990</v>
       </c>
       <c r="D702" t="n">
-        <v>3957602</v>
+        <v>3963762</v>
       </c>
       <c r="E702" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
[Fonds de solidarite] Add 2020-07-18 data
</commit_message>
<xml_diff>
--- a/published-data/fonds-solidarite-volet-1-departemental-classe-effectif-latest.xlsx
+++ b/published-data/fonds-solidarite-volet-1-departemental-classe-effectif-latest.xlsx
@@ -718,10 +718,10 @@
         </is>
       </c>
       <c r="C8" t="n">
-        <v>520</v>
+        <v>522</v>
       </c>
       <c r="D8" t="n">
-        <v>688556</v>
+        <v>691556</v>
       </c>
       <c r="E8" t="inlineStr">
         <is>
@@ -862,10 +862,10 @@
         </is>
       </c>
       <c r="C11" t="n">
-        <v>875</v>
+        <v>876</v>
       </c>
       <c r="D11" t="n">
-        <v>1292379</v>
+        <v>1293786</v>
       </c>
       <c r="E11" t="inlineStr">
         <is>
@@ -1006,10 +1006,10 @@
         </is>
       </c>
       <c r="C14" t="n">
-        <v>1744</v>
+        <v>1745</v>
       </c>
       <c r="D14" t="n">
-        <v>2292992</v>
+        <v>2294236</v>
       </c>
       <c r="E14" t="inlineStr">
         <is>
@@ -1054,10 +1054,10 @@
         </is>
       </c>
       <c r="C15" t="n">
-        <v>2327</v>
+        <v>2331</v>
       </c>
       <c r="D15" t="n">
-        <v>3370770</v>
+        <v>3376770</v>
       </c>
       <c r="E15" t="inlineStr">
         <is>
@@ -1102,10 +1102,10 @@
         </is>
       </c>
       <c r="C16" t="n">
-        <v>3932</v>
+        <v>3934</v>
       </c>
       <c r="D16" t="n">
-        <v>5749950</v>
+        <v>5752950</v>
       </c>
       <c r="E16" t="inlineStr">
         <is>
@@ -1198,10 +1198,10 @@
         </is>
       </c>
       <c r="C18" t="n">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="D18" t="n">
-        <v>325604</v>
+        <v>327104</v>
       </c>
       <c r="E18" t="inlineStr">
         <is>
@@ -1390,10 +1390,10 @@
         </is>
       </c>
       <c r="C22" t="n">
-        <v>1823</v>
+        <v>1827</v>
       </c>
       <c r="D22" t="n">
-        <v>2647233</v>
+        <v>2651842</v>
       </c>
       <c r="E22" t="inlineStr">
         <is>
@@ -1726,10 +1726,10 @@
         </is>
       </c>
       <c r="C29" t="n">
-        <v>6048</v>
+        <v>6053</v>
       </c>
       <c r="D29" t="n">
-        <v>8868775</v>
+        <v>8876275</v>
       </c>
       <c r="E29" t="inlineStr">
         <is>
@@ -1774,10 +1774,10 @@
         </is>
       </c>
       <c r="C30" t="n">
-        <v>1882</v>
+        <v>1883</v>
       </c>
       <c r="D30" t="n">
-        <v>2790329</v>
+        <v>2791829</v>
       </c>
       <c r="E30" t="inlineStr">
         <is>
@@ -1822,10 +1822,10 @@
         </is>
       </c>
       <c r="C31" t="n">
-        <v>459</v>
+        <v>461</v>
       </c>
       <c r="D31" t="n">
-        <v>683904</v>
+        <v>686904</v>
       </c>
       <c r="E31" t="inlineStr">
         <is>
@@ -2062,10 +2062,10 @@
         </is>
       </c>
       <c r="C36" t="n">
-        <v>2645</v>
+        <v>2646</v>
       </c>
       <c r="D36" t="n">
-        <v>3857239</v>
+        <v>3858739</v>
       </c>
       <c r="E36" t="inlineStr">
         <is>
@@ -2110,10 +2110,10 @@
         </is>
       </c>
       <c r="C37" t="n">
-        <v>748</v>
+        <v>749</v>
       </c>
       <c r="D37" t="n">
-        <v>1101317</v>
+        <v>1102817</v>
       </c>
       <c r="E37" t="inlineStr">
         <is>
@@ -2302,10 +2302,10 @@
         </is>
       </c>
       <c r="C41" t="n">
-        <v>1270</v>
+        <v>1272</v>
       </c>
       <c r="D41" t="n">
-        <v>1720358</v>
+        <v>1723358</v>
       </c>
       <c r="E41" t="inlineStr">
         <is>
@@ -2398,10 +2398,10 @@
         </is>
       </c>
       <c r="C43" t="n">
-        <v>8349</v>
+        <v>8353</v>
       </c>
       <c r="D43" t="n">
-        <v>12256923</v>
+        <v>12262923</v>
       </c>
       <c r="E43" t="inlineStr">
         <is>
@@ -2446,10 +2446,10 @@
         </is>
       </c>
       <c r="C44" t="n">
-        <v>3385</v>
+        <v>3386</v>
       </c>
       <c r="D44" t="n">
-        <v>5015354</v>
+        <v>5016854</v>
       </c>
       <c r="E44" t="inlineStr">
         <is>
@@ -2542,10 +2542,10 @@
         </is>
       </c>
       <c r="C46" t="n">
-        <v>277</v>
+        <v>278</v>
       </c>
       <c r="D46" t="n">
-        <v>412537</v>
+        <v>414037</v>
       </c>
       <c r="E46" t="inlineStr">
         <is>
@@ -2638,10 +2638,10 @@
         </is>
       </c>
       <c r="C48" t="n">
-        <v>4632</v>
+        <v>4633</v>
       </c>
       <c r="D48" t="n">
-        <v>6345484</v>
+        <v>6346984</v>
       </c>
       <c r="E48" t="inlineStr">
         <is>
@@ -2686,10 +2686,10 @@
         </is>
       </c>
       <c r="C49" t="n">
-        <v>5440</v>
+        <v>5444</v>
       </c>
       <c r="D49" t="n">
-        <v>7883906</v>
+        <v>7889906</v>
       </c>
       <c r="E49" t="inlineStr">
         <is>
@@ -2734,10 +2734,10 @@
         </is>
       </c>
       <c r="C50" t="n">
-        <v>12874</v>
+        <v>12885</v>
       </c>
       <c r="D50" t="n">
-        <v>18951821</v>
+        <v>18968321</v>
       </c>
       <c r="E50" t="inlineStr">
         <is>
@@ -2782,10 +2782,10 @@
         </is>
       </c>
       <c r="C51" t="n">
-        <v>4368</v>
+        <v>4369</v>
       </c>
       <c r="D51" t="n">
-        <v>6477713</v>
+        <v>6479213</v>
       </c>
       <c r="E51" t="inlineStr">
         <is>
@@ -2830,10 +2830,10 @@
         </is>
       </c>
       <c r="C52" t="n">
-        <v>1158</v>
+        <v>1160</v>
       </c>
       <c r="D52" t="n">
-        <v>1719195</v>
+        <v>1722195</v>
       </c>
       <c r="E52" t="inlineStr">
         <is>
@@ -3022,10 +3022,10 @@
         </is>
       </c>
       <c r="C56" t="n">
-        <v>5241</v>
+        <v>5248</v>
       </c>
       <c r="D56" t="n">
-        <v>7201646</v>
+        <v>7211597</v>
       </c>
       <c r="E56" t="inlineStr">
         <is>
@@ -3070,10 +3070,10 @@
         </is>
       </c>
       <c r="C57" t="n">
-        <v>2947</v>
+        <v>2949</v>
       </c>
       <c r="D57" t="n">
-        <v>4261452</v>
+        <v>4264452</v>
       </c>
       <c r="E57" t="inlineStr">
         <is>
@@ -3118,10 +3118,10 @@
         </is>
       </c>
       <c r="C58" t="n">
-        <v>7405</v>
+        <v>7408</v>
       </c>
       <c r="D58" t="n">
-        <v>10866770</v>
+        <v>10871265</v>
       </c>
       <c r="E58" t="inlineStr">
         <is>
@@ -3166,10 +3166,10 @@
         </is>
       </c>
       <c r="C59" t="n">
-        <v>2348</v>
+        <v>2349</v>
       </c>
       <c r="D59" t="n">
-        <v>3468995</v>
+        <v>3470495</v>
       </c>
       <c r="E59" t="inlineStr">
         <is>
@@ -3262,10 +3262,10 @@
         </is>
       </c>
       <c r="C61" t="n">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="D61" t="n">
-        <v>206761</v>
+        <v>208261</v>
       </c>
       <c r="E61" t="inlineStr">
         <is>
@@ -3406,10 +3406,10 @@
         </is>
       </c>
       <c r="C64" t="n">
-        <v>2466</v>
+        <v>2468</v>
       </c>
       <c r="D64" t="n">
-        <v>3552898</v>
+        <v>3555598</v>
       </c>
       <c r="E64" t="inlineStr">
         <is>
@@ -3454,10 +3454,10 @@
         </is>
       </c>
       <c r="C65" t="n">
-        <v>6594</v>
+        <v>6595</v>
       </c>
       <c r="D65" t="n">
-        <v>9652984</v>
+        <v>9654484</v>
       </c>
       <c r="E65" t="inlineStr">
         <is>
@@ -3502,10 +3502,10 @@
         </is>
       </c>
       <c r="C66" t="n">
-        <v>2222</v>
+        <v>2223</v>
       </c>
       <c r="D66" t="n">
-        <v>3290233</v>
+        <v>3291733</v>
       </c>
       <c r="E66" t="inlineStr">
         <is>
@@ -3598,10 +3598,10 @@
         </is>
       </c>
       <c r="C68" t="n">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="D68" t="n">
-        <v>150986</v>
+        <v>152486</v>
       </c>
       <c r="E68" t="inlineStr">
         <is>
@@ -3742,10 +3742,10 @@
         </is>
       </c>
       <c r="C71" t="n">
-        <v>8394</v>
+        <v>8398</v>
       </c>
       <c r="D71" t="n">
-        <v>12191381</v>
+        <v>12196659</v>
       </c>
       <c r="E71" t="inlineStr">
         <is>
@@ -3790,10 +3790,10 @@
         </is>
       </c>
       <c r="C72" t="n">
-        <v>20977</v>
+        <v>20983</v>
       </c>
       <c r="D72" t="n">
-        <v>30848649</v>
+        <v>30855622</v>
       </c>
       <c r="E72" t="inlineStr">
         <is>
@@ -3838,10 +3838,10 @@
         </is>
       </c>
       <c r="C73" t="n">
-        <v>7291</v>
+        <v>7294</v>
       </c>
       <c r="D73" t="n">
-        <v>10830703</v>
+        <v>10835203</v>
       </c>
       <c r="E73" t="inlineStr">
         <is>
@@ -3934,10 +3934,10 @@
         </is>
       </c>
       <c r="C75" t="n">
-        <v>388</v>
+        <v>390</v>
       </c>
       <c r="D75" t="n">
-        <v>579983</v>
+        <v>582983</v>
       </c>
       <c r="E75" t="inlineStr">
         <is>
@@ -4126,10 +4126,10 @@
         </is>
       </c>
       <c r="C79" t="n">
-        <v>6897</v>
+        <v>6903</v>
       </c>
       <c r="D79" t="n">
-        <v>9518081</v>
+        <v>9526671</v>
       </c>
       <c r="E79" t="inlineStr">
         <is>
@@ -4174,10 +4174,10 @@
         </is>
       </c>
       <c r="C80" t="n">
-        <v>2525</v>
+        <v>2527</v>
       </c>
       <c r="D80" t="n">
-        <v>3667401</v>
+        <v>3670401</v>
       </c>
       <c r="E80" t="inlineStr">
         <is>
@@ -4222,10 +4222,10 @@
         </is>
       </c>
       <c r="C81" t="n">
-        <v>5993</v>
+        <v>5995</v>
       </c>
       <c r="D81" t="n">
-        <v>8791895</v>
+        <v>8794743</v>
       </c>
       <c r="E81" t="inlineStr">
         <is>
@@ -4270,10 +4270,10 @@
         </is>
       </c>
       <c r="C82" t="n">
-        <v>2656</v>
+        <v>2657</v>
       </c>
       <c r="D82" t="n">
-        <v>3936813</v>
+        <v>3938313</v>
       </c>
       <c r="E82" t="inlineStr">
         <is>
@@ -4462,10 +4462,10 @@
         </is>
       </c>
       <c r="C86" t="n">
-        <v>6093</v>
+        <v>6097</v>
       </c>
       <c r="D86" t="n">
-        <v>8582104</v>
+        <v>8586781</v>
       </c>
       <c r="E86" t="inlineStr">
         <is>
@@ -4510,10 +4510,10 @@
         </is>
       </c>
       <c r="C87" t="n">
-        <v>1794</v>
+        <v>1796</v>
       </c>
       <c r="D87" t="n">
-        <v>2607184</v>
+        <v>2610184</v>
       </c>
       <c r="E87" t="inlineStr">
         <is>
@@ -4558,10 +4558,10 @@
         </is>
       </c>
       <c r="C88" t="n">
-        <v>4636</v>
+        <v>4638</v>
       </c>
       <c r="D88" t="n">
-        <v>6813532</v>
+        <v>6816532</v>
       </c>
       <c r="E88" t="inlineStr">
         <is>
@@ -4606,10 +4606,10 @@
         </is>
       </c>
       <c r="C89" t="n">
-        <v>1634</v>
+        <v>1636</v>
       </c>
       <c r="D89" t="n">
-        <v>2431936</v>
+        <v>2434936</v>
       </c>
       <c r="E89" t="inlineStr">
         <is>
@@ -4894,10 +4894,10 @@
         </is>
       </c>
       <c r="C95" t="n">
-        <v>4304</v>
+        <v>4306</v>
       </c>
       <c r="D95" t="n">
-        <v>6322977</v>
+        <v>6325427</v>
       </c>
       <c r="E95" t="inlineStr">
         <is>
@@ -5518,10 +5518,10 @@
         </is>
       </c>
       <c r="C108" t="n">
-        <v>1037</v>
+        <v>1038</v>
       </c>
       <c r="D108" t="n">
-        <v>1499603</v>
+        <v>1501103</v>
       </c>
       <c r="E108" t="inlineStr">
         <is>
@@ -5566,10 +5566,10 @@
         </is>
       </c>
       <c r="C109" t="n">
-        <v>2551</v>
+        <v>2553</v>
       </c>
       <c r="D109" t="n">
-        <v>3739130</v>
+        <v>3741538</v>
       </c>
       <c r="E109" t="inlineStr">
         <is>
@@ -5710,10 +5710,10 @@
         </is>
       </c>
       <c r="C112" t="n">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="D112" t="n">
-        <v>48455</v>
+        <v>49955</v>
       </c>
       <c r="E112" t="inlineStr">
         <is>
@@ -5806,10 +5806,10 @@
         </is>
       </c>
       <c r="C114" t="n">
-        <v>896</v>
+        <v>897</v>
       </c>
       <c r="D114" t="n">
-        <v>1187311</v>
+        <v>1188605</v>
       </c>
       <c r="E114" t="inlineStr">
         <is>
@@ -5902,10 +5902,10 @@
         </is>
       </c>
       <c r="C116" t="n">
-        <v>1834</v>
+        <v>1835</v>
       </c>
       <c r="D116" t="n">
-        <v>2674523</v>
+        <v>2676023</v>
       </c>
       <c r="E116" t="inlineStr">
         <is>
@@ -6142,10 +6142,10 @@
         </is>
       </c>
       <c r="C121" t="n">
-        <v>1822</v>
+        <v>1823</v>
       </c>
       <c r="D121" t="n">
-        <v>2638413</v>
+        <v>2639013</v>
       </c>
       <c r="E121" t="inlineStr">
         <is>
@@ -6190,10 +6190,10 @@
         </is>
       </c>
       <c r="C122" t="n">
-        <v>5437</v>
+        <v>5440</v>
       </c>
       <c r="D122" t="n">
-        <v>7972179</v>
+        <v>7976679</v>
       </c>
       <c r="E122" t="inlineStr">
         <is>
@@ -6382,10 +6382,10 @@
         </is>
       </c>
       <c r="C126" t="n">
-        <v>2271</v>
+        <v>2272</v>
       </c>
       <c r="D126" t="n">
-        <v>3066017</v>
+        <v>3067517</v>
       </c>
       <c r="E126" t="inlineStr">
         <is>
@@ -7054,10 +7054,10 @@
         </is>
       </c>
       <c r="C140" t="n">
-        <v>2469</v>
+        <v>2471</v>
       </c>
       <c r="D140" t="n">
-        <v>3572766</v>
+        <v>3575766</v>
       </c>
       <c r="E140" t="inlineStr">
         <is>
@@ -7438,10 +7438,10 @@
         </is>
       </c>
       <c r="C148" t="n">
-        <v>7806</v>
+        <v>7809</v>
       </c>
       <c r="D148" t="n">
-        <v>11441444</v>
+        <v>11444915</v>
       </c>
       <c r="E148" t="inlineStr">
         <is>
@@ -7486,10 +7486,10 @@
         </is>
       </c>
       <c r="C149" t="n">
-        <v>2750</v>
+        <v>2751</v>
       </c>
       <c r="D149" t="n">
-        <v>4082170</v>
+        <v>4083670</v>
       </c>
       <c r="E149" t="inlineStr">
         <is>
@@ -7534,10 +7534,10 @@
         </is>
       </c>
       <c r="C150" t="n">
-        <v>651</v>
+        <v>652</v>
       </c>
       <c r="D150" t="n">
-        <v>965826</v>
+        <v>967326</v>
       </c>
       <c r="E150" t="inlineStr">
         <is>
@@ -7678,10 +7678,10 @@
         </is>
       </c>
       <c r="C153" t="n">
-        <v>2965</v>
+        <v>2966</v>
       </c>
       <c r="D153" t="n">
-        <v>3971546</v>
+        <v>3973046</v>
       </c>
       <c r="E153" t="inlineStr">
         <is>
@@ -7726,10 +7726,10 @@
         </is>
       </c>
       <c r="C154" t="n">
-        <v>3171</v>
+        <v>3172</v>
       </c>
       <c r="D154" t="n">
-        <v>4600299</v>
+        <v>4601799</v>
       </c>
       <c r="E154" t="inlineStr">
         <is>
@@ -7774,10 +7774,10 @@
         </is>
       </c>
       <c r="C155" t="n">
-        <v>8968</v>
+        <v>8974</v>
       </c>
       <c r="D155" t="n">
-        <v>13238626</v>
+        <v>13247626</v>
       </c>
       <c r="E155" t="inlineStr">
         <is>
@@ -8014,10 +8014,10 @@
         </is>
       </c>
       <c r="C160" t="n">
-        <v>2957</v>
+        <v>2963</v>
       </c>
       <c r="D160" t="n">
-        <v>4011638</v>
+        <v>4014333</v>
       </c>
       <c r="E160" t="inlineStr">
         <is>
@@ -8062,10 +8062,10 @@
         </is>
       </c>
       <c r="C161" t="n">
-        <v>3485</v>
+        <v>3487</v>
       </c>
       <c r="D161" t="n">
-        <v>5020449</v>
+        <v>5023449</v>
       </c>
       <c r="E161" t="inlineStr">
         <is>
@@ -8110,10 +8110,10 @@
         </is>
       </c>
       <c r="C162" t="n">
-        <v>7484</v>
+        <v>7485</v>
       </c>
       <c r="D162" t="n">
-        <v>10987220</v>
+        <v>10988720</v>
       </c>
       <c r="E162" t="inlineStr">
         <is>
@@ -8206,10 +8206,10 @@
         </is>
       </c>
       <c r="C164" t="n">
-        <v>574</v>
+        <v>575</v>
       </c>
       <c r="D164" t="n">
-        <v>850212</v>
+        <v>851712</v>
       </c>
       <c r="E164" t="inlineStr">
         <is>
@@ -8350,10 +8350,10 @@
         </is>
       </c>
       <c r="C167" t="n">
-        <v>2788</v>
+        <v>2789</v>
       </c>
       <c r="D167" t="n">
-        <v>3758856</v>
+        <v>3760356</v>
       </c>
       <c r="E167" t="inlineStr">
         <is>
@@ -8446,10 +8446,10 @@
         </is>
       </c>
       <c r="C169" t="n">
-        <v>2373</v>
+        <v>2375</v>
       </c>
       <c r="D169" t="n">
-        <v>3479653</v>
+        <v>3482653</v>
       </c>
       <c r="E169" t="inlineStr">
         <is>
@@ -8590,10 +8590,10 @@
         </is>
       </c>
       <c r="C172" t="n">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="D172" t="n">
-        <v>49721</v>
+        <v>51221</v>
       </c>
       <c r="E172" t="inlineStr">
         <is>
@@ -8782,10 +8782,10 @@
         </is>
       </c>
       <c r="C176" t="n">
-        <v>3316</v>
+        <v>3317</v>
       </c>
       <c r="D176" t="n">
-        <v>4894166</v>
+        <v>4895666</v>
       </c>
       <c r="E176" t="inlineStr">
         <is>
@@ -9214,10 +9214,10 @@
         </is>
       </c>
       <c r="C185" t="n">
-        <v>162</v>
+        <v>164</v>
       </c>
       <c r="D185" t="n">
-        <v>242990</v>
+        <v>245990</v>
       </c>
       <c r="E185" t="inlineStr">
         <is>
@@ -9742,10 +9742,10 @@
         </is>
       </c>
       <c r="C196" t="n">
-        <v>5325</v>
+        <v>5327</v>
       </c>
       <c r="D196" t="n">
-        <v>7838145</v>
+        <v>7841145</v>
       </c>
       <c r="E196" t="inlineStr">
         <is>
@@ -9790,10 +9790,10 @@
         </is>
       </c>
       <c r="C197" t="n">
-        <v>1973</v>
+        <v>1974</v>
       </c>
       <c r="D197" t="n">
-        <v>2937930</v>
+        <v>2939430</v>
       </c>
       <c r="E197" t="inlineStr">
         <is>
@@ -9838,10 +9838,10 @@
         </is>
       </c>
       <c r="C198" t="n">
-        <v>462</v>
+        <v>463</v>
       </c>
       <c r="D198" t="n">
-        <v>685875</v>
+        <v>687375</v>
       </c>
       <c r="E198" t="inlineStr">
         <is>
@@ -9982,10 +9982,10 @@
         </is>
       </c>
       <c r="C201" t="n">
-        <v>1761</v>
+        <v>1762</v>
       </c>
       <c r="D201" t="n">
-        <v>2320398</v>
+        <v>2321898</v>
       </c>
       <c r="E201" t="inlineStr">
         <is>
@@ -10078,10 +10078,10 @@
         </is>
       </c>
       <c r="C203" t="n">
-        <v>3000</v>
+        <v>3001</v>
       </c>
       <c r="D203" t="n">
-        <v>4415574</v>
+        <v>4417074</v>
       </c>
       <c r="E203" t="inlineStr">
         <is>
@@ -10270,10 +10270,10 @@
         </is>
       </c>
       <c r="C207" t="n">
-        <v>1049</v>
+        <v>1050</v>
       </c>
       <c r="D207" t="n">
-        <v>1418035</v>
+        <v>1419535</v>
       </c>
       <c r="E207" t="inlineStr">
         <is>
@@ -10318,10 +10318,10 @@
         </is>
       </c>
       <c r="C208" t="n">
-        <v>828</v>
+        <v>829</v>
       </c>
       <c r="D208" t="n">
-        <v>1187526</v>
+        <v>1189026</v>
       </c>
       <c r="E208" t="inlineStr">
         <is>
@@ -10366,10 +10366,10 @@
         </is>
       </c>
       <c r="C209" t="n">
-        <v>3280</v>
+        <v>3282</v>
       </c>
       <c r="D209" t="n">
-        <v>4795542</v>
+        <v>4798542</v>
       </c>
       <c r="E209" t="inlineStr">
         <is>
@@ -10414,10 +10414,10 @@
         </is>
       </c>
       <c r="C210" t="n">
-        <v>1676</v>
+        <v>1678</v>
       </c>
       <c r="D210" t="n">
-        <v>2479481</v>
+        <v>2482481</v>
       </c>
       <c r="E210" t="inlineStr">
         <is>
@@ -10654,10 +10654,10 @@
         </is>
       </c>
       <c r="C215" t="n">
-        <v>3716</v>
+        <v>3718</v>
       </c>
       <c r="D215" t="n">
-        <v>5428805</v>
+        <v>5431805</v>
       </c>
       <c r="E215" t="inlineStr">
         <is>
@@ -10846,10 +10846,10 @@
         </is>
       </c>
       <c r="C219" t="n">
-        <v>1516</v>
+        <v>1517</v>
       </c>
       <c r="D219" t="n">
-        <v>2054002</v>
+        <v>2055502</v>
       </c>
       <c r="E219" t="inlineStr">
         <is>
@@ -10942,10 +10942,10 @@
         </is>
       </c>
       <c r="C221" t="n">
-        <v>2125</v>
+        <v>2126</v>
       </c>
       <c r="D221" t="n">
-        <v>3093971</v>
+        <v>3095471</v>
       </c>
       <c r="E221" t="inlineStr">
         <is>
@@ -11182,10 +11182,10 @@
         </is>
       </c>
       <c r="C226" t="n">
-        <v>879</v>
+        <v>883</v>
       </c>
       <c r="D226" t="n">
-        <v>1274106</v>
+        <v>1278784</v>
       </c>
       <c r="E226" t="inlineStr">
         <is>
@@ -11278,10 +11278,10 @@
         </is>
       </c>
       <c r="C228" t="n">
-        <v>784</v>
+        <v>785</v>
       </c>
       <c r="D228" t="n">
-        <v>1166840</v>
+        <v>1168340</v>
       </c>
       <c r="E228" t="inlineStr">
         <is>
@@ -11470,10 +11470,10 @@
         </is>
       </c>
       <c r="C232" t="n">
-        <v>3631</v>
+        <v>3633</v>
       </c>
       <c r="D232" t="n">
-        <v>5261626</v>
+        <v>5264626</v>
       </c>
       <c r="E232" t="inlineStr">
         <is>
@@ -11518,10 +11518,10 @@
         </is>
       </c>
       <c r="C233" t="n">
-        <v>11670</v>
+        <v>11676</v>
       </c>
       <c r="D233" t="n">
-        <v>17132192</v>
+        <v>17141192</v>
       </c>
       <c r="E233" t="inlineStr">
         <is>
@@ -11566,10 +11566,10 @@
         </is>
       </c>
       <c r="C234" t="n">
-        <v>4538</v>
+        <v>4540</v>
       </c>
       <c r="D234" t="n">
-        <v>6736653</v>
+        <v>6739653</v>
       </c>
       <c r="E234" t="inlineStr">
         <is>
@@ -11614,10 +11614,10 @@
         </is>
       </c>
       <c r="C235" t="n">
-        <v>1379</v>
+        <v>1380</v>
       </c>
       <c r="D235" t="n">
-        <v>2051790</v>
+        <v>2053290</v>
       </c>
       <c r="E235" t="inlineStr">
         <is>
@@ -11758,10 +11758,10 @@
         </is>
       </c>
       <c r="C238" t="n">
-        <v>3151</v>
+        <v>3154</v>
       </c>
       <c r="D238" t="n">
-        <v>4286204</v>
+        <v>4289444</v>
       </c>
       <c r="E238" t="inlineStr">
         <is>
@@ -12238,10 +12238,10 @@
         </is>
       </c>
       <c r="C248" t="n">
-        <v>3026</v>
+        <v>3030</v>
       </c>
       <c r="D248" t="n">
-        <v>4494614</v>
+        <v>4500614</v>
       </c>
       <c r="E248" t="inlineStr">
         <is>
@@ -12526,10 +12526,10 @@
         </is>
       </c>
       <c r="C254" t="n">
-        <v>1923</v>
+        <v>1924</v>
       </c>
       <c r="D254" t="n">
-        <v>2541499</v>
+        <v>2542104</v>
       </c>
       <c r="E254" t="inlineStr">
         <is>
@@ -13006,10 +13006,10 @@
         </is>
       </c>
       <c r="C264" t="n">
-        <v>1842</v>
+        <v>1843</v>
       </c>
       <c r="D264" t="n">
-        <v>2735153</v>
+        <v>2736653</v>
       </c>
       <c r="E264" t="inlineStr">
         <is>
@@ -13198,10 +13198,10 @@
         </is>
       </c>
       <c r="C268" t="n">
-        <v>2033</v>
+        <v>2034</v>
       </c>
       <c r="D268" t="n">
-        <v>2752067</v>
+        <v>2752548</v>
       </c>
       <c r="E268" t="inlineStr">
         <is>
@@ -13534,10 +13534,10 @@
         </is>
       </c>
       <c r="C275" t="n">
-        <v>2476</v>
+        <v>2479</v>
       </c>
       <c r="D275" t="n">
-        <v>3586299</v>
+        <v>3590799</v>
       </c>
       <c r="E275" t="inlineStr">
         <is>
@@ -13582,10 +13582,10 @@
         </is>
       </c>
       <c r="C276" t="n">
-        <v>8163</v>
+        <v>8168</v>
       </c>
       <c r="D276" t="n">
-        <v>11967857</v>
+        <v>11975357</v>
       </c>
       <c r="E276" t="inlineStr">
         <is>
@@ -13822,10 +13822,10 @@
         </is>
       </c>
       <c r="C281" t="n">
-        <v>2246</v>
+        <v>2247</v>
       </c>
       <c r="D281" t="n">
-        <v>3008986</v>
+        <v>3010043</v>
       </c>
       <c r="E281" t="inlineStr">
         <is>
@@ -14158,10 +14158,10 @@
         </is>
       </c>
       <c r="C288" t="n">
-        <v>1527</v>
+        <v>1529</v>
       </c>
       <c r="D288" t="n">
-        <v>2017043</v>
+        <v>2020043</v>
       </c>
       <c r="E288" t="inlineStr">
         <is>
@@ -14206,10 +14206,10 @@
         </is>
       </c>
       <c r="C289" t="n">
-        <v>1675</v>
+        <v>1682</v>
       </c>
       <c r="D289" t="n">
-        <v>2431133</v>
+        <v>2440833</v>
       </c>
       <c r="E289" t="inlineStr">
         <is>
@@ -14254,10 +14254,10 @@
         </is>
       </c>
       <c r="C290" t="n">
-        <v>5962</v>
+        <v>5976</v>
       </c>
       <c r="D290" t="n">
-        <v>8778326</v>
+        <v>8799326</v>
       </c>
       <c r="E290" t="inlineStr">
         <is>
@@ -14302,10 +14302,10 @@
         </is>
       </c>
       <c r="C291" t="n">
-        <v>2086</v>
+        <v>2090</v>
       </c>
       <c r="D291" t="n">
-        <v>3115750</v>
+        <v>3121750</v>
       </c>
       <c r="E291" t="inlineStr">
         <is>
@@ -14350,10 +14350,10 @@
         </is>
       </c>
       <c r="C292" t="n">
-        <v>678</v>
+        <v>683</v>
       </c>
       <c r="D292" t="n">
-        <v>1012305</v>
+        <v>1019805</v>
       </c>
       <c r="E292" t="inlineStr">
         <is>
@@ -14398,10 +14398,10 @@
         </is>
       </c>
       <c r="C293" t="n">
-        <v>150</v>
+        <v>153</v>
       </c>
       <c r="D293" t="n">
-        <v>222611</v>
+        <v>227111</v>
       </c>
       <c r="E293" t="inlineStr">
         <is>
@@ -14494,10 +14494,10 @@
         </is>
       </c>
       <c r="C295" t="n">
-        <v>5452</v>
+        <v>5483</v>
       </c>
       <c r="D295" t="n">
-        <v>7532638</v>
+        <v>7572623</v>
       </c>
       <c r="E295" t="inlineStr">
         <is>
@@ -14542,10 +14542,10 @@
         </is>
       </c>
       <c r="C296" t="n">
-        <v>685</v>
+        <v>690</v>
       </c>
       <c r="D296" t="n">
-        <v>1003840</v>
+        <v>1011340</v>
       </c>
       <c r="E296" t="inlineStr">
         <is>
@@ -14590,10 +14590,10 @@
         </is>
       </c>
       <c r="C297" t="n">
-        <v>1740</v>
+        <v>1743</v>
       </c>
       <c r="D297" t="n">
-        <v>2578414</v>
+        <v>2582914</v>
       </c>
       <c r="E297" t="inlineStr">
         <is>
@@ -14734,10 +14734,10 @@
         </is>
       </c>
       <c r="C300" t="n">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="D300" t="n">
-        <v>73500</v>
+        <v>76500</v>
       </c>
       <c r="E300" t="inlineStr">
         <is>
@@ -14830,10 +14830,10 @@
         </is>
       </c>
       <c r="C302" t="n">
-        <v>1007</v>
+        <v>1008</v>
       </c>
       <c r="D302" t="n">
-        <v>1428265</v>
+        <v>1429765</v>
       </c>
       <c r="E302" t="inlineStr">
         <is>
@@ -14926,10 +14926,10 @@
         </is>
       </c>
       <c r="C304" t="n">
-        <v>3411</v>
+        <v>3413</v>
       </c>
       <c r="D304" t="n">
-        <v>5004405</v>
+        <v>5007405</v>
       </c>
       <c r="E304" t="inlineStr">
         <is>
@@ -15166,10 +15166,10 @@
         </is>
       </c>
       <c r="C309" t="n">
-        <v>1337</v>
+        <v>1339</v>
       </c>
       <c r="D309" t="n">
-        <v>1784341</v>
+        <v>1787341</v>
       </c>
       <c r="E309" t="inlineStr">
         <is>
@@ -15214,10 +15214,10 @@
         </is>
       </c>
       <c r="C310" t="n">
-        <v>6474</v>
+        <v>6475</v>
       </c>
       <c r="D310" t="n">
-        <v>9345696</v>
+        <v>9347196</v>
       </c>
       <c r="E310" t="inlineStr">
         <is>
@@ -15262,10 +15262,10 @@
         </is>
       </c>
       <c r="C311" t="n">
-        <v>18530</v>
+        <v>18536</v>
       </c>
       <c r="D311" t="n">
-        <v>27131634</v>
+        <v>27139517</v>
       </c>
       <c r="E311" t="inlineStr">
         <is>
@@ -15310,10 +15310,10 @@
         </is>
       </c>
       <c r="C312" t="n">
-        <v>6604</v>
+        <v>6605</v>
       </c>
       <c r="D312" t="n">
-        <v>9832207</v>
+        <v>9833707</v>
       </c>
       <c r="E312" t="inlineStr">
         <is>
@@ -15406,10 +15406,10 @@
         </is>
       </c>
       <c r="C314" t="n">
-        <v>412</v>
+        <v>413</v>
       </c>
       <c r="D314" t="n">
-        <v>614470</v>
+        <v>615970</v>
       </c>
       <c r="E314" t="inlineStr">
         <is>
@@ -15502,10 +15502,10 @@
         </is>
       </c>
       <c r="C316" t="n">
-        <v>5803</v>
+        <v>5805</v>
       </c>
       <c r="D316" t="n">
-        <v>7674133</v>
+        <v>7677133</v>
       </c>
       <c r="E316" t="inlineStr">
         <is>
@@ -15550,10 +15550,10 @@
         </is>
       </c>
       <c r="C317" t="n">
-        <v>1946</v>
+        <v>1947</v>
       </c>
       <c r="D317" t="n">
-        <v>2849712</v>
+        <v>2851212</v>
       </c>
       <c r="E317" t="inlineStr">
         <is>
@@ -15598,10 +15598,10 @@
         </is>
       </c>
       <c r="C318" t="n">
-        <v>6093</v>
+        <v>6098</v>
       </c>
       <c r="D318" t="n">
-        <v>8953729</v>
+        <v>8961229</v>
       </c>
       <c r="E318" t="inlineStr">
         <is>
@@ -15646,10 +15646,10 @@
         </is>
       </c>
       <c r="C319" t="n">
-        <v>2174</v>
+        <v>2177</v>
       </c>
       <c r="D319" t="n">
-        <v>3236519</v>
+        <v>3241019</v>
       </c>
       <c r="E319" t="inlineStr">
         <is>
@@ -15934,10 +15934,10 @@
         </is>
       </c>
       <c r="C325" t="n">
-        <v>10276</v>
+        <v>10277</v>
       </c>
       <c r="D325" t="n">
-        <v>15029843</v>
+        <v>15031343</v>
       </c>
       <c r="E325" t="inlineStr">
         <is>
@@ -16030,10 +16030,10 @@
         </is>
       </c>
       <c r="C327" t="n">
-        <v>1028</v>
+        <v>1032</v>
       </c>
       <c r="D327" t="n">
-        <v>1528873</v>
+        <v>1534873</v>
       </c>
       <c r="E327" t="inlineStr">
         <is>
@@ -16078,10 +16078,10 @@
         </is>
       </c>
       <c r="C328" t="n">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="D328" t="n">
-        <v>238892</v>
+        <v>240392</v>
       </c>
       <c r="E328" t="inlineStr">
         <is>
@@ -16558,10 +16558,10 @@
         </is>
       </c>
       <c r="C338" t="n">
-        <v>1583</v>
+        <v>1584</v>
       </c>
       <c r="D338" t="n">
-        <v>2069987</v>
+        <v>2071487</v>
       </c>
       <c r="E338" t="inlineStr">
         <is>
@@ -16654,10 +16654,10 @@
         </is>
       </c>
       <c r="C340" t="n">
-        <v>9591</v>
+        <v>9598</v>
       </c>
       <c r="D340" t="n">
-        <v>14161039</v>
+        <v>14171539</v>
       </c>
       <c r="E340" t="inlineStr">
         <is>
@@ -16702,10 +16702,10 @@
         </is>
       </c>
       <c r="C341" t="n">
-        <v>3739</v>
+        <v>3741</v>
       </c>
       <c r="D341" t="n">
-        <v>5567927</v>
+        <v>5570927</v>
       </c>
       <c r="E341" t="inlineStr">
         <is>
@@ -16750,10 +16750,10 @@
         </is>
       </c>
       <c r="C342" t="n">
-        <v>1102</v>
+        <v>1105</v>
       </c>
       <c r="D342" t="n">
-        <v>1644679</v>
+        <v>1649179</v>
       </c>
       <c r="E342" t="inlineStr">
         <is>
@@ -16798,10 +16798,10 @@
         </is>
       </c>
       <c r="C343" t="n">
-        <v>191</v>
+        <v>193</v>
       </c>
       <c r="D343" t="n">
-        <v>286301</v>
+        <v>289301</v>
       </c>
       <c r="E343" t="inlineStr">
         <is>
@@ -16942,10 +16942,10 @@
         </is>
       </c>
       <c r="C346" t="n">
-        <v>5653</v>
+        <v>5660</v>
       </c>
       <c r="D346" t="n">
-        <v>8249684</v>
+        <v>8258478</v>
       </c>
       <c r="E346" t="inlineStr">
         <is>
@@ -16990,10 +16990,10 @@
         </is>
       </c>
       <c r="C347" t="n">
-        <v>14102</v>
+        <v>14109</v>
       </c>
       <c r="D347" t="n">
-        <v>20779254</v>
+        <v>20787451</v>
       </c>
       <c r="E347" t="inlineStr">
         <is>
@@ -17038,10 +17038,10 @@
         </is>
       </c>
       <c r="C348" t="n">
-        <v>6388</v>
+        <v>6391</v>
       </c>
       <c r="D348" t="n">
-        <v>9530540</v>
+        <v>9535040</v>
       </c>
       <c r="E348" t="inlineStr">
         <is>
@@ -17086,10 +17086,10 @@
         </is>
       </c>
       <c r="C349" t="n">
-        <v>1948</v>
+        <v>1949</v>
       </c>
       <c r="D349" t="n">
-        <v>2907872</v>
+        <v>2909372</v>
       </c>
       <c r="E349" t="inlineStr">
         <is>
@@ -17230,10 +17230,10 @@
         </is>
       </c>
       <c r="C352" t="n">
-        <v>5105</v>
+        <v>5111</v>
       </c>
       <c r="D352" t="n">
-        <v>7006631</v>
+        <v>7013012</v>
       </c>
       <c r="E352" t="inlineStr">
         <is>
@@ -17278,10 +17278,10 @@
         </is>
       </c>
       <c r="C353" t="n">
-        <v>16618</v>
+        <v>16622</v>
       </c>
       <c r="D353" t="n">
-        <v>24137012</v>
+        <v>24141283</v>
       </c>
       <c r="E353" t="inlineStr">
         <is>
@@ -17326,10 +17326,10 @@
         </is>
       </c>
       <c r="C354" t="n">
-        <v>46309</v>
+        <v>46343</v>
       </c>
       <c r="D354" t="n">
-        <v>68299418</v>
+        <v>68349427</v>
       </c>
       <c r="E354" t="inlineStr">
         <is>
@@ -17374,10 +17374,10 @@
         </is>
       </c>
       <c r="C355" t="n">
-        <v>21620</v>
+        <v>21639</v>
       </c>
       <c r="D355" t="n">
-        <v>32267530</v>
+        <v>32294246</v>
       </c>
       <c r="E355" t="inlineStr">
         <is>
@@ -17422,10 +17422,10 @@
         </is>
       </c>
       <c r="C356" t="n">
-        <v>7692</v>
+        <v>7702</v>
       </c>
       <c r="D356" t="n">
-        <v>11503483</v>
+        <v>11518483</v>
       </c>
       <c r="E356" t="inlineStr">
         <is>
@@ -17470,10 +17470,10 @@
         </is>
       </c>
       <c r="C357" t="n">
-        <v>1817</v>
+        <v>1822</v>
       </c>
       <c r="D357" t="n">
-        <v>2717416</v>
+        <v>2724916</v>
       </c>
       <c r="E357" t="inlineStr">
         <is>
@@ -17710,10 +17710,10 @@
         </is>
       </c>
       <c r="C362" t="n">
-        <v>16321</v>
+        <v>16330</v>
       </c>
       <c r="D362" t="n">
-        <v>22274455</v>
+        <v>22285736</v>
       </c>
       <c r="E362" t="inlineStr">
         <is>
@@ -17758,10 +17758,10 @@
         </is>
       </c>
       <c r="C363" t="n">
-        <v>3951</v>
+        <v>3954</v>
       </c>
       <c r="D363" t="n">
-        <v>5755510</v>
+        <v>5759910</v>
       </c>
       <c r="E363" t="inlineStr">
         <is>
@@ -17806,10 +17806,10 @@
         </is>
       </c>
       <c r="C364" t="n">
-        <v>11450</v>
+        <v>11457</v>
       </c>
       <c r="D364" t="n">
-        <v>16850328</v>
+        <v>16860828</v>
       </c>
       <c r="E364" t="inlineStr">
         <is>
@@ -17854,10 +17854,10 @@
         </is>
       </c>
       <c r="C365" t="n">
-        <v>4376</v>
+        <v>4378</v>
       </c>
       <c r="D365" t="n">
-        <v>6498827</v>
+        <v>6501827</v>
       </c>
       <c r="E365" t="inlineStr">
         <is>
@@ -17950,10 +17950,10 @@
         </is>
       </c>
       <c r="C367" t="n">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="D367" t="n">
-        <v>357000</v>
+        <v>358500</v>
       </c>
       <c r="E367" t="inlineStr">
         <is>
@@ -18046,10 +18046,10 @@
         </is>
       </c>
       <c r="C369" t="n">
-        <v>3903</v>
+        <v>3904</v>
       </c>
       <c r="D369" t="n">
-        <v>5349664</v>
+        <v>5351164</v>
       </c>
       <c r="E369" t="inlineStr">
         <is>
@@ -18094,10 +18094,10 @@
         </is>
       </c>
       <c r="C370" t="n">
-        <v>4706</v>
+        <v>4715</v>
       </c>
       <c r="D370" t="n">
-        <v>6848214</v>
+        <v>6861714</v>
       </c>
       <c r="E370" t="inlineStr">
         <is>
@@ -18142,10 +18142,10 @@
         </is>
       </c>
       <c r="C371" t="n">
-        <v>17189</v>
+        <v>17207</v>
       </c>
       <c r="D371" t="n">
-        <v>25336611</v>
+        <v>25363611</v>
       </c>
       <c r="E371" t="inlineStr">
         <is>
@@ -18190,10 +18190,10 @@
         </is>
       </c>
       <c r="C372" t="n">
-        <v>8244</v>
+        <v>8249</v>
       </c>
       <c r="D372" t="n">
-        <v>12294625</v>
+        <v>12302125</v>
       </c>
       <c r="E372" t="inlineStr">
         <is>
@@ -18238,10 +18238,10 @@
         </is>
       </c>
       <c r="C373" t="n">
-        <v>2317</v>
+        <v>2319</v>
       </c>
       <c r="D373" t="n">
-        <v>3464388</v>
+        <v>3467388</v>
       </c>
       <c r="E373" t="inlineStr">
         <is>
@@ -18286,10 +18286,10 @@
         </is>
       </c>
       <c r="C374" t="n">
-        <v>564</v>
+        <v>565</v>
       </c>
       <c r="D374" t="n">
-        <v>843095</v>
+        <v>844595</v>
       </c>
       <c r="E374" t="inlineStr">
         <is>
@@ -18382,10 +18382,10 @@
         </is>
       </c>
       <c r="C376" t="n">
-        <v>4827</v>
+        <v>4834</v>
       </c>
       <c r="D376" t="n">
-        <v>6551409</v>
+        <v>6560775</v>
       </c>
       <c r="E376" t="inlineStr">
         <is>
@@ -18430,10 +18430,10 @@
         </is>
       </c>
       <c r="C377" t="n">
-        <v>4294</v>
+        <v>4295</v>
       </c>
       <c r="D377" t="n">
-        <v>6260776</v>
+        <v>6262276</v>
       </c>
       <c r="E377" t="inlineStr">
         <is>
@@ -18478,10 +18478,10 @@
         </is>
       </c>
       <c r="C378" t="n">
-        <v>12617</v>
+        <v>12626</v>
       </c>
       <c r="D378" t="n">
-        <v>18586792</v>
+        <v>18600292</v>
       </c>
       <c r="E378" t="inlineStr">
         <is>
@@ -18526,10 +18526,10 @@
         </is>
       </c>
       <c r="C379" t="n">
-        <v>5290</v>
+        <v>5294</v>
       </c>
       <c r="D379" t="n">
-        <v>7886107</v>
+        <v>7892107</v>
       </c>
       <c r="E379" t="inlineStr">
         <is>
@@ -18574,10 +18574,10 @@
         </is>
       </c>
       <c r="C380" t="n">
-        <v>1514</v>
+        <v>1517</v>
       </c>
       <c r="D380" t="n">
-        <v>2260742</v>
+        <v>2265242</v>
       </c>
       <c r="E380" t="inlineStr">
         <is>
@@ -18718,10 +18718,10 @@
         </is>
       </c>
       <c r="C383" t="n">
-        <v>4420</v>
+        <v>4423</v>
       </c>
       <c r="D383" t="n">
-        <v>6072511</v>
+        <v>6077011</v>
       </c>
       <c r="E383" t="inlineStr">
         <is>
@@ -18766,10 +18766,10 @@
         </is>
       </c>
       <c r="C384" t="n">
-        <v>3259</v>
+        <v>3261</v>
       </c>
       <c r="D384" t="n">
-        <v>4755714</v>
+        <v>4758714</v>
       </c>
       <c r="E384" t="inlineStr">
         <is>
@@ -18814,10 +18814,10 @@
         </is>
       </c>
       <c r="C385" t="n">
-        <v>10551</v>
+        <v>10563</v>
       </c>
       <c r="D385" t="n">
-        <v>15568589</v>
+        <v>15586589</v>
       </c>
       <c r="E385" t="inlineStr">
         <is>
@@ -18862,10 +18862,10 @@
         </is>
       </c>
       <c r="C386" t="n">
-        <v>4501</v>
+        <v>4511</v>
       </c>
       <c r="D386" t="n">
-        <v>6694772</v>
+        <v>6709772</v>
       </c>
       <c r="E386" t="inlineStr">
         <is>
@@ -18910,10 +18910,10 @@
         </is>
       </c>
       <c r="C387" t="n">
-        <v>1279</v>
+        <v>1282</v>
       </c>
       <c r="D387" t="n">
-        <v>1909616</v>
+        <v>1914116</v>
       </c>
       <c r="E387" t="inlineStr">
         <is>
@@ -18958,10 +18958,10 @@
         </is>
       </c>
       <c r="C388" t="n">
-        <v>279</v>
+        <v>280</v>
       </c>
       <c r="D388" t="n">
-        <v>416100</v>
+        <v>417600</v>
       </c>
       <c r="E388" t="inlineStr">
         <is>
@@ -19054,10 +19054,10 @@
         </is>
       </c>
       <c r="C390" t="n">
-        <v>3478</v>
+        <v>3479</v>
       </c>
       <c r="D390" t="n">
-        <v>4719923</v>
+        <v>4721423</v>
       </c>
       <c r="E390" t="inlineStr">
         <is>
@@ -19102,10 +19102,10 @@
         </is>
       </c>
       <c r="C391" t="n">
-        <v>3797</v>
+        <v>3802</v>
       </c>
       <c r="D391" t="n">
-        <v>5535778</v>
+        <v>5543278</v>
       </c>
       <c r="E391" t="inlineStr">
         <is>
@@ -19150,10 +19150,10 @@
         </is>
       </c>
       <c r="C392" t="n">
-        <v>10443</v>
+        <v>10446</v>
       </c>
       <c r="D392" t="n">
-        <v>15392725</v>
+        <v>15397225</v>
       </c>
       <c r="E392" t="inlineStr">
         <is>
@@ -19198,10 +19198,10 @@
         </is>
       </c>
       <c r="C393" t="n">
-        <v>4039</v>
+        <v>4041</v>
       </c>
       <c r="D393" t="n">
-        <v>6011355</v>
+        <v>6014355</v>
       </c>
       <c r="E393" t="inlineStr">
         <is>
@@ -19390,10 +19390,10 @@
         </is>
       </c>
       <c r="C397" t="n">
-        <v>3794</v>
+        <v>3795</v>
       </c>
       <c r="D397" t="n">
-        <v>5217068</v>
+        <v>5218568</v>
       </c>
       <c r="E397" t="inlineStr">
         <is>
@@ -19438,10 +19438,10 @@
         </is>
       </c>
       <c r="C398" t="n">
-        <v>4078</v>
+        <v>4082</v>
       </c>
       <c r="D398" t="n">
-        <v>5915259</v>
+        <v>5920669</v>
       </c>
       <c r="E398" t="inlineStr">
         <is>
@@ -19486,10 +19486,10 @@
         </is>
       </c>
       <c r="C399" t="n">
-        <v>10578</v>
+        <v>10585</v>
       </c>
       <c r="D399" t="n">
-        <v>15549460</v>
+        <v>15559960</v>
       </c>
       <c r="E399" t="inlineStr">
         <is>
@@ -19534,10 +19534,10 @@
         </is>
       </c>
       <c r="C400" t="n">
-        <v>3623</v>
+        <v>3624</v>
       </c>
       <c r="D400" t="n">
-        <v>5400581</v>
+        <v>5402081</v>
       </c>
       <c r="E400" t="inlineStr">
         <is>
@@ -19822,10 +19822,10 @@
         </is>
       </c>
       <c r="C406" t="n">
-        <v>1384</v>
+        <v>1385</v>
       </c>
       <c r="D406" t="n">
-        <v>2000490</v>
+        <v>2001990</v>
       </c>
       <c r="E406" t="inlineStr">
         <is>
@@ -19870,10 +19870,10 @@
         </is>
       </c>
       <c r="C407" t="n">
-        <v>4580</v>
+        <v>4588</v>
       </c>
       <c r="D407" t="n">
-        <v>6749465</v>
+        <v>6761465</v>
       </c>
       <c r="E407" t="inlineStr">
         <is>
@@ -19918,10 +19918,10 @@
         </is>
       </c>
       <c r="C408" t="n">
-        <v>1776</v>
+        <v>1778</v>
       </c>
       <c r="D408" t="n">
-        <v>2648616</v>
+        <v>2651616</v>
       </c>
       <c r="E408" t="inlineStr">
         <is>
@@ -20158,10 +20158,10 @@
         </is>
       </c>
       <c r="C413" t="n">
-        <v>3035</v>
+        <v>3041</v>
       </c>
       <c r="D413" t="n">
-        <v>4030233</v>
+        <v>4037232</v>
       </c>
       <c r="E413" t="inlineStr">
         <is>
@@ -20206,10 +20206,10 @@
         </is>
       </c>
       <c r="C414" t="n">
-        <v>514</v>
+        <v>517</v>
       </c>
       <c r="D414" t="n">
-        <v>766464</v>
+        <v>770964</v>
       </c>
       <c r="E414" t="inlineStr">
         <is>
@@ -20254,10 +20254,10 @@
         </is>
       </c>
       <c r="C415" t="n">
-        <v>264</v>
+        <v>266</v>
       </c>
       <c r="D415" t="n">
-        <v>394265</v>
+        <v>397265</v>
       </c>
       <c r="E415" t="inlineStr">
         <is>
@@ -20446,10 +20446,10 @@
         </is>
       </c>
       <c r="C419" t="n">
-        <v>2881</v>
+        <v>2882</v>
       </c>
       <c r="D419" t="n">
-        <v>4183874</v>
+        <v>4185374</v>
       </c>
       <c r="E419" t="inlineStr">
         <is>
@@ -20494,10 +20494,10 @@
         </is>
       </c>
       <c r="C420" t="n">
-        <v>6977</v>
+        <v>6978</v>
       </c>
       <c r="D420" t="n">
-        <v>10246732</v>
+        <v>10248232</v>
       </c>
       <c r="E420" t="inlineStr">
         <is>
@@ -20590,10 +20590,10 @@
         </is>
       </c>
       <c r="C422" t="n">
-        <v>673</v>
+        <v>674</v>
       </c>
       <c r="D422" t="n">
-        <v>1004642</v>
+        <v>1006142</v>
       </c>
       <c r="E422" t="inlineStr">
         <is>
@@ -20638,10 +20638,10 @@
         </is>
       </c>
       <c r="C423" t="n">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="D423" t="n">
-        <v>184890</v>
+        <v>186390</v>
       </c>
       <c r="E423" t="inlineStr">
         <is>
@@ -20734,10 +20734,10 @@
         </is>
       </c>
       <c r="C425" t="n">
-        <v>2239</v>
+        <v>2240</v>
       </c>
       <c r="D425" t="n">
-        <v>2993632</v>
+        <v>2994303</v>
       </c>
       <c r="E425" t="inlineStr">
         <is>
@@ -21166,10 +21166,10 @@
         </is>
       </c>
       <c r="C434" t="n">
-        <v>4619</v>
+        <v>4622</v>
       </c>
       <c r="D434" t="n">
-        <v>6790780</v>
+        <v>6795020</v>
       </c>
       <c r="E434" t="inlineStr">
         <is>
@@ -21358,10 +21358,10 @@
         </is>
       </c>
       <c r="C438" t="n">
-        <v>1526</v>
+        <v>1529</v>
       </c>
       <c r="D438" t="n">
-        <v>2015897</v>
+        <v>2020397</v>
       </c>
       <c r="E438" t="inlineStr">
         <is>
@@ -21406,10 +21406,10 @@
         </is>
       </c>
       <c r="C439" t="n">
-        <v>869</v>
+        <v>870</v>
       </c>
       <c r="D439" t="n">
-        <v>1265959</v>
+        <v>1267459</v>
       </c>
       <c r="E439" t="inlineStr">
         <is>
@@ -21454,10 +21454,10 @@
         </is>
       </c>
       <c r="C440" t="n">
-        <v>2533</v>
+        <v>2534</v>
       </c>
       <c r="D440" t="n">
-        <v>3719457</v>
+        <v>3720957</v>
       </c>
       <c r="E440" t="inlineStr">
         <is>
@@ -21694,10 +21694,10 @@
         </is>
       </c>
       <c r="C445" t="n">
-        <v>2844</v>
+        <v>2847</v>
       </c>
       <c r="D445" t="n">
-        <v>4138927</v>
+        <v>4143079</v>
       </c>
       <c r="E445" t="inlineStr">
         <is>
@@ -21742,10 +21742,10 @@
         </is>
       </c>
       <c r="C446" t="n">
-        <v>8920</v>
+        <v>8926</v>
       </c>
       <c r="D446" t="n">
-        <v>13142592</v>
+        <v>13151592</v>
       </c>
       <c r="E446" t="inlineStr">
         <is>
@@ -21982,10 +21982,10 @@
         </is>
       </c>
       <c r="C451" t="n">
-        <v>2789</v>
+        <v>2790</v>
       </c>
       <c r="D451" t="n">
-        <v>3661544</v>
+        <v>3663044</v>
       </c>
       <c r="E451" t="inlineStr">
         <is>
@@ -22414,10 +22414,10 @@
         </is>
       </c>
       <c r="C460" t="n">
-        <v>7861</v>
+        <v>7862</v>
       </c>
       <c r="D460" t="n">
-        <v>11536981</v>
+        <v>11538481</v>
       </c>
       <c r="E460" t="inlineStr">
         <is>
@@ -22654,10 +22654,10 @@
         </is>
       </c>
       <c r="C465" t="n">
-        <v>2604</v>
+        <v>2607</v>
       </c>
       <c r="D465" t="n">
-        <v>3485704</v>
+        <v>3490202</v>
       </c>
       <c r="E465" t="inlineStr">
         <is>
@@ -22942,10 +22942,10 @@
         </is>
       </c>
       <c r="C471" t="n">
-        <v>1272</v>
+        <v>1273</v>
       </c>
       <c r="D471" t="n">
-        <v>1700797</v>
+        <v>1702279</v>
       </c>
       <c r="E471" t="inlineStr">
         <is>
@@ -23278,10 +23278,10 @@
         </is>
       </c>
       <c r="C478" t="n">
-        <v>868</v>
+        <v>871</v>
       </c>
       <c r="D478" t="n">
-        <v>1265559</v>
+        <v>1269459</v>
       </c>
       <c r="E478" t="inlineStr">
         <is>
@@ -23326,10 +23326,10 @@
         </is>
       </c>
       <c r="C479" t="n">
-        <v>2730</v>
+        <v>2731</v>
       </c>
       <c r="D479" t="n">
-        <v>4024445</v>
+        <v>4025945</v>
       </c>
       <c r="E479" t="inlineStr">
         <is>
@@ -23422,10 +23422,10 @@
         </is>
       </c>
       <c r="C481" t="n">
-        <v>232</v>
+        <v>235</v>
       </c>
       <c r="D481" t="n">
-        <v>347281</v>
+        <v>351781</v>
       </c>
       <c r="E481" t="inlineStr">
         <is>
@@ -23566,10 +23566,10 @@
         </is>
       </c>
       <c r="C484" t="n">
-        <v>2551</v>
+        <v>2555</v>
       </c>
       <c r="D484" t="n">
-        <v>3657469</v>
+        <v>3661535</v>
       </c>
       <c r="E484" t="inlineStr">
         <is>
@@ -23614,10 +23614,10 @@
         </is>
       </c>
       <c r="C485" t="n">
-        <v>5026</v>
+        <v>5028</v>
       </c>
       <c r="D485" t="n">
-        <v>7364865</v>
+        <v>7365285</v>
       </c>
       <c r="E485" t="inlineStr">
         <is>
@@ -23902,10 +23902,10 @@
         </is>
       </c>
       <c r="C491" t="n">
-        <v>8203</v>
+        <v>8205</v>
       </c>
       <c r="D491" t="n">
-        <v>11892618</v>
+        <v>11894323</v>
       </c>
       <c r="E491" t="inlineStr">
         <is>
@@ -23950,10 +23950,10 @@
         </is>
       </c>
       <c r="C492" t="n">
-        <v>17315</v>
+        <v>17321</v>
       </c>
       <c r="D492" t="n">
-        <v>25371306</v>
+        <v>25379256</v>
       </c>
       <c r="E492" t="inlineStr">
         <is>
@@ -23998,10 +23998,10 @@
         </is>
       </c>
       <c r="C493" t="n">
-        <v>5922</v>
+        <v>5926</v>
       </c>
       <c r="D493" t="n">
-        <v>8812851</v>
+        <v>8818139</v>
       </c>
       <c r="E493" t="inlineStr">
         <is>
@@ -24046,10 +24046,10 @@
         </is>
       </c>
       <c r="C494" t="n">
-        <v>1834</v>
+        <v>1835</v>
       </c>
       <c r="D494" t="n">
-        <v>2735699</v>
+        <v>2737199</v>
       </c>
       <c r="E494" t="inlineStr">
         <is>
@@ -24094,10 +24094,10 @@
         </is>
       </c>
       <c r="C495" t="n">
-        <v>359</v>
+        <v>360</v>
       </c>
       <c r="D495" t="n">
-        <v>538115</v>
+        <v>539615</v>
       </c>
       <c r="E495" t="inlineStr">
         <is>
@@ -24286,10 +24286,10 @@
         </is>
       </c>
       <c r="C499" t="n">
-        <v>6187</v>
+        <v>6195</v>
       </c>
       <c r="D499" t="n">
-        <v>8405766</v>
+        <v>8417297</v>
       </c>
       <c r="E499" t="inlineStr">
         <is>
@@ -24430,10 +24430,10 @@
         </is>
       </c>
       <c r="C502" t="n">
-        <v>1007</v>
+        <v>1008</v>
       </c>
       <c r="D502" t="n">
-        <v>1499741</v>
+        <v>1501241</v>
       </c>
       <c r="E502" t="inlineStr">
         <is>
@@ -24574,10 +24574,10 @@
         </is>
       </c>
       <c r="C505" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D505" t="n">
-        <v>4500</v>
+        <v>6000</v>
       </c>
       <c r="E505" t="inlineStr">
         <is>
@@ -24670,10 +24670,10 @@
         </is>
       </c>
       <c r="C507" t="n">
-        <v>2708</v>
+        <v>2709</v>
       </c>
       <c r="D507" t="n">
-        <v>3891139</v>
+        <v>3892639</v>
       </c>
       <c r="E507" t="inlineStr">
         <is>
@@ -24718,10 +24718,10 @@
         </is>
       </c>
       <c r="C508" t="n">
-        <v>4718</v>
+        <v>4719</v>
       </c>
       <c r="D508" t="n">
-        <v>6909603</v>
+        <v>6910116</v>
       </c>
       <c r="E508" t="inlineStr">
         <is>
@@ -24814,10 +24814,10 @@
         </is>
       </c>
       <c r="C510" t="n">
-        <v>366</v>
+        <v>367</v>
       </c>
       <c r="D510" t="n">
-        <v>545373</v>
+        <v>546873</v>
       </c>
       <c r="E510" t="inlineStr">
         <is>
@@ -25006,10 +25006,10 @@
         </is>
       </c>
       <c r="C514" t="n">
-        <v>1497</v>
+        <v>1498</v>
       </c>
       <c r="D514" t="n">
-        <v>2159168</v>
+        <v>2160668</v>
       </c>
       <c r="E514" t="inlineStr">
         <is>
@@ -25054,10 +25054,10 @@
         </is>
       </c>
       <c r="C515" t="n">
-        <v>3260</v>
+        <v>3261</v>
       </c>
       <c r="D515" t="n">
-        <v>4766926</v>
+        <v>4768426</v>
       </c>
       <c r="E515" t="inlineStr">
         <is>
@@ -25246,10 +25246,10 @@
         </is>
       </c>
       <c r="C519" t="n">
-        <v>1382</v>
+        <v>1384</v>
       </c>
       <c r="D519" t="n">
-        <v>1872166</v>
+        <v>1875166</v>
       </c>
       <c r="E519" t="inlineStr">
         <is>
@@ -25342,10 +25342,10 @@
         </is>
       </c>
       <c r="C521" t="n">
-        <v>8706</v>
+        <v>8709</v>
       </c>
       <c r="D521" t="n">
-        <v>12733108</v>
+        <v>12737608</v>
       </c>
       <c r="E521" t="inlineStr">
         <is>
@@ -25390,10 +25390,10 @@
         </is>
       </c>
       <c r="C522" t="n">
-        <v>2927</v>
+        <v>2930</v>
       </c>
       <c r="D522" t="n">
-        <v>4346740</v>
+        <v>4351240</v>
       </c>
       <c r="E522" t="inlineStr">
         <is>
@@ -25630,10 +25630,10 @@
         </is>
       </c>
       <c r="C527" t="n">
-        <v>3418</v>
+        <v>3421</v>
       </c>
       <c r="D527" t="n">
-        <v>4606930</v>
+        <v>4608450</v>
       </c>
       <c r="E527" t="inlineStr">
         <is>
@@ -25678,10 +25678,10 @@
         </is>
       </c>
       <c r="C528" t="n">
-        <v>1086</v>
+        <v>1087</v>
       </c>
       <c r="D528" t="n">
-        <v>1559097</v>
+        <v>1560367</v>
       </c>
       <c r="E528" t="inlineStr">
         <is>
@@ -25726,10 +25726,10 @@
         </is>
       </c>
       <c r="C529" t="n">
-        <v>3210</v>
+        <v>3215</v>
       </c>
       <c r="D529" t="n">
-        <v>4693014</v>
+        <v>4700514</v>
       </c>
       <c r="E529" t="inlineStr">
         <is>
@@ -25774,10 +25774,10 @@
         </is>
       </c>
       <c r="C530" t="n">
-        <v>1075</v>
+        <v>1076</v>
       </c>
       <c r="D530" t="n">
-        <v>1598454</v>
+        <v>1598854</v>
       </c>
       <c r="E530" t="inlineStr">
         <is>
@@ -26302,10 +26302,10 @@
         </is>
       </c>
       <c r="C541" t="n">
-        <v>800</v>
+        <v>801</v>
       </c>
       <c r="D541" t="n">
-        <v>1011158</v>
+        <v>1011598</v>
       </c>
       <c r="E541" t="inlineStr">
         <is>
@@ -26446,10 +26446,10 @@
         </is>
       </c>
       <c r="C544" t="n">
-        <v>1451</v>
+        <v>1453</v>
       </c>
       <c r="D544" t="n">
-        <v>2159109</v>
+        <v>2162109</v>
       </c>
       <c r="E544" t="inlineStr">
         <is>
@@ -26638,10 +26638,10 @@
         </is>
       </c>
       <c r="C548" t="n">
-        <v>1717</v>
+        <v>1721</v>
       </c>
       <c r="D548" t="n">
-        <v>2264575</v>
+        <v>2269040</v>
       </c>
       <c r="E548" t="inlineStr">
         <is>
@@ -26686,10 +26686,10 @@
         </is>
       </c>
       <c r="C549" t="n">
-        <v>1629</v>
+        <v>1630</v>
       </c>
       <c r="D549" t="n">
-        <v>2334759</v>
+        <v>2336259</v>
       </c>
       <c r="E549" t="inlineStr">
         <is>
@@ -26734,10 +26734,10 @@
         </is>
       </c>
       <c r="C550" t="n">
-        <v>3453</v>
+        <v>3458</v>
       </c>
       <c r="D550" t="n">
-        <v>5053839</v>
+        <v>5060040</v>
       </c>
       <c r="E550" t="inlineStr">
         <is>
@@ -26830,10 +26830,10 @@
         </is>
       </c>
       <c r="C552" t="n">
-        <v>279</v>
+        <v>281</v>
       </c>
       <c r="D552" t="n">
-        <v>414072</v>
+        <v>415582</v>
       </c>
       <c r="E552" t="inlineStr">
         <is>
@@ -26974,10 +26974,10 @@
         </is>
       </c>
       <c r="C555" t="n">
-        <v>1844</v>
+        <v>1845</v>
       </c>
       <c r="D555" t="n">
-        <v>2464719</v>
+        <v>2466219</v>
       </c>
       <c r="E555" t="inlineStr">
         <is>
@@ -27070,10 +27070,10 @@
         </is>
       </c>
       <c r="C557" t="n">
-        <v>9685</v>
+        <v>9687</v>
       </c>
       <c r="D557" t="n">
-        <v>14171142</v>
+        <v>14173272</v>
       </c>
       <c r="E557" t="inlineStr">
         <is>
@@ -27118,10 +27118,10 @@
         </is>
       </c>
       <c r="C558" t="n">
-        <v>2743</v>
+        <v>2744</v>
       </c>
       <c r="D558" t="n">
-        <v>4069858</v>
+        <v>4071058</v>
       </c>
       <c r="E558" t="inlineStr">
         <is>
@@ -27166,10 +27166,10 @@
         </is>
       </c>
       <c r="C559" t="n">
-        <v>629</v>
+        <v>631</v>
       </c>
       <c r="D559" t="n">
-        <v>932031</v>
+        <v>935031</v>
       </c>
       <c r="E559" t="inlineStr">
         <is>
@@ -27262,10 +27262,10 @@
         </is>
       </c>
       <c r="C561" t="n">
-        <v>3743</v>
+        <v>3745</v>
       </c>
       <c r="D561" t="n">
-        <v>4986511</v>
+        <v>4987614</v>
       </c>
       <c r="E561" t="inlineStr">
         <is>
@@ -27358,10 +27358,10 @@
         </is>
       </c>
       <c r="C563" t="n">
-        <v>2132</v>
+        <v>2134</v>
       </c>
       <c r="D563" t="n">
-        <v>3111808</v>
+        <v>3114808</v>
       </c>
       <c r="E563" t="inlineStr">
         <is>
@@ -27502,10 +27502,10 @@
         </is>
       </c>
       <c r="C566" t="n">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="D566" t="n">
-        <v>54472</v>
+        <v>57472</v>
       </c>
       <c r="E566" t="inlineStr">
         <is>
@@ -27598,10 +27598,10 @@
         </is>
       </c>
       <c r="C568" t="n">
-        <v>5780</v>
+        <v>5783</v>
       </c>
       <c r="D568" t="n">
-        <v>8360438</v>
+        <v>8363904</v>
       </c>
       <c r="E568" t="inlineStr">
         <is>
@@ -27646,10 +27646,10 @@
         </is>
       </c>
       <c r="C569" t="n">
-        <v>14053</v>
+        <v>14059</v>
       </c>
       <c r="D569" t="n">
-        <v>20619018</v>
+        <v>20628018</v>
       </c>
       <c r="E569" t="inlineStr">
         <is>
@@ -27694,10 +27694,10 @@
         </is>
       </c>
       <c r="C570" t="n">
-        <v>4980</v>
+        <v>4984</v>
       </c>
       <c r="D570" t="n">
-        <v>7400973</v>
+        <v>7406973</v>
       </c>
       <c r="E570" t="inlineStr">
         <is>
@@ -27790,10 +27790,10 @@
         </is>
       </c>
       <c r="C572" t="n">
-        <v>285</v>
+        <v>287</v>
       </c>
       <c r="D572" t="n">
-        <v>426085</v>
+        <v>429085</v>
       </c>
       <c r="E572" t="inlineStr">
         <is>
@@ -27934,10 +27934,10 @@
         </is>
       </c>
       <c r="C575" t="n">
-        <v>5650</v>
+        <v>5658</v>
       </c>
       <c r="D575" t="n">
-        <v>7574845</v>
+        <v>7586375</v>
       </c>
       <c r="E575" t="inlineStr">
         <is>
@@ -28030,10 +28030,10 @@
         </is>
       </c>
       <c r="C577" t="n">
-        <v>2978</v>
+        <v>2981</v>
       </c>
       <c r="D577" t="n">
-        <v>4324792</v>
+        <v>4329292</v>
       </c>
       <c r="E577" t="inlineStr">
         <is>
@@ -28126,10 +28126,10 @@
         </is>
       </c>
       <c r="C579" t="n">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="D579" t="n">
-        <v>359134</v>
+        <v>360634</v>
       </c>
       <c r="E579" t="inlineStr">
         <is>
@@ -28270,10 +28270,10 @@
         </is>
       </c>
       <c r="C582" t="n">
-        <v>7946</v>
+        <v>7949</v>
       </c>
       <c r="D582" t="n">
-        <v>11525304</v>
+        <v>11529804</v>
       </c>
       <c r="E582" t="inlineStr">
         <is>
@@ -28318,10 +28318,10 @@
         </is>
       </c>
       <c r="C583" t="n">
-        <v>17069</v>
+        <v>17075</v>
       </c>
       <c r="D583" t="n">
-        <v>25033251</v>
+        <v>25042251</v>
       </c>
       <c r="E583" t="inlineStr">
         <is>
@@ -28462,10 +28462,10 @@
         </is>
       </c>
       <c r="C586" t="n">
-        <v>237</v>
+        <v>239</v>
       </c>
       <c r="D586" t="n">
-        <v>353543</v>
+        <v>355325</v>
       </c>
       <c r="E586" t="inlineStr">
         <is>
@@ -28558,10 +28558,10 @@
         </is>
       </c>
       <c r="C588" t="n">
-        <v>5587</v>
+        <v>5588</v>
       </c>
       <c r="D588" t="n">
-        <v>7490842</v>
+        <v>7492342</v>
       </c>
       <c r="E588" t="inlineStr">
         <is>
@@ -28654,10 +28654,10 @@
         </is>
       </c>
       <c r="C590" t="n">
-        <v>2128</v>
+        <v>2129</v>
       </c>
       <c r="D590" t="n">
-        <v>3121645</v>
+        <v>3123145</v>
       </c>
       <c r="E590" t="inlineStr">
         <is>
@@ -28942,10 +28942,10 @@
         </is>
       </c>
       <c r="C596" t="n">
-        <v>652</v>
+        <v>653</v>
       </c>
       <c r="D596" t="n">
-        <v>935155</v>
+        <v>936655</v>
       </c>
       <c r="E596" t="inlineStr">
         <is>
@@ -29182,10 +29182,10 @@
         </is>
       </c>
       <c r="C601" t="n">
-        <v>632</v>
+        <v>633</v>
       </c>
       <c r="D601" t="n">
-        <v>873611</v>
+        <v>875111</v>
       </c>
       <c r="E601" t="inlineStr">
         <is>
@@ -29230,10 +29230,10 @@
         </is>
       </c>
       <c r="C602" t="n">
-        <v>3699</v>
+        <v>3700</v>
       </c>
       <c r="D602" t="n">
-        <v>5367714</v>
+        <v>5369214</v>
       </c>
       <c r="E602" t="inlineStr">
         <is>
@@ -29326,10 +29326,10 @@
         </is>
       </c>
       <c r="C604" t="n">
-        <v>1952</v>
+        <v>1954</v>
       </c>
       <c r="D604" t="n">
-        <v>2903350</v>
+        <v>2906350</v>
       </c>
       <c r="E604" t="inlineStr">
         <is>
@@ -29806,10 +29806,10 @@
         </is>
       </c>
       <c r="C614" t="n">
-        <v>1672</v>
+        <v>1674</v>
       </c>
       <c r="D614" t="n">
-        <v>2213836</v>
+        <v>2216188</v>
       </c>
       <c r="E614" t="inlineStr">
         <is>
@@ -30142,10 +30142,10 @@
         </is>
       </c>
       <c r="C621" t="n">
-        <v>1155</v>
+        <v>1156</v>
       </c>
       <c r="D621" t="n">
-        <v>1516956</v>
+        <v>1518456</v>
       </c>
       <c r="E621" t="inlineStr">
         <is>
@@ -30190,10 +30190,10 @@
         </is>
       </c>
       <c r="C622" t="n">
-        <v>4836</v>
+        <v>4839</v>
       </c>
       <c r="D622" t="n">
-        <v>7007296</v>
+        <v>7011796</v>
       </c>
       <c r="E622" t="inlineStr">
         <is>
@@ -30238,10 +30238,10 @@
         </is>
       </c>
       <c r="C623" t="n">
-        <v>11684</v>
+        <v>11694</v>
       </c>
       <c r="D623" t="n">
-        <v>17208224</v>
+        <v>17223124</v>
       </c>
       <c r="E623" t="inlineStr">
         <is>
@@ -30286,10 +30286,10 @@
         </is>
       </c>
       <c r="C624" t="n">
-        <v>4408</v>
+        <v>4409</v>
       </c>
       <c r="D624" t="n">
-        <v>6543953</v>
+        <v>6545453</v>
       </c>
       <c r="E624" t="inlineStr">
         <is>
@@ -30526,10 +30526,10 @@
         </is>
       </c>
       <c r="C629" t="n">
-        <v>2148</v>
+        <v>2150</v>
       </c>
       <c r="D629" t="n">
-        <v>3100953</v>
+        <v>3103953</v>
       </c>
       <c r="E629" t="inlineStr">
         <is>
@@ -30574,10 +30574,10 @@
         </is>
       </c>
       <c r="C630" t="n">
-        <v>6605</v>
+        <v>6607</v>
       </c>
       <c r="D630" t="n">
-        <v>9713114</v>
+        <v>9715464</v>
       </c>
       <c r="E630" t="inlineStr">
         <is>
@@ -31582,10 +31582,10 @@
         </is>
       </c>
       <c r="C651" t="n">
-        <v>3024</v>
+        <v>3025</v>
       </c>
       <c r="D651" t="n">
-        <v>4394040</v>
+        <v>4395540</v>
       </c>
       <c r="E651" t="inlineStr">
         <is>
@@ -31630,10 +31630,10 @@
         </is>
       </c>
       <c r="C652" t="n">
-        <v>6093</v>
+        <v>6095</v>
       </c>
       <c r="D652" t="n">
-        <v>8927248</v>
+        <v>8930248</v>
       </c>
       <c r="E652" t="inlineStr">
         <is>
@@ -31678,10 +31678,10 @@
         </is>
       </c>
       <c r="C653" t="n">
-        <v>2245</v>
+        <v>2246</v>
       </c>
       <c r="D653" t="n">
-        <v>3341689</v>
+        <v>3343189</v>
       </c>
       <c r="E653" t="inlineStr">
         <is>
@@ -31918,10 +31918,10 @@
         </is>
       </c>
       <c r="C658" t="n">
-        <v>1924</v>
+        <v>1927</v>
       </c>
       <c r="D658" t="n">
-        <v>2590357</v>
+        <v>2594237</v>
       </c>
       <c r="E658" t="inlineStr">
         <is>
@@ -31966,10 +31966,10 @@
         </is>
       </c>
       <c r="C659" t="n">
-        <v>1437</v>
+        <v>1438</v>
       </c>
       <c r="D659" t="n">
-        <v>2074259</v>
+        <v>2075759</v>
       </c>
       <c r="E659" t="inlineStr">
         <is>
@@ -32254,10 +32254,10 @@
         </is>
       </c>
       <c r="C665" t="n">
-        <v>1124</v>
+        <v>1125</v>
       </c>
       <c r="D665" t="n">
-        <v>1490948</v>
+        <v>1492061</v>
       </c>
       <c r="E665" t="inlineStr">
         <is>
@@ -32302,10 +32302,10 @@
         </is>
       </c>
       <c r="C666" t="n">
-        <v>7836</v>
+        <v>7846</v>
       </c>
       <c r="D666" t="n">
-        <v>11356503</v>
+        <v>11371503</v>
       </c>
       <c r="E666" t="inlineStr">
         <is>
@@ -32350,10 +32350,10 @@
         </is>
       </c>
       <c r="C667" t="n">
-        <v>19028</v>
+        <v>19040</v>
       </c>
       <c r="D667" t="n">
-        <v>27948902</v>
+        <v>27966902</v>
       </c>
       <c r="E667" t="inlineStr">
         <is>
@@ -32398,10 +32398,10 @@
         </is>
       </c>
       <c r="C668" t="n">
-        <v>5750</v>
+        <v>5752</v>
       </c>
       <c r="D668" t="n">
-        <v>8558811</v>
+        <v>8561811</v>
       </c>
       <c r="E668" t="inlineStr">
         <is>
@@ -32446,10 +32446,10 @@
         </is>
       </c>
       <c r="C669" t="n">
-        <v>1620</v>
+        <v>1621</v>
       </c>
       <c r="D669" t="n">
-        <v>2418787</v>
+        <v>2420287</v>
       </c>
       <c r="E669" t="inlineStr">
         <is>
@@ -32494,10 +32494,10 @@
         </is>
       </c>
       <c r="C670" t="n">
-        <v>363</v>
+        <v>364</v>
       </c>
       <c r="D670" t="n">
-        <v>539606</v>
+        <v>540286</v>
       </c>
       <c r="E670" t="inlineStr">
         <is>
@@ -32590,10 +32590,10 @@
         </is>
       </c>
       <c r="C672" t="n">
-        <v>6860</v>
+        <v>6869</v>
       </c>
       <c r="D672" t="n">
-        <v>9359156</v>
+        <v>9372400</v>
       </c>
       <c r="E672" t="inlineStr">
         <is>
@@ -32638,10 +32638,10 @@
         </is>
       </c>
       <c r="C673" t="n">
-        <v>9768</v>
+        <v>9773</v>
       </c>
       <c r="D673" t="n">
-        <v>14190190</v>
+        <v>14197690</v>
       </c>
       <c r="E673" t="inlineStr">
         <is>
@@ -32686,10 +32686,10 @@
         </is>
       </c>
       <c r="C674" t="n">
-        <v>26552</v>
+        <v>26562</v>
       </c>
       <c r="D674" t="n">
-        <v>39010042</v>
+        <v>39023278</v>
       </c>
       <c r="E674" t="inlineStr">
         <is>
@@ -32734,10 +32734,10 @@
         </is>
       </c>
       <c r="C675" t="n">
-        <v>8426</v>
+        <v>8430</v>
       </c>
       <c r="D675" t="n">
-        <v>12552155</v>
+        <v>12558155</v>
       </c>
       <c r="E675" t="inlineStr">
         <is>
@@ -32782,10 +32782,10 @@
         </is>
       </c>
       <c r="C676" t="n">
-        <v>2228</v>
+        <v>2232</v>
       </c>
       <c r="D676" t="n">
-        <v>3325602</v>
+        <v>3331602</v>
       </c>
       <c r="E676" t="inlineStr">
         <is>
@@ -32830,10 +32830,10 @@
         </is>
       </c>
       <c r="C677" t="n">
-        <v>489</v>
+        <v>490</v>
       </c>
       <c r="D677" t="n">
-        <v>729221</v>
+        <v>730721</v>
       </c>
       <c r="E677" t="inlineStr">
         <is>
@@ -32974,10 +32974,10 @@
         </is>
       </c>
       <c r="C680" t="n">
-        <v>8804</v>
+        <v>8809</v>
       </c>
       <c r="D680" t="n">
-        <v>11941110</v>
+        <v>11948610</v>
       </c>
       <c r="E680" t="inlineStr">
         <is>
@@ -33070,10 +33070,10 @@
         </is>
       </c>
       <c r="C682" t="n">
-        <v>2531</v>
+        <v>2536</v>
       </c>
       <c r="D682" t="n">
-        <v>3693560</v>
+        <v>3701060</v>
       </c>
       <c r="E682" t="inlineStr">
         <is>
@@ -33118,10 +33118,10 @@
         </is>
       </c>
       <c r="C683" t="n">
-        <v>962</v>
+        <v>963</v>
       </c>
       <c r="D683" t="n">
-        <v>1419169</v>
+        <v>1420669</v>
       </c>
       <c r="E683" t="inlineStr">
         <is>
@@ -33310,10 +33310,10 @@
         </is>
       </c>
       <c r="C687" t="n">
-        <v>1876</v>
+        <v>1878</v>
       </c>
       <c r="D687" t="n">
-        <v>2595495</v>
+        <v>2596383</v>
       </c>
       <c r="E687" t="inlineStr">
         <is>
@@ -33358,10 +33358,10 @@
         </is>
       </c>
       <c r="C688" t="n">
-        <v>8375</v>
+        <v>8379</v>
       </c>
       <c r="D688" t="n">
-        <v>12012323</v>
+        <v>12017913</v>
       </c>
       <c r="E688" t="inlineStr">
         <is>
@@ -33406,10 +33406,10 @@
         </is>
       </c>
       <c r="C689" t="n">
-        <v>16103</v>
+        <v>16107</v>
       </c>
       <c r="D689" t="n">
-        <v>23507301</v>
+        <v>23512390</v>
       </c>
       <c r="E689" t="inlineStr">
         <is>
@@ -33694,10 +33694,10 @@
         </is>
       </c>
       <c r="C695" t="n">
-        <v>5353</v>
+        <v>5355</v>
       </c>
       <c r="D695" t="n">
-        <v>7254126</v>
+        <v>7257126</v>
       </c>
       <c r="E695" t="inlineStr">
         <is>
@@ -33742,10 +33742,10 @@
         </is>
       </c>
       <c r="C696" t="n">
-        <v>3501</v>
+        <v>3504</v>
       </c>
       <c r="D696" t="n">
-        <v>5057956</v>
+        <v>5061443</v>
       </c>
       <c r="E696" t="inlineStr">
         <is>
@@ -33790,10 +33790,10 @@
         </is>
       </c>
       <c r="C697" t="n">
-        <v>8998</v>
+        <v>9002</v>
       </c>
       <c r="D697" t="n">
-        <v>13188932</v>
+        <v>13194202</v>
       </c>
       <c r="E697" t="inlineStr">
         <is>
@@ -34030,10 +34030,10 @@
         </is>
       </c>
       <c r="C702" t="n">
-        <v>2993</v>
+        <v>2998</v>
       </c>
       <c r="D702" t="n">
-        <v>3966978</v>
+        <v>3973023</v>
       </c>
       <c r="E702" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
[Fonds de solidarite] Add 2020-08-12 data
</commit_message>
<xml_diff>
--- a/published-data/fonds-solidarite-volet-1-departemental-classe-effectif-latest.xlsx
+++ b/published-data/fonds-solidarite-volet-1-departemental-classe-effectif-latest.xlsx
@@ -478,10 +478,10 @@
         </is>
       </c>
       <c r="C3" t="n">
-        <v>5716</v>
+        <v>5718</v>
       </c>
       <c r="D3" t="n">
-        <v>8396486</v>
+        <v>8399486</v>
       </c>
       <c r="E3" t="inlineStr">
         <is>
@@ -526,10 +526,10 @@
         </is>
       </c>
       <c r="C4" t="n">
-        <v>2044</v>
+        <v>2046</v>
       </c>
       <c r="D4" t="n">
-        <v>3036032</v>
+        <v>3039032</v>
       </c>
       <c r="E4" t="inlineStr">
         <is>
@@ -814,10 +814,10 @@
         </is>
       </c>
       <c r="C10" t="n">
-        <v>3558</v>
+        <v>3560</v>
       </c>
       <c r="D10" t="n">
-        <v>5201674</v>
+        <v>5204674</v>
       </c>
       <c r="E10" t="inlineStr">
         <is>
@@ -862,10 +862,10 @@
         </is>
       </c>
       <c r="C11" t="n">
-        <v>925</v>
+        <v>926</v>
       </c>
       <c r="D11" t="n">
-        <v>1364322</v>
+        <v>1364359</v>
       </c>
       <c r="E11" t="inlineStr">
         <is>
@@ -1006,10 +1006,10 @@
         </is>
       </c>
       <c r="C14" t="n">
-        <v>1937</v>
+        <v>1940</v>
       </c>
       <c r="D14" t="n">
-        <v>2552795</v>
+        <v>2556652</v>
       </c>
       <c r="E14" t="inlineStr">
         <is>
@@ -1438,10 +1438,10 @@
         </is>
       </c>
       <c r="C23" t="n">
-        <v>1927</v>
+        <v>1930</v>
       </c>
       <c r="D23" t="n">
-        <v>2794549</v>
+        <v>2799049</v>
       </c>
       <c r="E23" t="inlineStr">
         <is>
@@ -1534,10 +1534,10 @@
         </is>
       </c>
       <c r="C25" t="n">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="D25" t="n">
-        <v>200763</v>
+        <v>202263</v>
       </c>
       <c r="E25" t="inlineStr">
         <is>
@@ -1678,10 +1678,10 @@
         </is>
       </c>
       <c r="C28" t="n">
-        <v>2146</v>
+        <v>2149</v>
       </c>
       <c r="D28" t="n">
-        <v>2986627</v>
+        <v>2990283</v>
       </c>
       <c r="E28" t="inlineStr">
         <is>
@@ -1726,10 +1726,10 @@
         </is>
       </c>
       <c r="C29" t="n">
-        <v>3180</v>
+        <v>3183</v>
       </c>
       <c r="D29" t="n">
-        <v>4598685</v>
+        <v>4603185</v>
       </c>
       <c r="E29" t="inlineStr">
         <is>
@@ -1774,10 +1774,10 @@
         </is>
       </c>
       <c r="C30" t="n">
-        <v>6417</v>
+        <v>6422</v>
       </c>
       <c r="D30" t="n">
-        <v>9391146</v>
+        <v>9398646</v>
       </c>
       <c r="E30" t="inlineStr">
         <is>
@@ -2014,10 +2014,10 @@
         </is>
       </c>
       <c r="C35" t="n">
-        <v>2506</v>
+        <v>2509</v>
       </c>
       <c r="D35" t="n">
-        <v>3208290</v>
+        <v>3212790</v>
       </c>
       <c r="E35" t="inlineStr">
         <is>
@@ -2398,10 +2398,10 @@
         </is>
       </c>
       <c r="C43" t="n">
-        <v>3979</v>
+        <v>3980</v>
       </c>
       <c r="D43" t="n">
-        <v>5785635</v>
+        <v>5787135</v>
       </c>
       <c r="E43" t="inlineStr">
         <is>
@@ -2446,10 +2446,10 @@
         </is>
       </c>
       <c r="C44" t="n">
-        <v>8938</v>
+        <v>8940</v>
       </c>
       <c r="D44" t="n">
-        <v>13100163</v>
+        <v>13103163</v>
       </c>
       <c r="E44" t="inlineStr">
         <is>
@@ -2590,10 +2590,10 @@
         </is>
       </c>
       <c r="C47" t="n">
-        <v>327</v>
+        <v>329</v>
       </c>
       <c r="D47" t="n">
-        <v>486450</v>
+        <v>489450</v>
       </c>
       <c r="E47" t="inlineStr">
         <is>
@@ -2686,10 +2686,10 @@
         </is>
       </c>
       <c r="C49" t="n">
-        <v>4987</v>
+        <v>4992</v>
       </c>
       <c r="D49" t="n">
-        <v>6824845</v>
+        <v>6830895</v>
       </c>
       <c r="E49" t="inlineStr">
         <is>
@@ -2734,10 +2734,10 @@
         </is>
       </c>
       <c r="C50" t="n">
-        <v>5826</v>
+        <v>5830</v>
       </c>
       <c r="D50" t="n">
-        <v>8431626</v>
+        <v>8437610</v>
       </c>
       <c r="E50" t="inlineStr">
         <is>
@@ -2782,10 +2782,10 @@
         </is>
       </c>
       <c r="C51" t="n">
-        <v>13606</v>
+        <v>13613</v>
       </c>
       <c r="D51" t="n">
-        <v>20006634</v>
+        <v>20016173</v>
       </c>
       <c r="E51" t="inlineStr">
         <is>
@@ -2830,10 +2830,10 @@
         </is>
       </c>
       <c r="C52" t="n">
-        <v>4619</v>
+        <v>4620</v>
       </c>
       <c r="D52" t="n">
-        <v>6840250</v>
+        <v>6841750</v>
       </c>
       <c r="E52" t="inlineStr">
         <is>
@@ -2926,10 +2926,10 @@
         </is>
       </c>
       <c r="C54" t="n">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="D54" t="n">
-        <v>392366</v>
+        <v>393866</v>
       </c>
       <c r="E54" t="inlineStr">
         <is>
@@ -3070,10 +3070,10 @@
         </is>
       </c>
       <c r="C57" t="n">
-        <v>5618</v>
+        <v>5621</v>
       </c>
       <c r="D57" t="n">
-        <v>7696421</v>
+        <v>7699676</v>
       </c>
       <c r="E57" t="inlineStr">
         <is>
@@ -3166,10 +3166,10 @@
         </is>
       </c>
       <c r="C59" t="n">
-        <v>7824</v>
+        <v>7825</v>
       </c>
       <c r="D59" t="n">
-        <v>11469579</v>
+        <v>11471079</v>
       </c>
       <c r="E59" t="inlineStr">
         <is>
@@ -3214,10 +3214,10 @@
         </is>
       </c>
       <c r="C60" t="n">
-        <v>2488</v>
+        <v>2489</v>
       </c>
       <c r="D60" t="n">
-        <v>3667032</v>
+        <v>3668532</v>
       </c>
       <c r="E60" t="inlineStr">
         <is>
@@ -3406,10 +3406,10 @@
         </is>
       </c>
       <c r="C64" t="n">
-        <v>3378</v>
+        <v>3379</v>
       </c>
       <c r="D64" t="n">
-        <v>4406164</v>
+        <v>4407014</v>
       </c>
       <c r="E64" t="inlineStr">
         <is>
@@ -3454,10 +3454,10 @@
         </is>
       </c>
       <c r="C65" t="n">
-        <v>2684</v>
+        <v>2685</v>
       </c>
       <c r="D65" t="n">
-        <v>3857116</v>
+        <v>3857737</v>
       </c>
       <c r="E65" t="inlineStr">
         <is>
@@ -3502,10 +3502,10 @@
         </is>
       </c>
       <c r="C66" t="n">
-        <v>7023</v>
+        <v>7024</v>
       </c>
       <c r="D66" t="n">
-        <v>10274310</v>
+        <v>10275810</v>
       </c>
       <c r="E66" t="inlineStr">
         <is>
@@ -3598,10 +3598,10 @@
         </is>
       </c>
       <c r="C68" t="n">
-        <v>656</v>
+        <v>657</v>
       </c>
       <c r="D68" t="n">
-        <v>972698</v>
+        <v>974198</v>
       </c>
       <c r="E68" t="inlineStr">
         <is>
@@ -3742,10 +3742,10 @@
         </is>
       </c>
       <c r="C71" t="n">
-        <v>3001</v>
+        <v>3003</v>
       </c>
       <c r="D71" t="n">
-        <v>3963495</v>
+        <v>3966495</v>
       </c>
       <c r="E71" t="inlineStr">
         <is>
@@ -3790,10 +3790,10 @@
         </is>
       </c>
       <c r="C72" t="n">
-        <v>9138</v>
+        <v>9141</v>
       </c>
       <c r="D72" t="n">
-        <v>13252770</v>
+        <v>13257270</v>
       </c>
       <c r="E72" t="inlineStr">
         <is>
@@ -3838,10 +3838,10 @@
         </is>
       </c>
       <c r="C73" t="n">
-        <v>22444</v>
+        <v>22458</v>
       </c>
       <c r="D73" t="n">
-        <v>32972475</v>
+        <v>32993475</v>
       </c>
       <c r="E73" t="inlineStr">
         <is>
@@ -3886,10 +3886,10 @@
         </is>
       </c>
       <c r="C74" t="n">
-        <v>7733</v>
+        <v>7737</v>
       </c>
       <c r="D74" t="n">
-        <v>11479401</v>
+        <v>11485401</v>
       </c>
       <c r="E74" t="inlineStr">
         <is>
@@ -4222,10 +4222,10 @@
         </is>
       </c>
       <c r="C81" t="n">
-        <v>7441</v>
+        <v>7448</v>
       </c>
       <c r="D81" t="n">
-        <v>10233045</v>
+        <v>10241246</v>
       </c>
       <c r="E81" t="inlineStr">
         <is>
@@ -4270,10 +4270,10 @@
         </is>
       </c>
       <c r="C82" t="n">
-        <v>2758</v>
+        <v>2760</v>
       </c>
       <c r="D82" t="n">
-        <v>3998857</v>
+        <v>4001857</v>
       </c>
       <c r="E82" t="inlineStr">
         <is>
@@ -4366,10 +4366,10 @@
         </is>
       </c>
       <c r="C84" t="n">
-        <v>2870</v>
+        <v>2872</v>
       </c>
       <c r="D84" t="n">
-        <v>4253144</v>
+        <v>4256144</v>
       </c>
       <c r="E84" t="inlineStr">
         <is>
@@ -4558,10 +4558,10 @@
         </is>
       </c>
       <c r="C88" t="n">
-        <v>6455</v>
+        <v>6458</v>
       </c>
       <c r="D88" t="n">
-        <v>9062173</v>
+        <v>9065362</v>
       </c>
       <c r="E88" t="inlineStr">
         <is>
@@ -4606,10 +4606,10 @@
         </is>
       </c>
       <c r="C89" t="n">
-        <v>1919</v>
+        <v>1922</v>
       </c>
       <c r="D89" t="n">
-        <v>2788460</v>
+        <v>2792960</v>
       </c>
       <c r="E89" t="inlineStr">
         <is>
@@ -4654,10 +4654,10 @@
         </is>
       </c>
       <c r="C90" t="n">
-        <v>4916</v>
+        <v>4917</v>
       </c>
       <c r="D90" t="n">
-        <v>7220728</v>
+        <v>7222228</v>
       </c>
       <c r="E90" t="inlineStr">
         <is>
@@ -4894,10 +4894,10 @@
         </is>
       </c>
       <c r="C95" t="n">
-        <v>1990</v>
+        <v>1991</v>
       </c>
       <c r="D95" t="n">
-        <v>2618233</v>
+        <v>2619653</v>
       </c>
       <c r="E95" t="inlineStr">
         <is>
@@ -4942,10 +4942,10 @@
         </is>
       </c>
       <c r="C96" t="n">
-        <v>1703</v>
+        <v>1704</v>
       </c>
       <c r="D96" t="n">
-        <v>2461784</v>
+        <v>2463284</v>
       </c>
       <c r="E96" t="inlineStr">
         <is>
@@ -4990,10 +4990,10 @@
         </is>
       </c>
       <c r="C97" t="n">
-        <v>4538</v>
+        <v>4540</v>
       </c>
       <c r="D97" t="n">
-        <v>6659776</v>
+        <v>6662776</v>
       </c>
       <c r="E97" t="inlineStr">
         <is>
@@ -5662,10 +5662,10 @@
         </is>
       </c>
       <c r="C111" t="n">
-        <v>2669</v>
+        <v>2670</v>
       </c>
       <c r="D111" t="n">
-        <v>3914001</v>
+        <v>3915501</v>
       </c>
       <c r="E111" t="inlineStr">
         <is>
@@ -5710,10 +5710,10 @@
         </is>
       </c>
       <c r="C112" t="n">
-        <v>798</v>
+        <v>799</v>
       </c>
       <c r="D112" t="n">
-        <v>1177719</v>
+        <v>1178825</v>
       </c>
       <c r="E112" t="inlineStr">
         <is>
@@ -5758,10 +5758,10 @@
         </is>
       </c>
       <c r="C113" t="n">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="D113" t="n">
-        <v>309737</v>
+        <v>311019</v>
       </c>
       <c r="E113" t="inlineStr">
         <is>
@@ -6286,10 +6286,10 @@
         </is>
       </c>
       <c r="C124" t="n">
-        <v>5742</v>
+        <v>5745</v>
       </c>
       <c r="D124" t="n">
-        <v>8414304</v>
+        <v>8418804</v>
       </c>
       <c r="E124" t="inlineStr">
         <is>
@@ -6478,10 +6478,10 @@
         </is>
       </c>
       <c r="C128" t="n">
-        <v>2462</v>
+        <v>2463</v>
       </c>
       <c r="D128" t="n">
-        <v>3316586</v>
+        <v>3318086</v>
       </c>
       <c r="E128" t="inlineStr">
         <is>
@@ -6574,10 +6574,10 @@
         </is>
       </c>
       <c r="C130" t="n">
-        <v>1125</v>
+        <v>1126</v>
       </c>
       <c r="D130" t="n">
-        <v>1647890</v>
+        <v>1649390</v>
       </c>
       <c r="E130" t="inlineStr">
         <is>
@@ -6862,10 +6862,10 @@
         </is>
       </c>
       <c r="C136" t="n">
-        <v>3254</v>
+        <v>3255</v>
       </c>
       <c r="D136" t="n">
-        <v>4777078</v>
+        <v>4778578</v>
       </c>
       <c r="E136" t="inlineStr">
         <is>
@@ -6910,10 +6910,10 @@
         </is>
       </c>
       <c r="C137" t="n">
-        <v>937</v>
+        <v>938</v>
       </c>
       <c r="D137" t="n">
-        <v>1393524</v>
+        <v>1395024</v>
       </c>
       <c r="E137" t="inlineStr">
         <is>
@@ -7150,10 +7150,10 @@
         </is>
       </c>
       <c r="C142" t="n">
-        <v>2645</v>
+        <v>2646</v>
       </c>
       <c r="D142" t="n">
-        <v>3823741</v>
+        <v>3825241</v>
       </c>
       <c r="E142" t="inlineStr">
         <is>
@@ -7198,10 +7198,10 @@
         </is>
       </c>
       <c r="C143" t="n">
-        <v>6083</v>
+        <v>6086</v>
       </c>
       <c r="D143" t="n">
-        <v>8904451</v>
+        <v>8908951</v>
       </c>
       <c r="E143" t="inlineStr">
         <is>
@@ -7438,10 +7438,10 @@
         </is>
       </c>
       <c r="C148" t="n">
-        <v>2397</v>
+        <v>2398</v>
       </c>
       <c r="D148" t="n">
-        <v>3144609</v>
+        <v>3145691</v>
       </c>
       <c r="E148" t="inlineStr">
         <is>
@@ -7486,10 +7486,10 @@
         </is>
       </c>
       <c r="C149" t="n">
-        <v>3609</v>
+        <v>3610</v>
       </c>
       <c r="D149" t="n">
-        <v>5201625</v>
+        <v>5202713</v>
       </c>
       <c r="E149" t="inlineStr">
         <is>
@@ -7534,10 +7534,10 @@
         </is>
       </c>
       <c r="C150" t="n">
-        <v>8220</v>
+        <v>8223</v>
       </c>
       <c r="D150" t="n">
-        <v>12029284</v>
+        <v>12033677</v>
       </c>
       <c r="E150" t="inlineStr">
         <is>
@@ -7774,10 +7774,10 @@
         </is>
       </c>
       <c r="C155" t="n">
-        <v>3130</v>
+        <v>3131</v>
       </c>
       <c r="D155" t="n">
-        <v>4178437</v>
+        <v>4179937</v>
       </c>
       <c r="E155" t="inlineStr">
         <is>
@@ -7822,10 +7822,10 @@
         </is>
       </c>
       <c r="C156" t="n">
-        <v>3388</v>
+        <v>3390</v>
       </c>
       <c r="D156" t="n">
-        <v>4911582</v>
+        <v>4914582</v>
       </c>
       <c r="E156" t="inlineStr">
         <is>
@@ -7870,10 +7870,10 @@
         </is>
       </c>
       <c r="C157" t="n">
-        <v>9437</v>
+        <v>9438</v>
       </c>
       <c r="D157" t="n">
-        <v>13917058</v>
+        <v>13918558</v>
       </c>
       <c r="E157" t="inlineStr">
         <is>
@@ -7918,10 +7918,10 @@
         </is>
       </c>
       <c r="C158" t="n">
-        <v>3104</v>
+        <v>3105</v>
       </c>
       <c r="D158" t="n">
-        <v>4620999</v>
+        <v>4622499</v>
       </c>
       <c r="E158" t="inlineStr">
         <is>
@@ -8110,10 +8110,10 @@
         </is>
       </c>
       <c r="C162" t="n">
-        <v>3158</v>
+        <v>3159</v>
       </c>
       <c r="D162" t="n">
-        <v>4257622</v>
+        <v>4258012</v>
       </c>
       <c r="E162" t="inlineStr">
         <is>
@@ -8158,10 +8158,10 @@
         </is>
       </c>
       <c r="C163" t="n">
-        <v>3721</v>
+        <v>3724</v>
       </c>
       <c r="D163" t="n">
-        <v>5359526</v>
+        <v>5362756</v>
       </c>
       <c r="E163" t="inlineStr">
         <is>
@@ -8206,10 +8206,10 @@
         </is>
       </c>
       <c r="C164" t="n">
-        <v>7883</v>
+        <v>7885</v>
       </c>
       <c r="D164" t="n">
-        <v>11557409</v>
+        <v>11560409</v>
       </c>
       <c r="E164" t="inlineStr">
         <is>
@@ -8446,10 +8446,10 @@
         </is>
       </c>
       <c r="C169" t="n">
-        <v>2984</v>
+        <v>2985</v>
       </c>
       <c r="D169" t="n">
-        <v>4008269</v>
+        <v>4009769</v>
       </c>
       <c r="E169" t="inlineStr">
         <is>
@@ -8830,10 +8830,10 @@
         </is>
       </c>
       <c r="C177" t="n">
-        <v>1142</v>
+        <v>1143</v>
       </c>
       <c r="D177" t="n">
-        <v>1671239</v>
+        <v>1672739</v>
       </c>
       <c r="E177" t="inlineStr">
         <is>
@@ -8926,10 +8926,10 @@
         </is>
       </c>
       <c r="C179" t="n">
-        <v>1174</v>
+        <v>1175</v>
       </c>
       <c r="D179" t="n">
-        <v>1746807</v>
+        <v>1748307</v>
       </c>
       <c r="E179" t="inlineStr">
         <is>
@@ -9118,10 +9118,10 @@
         </is>
       </c>
       <c r="C183" t="n">
-        <v>1113</v>
+        <v>1114</v>
       </c>
       <c r="D183" t="n">
-        <v>1494113</v>
+        <v>1494413</v>
       </c>
       <c r="E183" t="inlineStr">
         <is>
@@ -9406,10 +9406,10 @@
         </is>
       </c>
       <c r="C189" t="n">
-        <v>844</v>
+        <v>847</v>
       </c>
       <c r="D189" t="n">
-        <v>1072363</v>
+        <v>1076323</v>
       </c>
       <c r="E189" t="inlineStr">
         <is>
@@ -9454,10 +9454,10 @@
         </is>
       </c>
       <c r="C190" t="n">
-        <v>2192</v>
+        <v>2193</v>
       </c>
       <c r="D190" t="n">
-        <v>3149336</v>
+        <v>3150836</v>
       </c>
       <c r="E190" t="inlineStr">
         <is>
@@ -9502,10 +9502,10 @@
         </is>
       </c>
       <c r="C191" t="n">
-        <v>5739</v>
+        <v>5740</v>
       </c>
       <c r="D191" t="n">
-        <v>8406319</v>
+        <v>8407819</v>
       </c>
       <c r="E191" t="inlineStr">
         <is>
@@ -9550,10 +9550,10 @@
         </is>
       </c>
       <c r="C192" t="n">
-        <v>2002</v>
+        <v>2005</v>
       </c>
       <c r="D192" t="n">
-        <v>2983404</v>
+        <v>2987904</v>
       </c>
       <c r="E192" t="inlineStr">
         <is>
@@ -9742,10 +9742,10 @@
         </is>
       </c>
       <c r="C196" t="n">
-        <v>2138</v>
+        <v>2141</v>
       </c>
       <c r="D196" t="n">
-        <v>2866970</v>
+        <v>2871325</v>
       </c>
       <c r="E196" t="inlineStr">
         <is>
@@ -9790,10 +9790,10 @@
         </is>
       </c>
       <c r="C197" t="n">
-        <v>1867</v>
+        <v>1868</v>
       </c>
       <c r="D197" t="n">
-        <v>2720059</v>
+        <v>2720721</v>
       </c>
       <c r="E197" t="inlineStr">
         <is>
@@ -9838,10 +9838,10 @@
         </is>
       </c>
       <c r="C198" t="n">
-        <v>5629</v>
+        <v>5633</v>
       </c>
       <c r="D198" t="n">
-        <v>8280989</v>
+        <v>8286989</v>
       </c>
       <c r="E198" t="inlineStr">
         <is>
@@ -9886,10 +9886,10 @@
         </is>
       </c>
       <c r="C199" t="n">
-        <v>2086</v>
+        <v>2089</v>
       </c>
       <c r="D199" t="n">
-        <v>3102537</v>
+        <v>3107037</v>
       </c>
       <c r="E199" t="inlineStr">
         <is>
@@ -10078,10 +10078,10 @@
         </is>
       </c>
       <c r="C203" t="n">
-        <v>1889</v>
+        <v>1891</v>
       </c>
       <c r="D203" t="n">
-        <v>2473296</v>
+        <v>2475519</v>
       </c>
       <c r="E203" t="inlineStr">
         <is>
@@ -10174,10 +10174,10 @@
         </is>
       </c>
       <c r="C205" t="n">
-        <v>3164</v>
+        <v>3167</v>
       </c>
       <c r="D205" t="n">
-        <v>4651250</v>
+        <v>4655750</v>
       </c>
       <c r="E205" t="inlineStr">
         <is>
@@ -10222,10 +10222,10 @@
         </is>
       </c>
       <c r="C206" t="n">
-        <v>1059</v>
+        <v>1060</v>
       </c>
       <c r="D206" t="n">
-        <v>1578003</v>
+        <v>1579503</v>
       </c>
       <c r="E206" t="inlineStr">
         <is>
@@ -10462,10 +10462,10 @@
         </is>
       </c>
       <c r="C211" t="n">
-        <v>956</v>
+        <v>957</v>
       </c>
       <c r="D211" t="n">
-        <v>1370986</v>
+        <v>1372486</v>
       </c>
       <c r="E211" t="inlineStr">
         <is>
@@ -10510,10 +10510,10 @@
         </is>
       </c>
       <c r="C212" t="n">
-        <v>3710</v>
+        <v>3714</v>
       </c>
       <c r="D212" t="n">
-        <v>5418719</v>
+        <v>5424719</v>
       </c>
       <c r="E212" t="inlineStr">
         <is>
@@ -10558,10 +10558,10 @@
         </is>
       </c>
       <c r="C213" t="n">
-        <v>1919</v>
+        <v>1920</v>
       </c>
       <c r="D213" t="n">
-        <v>2842953</v>
+        <v>2844453</v>
       </c>
       <c r="E213" t="inlineStr">
         <is>
@@ -10750,10 +10750,10 @@
         </is>
       </c>
       <c r="C217" t="n">
-        <v>2279</v>
+        <v>2282</v>
       </c>
       <c r="D217" t="n">
-        <v>3298651</v>
+        <v>3302708</v>
       </c>
       <c r="E217" t="inlineStr">
         <is>
@@ -10798,10 +10798,10 @@
         </is>
       </c>
       <c r="C218" t="n">
-        <v>4104</v>
+        <v>4105</v>
       </c>
       <c r="D218" t="n">
-        <v>5992737</v>
+        <v>5994237</v>
       </c>
       <c r="E218" t="inlineStr">
         <is>
@@ -10990,10 +10990,10 @@
         </is>
       </c>
       <c r="C222" t="n">
-        <v>1690</v>
+        <v>1691</v>
       </c>
       <c r="D222" t="n">
-        <v>2298862</v>
+        <v>2299526</v>
       </c>
       <c r="E222" t="inlineStr">
         <is>
@@ -11038,10 +11038,10 @@
         </is>
       </c>
       <c r="C223" t="n">
-        <v>732</v>
+        <v>733</v>
       </c>
       <c r="D223" t="n">
-        <v>1049327</v>
+        <v>1050827</v>
       </c>
       <c r="E223" t="inlineStr">
         <is>
@@ -11086,10 +11086,10 @@
         </is>
       </c>
       <c r="C224" t="n">
-        <v>2280</v>
+        <v>2281</v>
       </c>
       <c r="D224" t="n">
-        <v>3316605</v>
+        <v>3317621</v>
       </c>
       <c r="E224" t="inlineStr">
         <is>
@@ -11278,10 +11278,10 @@
         </is>
       </c>
       <c r="C228" t="n">
-        <v>938</v>
+        <v>943</v>
       </c>
       <c r="D228" t="n">
-        <v>1210733</v>
+        <v>1216603</v>
       </c>
       <c r="E228" t="inlineStr">
         <is>
@@ -11374,10 +11374,10 @@
         </is>
       </c>
       <c r="C230" t="n">
-        <v>2644</v>
+        <v>2646</v>
       </c>
       <c r="D230" t="n">
-        <v>3857093</v>
+        <v>3859166</v>
       </c>
       <c r="E230" t="inlineStr">
         <is>
@@ -11614,10 +11614,10 @@
         </is>
       </c>
       <c r="C235" t="n">
-        <v>3959</v>
+        <v>3964</v>
       </c>
       <c r="D235" t="n">
-        <v>5729443</v>
+        <v>5736721</v>
       </c>
       <c r="E235" t="inlineStr">
         <is>
@@ -11662,10 +11662,10 @@
         </is>
       </c>
       <c r="C236" t="n">
-        <v>12399</v>
+        <v>12406</v>
       </c>
       <c r="D236" t="n">
-        <v>18187662</v>
+        <v>18198162</v>
       </c>
       <c r="E236" t="inlineStr">
         <is>
@@ -11758,10 +11758,10 @@
         </is>
       </c>
       <c r="C238" t="n">
-        <v>1485</v>
+        <v>1487</v>
       </c>
       <c r="D238" t="n">
-        <v>2204818</v>
+        <v>2207818</v>
       </c>
       <c r="E238" t="inlineStr">
         <is>
@@ -11902,10 +11902,10 @@
         </is>
       </c>
       <c r="C241" t="n">
-        <v>3429</v>
+        <v>3430</v>
       </c>
       <c r="D241" t="n">
-        <v>4649747</v>
+        <v>4649947</v>
       </c>
       <c r="E241" t="inlineStr">
         <is>
@@ -12238,10 +12238,10 @@
         </is>
       </c>
       <c r="C248" t="n">
-        <v>567</v>
+        <v>568</v>
       </c>
       <c r="D248" t="n">
-        <v>754221</v>
+        <v>754919</v>
       </c>
       <c r="E248" t="inlineStr">
         <is>
@@ -12286,10 +12286,10 @@
         </is>
       </c>
       <c r="C249" t="n">
-        <v>2685</v>
+        <v>2686</v>
       </c>
       <c r="D249" t="n">
-        <v>3881126</v>
+        <v>3882626</v>
       </c>
       <c r="E249" t="inlineStr">
         <is>
@@ -12334,10 +12334,10 @@
         </is>
       </c>
       <c r="C250" t="n">
-        <v>7907</v>
+        <v>7909</v>
       </c>
       <c r="D250" t="n">
-        <v>11600840</v>
+        <v>11603840</v>
       </c>
       <c r="E250" t="inlineStr">
         <is>
@@ -12382,10 +12382,10 @@
         </is>
       </c>
       <c r="C251" t="n">
-        <v>3207</v>
+        <v>3210</v>
       </c>
       <c r="D251" t="n">
-        <v>4763482</v>
+        <v>4767982</v>
       </c>
       <c r="E251" t="inlineStr">
         <is>
@@ -12478,10 +12478,10 @@
         </is>
       </c>
       <c r="C253" t="n">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="D253" t="n">
-        <v>337230</v>
+        <v>338730</v>
       </c>
       <c r="E253" t="inlineStr">
         <is>
@@ -12670,10 +12670,10 @@
         </is>
       </c>
       <c r="C257" t="n">
-        <v>2062</v>
+        <v>2065</v>
       </c>
       <c r="D257" t="n">
-        <v>2713607</v>
+        <v>2716289</v>
       </c>
       <c r="E257" t="inlineStr">
         <is>
@@ -12766,10 +12766,10 @@
         </is>
       </c>
       <c r="C259" t="n">
-        <v>4945</v>
+        <v>4949</v>
       </c>
       <c r="D259" t="n">
-        <v>7279397</v>
+        <v>7285119</v>
       </c>
       <c r="E259" t="inlineStr">
         <is>
@@ -13006,10 +13006,10 @@
         </is>
       </c>
       <c r="C264" t="n">
-        <v>1931</v>
+        <v>1932</v>
       </c>
       <c r="D264" t="n">
-        <v>2530726</v>
+        <v>2531683</v>
       </c>
       <c r="E264" t="inlineStr">
         <is>
@@ -13726,10 +13726,10 @@
         </is>
       </c>
       <c r="C279" t="n">
-        <v>8568</v>
+        <v>8571</v>
       </c>
       <c r="D279" t="n">
-        <v>12557868</v>
+        <v>12562368</v>
       </c>
       <c r="E279" t="inlineStr">
         <is>
@@ -13966,10 +13966,10 @@
         </is>
       </c>
       <c r="C284" t="n">
-        <v>2410</v>
+        <v>2412</v>
       </c>
       <c r="D284" t="n">
-        <v>3215071</v>
+        <v>3218071</v>
       </c>
       <c r="E284" t="inlineStr">
         <is>
@@ -14014,10 +14014,10 @@
         </is>
       </c>
       <c r="C285" t="n">
-        <v>1595</v>
+        <v>1596</v>
       </c>
       <c r="D285" t="n">
-        <v>2290053</v>
+        <v>2290995</v>
       </c>
       <c r="E285" t="inlineStr">
         <is>
@@ -14062,10 +14062,10 @@
         </is>
       </c>
       <c r="C286" t="n">
-        <v>3955</v>
+        <v>3956</v>
       </c>
       <c r="D286" t="n">
-        <v>5804805</v>
+        <v>5806305</v>
       </c>
       <c r="E286" t="inlineStr">
         <is>
@@ -14350,10 +14350,10 @@
         </is>
       </c>
       <c r="C292" t="n">
-        <v>2009</v>
+        <v>2013</v>
       </c>
       <c r="D292" t="n">
-        <v>2913918</v>
+        <v>2919918</v>
       </c>
       <c r="E292" t="inlineStr">
         <is>
@@ -14398,10 +14398,10 @@
         </is>
       </c>
       <c r="C293" t="n">
-        <v>6872</v>
+        <v>6877</v>
       </c>
       <c r="D293" t="n">
-        <v>10101574</v>
+        <v>10109074</v>
       </c>
       <c r="E293" t="inlineStr">
         <is>
@@ -14446,10 +14446,10 @@
         </is>
       </c>
       <c r="C294" t="n">
-        <v>2343</v>
+        <v>2344</v>
       </c>
       <c r="D294" t="n">
-        <v>3499418</v>
+        <v>3500918</v>
       </c>
       <c r="E294" t="inlineStr">
         <is>
@@ -14494,10 +14494,10 @@
         </is>
       </c>
       <c r="C295" t="n">
-        <v>753</v>
+        <v>754</v>
       </c>
       <c r="D295" t="n">
-        <v>1124805</v>
+        <v>1126305</v>
       </c>
       <c r="E295" t="inlineStr">
         <is>
@@ -14542,10 +14542,10 @@
         </is>
       </c>
       <c r="C296" t="n">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="D296" t="n">
-        <v>272833</v>
+        <v>274333</v>
       </c>
       <c r="E296" t="inlineStr">
         <is>
@@ -14638,10 +14638,10 @@
         </is>
       </c>
       <c r="C298" t="n">
-        <v>6907</v>
+        <v>6936</v>
       </c>
       <c r="D298" t="n">
-        <v>9504082</v>
+        <v>9539107</v>
       </c>
       <c r="E298" t="inlineStr">
         <is>
@@ -14686,10 +14686,10 @@
         </is>
       </c>
       <c r="C299" t="n">
-        <v>933</v>
+        <v>935</v>
       </c>
       <c r="D299" t="n">
-        <v>1369079</v>
+        <v>1372079</v>
       </c>
       <c r="E299" t="inlineStr">
         <is>
@@ -14734,10 +14734,10 @@
         </is>
       </c>
       <c r="C300" t="n">
-        <v>2353</v>
+        <v>2362</v>
       </c>
       <c r="D300" t="n">
-        <v>3488337</v>
+        <v>3501837</v>
       </c>
       <c r="E300" t="inlineStr">
         <is>
@@ -14782,10 +14782,10 @@
         </is>
       </c>
       <c r="C301" t="n">
-        <v>936</v>
+        <v>938</v>
       </c>
       <c r="D301" t="n">
-        <v>1393501</v>
+        <v>1396501</v>
       </c>
       <c r="E301" t="inlineStr">
         <is>
@@ -14974,10 +14974,10 @@
         </is>
       </c>
       <c r="C305" t="n">
-        <v>1382</v>
+        <v>1384</v>
       </c>
       <c r="D305" t="n">
-        <v>1944206</v>
+        <v>1947206</v>
       </c>
       <c r="E305" t="inlineStr">
         <is>
@@ -15022,10 +15022,10 @@
         </is>
       </c>
       <c r="C306" t="n">
-        <v>1166</v>
+        <v>1167</v>
       </c>
       <c r="D306" t="n">
-        <v>1673659</v>
+        <v>1675148</v>
       </c>
       <c r="E306" t="inlineStr">
         <is>
@@ -15070,10 +15070,10 @@
         </is>
       </c>
       <c r="C307" t="n">
-        <v>3563</v>
+        <v>3564</v>
       </c>
       <c r="D307" t="n">
-        <v>5226785</v>
+        <v>5228062</v>
       </c>
       <c r="E307" t="inlineStr">
         <is>
@@ -15118,10 +15118,10 @@
         </is>
       </c>
       <c r="C308" t="n">
-        <v>1340</v>
+        <v>1343</v>
       </c>
       <c r="D308" t="n">
-        <v>1983853</v>
+        <v>1988253</v>
       </c>
       <c r="E308" t="inlineStr">
         <is>
@@ -15166,10 +15166,10 @@
         </is>
       </c>
       <c r="C309" t="n">
-        <v>329</v>
+        <v>330</v>
       </c>
       <c r="D309" t="n">
-        <v>490505</v>
+        <v>492005</v>
       </c>
       <c r="E309" t="inlineStr">
         <is>
@@ -15214,10 +15214,10 @@
         </is>
       </c>
       <c r="C310" t="n">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="D310" t="n">
-        <v>80937</v>
+        <v>82437</v>
       </c>
       <c r="E310" t="inlineStr">
         <is>
@@ -15358,10 +15358,10 @@
         </is>
       </c>
       <c r="C313" t="n">
-        <v>1423</v>
+        <v>1424</v>
       </c>
       <c r="D313" t="n">
-        <v>1897378</v>
+        <v>1898878</v>
       </c>
       <c r="E313" t="inlineStr">
         <is>
@@ -15406,10 +15406,10 @@
         </is>
       </c>
       <c r="C314" t="n">
-        <v>6985</v>
+        <v>6986</v>
       </c>
       <c r="D314" t="n">
-        <v>10079547</v>
+        <v>10081047</v>
       </c>
       <c r="E314" t="inlineStr">
         <is>
@@ -15454,10 +15454,10 @@
         </is>
       </c>
       <c r="C315" t="n">
-        <v>19563</v>
+        <v>19572</v>
       </c>
       <c r="D315" t="n">
-        <v>28619977</v>
+        <v>28632199</v>
       </c>
       <c r="E315" t="inlineStr">
         <is>
@@ -15502,10 +15502,10 @@
         </is>
       </c>
       <c r="C316" t="n">
-        <v>6938</v>
+        <v>6942</v>
       </c>
       <c r="D316" t="n">
-        <v>10325662</v>
+        <v>10331662</v>
       </c>
       <c r="E316" t="inlineStr">
         <is>
@@ -15550,10 +15550,10 @@
         </is>
       </c>
       <c r="C317" t="n">
-        <v>2127</v>
+        <v>2128</v>
       </c>
       <c r="D317" t="n">
-        <v>3173636</v>
+        <v>3175136</v>
       </c>
       <c r="E317" t="inlineStr">
         <is>
@@ -15742,10 +15742,10 @@
         </is>
       </c>
       <c r="C321" t="n">
-        <v>6199</v>
+        <v>6201</v>
       </c>
       <c r="D321" t="n">
-        <v>8154654</v>
+        <v>8156602</v>
       </c>
       <c r="E321" t="inlineStr">
         <is>
@@ -15790,10 +15790,10 @@
         </is>
       </c>
       <c r="C322" t="n">
-        <v>2087</v>
+        <v>2089</v>
       </c>
       <c r="D322" t="n">
-        <v>3056392</v>
+        <v>3059392</v>
       </c>
       <c r="E322" t="inlineStr">
         <is>
@@ -15838,10 +15838,10 @@
         </is>
       </c>
       <c r="C323" t="n">
-        <v>6490</v>
+        <v>6491</v>
       </c>
       <c r="D323" t="n">
-        <v>9528281</v>
+        <v>9529781</v>
       </c>
       <c r="E323" t="inlineStr">
         <is>
@@ -16078,10 +16078,10 @@
         </is>
       </c>
       <c r="C328" t="n">
-        <v>1978</v>
+        <v>1980</v>
       </c>
       <c r="D328" t="n">
-        <v>2687500</v>
+        <v>2689662</v>
       </c>
       <c r="E328" t="inlineStr">
         <is>
@@ -16126,10 +16126,10 @@
         </is>
       </c>
       <c r="C329" t="n">
-        <v>3573</v>
+        <v>3575</v>
       </c>
       <c r="D329" t="n">
-        <v>5137319</v>
+        <v>5140319</v>
       </c>
       <c r="E329" t="inlineStr">
         <is>
@@ -16174,10 +16174,10 @@
         </is>
       </c>
       <c r="C330" t="n">
-        <v>10774</v>
+        <v>10777</v>
       </c>
       <c r="D330" t="n">
-        <v>15742207</v>
+        <v>15746707</v>
       </c>
       <c r="E330" t="inlineStr">
         <is>
@@ -16510,10 +16510,10 @@
         </is>
       </c>
       <c r="C337" t="n">
-        <v>1513</v>
+        <v>1514</v>
       </c>
       <c r="D337" t="n">
-        <v>2189337</v>
+        <v>2190837</v>
       </c>
       <c r="E337" t="inlineStr">
         <is>
@@ -16558,10 +16558,10 @@
         </is>
       </c>
       <c r="C338" t="n">
-        <v>4230</v>
+        <v>4231</v>
       </c>
       <c r="D338" t="n">
-        <v>6178958</v>
+        <v>6180458</v>
       </c>
       <c r="E338" t="inlineStr">
         <is>
@@ -16606,10 +16606,10 @@
         </is>
       </c>
       <c r="C339" t="n">
-        <v>1611</v>
+        <v>1613</v>
       </c>
       <c r="D339" t="n">
-        <v>2394269</v>
+        <v>2397028</v>
       </c>
       <c r="E339" t="inlineStr">
         <is>
@@ -16702,10 +16702,10 @@
         </is>
       </c>
       <c r="C341" t="n">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="D341" t="n">
-        <v>159000</v>
+        <v>160500</v>
       </c>
       <c r="E341" t="inlineStr">
         <is>
@@ -16846,10 +16846,10 @@
         </is>
       </c>
       <c r="C344" t="n">
-        <v>3605</v>
+        <v>3606</v>
       </c>
       <c r="D344" t="n">
-        <v>5263560</v>
+        <v>5265060</v>
       </c>
       <c r="E344" t="inlineStr">
         <is>
@@ -16894,10 +16894,10 @@
         </is>
       </c>
       <c r="C345" t="n">
-        <v>10377</v>
+        <v>10386</v>
       </c>
       <c r="D345" t="n">
-        <v>15312965</v>
+        <v>15326465</v>
       </c>
       <c r="E345" t="inlineStr">
         <is>
@@ -16942,10 +16942,10 @@
         </is>
       </c>
       <c r="C346" t="n">
-        <v>3990</v>
+        <v>3994</v>
       </c>
       <c r="D346" t="n">
-        <v>5940455</v>
+        <v>5946455</v>
       </c>
       <c r="E346" t="inlineStr">
         <is>
@@ -17230,10 +17230,10 @@
         </is>
       </c>
       <c r="C352" t="n">
-        <v>3462</v>
+        <v>3464</v>
       </c>
       <c r="D352" t="n">
-        <v>4791088</v>
+        <v>4793412</v>
       </c>
       <c r="E352" t="inlineStr">
         <is>
@@ -17278,10 +17278,10 @@
         </is>
       </c>
       <c r="C353" t="n">
-        <v>6429</v>
+        <v>6436</v>
       </c>
       <c r="D353" t="n">
-        <v>9364275</v>
+        <v>9374775</v>
       </c>
       <c r="E353" t="inlineStr">
         <is>
@@ -17326,10 +17326,10 @@
         </is>
       </c>
       <c r="C354" t="n">
-        <v>15595</v>
+        <v>15610</v>
       </c>
       <c r="D354" t="n">
-        <v>22965863</v>
+        <v>22988363</v>
       </c>
       <c r="E354" t="inlineStr">
         <is>
@@ -17374,10 +17374,10 @@
         </is>
       </c>
       <c r="C355" t="n">
-        <v>6922</v>
+        <v>6925</v>
       </c>
       <c r="D355" t="n">
-        <v>10316390</v>
+        <v>10320890</v>
       </c>
       <c r="E355" t="inlineStr">
         <is>
@@ -17422,10 +17422,10 @@
         </is>
       </c>
       <c r="C356" t="n">
-        <v>2107</v>
+        <v>2108</v>
       </c>
       <c r="D356" t="n">
-        <v>3145151</v>
+        <v>3146651</v>
       </c>
       <c r="E356" t="inlineStr">
         <is>
@@ -17566,10 +17566,10 @@
         </is>
       </c>
       <c r="C359" t="n">
-        <v>5712</v>
+        <v>5720</v>
       </c>
       <c r="D359" t="n">
-        <v>7794403</v>
+        <v>7805423</v>
       </c>
       <c r="E359" t="inlineStr">
         <is>
@@ -17614,10 +17614,10 @@
         </is>
       </c>
       <c r="C360" t="n">
-        <v>18813</v>
+        <v>18831</v>
       </c>
       <c r="D360" t="n">
-        <v>27310696</v>
+        <v>27336641</v>
       </c>
       <c r="E360" t="inlineStr">
         <is>
@@ -17662,10 +17662,10 @@
         </is>
       </c>
       <c r="C361" t="n">
-        <v>51585</v>
+        <v>51622</v>
       </c>
       <c r="D361" t="n">
-        <v>76012580</v>
+        <v>76067559</v>
       </c>
       <c r="E361" t="inlineStr">
         <is>
@@ -17710,10 +17710,10 @@
         </is>
       </c>
       <c r="C362" t="n">
-        <v>24101</v>
+        <v>24117</v>
       </c>
       <c r="D362" t="n">
-        <v>35957108</v>
+        <v>35981108</v>
       </c>
       <c r="E362" t="inlineStr">
         <is>
@@ -17758,10 +17758,10 @@
         </is>
       </c>
       <c r="C363" t="n">
-        <v>8673</v>
+        <v>8679</v>
       </c>
       <c r="D363" t="n">
-        <v>12970204</v>
+        <v>12979204</v>
       </c>
       <c r="E363" t="inlineStr">
         <is>
@@ -17806,10 +17806,10 @@
         </is>
       </c>
       <c r="C364" t="n">
-        <v>2207</v>
+        <v>2210</v>
       </c>
       <c r="D364" t="n">
-        <v>3298459</v>
+        <v>3302959</v>
       </c>
       <c r="E364" t="inlineStr">
         <is>
@@ -18046,10 +18046,10 @@
         </is>
       </c>
       <c r="C369" t="n">
-        <v>18522</v>
+        <v>18532</v>
       </c>
       <c r="D369" t="n">
-        <v>25121689</v>
+        <v>25130890</v>
       </c>
       <c r="E369" t="inlineStr">
         <is>
@@ -18094,10 +18094,10 @@
         </is>
       </c>
       <c r="C370" t="n">
-        <v>4334</v>
+        <v>4335</v>
       </c>
       <c r="D370" t="n">
-        <v>6310477</v>
+        <v>6311977</v>
       </c>
       <c r="E370" t="inlineStr">
         <is>
@@ -18142,10 +18142,10 @@
         </is>
       </c>
       <c r="C371" t="n">
-        <v>12324</v>
+        <v>12329</v>
       </c>
       <c r="D371" t="n">
-        <v>18120864</v>
+        <v>18128364</v>
       </c>
       <c r="E371" t="inlineStr">
         <is>
@@ -18190,10 +18190,10 @@
         </is>
       </c>
       <c r="C372" t="n">
-        <v>4658</v>
+        <v>4660</v>
       </c>
       <c r="D372" t="n">
-        <v>6915788</v>
+        <v>6918788</v>
       </c>
       <c r="E372" t="inlineStr">
         <is>
@@ -18238,10 +18238,10 @@
         </is>
       </c>
       <c r="C373" t="n">
-        <v>1430</v>
+        <v>1431</v>
       </c>
       <c r="D373" t="n">
-        <v>2134981</v>
+        <v>2136481</v>
       </c>
       <c r="E373" t="inlineStr">
         <is>
@@ -18382,10 +18382,10 @@
         </is>
       </c>
       <c r="C376" t="n">
-        <v>4343</v>
+        <v>4346</v>
       </c>
       <c r="D376" t="n">
-        <v>5931812</v>
+        <v>5935554</v>
       </c>
       <c r="E376" t="inlineStr">
         <is>
@@ -18430,10 +18430,10 @@
         </is>
       </c>
       <c r="C377" t="n">
-        <v>5409</v>
+        <v>5412</v>
       </c>
       <c r="D377" t="n">
-        <v>7872071</v>
+        <v>7876571</v>
       </c>
       <c r="E377" t="inlineStr">
         <is>
@@ -18478,10 +18478,10 @@
         </is>
       </c>
       <c r="C378" t="n">
-        <v>19143</v>
+        <v>19152</v>
       </c>
       <c r="D378" t="n">
-        <v>28201804</v>
+        <v>28214545</v>
       </c>
       <c r="E378" t="inlineStr">
         <is>
@@ -18526,10 +18526,10 @@
         </is>
       </c>
       <c r="C379" t="n">
-        <v>8939</v>
+        <v>8941</v>
       </c>
       <c r="D379" t="n">
-        <v>13329534</v>
+        <v>13332534</v>
       </c>
       <c r="E379" t="inlineStr">
         <is>
@@ -18718,10 +18718,10 @@
         </is>
       </c>
       <c r="C383" t="n">
-        <v>5594</v>
+        <v>5596</v>
       </c>
       <c r="D383" t="n">
-        <v>7542467</v>
+        <v>7543532</v>
       </c>
       <c r="E383" t="inlineStr">
         <is>
@@ -18766,10 +18766,10 @@
         </is>
       </c>
       <c r="C384" t="n">
-        <v>4840</v>
+        <v>4845</v>
       </c>
       <c r="D384" t="n">
-        <v>7055009</v>
+        <v>7062509</v>
       </c>
       <c r="E384" t="inlineStr">
         <is>
@@ -18814,10 +18814,10 @@
         </is>
       </c>
       <c r="C385" t="n">
-        <v>13893</v>
+        <v>13902</v>
       </c>
       <c r="D385" t="n">
-        <v>20451767</v>
+        <v>20464982</v>
       </c>
       <c r="E385" t="inlineStr">
         <is>
@@ -18862,10 +18862,10 @@
         </is>
       </c>
       <c r="C386" t="n">
-        <v>5735</v>
+        <v>5736</v>
       </c>
       <c r="D386" t="n">
-        <v>8541999</v>
+        <v>8543239</v>
       </c>
       <c r="E386" t="inlineStr">
         <is>
@@ -18910,10 +18910,10 @@
         </is>
       </c>
       <c r="C387" t="n">
-        <v>1645</v>
+        <v>1647</v>
       </c>
       <c r="D387" t="n">
-        <v>2454622</v>
+        <v>2457622</v>
       </c>
       <c r="E387" t="inlineStr">
         <is>
@@ -18958,10 +18958,10 @@
         </is>
       </c>
       <c r="C388" t="n">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="D388" t="n">
-        <v>592606</v>
+        <v>594106</v>
       </c>
       <c r="E388" t="inlineStr">
         <is>
@@ -19102,10 +19102,10 @@
         </is>
       </c>
       <c r="C391" t="n">
-        <v>5011</v>
+        <v>5013</v>
       </c>
       <c r="D391" t="n">
-        <v>6835901</v>
+        <v>6838001</v>
       </c>
       <c r="E391" t="inlineStr">
         <is>
@@ -19150,10 +19150,10 @@
         </is>
       </c>
       <c r="C392" t="n">
-        <v>3653</v>
+        <v>3654</v>
       </c>
       <c r="D392" t="n">
-        <v>5330434</v>
+        <v>5331934</v>
       </c>
       <c r="E392" t="inlineStr">
         <is>
@@ -19198,10 +19198,10 @@
         </is>
       </c>
       <c r="C393" t="n">
-        <v>11522</v>
+        <v>11529</v>
       </c>
       <c r="D393" t="n">
-        <v>16996858</v>
+        <v>17006860</v>
       </c>
       <c r="E393" t="inlineStr">
         <is>
@@ -19246,10 +19246,10 @@
         </is>
       </c>
       <c r="C394" t="n">
-        <v>4831</v>
+        <v>4833</v>
       </c>
       <c r="D394" t="n">
-        <v>7188059</v>
+        <v>7191059</v>
       </c>
       <c r="E394" t="inlineStr">
         <is>
@@ -19486,10 +19486,10 @@
         </is>
       </c>
       <c r="C399" t="n">
-        <v>3918</v>
+        <v>3920</v>
       </c>
       <c r="D399" t="n">
-        <v>5291800</v>
+        <v>5293750</v>
       </c>
       <c r="E399" t="inlineStr">
         <is>
@@ -19534,10 +19534,10 @@
         </is>
       </c>
       <c r="C400" t="n">
-        <v>4152</v>
+        <v>4155</v>
       </c>
       <c r="D400" t="n">
-        <v>6051583</v>
+        <v>6056083</v>
       </c>
       <c r="E400" t="inlineStr">
         <is>
@@ -19582,10 +19582,10 @@
         </is>
       </c>
       <c r="C401" t="n">
-        <v>11229</v>
+        <v>11240</v>
       </c>
       <c r="D401" t="n">
-        <v>16542052</v>
+        <v>16558552</v>
       </c>
       <c r="E401" t="inlineStr">
         <is>
@@ -19726,10 +19726,10 @@
         </is>
       </c>
       <c r="C404" t="n">
-        <v>291</v>
+        <v>292</v>
       </c>
       <c r="D404" t="n">
-        <v>433510</v>
+        <v>433810</v>
       </c>
       <c r="E404" t="inlineStr">
         <is>
@@ -19822,10 +19822,10 @@
         </is>
       </c>
       <c r="C406" t="n">
-        <v>4115</v>
+        <v>4121</v>
       </c>
       <c r="D406" t="n">
-        <v>5637242</v>
+        <v>5646091</v>
       </c>
       <c r="E406" t="inlineStr">
         <is>
@@ -19870,10 +19870,10 @@
         </is>
       </c>
       <c r="C407" t="n">
-        <v>4581</v>
+        <v>4590</v>
       </c>
       <c r="D407" t="n">
-        <v>6637511</v>
+        <v>6650436</v>
       </c>
       <c r="E407" t="inlineStr">
         <is>
@@ -19918,10 +19918,10 @@
         </is>
       </c>
       <c r="C408" t="n">
-        <v>11539</v>
+        <v>11545</v>
       </c>
       <c r="D408" t="n">
-        <v>16952765</v>
+        <v>16961042</v>
       </c>
       <c r="E408" t="inlineStr">
         <is>
@@ -19966,10 +19966,10 @@
         </is>
       </c>
       <c r="C409" t="n">
-        <v>3879</v>
+        <v>3881</v>
       </c>
       <c r="D409" t="n">
-        <v>5781083</v>
+        <v>5784083</v>
       </c>
       <c r="E409" t="inlineStr">
         <is>
@@ -20206,10 +20206,10 @@
         </is>
       </c>
       <c r="C414" t="n">
-        <v>5390</v>
+        <v>5400</v>
       </c>
       <c r="D414" t="n">
-        <v>7248028</v>
+        <v>7259391</v>
       </c>
       <c r="E414" t="inlineStr">
         <is>
@@ -20254,10 +20254,10 @@
         </is>
       </c>
       <c r="C415" t="n">
-        <v>1588</v>
+        <v>1591</v>
       </c>
       <c r="D415" t="n">
-        <v>2286932</v>
+        <v>2291432</v>
       </c>
       <c r="E415" t="inlineStr">
         <is>
@@ -20302,10 +20302,10 @@
         </is>
       </c>
       <c r="C416" t="n">
-        <v>5137</v>
+        <v>5146</v>
       </c>
       <c r="D416" t="n">
-        <v>7564243</v>
+        <v>7577743</v>
       </c>
       <c r="E416" t="inlineStr">
         <is>
@@ -20350,10 +20350,10 @@
         </is>
       </c>
       <c r="C417" t="n">
-        <v>1937</v>
+        <v>1938</v>
       </c>
       <c r="D417" t="n">
-        <v>2885437</v>
+        <v>2886937</v>
       </c>
       <c r="E417" t="inlineStr">
         <is>
@@ -20590,10 +20590,10 @@
         </is>
       </c>
       <c r="C422" t="n">
-        <v>3536</v>
+        <v>3543</v>
       </c>
       <c r="D422" t="n">
-        <v>4678902</v>
+        <v>4687961</v>
       </c>
       <c r="E422" t="inlineStr">
         <is>
@@ -20638,10 +20638,10 @@
         </is>
       </c>
       <c r="C423" t="n">
-        <v>599</v>
+        <v>600</v>
       </c>
       <c r="D423" t="n">
-        <v>892164</v>
+        <v>893664</v>
       </c>
       <c r="E423" t="inlineStr">
         <is>
@@ -20686,10 +20686,10 @@
         </is>
       </c>
       <c r="C424" t="n">
-        <v>349</v>
+        <v>350</v>
       </c>
       <c r="D424" t="n">
-        <v>521030</v>
+        <v>522530</v>
       </c>
       <c r="E424" t="inlineStr">
         <is>
@@ -20782,10 +20782,10 @@
         </is>
       </c>
       <c r="C426" t="n">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="D426" t="n">
-        <v>64500</v>
+        <v>66000</v>
       </c>
       <c r="E426" t="inlineStr">
         <is>
@@ -20878,10 +20878,10 @@
         </is>
       </c>
       <c r="C428" t="n">
-        <v>3078</v>
+        <v>3080</v>
       </c>
       <c r="D428" t="n">
-        <v>4458502</v>
+        <v>4460672</v>
       </c>
       <c r="E428" t="inlineStr">
         <is>
@@ -20926,10 +20926,10 @@
         </is>
       </c>
       <c r="C429" t="n">
-        <v>7359</v>
+        <v>7364</v>
       </c>
       <c r="D429" t="n">
-        <v>10799909</v>
+        <v>10806745</v>
       </c>
       <c r="E429" t="inlineStr">
         <is>
@@ -20974,10 +20974,10 @@
         </is>
       </c>
       <c r="C430" t="n">
-        <v>2435</v>
+        <v>2437</v>
       </c>
       <c r="D430" t="n">
-        <v>3629588</v>
+        <v>3632588</v>
       </c>
       <c r="E430" t="inlineStr">
         <is>
@@ -21166,10 +21166,10 @@
         </is>
       </c>
       <c r="C434" t="n">
-        <v>2418</v>
+        <v>2419</v>
       </c>
       <c r="D434" t="n">
-        <v>3229133</v>
+        <v>3230633</v>
       </c>
       <c r="E434" t="inlineStr">
         <is>
@@ -21214,10 +21214,10 @@
         </is>
       </c>
       <c r="C435" t="n">
-        <v>1733</v>
+        <v>1734</v>
       </c>
       <c r="D435" t="n">
-        <v>2518468</v>
+        <v>2518809</v>
       </c>
       <c r="E435" t="inlineStr">
         <is>
@@ -21310,10 +21310,10 @@
         </is>
       </c>
       <c r="C437" t="n">
-        <v>1607</v>
+        <v>1608</v>
       </c>
       <c r="D437" t="n">
-        <v>2393727</v>
+        <v>2395227</v>
       </c>
       <c r="E437" t="inlineStr">
         <is>
@@ -21502,10 +21502,10 @@
         </is>
       </c>
       <c r="C441" t="n">
-        <v>1681</v>
+        <v>1685</v>
       </c>
       <c r="D441" t="n">
-        <v>2206261</v>
+        <v>2210645</v>
       </c>
       <c r="E441" t="inlineStr">
         <is>
@@ -21550,10 +21550,10 @@
         </is>
       </c>
       <c r="C442" t="n">
-        <v>1955</v>
+        <v>1956</v>
       </c>
       <c r="D442" t="n">
-        <v>2822711</v>
+        <v>2824211</v>
       </c>
       <c r="E442" t="inlineStr">
         <is>
@@ -21790,10 +21790,10 @@
         </is>
       </c>
       <c r="C447" t="n">
-        <v>1632</v>
+        <v>1633</v>
       </c>
       <c r="D447" t="n">
-        <v>2146899</v>
+        <v>2147325</v>
       </c>
       <c r="E447" t="inlineStr">
         <is>
@@ -21886,10 +21886,10 @@
         </is>
       </c>
       <c r="C449" t="n">
-        <v>2662</v>
+        <v>2664</v>
       </c>
       <c r="D449" t="n">
-        <v>3905171</v>
+        <v>3907031</v>
       </c>
       <c r="E449" t="inlineStr">
         <is>
@@ -22078,10 +22078,10 @@
         </is>
       </c>
       <c r="C453" t="n">
-        <v>1071</v>
+        <v>1072</v>
       </c>
       <c r="D453" t="n">
-        <v>1447561</v>
+        <v>1449061</v>
       </c>
       <c r="E453" t="inlineStr">
         <is>
@@ -22126,10 +22126,10 @@
         </is>
       </c>
       <c r="C454" t="n">
-        <v>3036</v>
+        <v>3037</v>
       </c>
       <c r="D454" t="n">
-        <v>4418711</v>
+        <v>4420211</v>
       </c>
       <c r="E454" t="inlineStr">
         <is>
@@ -22174,10 +22174,10 @@
         </is>
       </c>
       <c r="C455" t="n">
-        <v>9359</v>
+        <v>9369</v>
       </c>
       <c r="D455" t="n">
-        <v>13779417</v>
+        <v>13794281</v>
       </c>
       <c r="E455" t="inlineStr">
         <is>
@@ -22222,10 +22222,10 @@
         </is>
       </c>
       <c r="C456" t="n">
-        <v>3401</v>
+        <v>3402</v>
       </c>
       <c r="D456" t="n">
-        <v>5055394</v>
+        <v>5056894</v>
       </c>
       <c r="E456" t="inlineStr">
         <is>
@@ -22270,10 +22270,10 @@
         </is>
       </c>
       <c r="C457" t="n">
-        <v>931</v>
+        <v>932</v>
       </c>
       <c r="D457" t="n">
-        <v>1389237</v>
+        <v>1390737</v>
       </c>
       <c r="E457" t="inlineStr">
         <is>
@@ -22414,10 +22414,10 @@
         </is>
       </c>
       <c r="C460" t="n">
-        <v>2968</v>
+        <v>2970</v>
       </c>
       <c r="D460" t="n">
-        <v>3879649</v>
+        <v>3882649</v>
       </c>
       <c r="E460" t="inlineStr">
         <is>
@@ -22798,10 +22798,10 @@
         </is>
       </c>
       <c r="C468" t="n">
-        <v>4415</v>
+        <v>4416</v>
       </c>
       <c r="D468" t="n">
-        <v>6390366</v>
+        <v>6391866</v>
       </c>
       <c r="E468" t="inlineStr">
         <is>
@@ -22846,10 +22846,10 @@
         </is>
       </c>
       <c r="C469" t="n">
-        <v>8232</v>
+        <v>8234</v>
       </c>
       <c r="D469" t="n">
-        <v>12071075</v>
+        <v>12074075</v>
       </c>
       <c r="E469" t="inlineStr">
         <is>
@@ -22894,10 +22894,10 @@
         </is>
       </c>
       <c r="C470" t="n">
-        <v>2411</v>
+        <v>2412</v>
       </c>
       <c r="D470" t="n">
-        <v>3585210</v>
+        <v>3586710</v>
       </c>
       <c r="E470" t="inlineStr">
         <is>
@@ -22942,10 +22942,10 @@
         </is>
       </c>
       <c r="C471" t="n">
-        <v>614</v>
+        <v>615</v>
       </c>
       <c r="D471" t="n">
-        <v>912588</v>
+        <v>914088</v>
       </c>
       <c r="E471" t="inlineStr">
         <is>
@@ -23086,10 +23086,10 @@
         </is>
       </c>
       <c r="C474" t="n">
-        <v>2775</v>
+        <v>2777</v>
       </c>
       <c r="D474" t="n">
-        <v>3705521</v>
+        <v>3707174</v>
       </c>
       <c r="E474" t="inlineStr">
         <is>
@@ -23230,10 +23230,10 @@
         </is>
       </c>
       <c r="C477" t="n">
-        <v>780</v>
+        <v>781</v>
       </c>
       <c r="D477" t="n">
-        <v>1153507</v>
+        <v>1155007</v>
       </c>
       <c r="E477" t="inlineStr">
         <is>
@@ -23374,10 +23374,10 @@
         </is>
       </c>
       <c r="C480" t="n">
-        <v>1391</v>
+        <v>1392</v>
       </c>
       <c r="D480" t="n">
-        <v>1856242</v>
+        <v>1857742</v>
       </c>
       <c r="E480" t="inlineStr">
         <is>
@@ -23422,10 +23422,10 @@
         </is>
       </c>
       <c r="C481" t="n">
-        <v>377</v>
+        <v>378</v>
       </c>
       <c r="D481" t="n">
-        <v>538548</v>
+        <v>540048</v>
       </c>
       <c r="E481" t="inlineStr">
         <is>
@@ -23470,10 +23470,10 @@
         </is>
       </c>
       <c r="C482" t="n">
-        <v>1075</v>
+        <v>1076</v>
       </c>
       <c r="D482" t="n">
-        <v>1546761</v>
+        <v>1548261</v>
       </c>
       <c r="E482" t="inlineStr">
         <is>
@@ -23806,10 +23806,10 @@
         </is>
       </c>
       <c r="C489" t="n">
-        <v>969</v>
+        <v>970</v>
       </c>
       <c r="D489" t="n">
-        <v>1447793</v>
+        <v>1449293</v>
       </c>
       <c r="E489" t="inlineStr">
         <is>
@@ -24046,10 +24046,10 @@
         </is>
       </c>
       <c r="C494" t="n">
-        <v>5319</v>
+        <v>5321</v>
       </c>
       <c r="D494" t="n">
-        <v>7787936</v>
+        <v>7790562</v>
       </c>
       <c r="E494" t="inlineStr">
         <is>
@@ -24286,10 +24286,10 @@
         </is>
       </c>
       <c r="C499" t="n">
-        <v>2397</v>
+        <v>2399</v>
       </c>
       <c r="D499" t="n">
-        <v>3137033</v>
+        <v>3140033</v>
       </c>
       <c r="E499" t="inlineStr">
         <is>
@@ -24334,10 +24334,10 @@
         </is>
       </c>
       <c r="C500" t="n">
-        <v>8824</v>
+        <v>8828</v>
       </c>
       <c r="D500" t="n">
-        <v>12782350</v>
+        <v>12788350</v>
       </c>
       <c r="E500" t="inlineStr">
         <is>
@@ -24382,10 +24382,10 @@
         </is>
       </c>
       <c r="C501" t="n">
-        <v>18392</v>
+        <v>18401</v>
       </c>
       <c r="D501" t="n">
-        <v>26928991</v>
+        <v>26940859</v>
       </c>
       <c r="E501" t="inlineStr">
         <is>
@@ -24430,10 +24430,10 @@
         </is>
       </c>
       <c r="C502" t="n">
-        <v>6251</v>
+        <v>6252</v>
       </c>
       <c r="D502" t="n">
-        <v>9299427</v>
+        <v>9300927</v>
       </c>
       <c r="E502" t="inlineStr">
         <is>
@@ -24478,10 +24478,10 @@
         </is>
       </c>
       <c r="C503" t="n">
-        <v>1963</v>
+        <v>1964</v>
       </c>
       <c r="D503" t="n">
-        <v>2926772</v>
+        <v>2928272</v>
       </c>
       <c r="E503" t="inlineStr">
         <is>
@@ -24718,10 +24718,10 @@
         </is>
       </c>
       <c r="C508" t="n">
-        <v>6625</v>
+        <v>6627</v>
       </c>
       <c r="D508" t="n">
-        <v>8970980</v>
+        <v>8973136</v>
       </c>
       <c r="E508" t="inlineStr">
         <is>
@@ -24766,10 +24766,10 @@
         </is>
       </c>
       <c r="C509" t="n">
-        <v>1283</v>
+        <v>1284</v>
       </c>
       <c r="D509" t="n">
-        <v>1847115</v>
+        <v>1848615</v>
       </c>
       <c r="E509" t="inlineStr">
         <is>
@@ -24862,10 +24862,10 @@
         </is>
       </c>
       <c r="C511" t="n">
-        <v>1053</v>
+        <v>1054</v>
       </c>
       <c r="D511" t="n">
-        <v>1565669</v>
+        <v>1567169</v>
       </c>
       <c r="E511" t="inlineStr">
         <is>
@@ -24910,10 +24910,10 @@
         </is>
       </c>
       <c r="C512" t="n">
-        <v>349</v>
+        <v>350</v>
       </c>
       <c r="D512" t="n">
-        <v>520432</v>
+        <v>521932</v>
       </c>
       <c r="E512" t="inlineStr">
         <is>
@@ -25102,10 +25102,10 @@
         </is>
       </c>
       <c r="C516" t="n">
-        <v>2908</v>
+        <v>2910</v>
       </c>
       <c r="D516" t="n">
-        <v>4172234</v>
+        <v>4175234</v>
       </c>
       <c r="E516" t="inlineStr">
         <is>
@@ -25150,10 +25150,10 @@
         </is>
       </c>
       <c r="C517" t="n">
-        <v>4983</v>
+        <v>4984</v>
       </c>
       <c r="D517" t="n">
-        <v>7292562</v>
+        <v>7293497</v>
       </c>
       <c r="E517" t="inlineStr">
         <is>
@@ -25390,10 +25390,10 @@
         </is>
       </c>
       <c r="C522" t="n">
-        <v>1653</v>
+        <v>1655</v>
       </c>
       <c r="D522" t="n">
-        <v>2188678</v>
+        <v>2191678</v>
       </c>
       <c r="E522" t="inlineStr">
         <is>
@@ -25438,10 +25438,10 @@
         </is>
       </c>
       <c r="C523" t="n">
-        <v>1612</v>
+        <v>1613</v>
       </c>
       <c r="D523" t="n">
-        <v>2324683</v>
+        <v>2326183</v>
       </c>
       <c r="E523" t="inlineStr">
         <is>
@@ -25486,10 +25486,10 @@
         </is>
       </c>
       <c r="C524" t="n">
-        <v>3441</v>
+        <v>3442</v>
       </c>
       <c r="D524" t="n">
-        <v>5029245</v>
+        <v>5029765</v>
       </c>
       <c r="E524" t="inlineStr">
         <is>
@@ -25726,10 +25726,10 @@
         </is>
       </c>
       <c r="C529" t="n">
-        <v>1481</v>
+        <v>1482</v>
       </c>
       <c r="D529" t="n">
-        <v>1998436</v>
+        <v>1998948</v>
       </c>
       <c r="E529" t="inlineStr">
         <is>
@@ -25774,10 +25774,10 @@
         </is>
       </c>
       <c r="C530" t="n">
-        <v>3775</v>
+        <v>3778</v>
       </c>
       <c r="D530" t="n">
-        <v>5429880</v>
+        <v>5434380</v>
       </c>
       <c r="E530" t="inlineStr">
         <is>
@@ -25822,10 +25822,10 @@
         </is>
       </c>
       <c r="C531" t="n">
-        <v>9236</v>
+        <v>9241</v>
       </c>
       <c r="D531" t="n">
-        <v>13500727</v>
+        <v>13508227</v>
       </c>
       <c r="E531" t="inlineStr">
         <is>
@@ -26110,10 +26110,10 @@
         </is>
       </c>
       <c r="C537" t="n">
-        <v>3656</v>
+        <v>3658</v>
       </c>
       <c r="D537" t="n">
-        <v>4922206</v>
+        <v>4923386</v>
       </c>
       <c r="E537" t="inlineStr">
         <is>
@@ -26158,10 +26158,10 @@
         </is>
       </c>
       <c r="C538" t="n">
-        <v>1174</v>
+        <v>1175</v>
       </c>
       <c r="D538" t="n">
-        <v>1682770</v>
+        <v>1683765</v>
       </c>
       <c r="E538" t="inlineStr">
         <is>
@@ -26206,10 +26206,10 @@
         </is>
       </c>
       <c r="C539" t="n">
-        <v>3435</v>
+        <v>3436</v>
       </c>
       <c r="D539" t="n">
-        <v>5008941</v>
+        <v>5010441</v>
       </c>
       <c r="E539" t="inlineStr">
         <is>
@@ -26254,10 +26254,10 @@
         </is>
       </c>
       <c r="C540" t="n">
-        <v>1135</v>
+        <v>1136</v>
       </c>
       <c r="D540" t="n">
-        <v>1685183</v>
+        <v>1686683</v>
       </c>
       <c r="E540" t="inlineStr">
         <is>
@@ -26590,10 +26590,10 @@
         </is>
       </c>
       <c r="C547" t="n">
-        <v>625</v>
+        <v>626</v>
       </c>
       <c r="D547" t="n">
-        <v>932906</v>
+        <v>934406</v>
       </c>
       <c r="E547" t="inlineStr">
         <is>
@@ -26830,10 +26830,10 @@
         </is>
       </c>
       <c r="C552" t="n">
-        <v>2840</v>
+        <v>2841</v>
       </c>
       <c r="D552" t="n">
-        <v>4074708</v>
+        <v>4076049</v>
       </c>
       <c r="E552" t="inlineStr">
         <is>
@@ -26878,10 +26878,10 @@
         </is>
       </c>
       <c r="C553" t="n">
-        <v>5108</v>
+        <v>5110</v>
       </c>
       <c r="D553" t="n">
-        <v>7476049</v>
+        <v>7479049</v>
       </c>
       <c r="E553" t="inlineStr">
         <is>
@@ -26926,10 +26926,10 @@
         </is>
       </c>
       <c r="C554" t="n">
-        <v>1558</v>
+        <v>1559</v>
       </c>
       <c r="D554" t="n">
-        <v>2313122</v>
+        <v>2314622</v>
       </c>
       <c r="E554" t="inlineStr">
         <is>
@@ -27118,10 +27118,10 @@
         </is>
       </c>
       <c r="C558" t="n">
-        <v>1854</v>
+        <v>1856</v>
       </c>
       <c r="D558" t="n">
-        <v>2440277</v>
+        <v>2441927</v>
       </c>
       <c r="E558" t="inlineStr">
         <is>
@@ -27166,10 +27166,10 @@
         </is>
       </c>
       <c r="C559" t="n">
-        <v>1780</v>
+        <v>1781</v>
       </c>
       <c r="D559" t="n">
-        <v>2551381</v>
+        <v>2551856</v>
       </c>
       <c r="E559" t="inlineStr">
         <is>
@@ -27214,10 +27214,10 @@
         </is>
       </c>
       <c r="C560" t="n">
-        <v>3650</v>
+        <v>3651</v>
       </c>
       <c r="D560" t="n">
-        <v>5336224</v>
+        <v>5337724</v>
       </c>
       <c r="E560" t="inlineStr">
         <is>
@@ -27454,10 +27454,10 @@
         </is>
       </c>
       <c r="C565" t="n">
-        <v>1993</v>
+        <v>1994</v>
       </c>
       <c r="D565" t="n">
-        <v>2643039</v>
+        <v>2644539</v>
       </c>
       <c r="E565" t="inlineStr">
         <is>
@@ -27502,10 +27502,10 @@
         </is>
       </c>
       <c r="C566" t="n">
-        <v>4427</v>
+        <v>4429</v>
       </c>
       <c r="D566" t="n">
-        <v>6394237</v>
+        <v>6396387</v>
       </c>
       <c r="E566" t="inlineStr">
         <is>
@@ -27550,10 +27550,10 @@
         </is>
       </c>
       <c r="C567" t="n">
-        <v>10319</v>
+        <v>10327</v>
       </c>
       <c r="D567" t="n">
-        <v>15093001</v>
+        <v>15103702</v>
       </c>
       <c r="E567" t="inlineStr">
         <is>
@@ -27790,10 +27790,10 @@
         </is>
       </c>
       <c r="C572" t="n">
-        <v>4050</v>
+        <v>4052</v>
       </c>
       <c r="D572" t="n">
-        <v>5364650</v>
+        <v>5366800</v>
       </c>
       <c r="E572" t="inlineStr">
         <is>
@@ -27838,10 +27838,10 @@
         </is>
       </c>
       <c r="C573" t="n">
-        <v>1008</v>
+        <v>1009</v>
       </c>
       <c r="D573" t="n">
-        <v>1461706</v>
+        <v>1463206</v>
       </c>
       <c r="E573" t="inlineStr">
         <is>
@@ -27886,10 +27886,10 @@
         </is>
       </c>
       <c r="C574" t="n">
-        <v>2299</v>
+        <v>2300</v>
       </c>
       <c r="D574" t="n">
-        <v>3340121</v>
+        <v>3341621</v>
       </c>
       <c r="E574" t="inlineStr">
         <is>
@@ -28126,10 +28126,10 @@
         </is>
       </c>
       <c r="C579" t="n">
-        <v>6276</v>
+        <v>6282</v>
       </c>
       <c r="D579" t="n">
-        <v>9065044</v>
+        <v>9072776</v>
       </c>
       <c r="E579" t="inlineStr">
         <is>
@@ -28174,10 +28174,10 @@
         </is>
       </c>
       <c r="C580" t="n">
-        <v>15056</v>
+        <v>15061</v>
       </c>
       <c r="D580" t="n">
-        <v>22070563</v>
+        <v>22077958</v>
       </c>
       <c r="E580" t="inlineStr">
         <is>
@@ -28222,10 +28222,10 @@
         </is>
       </c>
       <c r="C581" t="n">
-        <v>5291</v>
+        <v>5292</v>
       </c>
       <c r="D581" t="n">
-        <v>7863178</v>
+        <v>7864678</v>
       </c>
       <c r="E581" t="inlineStr">
         <is>
@@ -28270,10 +28270,10 @@
         </is>
       </c>
       <c r="C582" t="n">
-        <v>1617</v>
+        <v>1619</v>
       </c>
       <c r="D582" t="n">
-        <v>2409491</v>
+        <v>2412178</v>
       </c>
       <c r="E582" t="inlineStr">
         <is>
@@ -28462,10 +28462,10 @@
         </is>
       </c>
       <c r="C586" t="n">
-        <v>6124</v>
+        <v>6128</v>
       </c>
       <c r="D586" t="n">
-        <v>8178235</v>
+        <v>8183778</v>
       </c>
       <c r="E586" t="inlineStr">
         <is>
@@ -28558,10 +28558,10 @@
         </is>
       </c>
       <c r="C588" t="n">
-        <v>3282</v>
+        <v>3286</v>
       </c>
       <c r="D588" t="n">
-        <v>4746234</v>
+        <v>4751061</v>
       </c>
       <c r="E588" t="inlineStr">
         <is>
@@ -28750,10 +28750,10 @@
         </is>
       </c>
       <c r="C592" t="n">
-        <v>1808</v>
+        <v>1810</v>
       </c>
       <c r="D592" t="n">
-        <v>2424078</v>
+        <v>2426228</v>
       </c>
       <c r="E592" t="inlineStr">
         <is>
@@ -28798,10 +28798,10 @@
         </is>
       </c>
       <c r="C593" t="n">
-        <v>8677</v>
+        <v>8684</v>
       </c>
       <c r="D593" t="n">
-        <v>12581258</v>
+        <v>12590776</v>
       </c>
       <c r="E593" t="inlineStr">
         <is>
@@ -28846,10 +28846,10 @@
         </is>
       </c>
       <c r="C594" t="n">
-        <v>18290</v>
+        <v>18301</v>
       </c>
       <c r="D594" t="n">
-        <v>26793145</v>
+        <v>26809645</v>
       </c>
       <c r="E594" t="inlineStr">
         <is>
@@ -28894,10 +28894,10 @@
         </is>
       </c>
       <c r="C595" t="n">
-        <v>5500</v>
+        <v>5503</v>
       </c>
       <c r="D595" t="n">
-        <v>8178215</v>
+        <v>8182715</v>
       </c>
       <c r="E595" t="inlineStr">
         <is>
@@ -28942,10 +28942,10 @@
         </is>
       </c>
       <c r="C596" t="n">
-        <v>1416</v>
+        <v>1418</v>
       </c>
       <c r="D596" t="n">
-        <v>2102736</v>
+        <v>2105736</v>
       </c>
       <c r="E596" t="inlineStr">
         <is>
@@ -29086,10 +29086,10 @@
         </is>
       </c>
       <c r="C599" t="n">
-        <v>6022</v>
+        <v>6029</v>
       </c>
       <c r="D599" t="n">
-        <v>8032673</v>
+        <v>8042673</v>
       </c>
       <c r="E599" t="inlineStr">
         <is>
@@ -29470,10 +29470,10 @@
         </is>
       </c>
       <c r="C607" t="n">
-        <v>712</v>
+        <v>713</v>
       </c>
       <c r="D607" t="n">
-        <v>1020522</v>
+        <v>1022022</v>
       </c>
       <c r="E607" t="inlineStr">
         <is>
@@ -29518,10 +29518,10 @@
         </is>
       </c>
       <c r="C608" t="n">
-        <v>1074</v>
+        <v>1075</v>
       </c>
       <c r="D608" t="n">
-        <v>1554770</v>
+        <v>1556270</v>
       </c>
       <c r="E608" t="inlineStr">
         <is>
@@ -29758,10 +29758,10 @@
         </is>
       </c>
       <c r="C613" t="n">
-        <v>4075</v>
+        <v>4076</v>
       </c>
       <c r="D613" t="n">
-        <v>5915602</v>
+        <v>5917102</v>
       </c>
       <c r="E613" t="inlineStr">
         <is>
@@ -29806,10 +29806,10 @@
         </is>
       </c>
       <c r="C614" t="n">
-        <v>6656</v>
+        <v>6659</v>
       </c>
       <c r="D614" t="n">
-        <v>9686013</v>
+        <v>9690026</v>
       </c>
       <c r="E614" t="inlineStr">
         <is>
@@ -29854,10 +29854,10 @@
         </is>
       </c>
       <c r="C615" t="n">
-        <v>2080</v>
+        <v>2081</v>
       </c>
       <c r="D615" t="n">
-        <v>3092365</v>
+        <v>3093865</v>
       </c>
       <c r="E615" t="inlineStr">
         <is>
@@ -30142,10 +30142,10 @@
         </is>
       </c>
       <c r="C621" t="n">
-        <v>4161</v>
+        <v>4162</v>
       </c>
       <c r="D621" t="n">
-        <v>6111245</v>
+        <v>6112745</v>
       </c>
       <c r="E621" t="inlineStr">
         <is>
@@ -30382,10 +30382,10 @@
         </is>
       </c>
       <c r="C626" t="n">
-        <v>1775</v>
+        <v>1776</v>
       </c>
       <c r="D626" t="n">
-        <v>2340021</v>
+        <v>2340532</v>
       </c>
       <c r="E626" t="inlineStr">
         <is>
@@ -30430,10 +30430,10 @@
         </is>
       </c>
       <c r="C627" t="n">
-        <v>1133</v>
+        <v>1134</v>
       </c>
       <c r="D627" t="n">
-        <v>1632730</v>
+        <v>1634230</v>
       </c>
       <c r="E627" t="inlineStr">
         <is>
@@ -30478,10 +30478,10 @@
         </is>
       </c>
       <c r="C628" t="n">
-        <v>2673</v>
+        <v>2674</v>
       </c>
       <c r="D628" t="n">
-        <v>3911954</v>
+        <v>3913454</v>
       </c>
       <c r="E628" t="inlineStr">
         <is>
@@ -30718,10 +30718,10 @@
         </is>
       </c>
       <c r="C633" t="n">
-        <v>1229</v>
+        <v>1231</v>
       </c>
       <c r="D633" t="n">
-        <v>1617158</v>
+        <v>1618958</v>
       </c>
       <c r="E633" t="inlineStr">
         <is>
@@ -30766,10 +30766,10 @@
         </is>
       </c>
       <c r="C634" t="n">
-        <v>5218</v>
+        <v>5224</v>
       </c>
       <c r="D634" t="n">
-        <v>7562573</v>
+        <v>7571573</v>
       </c>
       <c r="E634" t="inlineStr">
         <is>
@@ -30814,10 +30814,10 @@
         </is>
       </c>
       <c r="C635" t="n">
-        <v>12319</v>
+        <v>12328</v>
       </c>
       <c r="D635" t="n">
-        <v>18127586</v>
+        <v>18140386</v>
       </c>
       <c r="E635" t="inlineStr">
         <is>
@@ -30862,10 +30862,10 @@
         </is>
       </c>
       <c r="C636" t="n">
-        <v>4631</v>
+        <v>4633</v>
       </c>
       <c r="D636" t="n">
-        <v>6872528</v>
+        <v>6875528</v>
       </c>
       <c r="E636" t="inlineStr">
         <is>
@@ -30910,10 +30910,10 @@
         </is>
       </c>
       <c r="C637" t="n">
-        <v>1229</v>
+        <v>1230</v>
       </c>
       <c r="D637" t="n">
-        <v>1834766</v>
+        <v>1836266</v>
       </c>
       <c r="E637" t="inlineStr">
         <is>
@@ -31054,10 +31054,10 @@
         </is>
       </c>
       <c r="C640" t="n">
-        <v>4232</v>
+        <v>4233</v>
       </c>
       <c r="D640" t="n">
-        <v>5647781</v>
+        <v>5649281</v>
       </c>
       <c r="E640" t="inlineStr">
         <is>
@@ -31102,10 +31102,10 @@
         </is>
       </c>
       <c r="C641" t="n">
-        <v>2268</v>
+        <v>2270</v>
       </c>
       <c r="D641" t="n">
-        <v>3270023</v>
+        <v>3273023</v>
       </c>
       <c r="E641" t="inlineStr">
         <is>
@@ -31150,10 +31150,10 @@
         </is>
       </c>
       <c r="C642" t="n">
-        <v>6933</v>
+        <v>6936</v>
       </c>
       <c r="D642" t="n">
-        <v>10190319</v>
+        <v>10194819</v>
       </c>
       <c r="E642" t="inlineStr">
         <is>
@@ -31198,10 +31198,10 @@
         </is>
       </c>
       <c r="C643" t="n">
-        <v>2284</v>
+        <v>2285</v>
       </c>
       <c r="D643" t="n">
-        <v>3391540</v>
+        <v>3393040</v>
       </c>
       <c r="E643" t="inlineStr">
         <is>
@@ -31438,10 +31438,10 @@
         </is>
       </c>
       <c r="C648" t="n">
-        <v>2279</v>
+        <v>2280</v>
       </c>
       <c r="D648" t="n">
-        <v>3078647</v>
+        <v>3079816</v>
       </c>
       <c r="E648" t="inlineStr">
         <is>
@@ -31534,10 +31534,10 @@
         </is>
       </c>
       <c r="C650" t="n">
-        <v>2468</v>
+        <v>2469</v>
       </c>
       <c r="D650" t="n">
-        <v>3614879</v>
+        <v>3616379</v>
       </c>
       <c r="E650" t="inlineStr">
         <is>
@@ -31870,10 +31870,10 @@
         </is>
       </c>
       <c r="C657" t="n">
-        <v>4136</v>
+        <v>4139</v>
       </c>
       <c r="D657" t="n">
-        <v>6078658</v>
+        <v>6083158</v>
       </c>
       <c r="E657" t="inlineStr">
         <is>
@@ -32014,10 +32014,10 @@
         </is>
       </c>
       <c r="C660" t="n">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="D660" t="n">
-        <v>102000</v>
+        <v>103500</v>
       </c>
       <c r="E660" t="inlineStr">
         <is>
@@ -32206,10 +32206,10 @@
         </is>
       </c>
       <c r="C664" t="n">
-        <v>6407</v>
+        <v>6408</v>
       </c>
       <c r="D664" t="n">
-        <v>9377651</v>
+        <v>9379151</v>
       </c>
       <c r="E664" t="inlineStr">
         <is>
@@ -32494,10 +32494,10 @@
         </is>
       </c>
       <c r="C670" t="n">
-        <v>2061</v>
+        <v>2062</v>
       </c>
       <c r="D670" t="n">
-        <v>2758854</v>
+        <v>2760354</v>
       </c>
       <c r="E670" t="inlineStr">
         <is>
@@ -32590,10 +32590,10 @@
         </is>
       </c>
       <c r="C672" t="n">
-        <v>2865</v>
+        <v>2869</v>
       </c>
       <c r="D672" t="n">
-        <v>4178800</v>
+        <v>4184451</v>
       </c>
       <c r="E672" t="inlineStr">
         <is>
@@ -32878,10 +32878,10 @@
         </is>
       </c>
       <c r="C678" t="n">
-        <v>8629</v>
+        <v>8634</v>
       </c>
       <c r="D678" t="n">
-        <v>12491893</v>
+        <v>12498773</v>
       </c>
       <c r="E678" t="inlineStr">
         <is>
@@ -32926,10 +32926,10 @@
         </is>
       </c>
       <c r="C679" t="n">
-        <v>20667</v>
+        <v>20672</v>
       </c>
       <c r="D679" t="n">
-        <v>30322616</v>
+        <v>30330116</v>
       </c>
       <c r="E679" t="inlineStr">
         <is>
@@ -32974,10 +32974,10 @@
         </is>
       </c>
       <c r="C680" t="n">
-        <v>6157</v>
+        <v>6161</v>
       </c>
       <c r="D680" t="n">
-        <v>9154048</v>
+        <v>9160048</v>
       </c>
       <c r="E680" t="inlineStr">
         <is>
@@ -33022,10 +33022,10 @@
         </is>
       </c>
       <c r="C681" t="n">
-        <v>1774</v>
+        <v>1776</v>
       </c>
       <c r="D681" t="n">
-        <v>2649374</v>
+        <v>2652374</v>
       </c>
       <c r="E681" t="inlineStr">
         <is>
@@ -33166,10 +33166,10 @@
         </is>
       </c>
       <c r="C684" t="n">
-        <v>7478</v>
+        <v>7484</v>
       </c>
       <c r="D684" t="n">
-        <v>10169143</v>
+        <v>10176833</v>
       </c>
       <c r="E684" t="inlineStr">
         <is>
@@ -33214,10 +33214,10 @@
         </is>
       </c>
       <c r="C685" t="n">
-        <v>10570</v>
+        <v>10579</v>
       </c>
       <c r="D685" t="n">
-        <v>15347143</v>
+        <v>15358866</v>
       </c>
       <c r="E685" t="inlineStr">
         <is>
@@ -33262,10 +33262,10 @@
         </is>
       </c>
       <c r="C686" t="n">
-        <v>28293</v>
+        <v>28302</v>
       </c>
       <c r="D686" t="n">
-        <v>41542550</v>
+        <v>41554703</v>
       </c>
       <c r="E686" t="inlineStr">
         <is>
@@ -33310,10 +33310,10 @@
         </is>
       </c>
       <c r="C687" t="n">
-        <v>8909</v>
+        <v>8911</v>
       </c>
       <c r="D687" t="n">
-        <v>13263433</v>
+        <v>13266433</v>
       </c>
       <c r="E687" t="inlineStr">
         <is>
@@ -33550,10 +33550,10 @@
         </is>
       </c>
       <c r="C692" t="n">
-        <v>9470</v>
+        <v>9477</v>
       </c>
       <c r="D692" t="n">
-        <v>12779430</v>
+        <v>12787936</v>
       </c>
       <c r="E692" t="inlineStr">
         <is>
@@ -33598,10 +33598,10 @@
         </is>
       </c>
       <c r="C693" t="n">
-        <v>1295</v>
+        <v>1296</v>
       </c>
       <c r="D693" t="n">
-        <v>1864440</v>
+        <v>1865940</v>
       </c>
       <c r="E693" t="inlineStr">
         <is>
@@ -33646,10 +33646,10 @@
         </is>
       </c>
       <c r="C694" t="n">
-        <v>2694</v>
+        <v>2696</v>
       </c>
       <c r="D694" t="n">
-        <v>3934980</v>
+        <v>3937300</v>
       </c>
       <c r="E694" t="inlineStr">
         <is>
@@ -33694,10 +33694,10 @@
         </is>
       </c>
       <c r="C695" t="n">
-        <v>1039</v>
+        <v>1040</v>
       </c>
       <c r="D695" t="n">
-        <v>1530400</v>
+        <v>1531900</v>
       </c>
       <c r="E695" t="inlineStr">
         <is>
@@ -33790,10 +33790,10 @@
         </is>
       </c>
       <c r="C697" t="n">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="D697" t="n">
-        <v>134121</v>
+        <v>135621</v>
       </c>
       <c r="E697" t="inlineStr">
         <is>
@@ -33934,10 +33934,10 @@
         </is>
       </c>
       <c r="C700" t="n">
-        <v>9058</v>
+        <v>9062</v>
       </c>
       <c r="D700" t="n">
-        <v>12973750</v>
+        <v>12979565</v>
       </c>
       <c r="E700" t="inlineStr">
         <is>
@@ -33982,10 +33982,10 @@
         </is>
       </c>
       <c r="C701" t="n">
-        <v>16947</v>
+        <v>16954</v>
       </c>
       <c r="D701" t="n">
-        <v>24726717</v>
+        <v>24737217</v>
       </c>
       <c r="E701" t="inlineStr">
         <is>
@@ -34270,10 +34270,10 @@
         </is>
       </c>
       <c r="C707" t="n">
-        <v>5685</v>
+        <v>5692</v>
       </c>
       <c r="D707" t="n">
-        <v>7670766</v>
+        <v>7679123</v>
       </c>
       <c r="E707" t="inlineStr">
         <is>
@@ -34366,10 +34366,10 @@
         </is>
       </c>
       <c r="C709" t="n">
-        <v>9601</v>
+        <v>9607</v>
       </c>
       <c r="D709" t="n">
-        <v>14071699</v>
+        <v>14080699</v>
       </c>
       <c r="E709" t="inlineStr">
         <is>
@@ -34414,10 +34414,10 @@
         </is>
       </c>
       <c r="C710" t="n">
-        <v>2646</v>
+        <v>2647</v>
       </c>
       <c r="D710" t="n">
-        <v>3923710</v>
+        <v>3925210</v>
       </c>
       <c r="E710" t="inlineStr">
         <is>
@@ -34462,10 +34462,10 @@
         </is>
       </c>
       <c r="C711" t="n">
-        <v>593</v>
+        <v>594</v>
       </c>
       <c r="D711" t="n">
-        <v>880391</v>
+        <v>881891</v>
       </c>
       <c r="E711" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
[Fonds de solidarite] Add 2020-08-16 data
</commit_message>
<xml_diff>
--- a/published-data/fonds-solidarite-volet-1-departemental-classe-effectif-latest.xlsx
+++ b/published-data/fonds-solidarite-volet-1-departemental-classe-effectif-latest.xlsx
@@ -430,10 +430,10 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>1285</v>
+        <v>1286</v>
       </c>
       <c r="D2" t="n">
-        <v>1861635</v>
+        <v>1863135</v>
       </c>
       <c r="E2" t="inlineStr">
         <is>
@@ -478,10 +478,10 @@
         </is>
       </c>
       <c r="C3" t="n">
-        <v>5722</v>
+        <v>5726</v>
       </c>
       <c r="D3" t="n">
-        <v>8405486</v>
+        <v>8411486</v>
       </c>
       <c r="E3" t="inlineStr">
         <is>
@@ -526,10 +526,10 @@
         </is>
       </c>
       <c r="C4" t="n">
-        <v>2051</v>
+        <v>2052</v>
       </c>
       <c r="D4" t="n">
-        <v>3046532</v>
+        <v>3048032</v>
       </c>
       <c r="E4" t="inlineStr">
         <is>
@@ -622,10 +622,10 @@
         </is>
       </c>
       <c r="C6" t="n">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="D6" t="n">
-        <v>154944</v>
+        <v>156444</v>
       </c>
       <c r="E6" t="inlineStr">
         <is>
@@ -718,10 +718,10 @@
         </is>
       </c>
       <c r="C8" t="n">
-        <v>638</v>
+        <v>639</v>
       </c>
       <c r="D8" t="n">
-        <v>835457</v>
+        <v>836957</v>
       </c>
       <c r="E8" t="inlineStr">
         <is>
@@ -766,10 +766,10 @@
         </is>
       </c>
       <c r="C9" t="n">
-        <v>1191</v>
+        <v>1192</v>
       </c>
       <c r="D9" t="n">
-        <v>1720488</v>
+        <v>1721988</v>
       </c>
       <c r="E9" t="inlineStr">
         <is>
@@ -1006,10 +1006,10 @@
         </is>
       </c>
       <c r="C14" t="n">
-        <v>1947</v>
+        <v>1948</v>
       </c>
       <c r="D14" t="n">
-        <v>2567152</v>
+        <v>2567667</v>
       </c>
       <c r="E14" t="inlineStr">
         <is>
@@ -1102,10 +1102,10 @@
         </is>
       </c>
       <c r="C16" t="n">
-        <v>4206</v>
+        <v>4208</v>
       </c>
       <c r="D16" t="n">
-        <v>6139708</v>
+        <v>6141995</v>
       </c>
       <c r="E16" t="inlineStr">
         <is>
@@ -1342,10 +1342,10 @@
         </is>
       </c>
       <c r="C21" t="n">
-        <v>1785</v>
+        <v>1786</v>
       </c>
       <c r="D21" t="n">
-        <v>2368579</v>
+        <v>2370079</v>
       </c>
       <c r="E21" t="inlineStr">
         <is>
@@ -2014,10 +2014,10 @@
         </is>
       </c>
       <c r="C35" t="n">
-        <v>2509</v>
+        <v>2510</v>
       </c>
       <c r="D35" t="n">
-        <v>3212790</v>
+        <v>3214290</v>
       </c>
       <c r="E35" t="inlineStr">
         <is>
@@ -2350,10 +2350,10 @@
         </is>
       </c>
       <c r="C42" t="n">
-        <v>1358</v>
+        <v>1359</v>
       </c>
       <c r="D42" t="n">
-        <v>1835240</v>
+        <v>1836740</v>
       </c>
       <c r="E42" t="inlineStr">
         <is>
@@ -2446,10 +2446,10 @@
         </is>
       </c>
       <c r="C44" t="n">
-        <v>8947</v>
+        <v>8949</v>
       </c>
       <c r="D44" t="n">
-        <v>13113663</v>
+        <v>13116663</v>
       </c>
       <c r="E44" t="inlineStr">
         <is>
@@ -2494,10 +2494,10 @@
         </is>
       </c>
       <c r="C45" t="n">
-        <v>3651</v>
+        <v>3652</v>
       </c>
       <c r="D45" t="n">
-        <v>5402570</v>
+        <v>5404070</v>
       </c>
       <c r="E45" t="inlineStr">
         <is>
@@ -2686,10 +2686,10 @@
         </is>
       </c>
       <c r="C49" t="n">
-        <v>4997</v>
+        <v>4998</v>
       </c>
       <c r="D49" t="n">
-        <v>6837320</v>
+        <v>6838820</v>
       </c>
       <c r="E49" t="inlineStr">
         <is>
@@ -2782,10 +2782,10 @@
         </is>
       </c>
       <c r="C51" t="n">
-        <v>13624</v>
+        <v>13628</v>
       </c>
       <c r="D51" t="n">
-        <v>20031749</v>
+        <v>20037749</v>
       </c>
       <c r="E51" t="inlineStr">
         <is>
@@ -2830,10 +2830,10 @@
         </is>
       </c>
       <c r="C52" t="n">
-        <v>4621</v>
+        <v>4622</v>
       </c>
       <c r="D52" t="n">
-        <v>6843250</v>
+        <v>6844750</v>
       </c>
       <c r="E52" t="inlineStr">
         <is>
@@ -2878,10 +2878,10 @@
         </is>
       </c>
       <c r="C53" t="n">
-        <v>1248</v>
+        <v>1249</v>
       </c>
       <c r="D53" t="n">
-        <v>1853997</v>
+        <v>1855497</v>
       </c>
       <c r="E53" t="inlineStr">
         <is>
@@ -3118,10 +3118,10 @@
         </is>
       </c>
       <c r="C58" t="n">
-        <v>3171</v>
+        <v>3172</v>
       </c>
       <c r="D58" t="n">
-        <v>4577239</v>
+        <v>4578739</v>
       </c>
       <c r="E58" t="inlineStr">
         <is>
@@ -3166,10 +3166,10 @@
         </is>
       </c>
       <c r="C59" t="n">
-        <v>7830</v>
+        <v>7832</v>
       </c>
       <c r="D59" t="n">
-        <v>11477705</v>
+        <v>11480705</v>
       </c>
       <c r="E59" t="inlineStr">
         <is>
@@ -3214,10 +3214,10 @@
         </is>
       </c>
       <c r="C60" t="n">
-        <v>2490</v>
+        <v>2491</v>
       </c>
       <c r="D60" t="n">
-        <v>3670032</v>
+        <v>3671532</v>
       </c>
       <c r="E60" t="inlineStr">
         <is>
@@ -3406,10 +3406,10 @@
         </is>
       </c>
       <c r="C64" t="n">
-        <v>3379</v>
+        <v>3383</v>
       </c>
       <c r="D64" t="n">
-        <v>4407014</v>
+        <v>4410514</v>
       </c>
       <c r="E64" t="inlineStr">
         <is>
@@ -3454,10 +3454,10 @@
         </is>
       </c>
       <c r="C65" t="n">
-        <v>2687</v>
+        <v>2688</v>
       </c>
       <c r="D65" t="n">
-        <v>3860737</v>
+        <v>3862237</v>
       </c>
       <c r="E65" t="inlineStr">
         <is>
@@ -3502,10 +3502,10 @@
         </is>
       </c>
       <c r="C66" t="n">
-        <v>7025</v>
+        <v>7028</v>
       </c>
       <c r="D66" t="n">
-        <v>10277310</v>
+        <v>10281810</v>
       </c>
       <c r="E66" t="inlineStr">
         <is>
@@ -3742,10 +3742,10 @@
         </is>
       </c>
       <c r="C71" t="n">
-        <v>3004</v>
+        <v>3007</v>
       </c>
       <c r="D71" t="n">
-        <v>3967995</v>
+        <v>3971701</v>
       </c>
       <c r="E71" t="inlineStr">
         <is>
@@ -3790,10 +3790,10 @@
         </is>
       </c>
       <c r="C72" t="n">
-        <v>9151</v>
+        <v>9157</v>
       </c>
       <c r="D72" t="n">
-        <v>13272270</v>
+        <v>13280220</v>
       </c>
       <c r="E72" t="inlineStr">
         <is>
@@ -3838,10 +3838,10 @@
         </is>
       </c>
       <c r="C73" t="n">
-        <v>22475</v>
+        <v>22483</v>
       </c>
       <c r="D73" t="n">
-        <v>33018975</v>
+        <v>33030016</v>
       </c>
       <c r="E73" t="inlineStr">
         <is>
@@ -3886,10 +3886,10 @@
         </is>
       </c>
       <c r="C74" t="n">
-        <v>7743</v>
+        <v>7744</v>
       </c>
       <c r="D74" t="n">
-        <v>11494401</v>
+        <v>11495901</v>
       </c>
       <c r="E74" t="inlineStr">
         <is>
@@ -4222,10 +4222,10 @@
         </is>
       </c>
       <c r="C81" t="n">
-        <v>7463</v>
+        <v>7465</v>
       </c>
       <c r="D81" t="n">
-        <v>10261324</v>
+        <v>10264324</v>
       </c>
       <c r="E81" t="inlineStr">
         <is>
@@ -4270,10 +4270,10 @@
         </is>
       </c>
       <c r="C82" t="n">
-        <v>2762</v>
+        <v>2763</v>
       </c>
       <c r="D82" t="n">
-        <v>4004857</v>
+        <v>4006357</v>
       </c>
       <c r="E82" t="inlineStr">
         <is>
@@ -4318,10 +4318,10 @@
         </is>
       </c>
       <c r="C83" t="n">
-        <v>6436</v>
+        <v>6439</v>
       </c>
       <c r="D83" t="n">
-        <v>9419739</v>
+        <v>9424239</v>
       </c>
       <c r="E83" t="inlineStr">
         <is>
@@ -4414,10 +4414,10 @@
         </is>
       </c>
       <c r="C85" t="n">
-        <v>1031</v>
+        <v>1033</v>
       </c>
       <c r="D85" t="n">
-        <v>1526993</v>
+        <v>1529993</v>
       </c>
       <c r="E85" t="inlineStr">
         <is>
@@ -4462,10 +4462,10 @@
         </is>
       </c>
       <c r="C86" t="n">
-        <v>309</v>
+        <v>310</v>
       </c>
       <c r="D86" t="n">
-        <v>459275</v>
+        <v>460775</v>
       </c>
       <c r="E86" t="inlineStr">
         <is>
@@ -4558,10 +4558,10 @@
         </is>
       </c>
       <c r="C88" t="n">
-        <v>6459</v>
+        <v>6461</v>
       </c>
       <c r="D88" t="n">
-        <v>9066862</v>
+        <v>9069498</v>
       </c>
       <c r="E88" t="inlineStr">
         <is>
@@ -4654,10 +4654,10 @@
         </is>
       </c>
       <c r="C90" t="n">
-        <v>4918</v>
+        <v>4921</v>
       </c>
       <c r="D90" t="n">
-        <v>7222644</v>
+        <v>7226534</v>
       </c>
       <c r="E90" t="inlineStr">
         <is>
@@ -4750,10 +4750,10 @@
         </is>
       </c>
       <c r="C92" t="n">
-        <v>477</v>
+        <v>478</v>
       </c>
       <c r="D92" t="n">
-        <v>710008</v>
+        <v>711508</v>
       </c>
       <c r="E92" t="inlineStr">
         <is>
@@ -4894,10 +4894,10 @@
         </is>
       </c>
       <c r="C95" t="n">
-        <v>1994</v>
+        <v>1995</v>
       </c>
       <c r="D95" t="n">
-        <v>2623089</v>
+        <v>2624227</v>
       </c>
       <c r="E95" t="inlineStr">
         <is>
@@ -4990,10 +4990,10 @@
         </is>
       </c>
       <c r="C97" t="n">
-        <v>4542</v>
+        <v>4545</v>
       </c>
       <c r="D97" t="n">
-        <v>6665106</v>
+        <v>6669046</v>
       </c>
       <c r="E97" t="inlineStr">
         <is>
@@ -5278,10 +5278,10 @@
         </is>
       </c>
       <c r="C103" t="n">
-        <v>1546</v>
+        <v>1547</v>
       </c>
       <c r="D103" t="n">
-        <v>2087305</v>
+        <v>2088805</v>
       </c>
       <c r="E103" t="inlineStr">
         <is>
@@ -5374,10 +5374,10 @@
         </is>
       </c>
       <c r="C105" t="n">
-        <v>1756</v>
+        <v>1757</v>
       </c>
       <c r="D105" t="n">
-        <v>2583321</v>
+        <v>2584821</v>
       </c>
       <c r="E105" t="inlineStr">
         <is>
@@ -5566,10 +5566,10 @@
         </is>
       </c>
       <c r="C109" t="n">
-        <v>878</v>
+        <v>879</v>
       </c>
       <c r="D109" t="n">
-        <v>1112962</v>
+        <v>1114462</v>
       </c>
       <c r="E109" t="inlineStr">
         <is>
@@ -6238,10 +6238,10 @@
         </is>
       </c>
       <c r="C123" t="n">
-        <v>1965</v>
+        <v>1966</v>
       </c>
       <c r="D123" t="n">
-        <v>2840713</v>
+        <v>2842213</v>
       </c>
       <c r="E123" t="inlineStr">
         <is>
@@ -6286,10 +6286,10 @@
         </is>
       </c>
       <c r="C124" t="n">
-        <v>5745</v>
+        <v>5746</v>
       </c>
       <c r="D124" t="n">
-        <v>8418804</v>
+        <v>8420304</v>
       </c>
       <c r="E124" t="inlineStr">
         <is>
@@ -6478,10 +6478,10 @@
         </is>
       </c>
       <c r="C128" t="n">
-        <v>2464</v>
+        <v>2465</v>
       </c>
       <c r="D128" t="n">
-        <v>3318362</v>
+        <v>3319362</v>
       </c>
       <c r="E128" t="inlineStr">
         <is>
@@ -7102,10 +7102,10 @@
         </is>
       </c>
       <c r="C141" t="n">
-        <v>1137</v>
+        <v>1138</v>
       </c>
       <c r="D141" t="n">
-        <v>1490541</v>
+        <v>1492041</v>
       </c>
       <c r="E141" t="inlineStr">
         <is>
@@ -7198,10 +7198,10 @@
         </is>
       </c>
       <c r="C143" t="n">
-        <v>6087</v>
+        <v>6089</v>
       </c>
       <c r="D143" t="n">
-        <v>8910451</v>
+        <v>8913451</v>
       </c>
       <c r="E143" t="inlineStr">
         <is>
@@ -7438,10 +7438,10 @@
         </is>
       </c>
       <c r="C148" t="n">
-        <v>2398</v>
+        <v>2399</v>
       </c>
       <c r="D148" t="n">
-        <v>3145691</v>
+        <v>3147191</v>
       </c>
       <c r="E148" t="inlineStr">
         <is>
@@ -7486,10 +7486,10 @@
         </is>
       </c>
       <c r="C149" t="n">
-        <v>3610</v>
+        <v>3611</v>
       </c>
       <c r="D149" t="n">
-        <v>5202713</v>
+        <v>5203913</v>
       </c>
       <c r="E149" t="inlineStr">
         <is>
@@ -7534,10 +7534,10 @@
         </is>
       </c>
       <c r="C150" t="n">
-        <v>8230</v>
+        <v>8232</v>
       </c>
       <c r="D150" t="n">
-        <v>12043135</v>
+        <v>12046135</v>
       </c>
       <c r="E150" t="inlineStr">
         <is>
@@ -7822,10 +7822,10 @@
         </is>
       </c>
       <c r="C156" t="n">
-        <v>3392</v>
+        <v>3393</v>
       </c>
       <c r="D156" t="n">
-        <v>4917582</v>
+        <v>4919082</v>
       </c>
       <c r="E156" t="inlineStr">
         <is>
@@ -7870,10 +7870,10 @@
         </is>
       </c>
       <c r="C157" t="n">
-        <v>9442</v>
+        <v>9443</v>
       </c>
       <c r="D157" t="n">
-        <v>13924558</v>
+        <v>13926058</v>
       </c>
       <c r="E157" t="inlineStr">
         <is>
@@ -7918,10 +7918,10 @@
         </is>
       </c>
       <c r="C158" t="n">
-        <v>3107</v>
+        <v>3110</v>
       </c>
       <c r="D158" t="n">
-        <v>4625122</v>
+        <v>4629622</v>
       </c>
       <c r="E158" t="inlineStr">
         <is>
@@ -7966,10 +7966,10 @@
         </is>
       </c>
       <c r="C159" t="n">
-        <v>925</v>
+        <v>926</v>
       </c>
       <c r="D159" t="n">
-        <v>1382975</v>
+        <v>1384475</v>
       </c>
       <c r="E159" t="inlineStr">
         <is>
@@ -8110,10 +8110,10 @@
         </is>
       </c>
       <c r="C162" t="n">
-        <v>3163</v>
+        <v>3164</v>
       </c>
       <c r="D162" t="n">
-        <v>4262862</v>
+        <v>4263721</v>
       </c>
       <c r="E162" t="inlineStr">
         <is>
@@ -8158,10 +8158,10 @@
         </is>
       </c>
       <c r="C163" t="n">
-        <v>3726</v>
+        <v>3728</v>
       </c>
       <c r="D163" t="n">
-        <v>5365756</v>
+        <v>5368756</v>
       </c>
       <c r="E163" t="inlineStr">
         <is>
@@ -8206,10 +8206,10 @@
         </is>
       </c>
       <c r="C164" t="n">
-        <v>7891</v>
+        <v>7892</v>
       </c>
       <c r="D164" t="n">
-        <v>11567676</v>
+        <v>11569176</v>
       </c>
       <c r="E164" t="inlineStr">
         <is>
@@ -8494,10 +8494,10 @@
         </is>
       </c>
       <c r="C170" t="n">
-        <v>842</v>
+        <v>843</v>
       </c>
       <c r="D170" t="n">
-        <v>1221251</v>
+        <v>1222751</v>
       </c>
       <c r="E170" t="inlineStr">
         <is>
@@ -9118,10 +9118,10 @@
         </is>
       </c>
       <c r="C183" t="n">
-        <v>1114</v>
+        <v>1115</v>
       </c>
       <c r="D183" t="n">
-        <v>1494413</v>
+        <v>1495913</v>
       </c>
       <c r="E183" t="inlineStr">
         <is>
@@ -9214,10 +9214,10 @@
         </is>
       </c>
       <c r="C185" t="n">
-        <v>1923</v>
+        <v>1924</v>
       </c>
       <c r="D185" t="n">
-        <v>2801097</v>
+        <v>2802597</v>
       </c>
       <c r="E185" t="inlineStr">
         <is>
@@ -9406,10 +9406,10 @@
         </is>
       </c>
       <c r="C189" t="n">
-        <v>847</v>
+        <v>848</v>
       </c>
       <c r="D189" t="n">
-        <v>1076323</v>
+        <v>1076670</v>
       </c>
       <c r="E189" t="inlineStr">
         <is>
@@ -9454,10 +9454,10 @@
         </is>
       </c>
       <c r="C190" t="n">
-        <v>2194</v>
+        <v>2195</v>
       </c>
       <c r="D190" t="n">
-        <v>3151576</v>
+        <v>3153076</v>
       </c>
       <c r="E190" t="inlineStr">
         <is>
@@ -9502,10 +9502,10 @@
         </is>
       </c>
       <c r="C191" t="n">
-        <v>5742</v>
+        <v>5745</v>
       </c>
       <c r="D191" t="n">
-        <v>8410819</v>
+        <v>8415319</v>
       </c>
       <c r="E191" t="inlineStr">
         <is>
@@ -9742,10 +9742,10 @@
         </is>
       </c>
       <c r="C196" t="n">
-        <v>2144</v>
+        <v>2146</v>
       </c>
       <c r="D196" t="n">
-        <v>2875504</v>
+        <v>2877926</v>
       </c>
       <c r="E196" t="inlineStr">
         <is>
@@ -9838,10 +9838,10 @@
         </is>
       </c>
       <c r="C198" t="n">
-        <v>5635</v>
+        <v>5637</v>
       </c>
       <c r="D198" t="n">
-        <v>8289989</v>
+        <v>8292989</v>
       </c>
       <c r="E198" t="inlineStr">
         <is>
@@ -9934,10 +9934,10 @@
         </is>
       </c>
       <c r="C200" t="n">
-        <v>486</v>
+        <v>487</v>
       </c>
       <c r="D200" t="n">
-        <v>721874</v>
+        <v>723374</v>
       </c>
       <c r="E200" t="inlineStr">
         <is>
@@ -10222,10 +10222,10 @@
         </is>
       </c>
       <c r="C206" t="n">
-        <v>1060</v>
+        <v>1062</v>
       </c>
       <c r="D206" t="n">
-        <v>1579503</v>
+        <v>1582503</v>
       </c>
       <c r="E206" t="inlineStr">
         <is>
@@ -10414,10 +10414,10 @@
         </is>
       </c>
       <c r="C210" t="n">
-        <v>1111</v>
+        <v>1112</v>
       </c>
       <c r="D210" t="n">
-        <v>1494844</v>
+        <v>1496344</v>
       </c>
       <c r="E210" t="inlineStr">
         <is>
@@ -10510,10 +10510,10 @@
         </is>
       </c>
       <c r="C212" t="n">
-        <v>3716</v>
+        <v>3719</v>
       </c>
       <c r="D212" t="n">
-        <v>5427719</v>
+        <v>5432219</v>
       </c>
       <c r="E212" t="inlineStr">
         <is>
@@ -10558,10 +10558,10 @@
         </is>
       </c>
       <c r="C213" t="n">
-        <v>1921</v>
+        <v>1922</v>
       </c>
       <c r="D213" t="n">
-        <v>2845953</v>
+        <v>2847453</v>
       </c>
       <c r="E213" t="inlineStr">
         <is>
@@ -10798,10 +10798,10 @@
         </is>
       </c>
       <c r="C218" t="n">
-        <v>4107</v>
+        <v>4109</v>
       </c>
       <c r="D218" t="n">
-        <v>5996715</v>
+        <v>5999715</v>
       </c>
       <c r="E218" t="inlineStr">
         <is>
@@ -10990,10 +10990,10 @@
         </is>
       </c>
       <c r="C222" t="n">
-        <v>1691</v>
+        <v>1692</v>
       </c>
       <c r="D222" t="n">
-        <v>2299526</v>
+        <v>2301026</v>
       </c>
       <c r="E222" t="inlineStr">
         <is>
@@ -11086,10 +11086,10 @@
         </is>
       </c>
       <c r="C224" t="n">
-        <v>2285</v>
+        <v>2286</v>
       </c>
       <c r="D224" t="n">
-        <v>3323621</v>
+        <v>3325121</v>
       </c>
       <c r="E224" t="inlineStr">
         <is>
@@ -11614,10 +11614,10 @@
         </is>
       </c>
       <c r="C235" t="n">
-        <v>3968</v>
+        <v>3970</v>
       </c>
       <c r="D235" t="n">
-        <v>5740730</v>
+        <v>5743730</v>
       </c>
       <c r="E235" t="inlineStr">
         <is>
@@ -11662,10 +11662,10 @@
         </is>
       </c>
       <c r="C236" t="n">
-        <v>12413</v>
+        <v>12419</v>
       </c>
       <c r="D236" t="n">
-        <v>18207772</v>
+        <v>18216772</v>
       </c>
       <c r="E236" t="inlineStr">
         <is>
@@ -11710,10 +11710,10 @@
         </is>
       </c>
       <c r="C237" t="n">
-        <v>4803</v>
+        <v>4807</v>
       </c>
       <c r="D237" t="n">
-        <v>7127375</v>
+        <v>7133375</v>
       </c>
       <c r="E237" t="inlineStr">
         <is>
@@ -11902,10 +11902,10 @@
         </is>
       </c>
       <c r="C241" t="n">
-        <v>3435</v>
+        <v>3437</v>
       </c>
       <c r="D241" t="n">
-        <v>4656458</v>
+        <v>4658218</v>
       </c>
       <c r="E241" t="inlineStr">
         <is>
@@ -12238,10 +12238,10 @@
         </is>
       </c>
       <c r="C248" t="n">
-        <v>568</v>
+        <v>569</v>
       </c>
       <c r="D248" t="n">
-        <v>754919</v>
+        <v>756419</v>
       </c>
       <c r="E248" t="inlineStr">
         <is>
@@ -12286,10 +12286,10 @@
         </is>
       </c>
       <c r="C249" t="n">
-        <v>2686</v>
+        <v>2688</v>
       </c>
       <c r="D249" t="n">
-        <v>3882626</v>
+        <v>3885626</v>
       </c>
       <c r="E249" t="inlineStr">
         <is>
@@ -12334,10 +12334,10 @@
         </is>
       </c>
       <c r="C250" t="n">
-        <v>7912</v>
+        <v>7920</v>
       </c>
       <c r="D250" t="n">
-        <v>11608340</v>
+        <v>11620340</v>
       </c>
       <c r="E250" t="inlineStr">
         <is>
@@ -12382,10 +12382,10 @@
         </is>
       </c>
       <c r="C251" t="n">
-        <v>3211</v>
+        <v>3213</v>
       </c>
       <c r="D251" t="n">
-        <v>4769482</v>
+        <v>4772482</v>
       </c>
       <c r="E251" t="inlineStr">
         <is>
@@ -12670,10 +12670,10 @@
         </is>
       </c>
       <c r="C257" t="n">
-        <v>2068</v>
+        <v>2069</v>
       </c>
       <c r="D257" t="n">
-        <v>2720789</v>
+        <v>2722289</v>
       </c>
       <c r="E257" t="inlineStr">
         <is>
@@ -12862,10 +12862,10 @@
         </is>
       </c>
       <c r="C261" t="n">
-        <v>540</v>
+        <v>541</v>
       </c>
       <c r="D261" t="n">
-        <v>803539</v>
+        <v>805039</v>
       </c>
       <c r="E261" t="inlineStr">
         <is>
@@ -13102,10 +13102,10 @@
         </is>
       </c>
       <c r="C266" t="n">
-        <v>5551</v>
+        <v>5552</v>
       </c>
       <c r="D266" t="n">
-        <v>8159844</v>
+        <v>8161344</v>
       </c>
       <c r="E266" t="inlineStr">
         <is>
@@ -13438,10 +13438,10 @@
         </is>
       </c>
       <c r="C273" t="n">
-        <v>1405</v>
+        <v>1406</v>
       </c>
       <c r="D273" t="n">
-        <v>2043146</v>
+        <v>2044346</v>
       </c>
       <c r="E273" t="inlineStr">
         <is>
@@ -13678,10 +13678,10 @@
         </is>
       </c>
       <c r="C278" t="n">
-        <v>2640</v>
+        <v>2641</v>
       </c>
       <c r="D278" t="n">
-        <v>3822700</v>
+        <v>3824200</v>
       </c>
       <c r="E278" t="inlineStr">
         <is>
@@ -13726,10 +13726,10 @@
         </is>
       </c>
       <c r="C279" t="n">
-        <v>8580</v>
+        <v>8584</v>
       </c>
       <c r="D279" t="n">
-        <v>12575868</v>
+        <v>12581868</v>
       </c>
       <c r="E279" t="inlineStr">
         <is>
@@ -13774,10 +13774,10 @@
         </is>
       </c>
       <c r="C280" t="n">
-        <v>3546</v>
+        <v>3547</v>
       </c>
       <c r="D280" t="n">
-        <v>5273758</v>
+        <v>5275258</v>
       </c>
       <c r="E280" t="inlineStr">
         <is>
@@ -13966,10 +13966,10 @@
         </is>
       </c>
       <c r="C284" t="n">
-        <v>2415</v>
+        <v>2416</v>
       </c>
       <c r="D284" t="n">
-        <v>3222347</v>
+        <v>3223847</v>
       </c>
       <c r="E284" t="inlineStr">
         <is>
@@ -14062,10 +14062,10 @@
         </is>
       </c>
       <c r="C286" t="n">
-        <v>3958</v>
+        <v>3959</v>
       </c>
       <c r="D286" t="n">
-        <v>5809305</v>
+        <v>5810805</v>
       </c>
       <c r="E286" t="inlineStr">
         <is>
@@ -14350,10 +14350,10 @@
         </is>
       </c>
       <c r="C292" t="n">
-        <v>2020</v>
+        <v>2022</v>
       </c>
       <c r="D292" t="n">
-        <v>2929471</v>
+        <v>2932471</v>
       </c>
       <c r="E292" t="inlineStr">
         <is>
@@ -14398,10 +14398,10 @@
         </is>
       </c>
       <c r="C293" t="n">
-        <v>6893</v>
+        <v>6901</v>
       </c>
       <c r="D293" t="n">
-        <v>10132824</v>
+        <v>10144579</v>
       </c>
       <c r="E293" t="inlineStr">
         <is>
@@ -14638,10 +14638,10 @@
         </is>
       </c>
       <c r="C298" t="n">
-        <v>6972</v>
+        <v>6985</v>
       </c>
       <c r="D298" t="n">
-        <v>9586294</v>
+        <v>9601687</v>
       </c>
       <c r="E298" t="inlineStr">
         <is>
@@ -14686,10 +14686,10 @@
         </is>
       </c>
       <c r="C299" t="n">
-        <v>945</v>
+        <v>946</v>
       </c>
       <c r="D299" t="n">
-        <v>1387079</v>
+        <v>1388579</v>
       </c>
       <c r="E299" t="inlineStr">
         <is>
@@ -14734,10 +14734,10 @@
         </is>
       </c>
       <c r="C300" t="n">
-        <v>2374</v>
+        <v>2381</v>
       </c>
       <c r="D300" t="n">
-        <v>3519837</v>
+        <v>3530337</v>
       </c>
       <c r="E300" t="inlineStr">
         <is>
@@ -14782,10 +14782,10 @@
         </is>
       </c>
       <c r="C301" t="n">
-        <v>943</v>
+        <v>945</v>
       </c>
       <c r="D301" t="n">
-        <v>1404001</v>
+        <v>1407001</v>
       </c>
       <c r="E301" t="inlineStr">
         <is>
@@ -14974,10 +14974,10 @@
         </is>
       </c>
       <c r="C305" t="n">
-        <v>1392</v>
+        <v>1393</v>
       </c>
       <c r="D305" t="n">
-        <v>1959206</v>
+        <v>1960706</v>
       </c>
       <c r="E305" t="inlineStr">
         <is>
@@ -15070,10 +15070,10 @@
         </is>
       </c>
       <c r="C307" t="n">
-        <v>3566</v>
+        <v>3567</v>
       </c>
       <c r="D307" t="n">
-        <v>5231062</v>
+        <v>5232523</v>
       </c>
       <c r="E307" t="inlineStr">
         <is>
@@ -15358,10 +15358,10 @@
         </is>
       </c>
       <c r="C313" t="n">
-        <v>1425</v>
+        <v>1427</v>
       </c>
       <c r="D313" t="n">
-        <v>1900378</v>
+        <v>1902583</v>
       </c>
       <c r="E313" t="inlineStr">
         <is>
@@ -15406,10 +15406,10 @@
         </is>
       </c>
       <c r="C314" t="n">
-        <v>6993</v>
+        <v>6997</v>
       </c>
       <c r="D314" t="n">
-        <v>10091408</v>
+        <v>10094951</v>
       </c>
       <c r="E314" t="inlineStr">
         <is>
@@ -15454,10 +15454,10 @@
         </is>
       </c>
       <c r="C315" t="n">
-        <v>19582</v>
+        <v>19589</v>
       </c>
       <c r="D315" t="n">
-        <v>28647199</v>
+        <v>28656684</v>
       </c>
       <c r="E315" t="inlineStr">
         <is>
@@ -15502,10 +15502,10 @@
         </is>
       </c>
       <c r="C316" t="n">
-        <v>6945</v>
+        <v>6947</v>
       </c>
       <c r="D316" t="n">
-        <v>10336162</v>
+        <v>10339162</v>
       </c>
       <c r="E316" t="inlineStr">
         <is>
@@ -15598,10 +15598,10 @@
         </is>
       </c>
       <c r="C318" t="n">
-        <v>453</v>
+        <v>454</v>
       </c>
       <c r="D318" t="n">
-        <v>674542</v>
+        <v>676042</v>
       </c>
       <c r="E318" t="inlineStr">
         <is>
@@ -15742,10 +15742,10 @@
         </is>
       </c>
       <c r="C321" t="n">
-        <v>6206</v>
+        <v>6210</v>
       </c>
       <c r="D321" t="n">
-        <v>8161530</v>
+        <v>8166090</v>
       </c>
       <c r="E321" t="inlineStr">
         <is>
@@ -15790,10 +15790,10 @@
         </is>
       </c>
       <c r="C322" t="n">
-        <v>2091</v>
+        <v>2092</v>
       </c>
       <c r="D322" t="n">
-        <v>3062392</v>
+        <v>3063892</v>
       </c>
       <c r="E322" t="inlineStr">
         <is>
@@ -15838,10 +15838,10 @@
         </is>
       </c>
       <c r="C323" t="n">
-        <v>6499</v>
+        <v>6500</v>
       </c>
       <c r="D323" t="n">
-        <v>9541781</v>
+        <v>9543281</v>
       </c>
       <c r="E323" t="inlineStr">
         <is>
@@ -15886,10 +15886,10 @@
         </is>
       </c>
       <c r="C324" t="n">
-        <v>2288</v>
+        <v>2289</v>
       </c>
       <c r="D324" t="n">
-        <v>3404030</v>
+        <v>3405530</v>
       </c>
       <c r="E324" t="inlineStr">
         <is>
@@ -16126,10 +16126,10 @@
         </is>
       </c>
       <c r="C329" t="n">
-        <v>3583</v>
+        <v>3584</v>
       </c>
       <c r="D329" t="n">
-        <v>5151251</v>
+        <v>5152751</v>
       </c>
       <c r="E329" t="inlineStr">
         <is>
@@ -16222,10 +16222,10 @@
         </is>
       </c>
       <c r="C331" t="n">
-        <v>3505</v>
+        <v>3506</v>
       </c>
       <c r="D331" t="n">
-        <v>5197713</v>
+        <v>5199213</v>
       </c>
       <c r="E331" t="inlineStr">
         <is>
@@ -16270,10 +16270,10 @@
         </is>
       </c>
       <c r="C332" t="n">
-        <v>1090</v>
+        <v>1091</v>
       </c>
       <c r="D332" t="n">
-        <v>1620373</v>
+        <v>1621873</v>
       </c>
       <c r="E332" t="inlineStr">
         <is>
@@ -16558,10 +16558,10 @@
         </is>
       </c>
       <c r="C338" t="n">
-        <v>4233</v>
+        <v>4235</v>
       </c>
       <c r="D338" t="n">
-        <v>6183458</v>
+        <v>6186458</v>
       </c>
       <c r="E338" t="inlineStr">
         <is>
@@ -16846,10 +16846,10 @@
         </is>
       </c>
       <c r="C344" t="n">
-        <v>3610</v>
+        <v>3613</v>
       </c>
       <c r="D344" t="n">
-        <v>5271060</v>
+        <v>5275560</v>
       </c>
       <c r="E344" t="inlineStr">
         <is>
@@ -16894,10 +16894,10 @@
         </is>
       </c>
       <c r="C345" t="n">
-        <v>10398</v>
+        <v>10402</v>
       </c>
       <c r="D345" t="n">
-        <v>15342602</v>
+        <v>15348602</v>
       </c>
       <c r="E345" t="inlineStr">
         <is>
@@ -16942,10 +16942,10 @@
         </is>
       </c>
       <c r="C346" t="n">
-        <v>3995</v>
+        <v>3996</v>
       </c>
       <c r="D346" t="n">
-        <v>5947955</v>
+        <v>5949455</v>
       </c>
       <c r="E346" t="inlineStr">
         <is>
@@ -17278,10 +17278,10 @@
         </is>
       </c>
       <c r="C353" t="n">
-        <v>6449</v>
+        <v>6459</v>
       </c>
       <c r="D353" t="n">
-        <v>9393203</v>
+        <v>9407370</v>
       </c>
       <c r="E353" t="inlineStr">
         <is>
@@ -17326,10 +17326,10 @@
         </is>
       </c>
       <c r="C354" t="n">
-        <v>15619</v>
+        <v>15631</v>
       </c>
       <c r="D354" t="n">
-        <v>23001813</v>
+        <v>23019813</v>
       </c>
       <c r="E354" t="inlineStr">
         <is>
@@ -17374,10 +17374,10 @@
         </is>
       </c>
       <c r="C355" t="n">
-        <v>6934</v>
+        <v>6936</v>
       </c>
       <c r="D355" t="n">
-        <v>10334390</v>
+        <v>10337390</v>
       </c>
       <c r="E355" t="inlineStr">
         <is>
@@ -17422,10 +17422,10 @@
         </is>
       </c>
       <c r="C356" t="n">
-        <v>2112</v>
+        <v>2114</v>
       </c>
       <c r="D356" t="n">
-        <v>3152651</v>
+        <v>3155651</v>
       </c>
       <c r="E356" t="inlineStr">
         <is>
@@ -17566,10 +17566,10 @@
         </is>
       </c>
       <c r="C359" t="n">
-        <v>5730</v>
+        <v>5731</v>
       </c>
       <c r="D359" t="n">
-        <v>7819903</v>
+        <v>7820408</v>
       </c>
       <c r="E359" t="inlineStr">
         <is>
@@ -17614,10 +17614,10 @@
         </is>
       </c>
       <c r="C360" t="n">
-        <v>18862</v>
+        <v>18869</v>
       </c>
       <c r="D360" t="n">
-        <v>27382106</v>
+        <v>27391648</v>
       </c>
       <c r="E360" t="inlineStr">
         <is>
@@ -17662,10 +17662,10 @@
         </is>
       </c>
       <c r="C361" t="n">
-        <v>51680</v>
+        <v>51711</v>
       </c>
       <c r="D361" t="n">
-        <v>76153510</v>
+        <v>76198388</v>
       </c>
       <c r="E361" t="inlineStr">
         <is>
@@ -17710,10 +17710,10 @@
         </is>
       </c>
       <c r="C362" t="n">
-        <v>24151</v>
+        <v>24160</v>
       </c>
       <c r="D362" t="n">
-        <v>36031800</v>
+        <v>36045300</v>
       </c>
       <c r="E362" t="inlineStr">
         <is>
@@ -17758,10 +17758,10 @@
         </is>
       </c>
       <c r="C363" t="n">
-        <v>8691</v>
+        <v>8692</v>
       </c>
       <c r="D363" t="n">
-        <v>12997204</v>
+        <v>12998704</v>
       </c>
       <c r="E363" t="inlineStr">
         <is>
@@ -17806,10 +17806,10 @@
         </is>
       </c>
       <c r="C364" t="n">
-        <v>2214</v>
+        <v>2215</v>
       </c>
       <c r="D364" t="n">
-        <v>3308959</v>
+        <v>3310459</v>
       </c>
       <c r="E364" t="inlineStr">
         <is>
@@ -18046,10 +18046,10 @@
         </is>
       </c>
       <c r="C369" t="n">
-        <v>18547</v>
+        <v>18562</v>
       </c>
       <c r="D369" t="n">
-        <v>25150154</v>
+        <v>25167693</v>
       </c>
       <c r="E369" t="inlineStr">
         <is>
@@ -18094,10 +18094,10 @@
         </is>
       </c>
       <c r="C370" t="n">
-        <v>4335</v>
+        <v>4336</v>
       </c>
       <c r="D370" t="n">
-        <v>6311977</v>
+        <v>6312694</v>
       </c>
       <c r="E370" t="inlineStr">
         <is>
@@ -18142,10 +18142,10 @@
         </is>
       </c>
       <c r="C371" t="n">
-        <v>12343</v>
+        <v>12348</v>
       </c>
       <c r="D371" t="n">
-        <v>18148681</v>
+        <v>18155250</v>
       </c>
       <c r="E371" t="inlineStr">
         <is>
@@ -18430,10 +18430,10 @@
         </is>
       </c>
       <c r="C377" t="n">
-        <v>5421</v>
+        <v>5425</v>
       </c>
       <c r="D377" t="n">
-        <v>7889771</v>
+        <v>7895771</v>
       </c>
       <c r="E377" t="inlineStr">
         <is>
@@ -18478,10 +18478,10 @@
         </is>
       </c>
       <c r="C378" t="n">
-        <v>19189</v>
+        <v>19207</v>
       </c>
       <c r="D378" t="n">
-        <v>28268965</v>
+        <v>28294727</v>
       </c>
       <c r="E378" t="inlineStr">
         <is>
@@ -18526,10 +18526,10 @@
         </is>
       </c>
       <c r="C379" t="n">
-        <v>8951</v>
+        <v>8954</v>
       </c>
       <c r="D379" t="n">
-        <v>13347534</v>
+        <v>13352034</v>
       </c>
       <c r="E379" t="inlineStr">
         <is>
@@ -18574,10 +18574,10 @@
         </is>
       </c>
       <c r="C380" t="n">
-        <v>2499</v>
+        <v>2501</v>
       </c>
       <c r="D380" t="n">
-        <v>3735452</v>
+        <v>3738452</v>
       </c>
       <c r="E380" t="inlineStr">
         <is>
@@ -18718,10 +18718,10 @@
         </is>
       </c>
       <c r="C383" t="n">
-        <v>5607</v>
+        <v>5613</v>
       </c>
       <c r="D383" t="n">
-        <v>7558453</v>
+        <v>7566306</v>
       </c>
       <c r="E383" t="inlineStr">
         <is>
@@ -18766,10 +18766,10 @@
         </is>
       </c>
       <c r="C384" t="n">
-        <v>4853</v>
+        <v>4855</v>
       </c>
       <c r="D384" t="n">
-        <v>7073666</v>
+        <v>7076666</v>
       </c>
       <c r="E384" t="inlineStr">
         <is>
@@ -18814,10 +18814,10 @@
         </is>
       </c>
       <c r="C385" t="n">
-        <v>13918</v>
+        <v>13927</v>
       </c>
       <c r="D385" t="n">
-        <v>20488682</v>
+        <v>20501724</v>
       </c>
       <c r="E385" t="inlineStr">
         <is>
@@ -18862,10 +18862,10 @@
         </is>
       </c>
       <c r="C386" t="n">
-        <v>5739</v>
+        <v>5742</v>
       </c>
       <c r="D386" t="n">
-        <v>8547739</v>
+        <v>8552239</v>
       </c>
       <c r="E386" t="inlineStr">
         <is>
@@ -18958,10 +18958,10 @@
         </is>
       </c>
       <c r="C388" t="n">
-        <v>398</v>
+        <v>399</v>
       </c>
       <c r="D388" t="n">
-        <v>594106</v>
+        <v>595606</v>
       </c>
       <c r="E388" t="inlineStr">
         <is>
@@ -19102,10 +19102,10 @@
         </is>
       </c>
       <c r="C391" t="n">
-        <v>5020</v>
+        <v>5024</v>
       </c>
       <c r="D391" t="n">
-        <v>6847091</v>
+        <v>6852145</v>
       </c>
       <c r="E391" t="inlineStr">
         <is>
@@ -19150,10 +19150,10 @@
         </is>
       </c>
       <c r="C392" t="n">
-        <v>3659</v>
+        <v>3662</v>
       </c>
       <c r="D392" t="n">
-        <v>5339434</v>
+        <v>5342700</v>
       </c>
       <c r="E392" t="inlineStr">
         <is>
@@ -19198,10 +19198,10 @@
         </is>
       </c>
       <c r="C393" t="n">
-        <v>11542</v>
+        <v>11547</v>
       </c>
       <c r="D393" t="n">
-        <v>17025084</v>
+        <v>17032584</v>
       </c>
       <c r="E393" t="inlineStr">
         <is>
@@ -19246,10 +19246,10 @@
         </is>
       </c>
       <c r="C394" t="n">
-        <v>4836</v>
+        <v>4838</v>
       </c>
       <c r="D394" t="n">
-        <v>7195559</v>
+        <v>7198559</v>
       </c>
       <c r="E394" t="inlineStr">
         <is>
@@ -19486,10 +19486,10 @@
         </is>
       </c>
       <c r="C399" t="n">
-        <v>3923</v>
+        <v>3924</v>
       </c>
       <c r="D399" t="n">
-        <v>5297415</v>
+        <v>5298876</v>
       </c>
       <c r="E399" t="inlineStr">
         <is>
@@ -19534,10 +19534,10 @@
         </is>
       </c>
       <c r="C400" t="n">
-        <v>4161</v>
+        <v>4163</v>
       </c>
       <c r="D400" t="n">
-        <v>6065083</v>
+        <v>6068083</v>
       </c>
       <c r="E400" t="inlineStr">
         <is>
@@ -19582,10 +19582,10 @@
         </is>
       </c>
       <c r="C401" t="n">
-        <v>11255</v>
+        <v>11263</v>
       </c>
       <c r="D401" t="n">
-        <v>16580382</v>
+        <v>16591995</v>
       </c>
       <c r="E401" t="inlineStr">
         <is>
@@ -19630,10 +19630,10 @@
         </is>
       </c>
       <c r="C402" t="n">
-        <v>4329</v>
+        <v>4332</v>
       </c>
       <c r="D402" t="n">
-        <v>6441542</v>
+        <v>6445892</v>
       </c>
       <c r="E402" t="inlineStr">
         <is>
@@ -19678,10 +19678,10 @@
         </is>
       </c>
       <c r="C403" t="n">
-        <v>1360</v>
+        <v>1362</v>
       </c>
       <c r="D403" t="n">
-        <v>2032820</v>
+        <v>2035820</v>
       </c>
       <c r="E403" t="inlineStr">
         <is>
@@ -19822,10 +19822,10 @@
         </is>
       </c>
       <c r="C406" t="n">
-        <v>4128</v>
+        <v>4131</v>
       </c>
       <c r="D406" t="n">
-        <v>5655621</v>
+        <v>5658949</v>
       </c>
       <c r="E406" t="inlineStr">
         <is>
@@ -19870,10 +19870,10 @@
         </is>
       </c>
       <c r="C407" t="n">
-        <v>4596</v>
+        <v>4602</v>
       </c>
       <c r="D407" t="n">
-        <v>6658911</v>
+        <v>6667513</v>
       </c>
       <c r="E407" t="inlineStr">
         <is>
@@ -19918,10 +19918,10 @@
         </is>
       </c>
       <c r="C408" t="n">
-        <v>11556</v>
+        <v>11563</v>
       </c>
       <c r="D408" t="n">
-        <v>16976869</v>
+        <v>16987319</v>
       </c>
       <c r="E408" t="inlineStr">
         <is>
@@ -19966,10 +19966,10 @@
         </is>
       </c>
       <c r="C409" t="n">
-        <v>3881</v>
+        <v>3883</v>
       </c>
       <c r="D409" t="n">
-        <v>5784083</v>
+        <v>5787083</v>
       </c>
       <c r="E409" t="inlineStr">
         <is>
@@ -20014,10 +20014,10 @@
         </is>
       </c>
       <c r="C410" t="n">
-        <v>1343</v>
+        <v>1344</v>
       </c>
       <c r="D410" t="n">
-        <v>2006989</v>
+        <v>2008489</v>
       </c>
       <c r="E410" t="inlineStr">
         <is>
@@ -20206,10 +20206,10 @@
         </is>
       </c>
       <c r="C414" t="n">
-        <v>5409</v>
+        <v>5411</v>
       </c>
       <c r="D414" t="n">
-        <v>7271613</v>
+        <v>7274275</v>
       </c>
       <c r="E414" t="inlineStr">
         <is>
@@ -20254,10 +20254,10 @@
         </is>
       </c>
       <c r="C415" t="n">
-        <v>1595</v>
+        <v>1596</v>
       </c>
       <c r="D415" t="n">
-        <v>2297432</v>
+        <v>2298932</v>
       </c>
       <c r="E415" t="inlineStr">
         <is>
@@ -20302,10 +20302,10 @@
         </is>
       </c>
       <c r="C416" t="n">
-        <v>5161</v>
+        <v>5164</v>
       </c>
       <c r="D416" t="n">
-        <v>7600243</v>
+        <v>7604743</v>
       </c>
       <c r="E416" t="inlineStr">
         <is>
@@ -20590,10 +20590,10 @@
         </is>
       </c>
       <c r="C422" t="n">
-        <v>3557</v>
+        <v>3562</v>
       </c>
       <c r="D422" t="n">
-        <v>4707764</v>
+        <v>4715264</v>
       </c>
       <c r="E422" t="inlineStr">
         <is>
@@ -20638,10 +20638,10 @@
         </is>
       </c>
       <c r="C423" t="n">
-        <v>601</v>
+        <v>602</v>
       </c>
       <c r="D423" t="n">
-        <v>895164</v>
+        <v>896664</v>
       </c>
       <c r="E423" t="inlineStr">
         <is>
@@ -20878,10 +20878,10 @@
         </is>
       </c>
       <c r="C428" t="n">
-        <v>3082</v>
+        <v>3083</v>
       </c>
       <c r="D428" t="n">
-        <v>4463672</v>
+        <v>4465172</v>
       </c>
       <c r="E428" t="inlineStr">
         <is>
@@ -20926,10 +20926,10 @@
         </is>
       </c>
       <c r="C429" t="n">
-        <v>7372</v>
+        <v>7377</v>
       </c>
       <c r="D429" t="n">
-        <v>10817548</v>
+        <v>10825048</v>
       </c>
       <c r="E429" t="inlineStr">
         <is>
@@ -20974,10 +20974,10 @@
         </is>
       </c>
       <c r="C430" t="n">
-        <v>2438</v>
+        <v>2439</v>
       </c>
       <c r="D430" t="n">
-        <v>3634088</v>
+        <v>3635588</v>
       </c>
       <c r="E430" t="inlineStr">
         <is>
@@ -21166,10 +21166,10 @@
         </is>
       </c>
       <c r="C434" t="n">
-        <v>2422</v>
+        <v>2423</v>
       </c>
       <c r="D434" t="n">
-        <v>3233482</v>
+        <v>3234899</v>
       </c>
       <c r="E434" t="inlineStr">
         <is>
@@ -21358,10 +21358,10 @@
         </is>
       </c>
       <c r="C438" t="n">
-        <v>416</v>
+        <v>418</v>
       </c>
       <c r="D438" t="n">
-        <v>621188</v>
+        <v>624188</v>
       </c>
       <c r="E438" t="inlineStr">
         <is>
@@ -21502,10 +21502,10 @@
         </is>
       </c>
       <c r="C441" t="n">
-        <v>1686</v>
+        <v>1688</v>
       </c>
       <c r="D441" t="n">
-        <v>2212145</v>
+        <v>2214929</v>
       </c>
       <c r="E441" t="inlineStr">
         <is>
@@ -21598,10 +21598,10 @@
         </is>
       </c>
       <c r="C443" t="n">
-        <v>4875</v>
+        <v>4877</v>
       </c>
       <c r="D443" t="n">
-        <v>7161381</v>
+        <v>7164381</v>
       </c>
       <c r="E443" t="inlineStr">
         <is>
@@ -21886,10 +21886,10 @@
         </is>
       </c>
       <c r="C449" t="n">
-        <v>2665</v>
+        <v>2666</v>
       </c>
       <c r="D449" t="n">
-        <v>3908531</v>
+        <v>3910031</v>
       </c>
       <c r="E449" t="inlineStr">
         <is>
@@ -22126,10 +22126,10 @@
         </is>
       </c>
       <c r="C454" t="n">
-        <v>3040</v>
+        <v>3041</v>
       </c>
       <c r="D454" t="n">
-        <v>4424711</v>
+        <v>4426211</v>
       </c>
       <c r="E454" t="inlineStr">
         <is>
@@ -22174,10 +22174,10 @@
         </is>
       </c>
       <c r="C455" t="n">
-        <v>9377</v>
+        <v>9380</v>
       </c>
       <c r="D455" t="n">
-        <v>13806281</v>
+        <v>13810000</v>
       </c>
       <c r="E455" t="inlineStr">
         <is>
@@ -22270,10 +22270,10 @@
         </is>
       </c>
       <c r="C457" t="n">
-        <v>934</v>
+        <v>935</v>
       </c>
       <c r="D457" t="n">
-        <v>1393737</v>
+        <v>1395237</v>
       </c>
       <c r="E457" t="inlineStr">
         <is>
@@ -22414,10 +22414,10 @@
         </is>
       </c>
       <c r="C460" t="n">
-        <v>2974</v>
+        <v>2975</v>
       </c>
       <c r="D460" t="n">
-        <v>3886949</v>
+        <v>3887679</v>
       </c>
       <c r="E460" t="inlineStr">
         <is>
@@ -22462,10 +22462,10 @@
         </is>
       </c>
       <c r="C461" t="n">
-        <v>1215</v>
+        <v>1217</v>
       </c>
       <c r="D461" t="n">
-        <v>1745235</v>
+        <v>1747259</v>
       </c>
       <c r="E461" t="inlineStr">
         <is>
@@ -22750,10 +22750,10 @@
         </is>
       </c>
       <c r="C467" t="n">
-        <v>1345</v>
+        <v>1346</v>
       </c>
       <c r="D467" t="n">
-        <v>1711057</v>
+        <v>1712557</v>
       </c>
       <c r="E467" t="inlineStr">
         <is>
@@ -22798,10 +22798,10 @@
         </is>
       </c>
       <c r="C468" t="n">
-        <v>4423</v>
+        <v>4426</v>
       </c>
       <c r="D468" t="n">
-        <v>6402366</v>
+        <v>6406866</v>
       </c>
       <c r="E468" t="inlineStr">
         <is>
@@ -22846,10 +22846,10 @@
         </is>
       </c>
       <c r="C469" t="n">
-        <v>8237</v>
+        <v>8239</v>
       </c>
       <c r="D469" t="n">
-        <v>12078575</v>
+        <v>12081575</v>
       </c>
       <c r="E469" t="inlineStr">
         <is>
@@ -23086,10 +23086,10 @@
         </is>
       </c>
       <c r="C474" t="n">
-        <v>2781</v>
+        <v>2784</v>
       </c>
       <c r="D474" t="n">
-        <v>3711733</v>
+        <v>3714502</v>
       </c>
       <c r="E474" t="inlineStr">
         <is>
@@ -23470,10 +23470,10 @@
         </is>
       </c>
       <c r="C482" t="n">
-        <v>1076</v>
+        <v>1077</v>
       </c>
       <c r="D482" t="n">
-        <v>1548261</v>
+        <v>1549761</v>
       </c>
       <c r="E482" t="inlineStr">
         <is>
@@ -23806,10 +23806,10 @@
         </is>
       </c>
       <c r="C489" t="n">
-        <v>970</v>
+        <v>971</v>
       </c>
       <c r="D489" t="n">
-        <v>1449293</v>
+        <v>1450793</v>
       </c>
       <c r="E489" t="inlineStr">
         <is>
@@ -24286,10 +24286,10 @@
         </is>
       </c>
       <c r="C499" t="n">
-        <v>2402</v>
+        <v>2403</v>
       </c>
       <c r="D499" t="n">
-        <v>3143090</v>
+        <v>3143794</v>
       </c>
       <c r="E499" t="inlineStr">
         <is>
@@ -24334,10 +24334,10 @@
         </is>
       </c>
       <c r="C500" t="n">
-        <v>8842</v>
+        <v>8846</v>
       </c>
       <c r="D500" t="n">
-        <v>12807582</v>
+        <v>12813582</v>
       </c>
       <c r="E500" t="inlineStr">
         <is>
@@ -24382,10 +24382,10 @@
         </is>
       </c>
       <c r="C501" t="n">
-        <v>18418</v>
+        <v>18424</v>
       </c>
       <c r="D501" t="n">
-        <v>26964178</v>
+        <v>26971978</v>
       </c>
       <c r="E501" t="inlineStr">
         <is>
@@ -24430,10 +24430,10 @@
         </is>
       </c>
       <c r="C502" t="n">
-        <v>6255</v>
+        <v>6257</v>
       </c>
       <c r="D502" t="n">
-        <v>9305427</v>
+        <v>9308427</v>
       </c>
       <c r="E502" t="inlineStr">
         <is>
@@ -24718,10 +24718,10 @@
         </is>
       </c>
       <c r="C508" t="n">
-        <v>6633</v>
+        <v>6639</v>
       </c>
       <c r="D508" t="n">
-        <v>8980453</v>
+        <v>8988831</v>
       </c>
       <c r="E508" t="inlineStr">
         <is>
@@ -24862,10 +24862,10 @@
         </is>
       </c>
       <c r="C511" t="n">
-        <v>1055</v>
+        <v>1056</v>
       </c>
       <c r="D511" t="n">
-        <v>1568669</v>
+        <v>1570169</v>
       </c>
       <c r="E511" t="inlineStr">
         <is>
@@ -25102,10 +25102,10 @@
         </is>
       </c>
       <c r="C516" t="n">
-        <v>2917</v>
+        <v>2918</v>
       </c>
       <c r="D516" t="n">
-        <v>4183778</v>
+        <v>4185278</v>
       </c>
       <c r="E516" t="inlineStr">
         <is>
@@ -25198,10 +25198,10 @@
         </is>
       </c>
       <c r="C518" t="n">
-        <v>1523</v>
+        <v>1524</v>
       </c>
       <c r="D518" t="n">
-        <v>2264790</v>
+        <v>2266290</v>
       </c>
       <c r="E518" t="inlineStr">
         <is>
@@ -25438,10 +25438,10 @@
         </is>
       </c>
       <c r="C523" t="n">
-        <v>1617</v>
+        <v>1618</v>
       </c>
       <c r="D523" t="n">
-        <v>2332183</v>
+        <v>2333683</v>
       </c>
       <c r="E523" t="inlineStr">
         <is>
@@ -25486,10 +25486,10 @@
         </is>
       </c>
       <c r="C524" t="n">
-        <v>3444</v>
+        <v>3447</v>
       </c>
       <c r="D524" t="n">
-        <v>5032765</v>
+        <v>5036466</v>
       </c>
       <c r="E524" t="inlineStr">
         <is>
@@ -25534,10 +25534,10 @@
         </is>
       </c>
       <c r="C525" t="n">
-        <v>1175</v>
+        <v>1176</v>
       </c>
       <c r="D525" t="n">
-        <v>1744535</v>
+        <v>1746035</v>
       </c>
       <c r="E525" t="inlineStr">
         <is>
@@ -25726,10 +25726,10 @@
         </is>
       </c>
       <c r="C529" t="n">
-        <v>1482</v>
+        <v>1483</v>
       </c>
       <c r="D529" t="n">
-        <v>1998948</v>
+        <v>2000384</v>
       </c>
       <c r="E529" t="inlineStr">
         <is>
@@ -25774,10 +25774,10 @@
         </is>
       </c>
       <c r="C530" t="n">
-        <v>3783</v>
+        <v>3788</v>
       </c>
       <c r="D530" t="n">
-        <v>5440920</v>
+        <v>5445670</v>
       </c>
       <c r="E530" t="inlineStr">
         <is>
@@ -25822,10 +25822,10 @@
         </is>
       </c>
       <c r="C531" t="n">
-        <v>9251</v>
+        <v>9254</v>
       </c>
       <c r="D531" t="n">
-        <v>13522119</v>
+        <v>13526619</v>
       </c>
       <c r="E531" t="inlineStr">
         <is>
@@ -25870,10 +25870,10 @@
         </is>
       </c>
       <c r="C532" t="n">
-        <v>3118</v>
+        <v>3119</v>
       </c>
       <c r="D532" t="n">
-        <v>4627898</v>
+        <v>4629398</v>
       </c>
       <c r="E532" t="inlineStr">
         <is>
@@ -26542,10 +26542,10 @@
         </is>
       </c>
       <c r="C546" t="n">
-        <v>1791</v>
+        <v>1792</v>
       </c>
       <c r="D546" t="n">
-        <v>2612834</v>
+        <v>2614334</v>
       </c>
       <c r="E546" t="inlineStr">
         <is>
@@ -26782,10 +26782,10 @@
         </is>
       </c>
       <c r="C551" t="n">
-        <v>875</v>
+        <v>876</v>
       </c>
       <c r="D551" t="n">
-        <v>1106531</v>
+        <v>1108031</v>
       </c>
       <c r="E551" t="inlineStr">
         <is>
@@ -26830,10 +26830,10 @@
         </is>
       </c>
       <c r="C552" t="n">
-        <v>2843</v>
+        <v>2845</v>
       </c>
       <c r="D552" t="n">
-        <v>4079049</v>
+        <v>4081048</v>
       </c>
       <c r="E552" t="inlineStr">
         <is>
@@ -26878,10 +26878,10 @@
         </is>
       </c>
       <c r="C553" t="n">
-        <v>5115</v>
+        <v>5117</v>
       </c>
       <c r="D553" t="n">
-        <v>7484805</v>
+        <v>7487805</v>
       </c>
       <c r="E553" t="inlineStr">
         <is>
@@ -27166,10 +27166,10 @@
         </is>
       </c>
       <c r="C559" t="n">
-        <v>1782</v>
+        <v>1783</v>
       </c>
       <c r="D559" t="n">
-        <v>2553356</v>
+        <v>2554756</v>
       </c>
       <c r="E559" t="inlineStr">
         <is>
@@ -27454,10 +27454,10 @@
         </is>
       </c>
       <c r="C565" t="n">
-        <v>1997</v>
+        <v>1999</v>
       </c>
       <c r="D565" t="n">
-        <v>2649039</v>
+        <v>2652039</v>
       </c>
       <c r="E565" t="inlineStr">
         <is>
@@ -27502,10 +27502,10 @@
         </is>
       </c>
       <c r="C566" t="n">
-        <v>4432</v>
+        <v>4434</v>
       </c>
       <c r="D566" t="n">
-        <v>6400887</v>
+        <v>6403887</v>
       </c>
       <c r="E566" t="inlineStr">
         <is>
@@ -27550,10 +27550,10 @@
         </is>
       </c>
       <c r="C567" t="n">
-        <v>10337</v>
+        <v>10338</v>
       </c>
       <c r="D567" t="n">
-        <v>15118462</v>
+        <v>15119962</v>
       </c>
       <c r="E567" t="inlineStr">
         <is>
@@ -27598,10 +27598,10 @@
         </is>
       </c>
       <c r="C568" t="n">
-        <v>2880</v>
+        <v>2881</v>
       </c>
       <c r="D568" t="n">
-        <v>4268268</v>
+        <v>4269768</v>
       </c>
       <c r="E568" t="inlineStr">
         <is>
@@ -27790,10 +27790,10 @@
         </is>
       </c>
       <c r="C572" t="n">
-        <v>4053</v>
+        <v>4056</v>
       </c>
       <c r="D572" t="n">
-        <v>5367525</v>
+        <v>5371129</v>
       </c>
       <c r="E572" t="inlineStr">
         <is>
@@ -27838,10 +27838,10 @@
         </is>
       </c>
       <c r="C573" t="n">
-        <v>1010</v>
+        <v>1012</v>
       </c>
       <c r="D573" t="n">
-        <v>1464706</v>
+        <v>1467706</v>
       </c>
       <c r="E573" t="inlineStr">
         <is>
@@ -28078,10 +28078,10 @@
         </is>
       </c>
       <c r="C578" t="n">
-        <v>1254</v>
+        <v>1256</v>
       </c>
       <c r="D578" t="n">
-        <v>1646719</v>
+        <v>1649719</v>
       </c>
       <c r="E578" t="inlineStr">
         <is>
@@ -28126,10 +28126,10 @@
         </is>
       </c>
       <c r="C579" t="n">
-        <v>6291</v>
+        <v>6293</v>
       </c>
       <c r="D579" t="n">
-        <v>9084861</v>
+        <v>9087861</v>
       </c>
       <c r="E579" t="inlineStr">
         <is>
@@ -28174,10 +28174,10 @@
         </is>
       </c>
       <c r="C580" t="n">
-        <v>15067</v>
+        <v>15076</v>
       </c>
       <c r="D580" t="n">
-        <v>22086343</v>
+        <v>22099740</v>
       </c>
       <c r="E580" t="inlineStr">
         <is>
@@ -28222,10 +28222,10 @@
         </is>
       </c>
       <c r="C581" t="n">
-        <v>5296</v>
+        <v>5300</v>
       </c>
       <c r="D581" t="n">
-        <v>7870678</v>
+        <v>7876678</v>
       </c>
       <c r="E581" t="inlineStr">
         <is>
@@ -28462,10 +28462,10 @@
         </is>
       </c>
       <c r="C586" t="n">
-        <v>6138</v>
+        <v>6144</v>
       </c>
       <c r="D586" t="n">
-        <v>8195533</v>
+        <v>8204033</v>
       </c>
       <c r="E586" t="inlineStr">
         <is>
@@ -28702,10 +28702,10 @@
         </is>
       </c>
       <c r="C591" t="n">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="D591" t="n">
-        <v>97834</v>
+        <v>99334</v>
       </c>
       <c r="E591" t="inlineStr">
         <is>
@@ -28750,10 +28750,10 @@
         </is>
       </c>
       <c r="C592" t="n">
-        <v>1812</v>
+        <v>1813</v>
       </c>
       <c r="D592" t="n">
-        <v>2428998</v>
+        <v>2430498</v>
       </c>
       <c r="E592" t="inlineStr">
         <is>
@@ -28798,10 +28798,10 @@
         </is>
       </c>
       <c r="C593" t="n">
-        <v>8689</v>
+        <v>8696</v>
       </c>
       <c r="D593" t="n">
-        <v>12597526</v>
+        <v>12608026</v>
       </c>
       <c r="E593" t="inlineStr">
         <is>
@@ -28846,10 +28846,10 @@
         </is>
       </c>
       <c r="C594" t="n">
-        <v>18315</v>
+        <v>18323</v>
       </c>
       <c r="D594" t="n">
-        <v>26830645</v>
+        <v>26841535</v>
       </c>
       <c r="E594" t="inlineStr">
         <is>
@@ -28894,10 +28894,10 @@
         </is>
       </c>
       <c r="C595" t="n">
-        <v>5508</v>
+        <v>5511</v>
       </c>
       <c r="D595" t="n">
-        <v>8190215</v>
+        <v>8194715</v>
       </c>
       <c r="E595" t="inlineStr">
         <is>
@@ -29086,10 +29086,10 @@
         </is>
       </c>
       <c r="C599" t="n">
-        <v>6035</v>
+        <v>6037</v>
       </c>
       <c r="D599" t="n">
-        <v>8049462</v>
+        <v>8051686</v>
       </c>
       <c r="E599" t="inlineStr">
         <is>
@@ -29134,10 +29134,10 @@
         </is>
       </c>
       <c r="C600" t="n">
-        <v>1305</v>
+        <v>1306</v>
       </c>
       <c r="D600" t="n">
-        <v>1878789</v>
+        <v>1880289</v>
       </c>
       <c r="E600" t="inlineStr">
         <is>
@@ -29422,10 +29422,10 @@
         </is>
       </c>
       <c r="C606" t="n">
-        <v>1227</v>
+        <v>1228</v>
       </c>
       <c r="D606" t="n">
-        <v>1616554</v>
+        <v>1618054</v>
       </c>
       <c r="E606" t="inlineStr">
         <is>
@@ -29758,10 +29758,10 @@
         </is>
       </c>
       <c r="C613" t="n">
-        <v>4079</v>
+        <v>4080</v>
       </c>
       <c r="D613" t="n">
-        <v>5921602</v>
+        <v>5923102</v>
       </c>
       <c r="E613" t="inlineStr">
         <is>
@@ -29806,10 +29806,10 @@
         </is>
       </c>
       <c r="C614" t="n">
-        <v>6665</v>
+        <v>6666</v>
       </c>
       <c r="D614" t="n">
-        <v>9698016</v>
+        <v>9699516</v>
       </c>
       <c r="E614" t="inlineStr">
         <is>
@@ -29854,10 +29854,10 @@
         </is>
       </c>
       <c r="C615" t="n">
-        <v>2083</v>
+        <v>2084</v>
       </c>
       <c r="D615" t="n">
-        <v>3096865</v>
+        <v>3098365</v>
       </c>
       <c r="E615" t="inlineStr">
         <is>
@@ -30046,10 +30046,10 @@
         </is>
       </c>
       <c r="C619" t="n">
-        <v>2615</v>
+        <v>2616</v>
       </c>
       <c r="D619" t="n">
-        <v>3476762</v>
+        <v>3478262</v>
       </c>
       <c r="E619" t="inlineStr">
         <is>
@@ -30142,10 +30142,10 @@
         </is>
       </c>
       <c r="C621" t="n">
-        <v>4165</v>
+        <v>4167</v>
       </c>
       <c r="D621" t="n">
-        <v>6117245</v>
+        <v>6120245</v>
       </c>
       <c r="E621" t="inlineStr">
         <is>
@@ -30382,10 +30382,10 @@
         </is>
       </c>
       <c r="C626" t="n">
-        <v>1778</v>
+        <v>1780</v>
       </c>
       <c r="D626" t="n">
-        <v>2342462</v>
+        <v>2344958</v>
       </c>
       <c r="E626" t="inlineStr">
         <is>
@@ -30478,10 +30478,10 @@
         </is>
       </c>
       <c r="C628" t="n">
-        <v>2678</v>
+        <v>2679</v>
       </c>
       <c r="D628" t="n">
-        <v>3918802</v>
+        <v>3920302</v>
       </c>
       <c r="E628" t="inlineStr">
         <is>
@@ -30622,10 +30622,10 @@
         </is>
       </c>
       <c r="C631" t="n">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="D631" t="n">
-        <v>58500</v>
+        <v>60000</v>
       </c>
       <c r="E631" t="inlineStr">
         <is>
@@ -30766,10 +30766,10 @@
         </is>
       </c>
       <c r="C634" t="n">
-        <v>5227</v>
+        <v>5229</v>
       </c>
       <c r="D634" t="n">
-        <v>7576073</v>
+        <v>7579073</v>
       </c>
       <c r="E634" t="inlineStr">
         <is>
@@ -30814,10 +30814,10 @@
         </is>
       </c>
       <c r="C635" t="n">
-        <v>12337</v>
+        <v>12339</v>
       </c>
       <c r="D635" t="n">
-        <v>18152526</v>
+        <v>18155526</v>
       </c>
       <c r="E635" t="inlineStr">
         <is>
@@ -30958,10 +30958,10 @@
         </is>
       </c>
       <c r="C638" t="n">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="D638" t="n">
-        <v>339262</v>
+        <v>340762</v>
       </c>
       <c r="E638" t="inlineStr">
         <is>
@@ -31054,10 +31054,10 @@
         </is>
       </c>
       <c r="C640" t="n">
-        <v>4234</v>
+        <v>4235</v>
       </c>
       <c r="D640" t="n">
-        <v>5649581</v>
+        <v>5651081</v>
       </c>
       <c r="E640" t="inlineStr">
         <is>
@@ -31102,10 +31102,10 @@
         </is>
       </c>
       <c r="C641" t="n">
-        <v>2271</v>
+        <v>2273</v>
       </c>
       <c r="D641" t="n">
-        <v>3274523</v>
+        <v>3277523</v>
       </c>
       <c r="E641" t="inlineStr">
         <is>
@@ -31150,10 +31150,10 @@
         </is>
       </c>
       <c r="C642" t="n">
-        <v>6938</v>
+        <v>6940</v>
       </c>
       <c r="D642" t="n">
-        <v>10197819</v>
+        <v>10200819</v>
       </c>
       <c r="E642" t="inlineStr">
         <is>
@@ -31438,10 +31438,10 @@
         </is>
       </c>
       <c r="C648" t="n">
-        <v>2280</v>
+        <v>2281</v>
       </c>
       <c r="D648" t="n">
-        <v>3079816</v>
+        <v>3081316</v>
       </c>
       <c r="E648" t="inlineStr">
         <is>
@@ -31486,10 +31486,10 @@
         </is>
       </c>
       <c r="C649" t="n">
-        <v>923</v>
+        <v>924</v>
       </c>
       <c r="D649" t="n">
-        <v>1332305</v>
+        <v>1333805</v>
       </c>
       <c r="E649" t="inlineStr">
         <is>
@@ -31774,10 +31774,10 @@
         </is>
       </c>
       <c r="C655" t="n">
-        <v>851</v>
+        <v>852</v>
       </c>
       <c r="D655" t="n">
-        <v>1125093</v>
+        <v>1125326</v>
       </c>
       <c r="E655" t="inlineStr">
         <is>
@@ -31966,10 +31966,10 @@
         </is>
       </c>
       <c r="C659" t="n">
-        <v>350</v>
+        <v>352</v>
       </c>
       <c r="D659" t="n">
-        <v>518265</v>
+        <v>521265</v>
       </c>
       <c r="E659" t="inlineStr">
         <is>
@@ -32110,10 +32110,10 @@
         </is>
       </c>
       <c r="C662" t="n">
-        <v>1375</v>
+        <v>1376</v>
       </c>
       <c r="D662" t="n">
-        <v>1790712</v>
+        <v>1791512</v>
       </c>
       <c r="E662" t="inlineStr">
         <is>
@@ -32158,10 +32158,10 @@
         </is>
       </c>
       <c r="C663" t="n">
-        <v>3241</v>
+        <v>3245</v>
       </c>
       <c r="D663" t="n">
-        <v>4705983</v>
+        <v>4711596</v>
       </c>
       <c r="E663" t="inlineStr">
         <is>
@@ -32206,10 +32206,10 @@
         </is>
       </c>
       <c r="C664" t="n">
-        <v>6414</v>
+        <v>6416</v>
       </c>
       <c r="D664" t="n">
-        <v>9388151</v>
+        <v>9391151</v>
       </c>
       <c r="E664" t="inlineStr">
         <is>
@@ -32302,10 +32302,10 @@
         </is>
       </c>
       <c r="C666" t="n">
-        <v>534</v>
+        <v>535</v>
       </c>
       <c r="D666" t="n">
-        <v>796161</v>
+        <v>797661</v>
       </c>
       <c r="E666" t="inlineStr">
         <is>
@@ -32494,10 +32494,10 @@
         </is>
       </c>
       <c r="C670" t="n">
-        <v>2062</v>
+        <v>2063</v>
       </c>
       <c r="D670" t="n">
-        <v>2760354</v>
+        <v>2761554</v>
       </c>
       <c r="E670" t="inlineStr">
         <is>
@@ -32542,10 +32542,10 @@
         </is>
       </c>
       <c r="C671" t="n">
-        <v>1566</v>
+        <v>1568</v>
       </c>
       <c r="D671" t="n">
-        <v>2261539</v>
+        <v>2264539</v>
       </c>
       <c r="E671" t="inlineStr">
         <is>
@@ -32686,10 +32686,10 @@
         </is>
       </c>
       <c r="C674" t="n">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="D674" t="n">
-        <v>268937</v>
+        <v>270437</v>
       </c>
       <c r="E674" t="inlineStr">
         <is>
@@ -32878,10 +32878,10 @@
         </is>
       </c>
       <c r="C678" t="n">
-        <v>8654</v>
+        <v>8660</v>
       </c>
       <c r="D678" t="n">
-        <v>12526707</v>
+        <v>12535707</v>
       </c>
       <c r="E678" t="inlineStr">
         <is>
@@ -32926,10 +32926,10 @@
         </is>
       </c>
       <c r="C679" t="n">
-        <v>20685</v>
+        <v>20690</v>
       </c>
       <c r="D679" t="n">
-        <v>30349330</v>
+        <v>30356830</v>
       </c>
       <c r="E679" t="inlineStr">
         <is>
@@ -32974,10 +32974,10 @@
         </is>
       </c>
       <c r="C680" t="n">
-        <v>6168</v>
+        <v>6170</v>
       </c>
       <c r="D680" t="n">
-        <v>9170548</v>
+        <v>9173548</v>
       </c>
       <c r="E680" t="inlineStr">
         <is>
@@ -33022,10 +33022,10 @@
         </is>
       </c>
       <c r="C681" t="n">
-        <v>1778</v>
+        <v>1779</v>
       </c>
       <c r="D681" t="n">
-        <v>2655374</v>
+        <v>2656874</v>
       </c>
       <c r="E681" t="inlineStr">
         <is>
@@ -33166,10 +33166,10 @@
         </is>
       </c>
       <c r="C684" t="n">
-        <v>7497</v>
+        <v>7500</v>
       </c>
       <c r="D684" t="n">
-        <v>10192018</v>
+        <v>10196518</v>
       </c>
       <c r="E684" t="inlineStr">
         <is>
@@ -33214,10 +33214,10 @@
         </is>
       </c>
       <c r="C685" t="n">
-        <v>10592</v>
+        <v>10600</v>
       </c>
       <c r="D685" t="n">
-        <v>15377322</v>
+        <v>15389322</v>
       </c>
       <c r="E685" t="inlineStr">
         <is>
@@ -33262,10 +33262,10 @@
         </is>
       </c>
       <c r="C686" t="n">
-        <v>28332</v>
+        <v>28337</v>
       </c>
       <c r="D686" t="n">
-        <v>41597768</v>
+        <v>41604168</v>
       </c>
       <c r="E686" t="inlineStr">
         <is>
@@ -33310,10 +33310,10 @@
         </is>
       </c>
       <c r="C687" t="n">
-        <v>8915</v>
+        <v>8919</v>
       </c>
       <c r="D687" t="n">
-        <v>13272033</v>
+        <v>13277653</v>
       </c>
       <c r="E687" t="inlineStr">
         <is>
@@ -33550,10 +33550,10 @@
         </is>
       </c>
       <c r="C692" t="n">
-        <v>9491</v>
+        <v>9499</v>
       </c>
       <c r="D692" t="n">
-        <v>12803786</v>
+        <v>12812583</v>
       </c>
       <c r="E692" t="inlineStr">
         <is>
@@ -33598,10 +33598,10 @@
         </is>
       </c>
       <c r="C693" t="n">
-        <v>1298</v>
+        <v>1300</v>
       </c>
       <c r="D693" t="n">
-        <v>1868940</v>
+        <v>1871940</v>
       </c>
       <c r="E693" t="inlineStr">
         <is>
@@ -33694,10 +33694,10 @@
         </is>
       </c>
       <c r="C695" t="n">
-        <v>1041</v>
+        <v>1042</v>
       </c>
       <c r="D695" t="n">
-        <v>1533400</v>
+        <v>1534900</v>
       </c>
       <c r="E695" t="inlineStr">
         <is>
@@ -33934,10 +33934,10 @@
         </is>
       </c>
       <c r="C700" t="n">
-        <v>9071</v>
+        <v>9074</v>
       </c>
       <c r="D700" t="n">
-        <v>12990362</v>
+        <v>12994862</v>
       </c>
       <c r="E700" t="inlineStr">
         <is>
@@ -33982,10 +33982,10 @@
         </is>
       </c>
       <c r="C701" t="n">
-        <v>16964</v>
+        <v>16969</v>
       </c>
       <c r="D701" t="n">
-        <v>24751294</v>
+        <v>24758728</v>
       </c>
       <c r="E701" t="inlineStr">
         <is>
@@ -34030,10 +34030,10 @@
         </is>
       </c>
       <c r="C702" t="n">
-        <v>4706</v>
+        <v>4708</v>
       </c>
       <c r="D702" t="n">
-        <v>6990367</v>
+        <v>6993367</v>
       </c>
       <c r="E702" t="inlineStr">
         <is>
@@ -34078,10 +34078,10 @@
         </is>
       </c>
       <c r="C703" t="n">
-        <v>1134</v>
+        <v>1136</v>
       </c>
       <c r="D703" t="n">
-        <v>1693876</v>
+        <v>1696876</v>
       </c>
       <c r="E703" t="inlineStr">
         <is>
@@ -34366,10 +34366,10 @@
         </is>
       </c>
       <c r="C709" t="n">
-        <v>9610</v>
+        <v>9614</v>
       </c>
       <c r="D709" t="n">
-        <v>14085199</v>
+        <v>14090899</v>
       </c>
       <c r="E709" t="inlineStr">
         <is>
@@ -34606,10 +34606,10 @@
         </is>
       </c>
       <c r="C714" t="n">
-        <v>3226</v>
+        <v>3229</v>
       </c>
       <c r="D714" t="n">
-        <v>4247801</v>
+        <v>4250974</v>
       </c>
       <c r="E714" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
[Fonds de solidarite] Add 2020-08-17 data
</commit_message>
<xml_diff>
--- a/published-data/fonds-solidarite-volet-1-departemental-classe-effectif-latest.xlsx
+++ b/published-data/fonds-solidarite-volet-1-departemental-classe-effectif-latest.xlsx
@@ -430,10 +430,10 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>1286</v>
+        <v>1287</v>
       </c>
       <c r="D2" t="n">
-        <v>1863135</v>
+        <v>1864635</v>
       </c>
       <c r="E2" t="inlineStr">
         <is>
@@ -478,10 +478,10 @@
         </is>
       </c>
       <c r="C3" t="n">
-        <v>5726</v>
+        <v>5727</v>
       </c>
       <c r="D3" t="n">
-        <v>8411486</v>
+        <v>8412986</v>
       </c>
       <c r="E3" t="inlineStr">
         <is>
@@ -622,10 +622,10 @@
         </is>
       </c>
       <c r="C6" t="n">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="D6" t="n">
-        <v>156444</v>
+        <v>157409</v>
       </c>
       <c r="E6" t="inlineStr">
         <is>
@@ -766,10 +766,10 @@
         </is>
       </c>
       <c r="C9" t="n">
-        <v>1192</v>
+        <v>1194</v>
       </c>
       <c r="D9" t="n">
-        <v>1721988</v>
+        <v>1724988</v>
       </c>
       <c r="E9" t="inlineStr">
         <is>
@@ -1006,10 +1006,10 @@
         </is>
       </c>
       <c r="C14" t="n">
-        <v>1948</v>
+        <v>1952</v>
       </c>
       <c r="D14" t="n">
-        <v>2567667</v>
+        <v>2572869</v>
       </c>
       <c r="E14" t="inlineStr">
         <is>
@@ -1054,10 +1054,10 @@
         </is>
       </c>
       <c r="C15" t="n">
-        <v>2555</v>
+        <v>2556</v>
       </c>
       <c r="D15" t="n">
-        <v>3692373</v>
+        <v>3693873</v>
       </c>
       <c r="E15" t="inlineStr">
         <is>
@@ -1102,10 +1102,10 @@
         </is>
       </c>
       <c r="C16" t="n">
-        <v>4208</v>
+        <v>4211</v>
       </c>
       <c r="D16" t="n">
-        <v>6141995</v>
+        <v>6146495</v>
       </c>
       <c r="E16" t="inlineStr">
         <is>
@@ -1150,10 +1150,10 @@
         </is>
       </c>
       <c r="C17" t="n">
-        <v>1154</v>
+        <v>1155</v>
       </c>
       <c r="D17" t="n">
-        <v>1713327</v>
+        <v>1714827</v>
       </c>
       <c r="E17" t="inlineStr">
         <is>
@@ -1342,10 +1342,10 @@
         </is>
       </c>
       <c r="C21" t="n">
-        <v>1786</v>
+        <v>1787</v>
       </c>
       <c r="D21" t="n">
-        <v>2370079</v>
+        <v>2371579</v>
       </c>
       <c r="E21" t="inlineStr">
         <is>
@@ -1438,10 +1438,10 @@
         </is>
       </c>
       <c r="C23" t="n">
-        <v>1932</v>
+        <v>1934</v>
       </c>
       <c r="D23" t="n">
-        <v>2801930</v>
+        <v>2803790</v>
       </c>
       <c r="E23" t="inlineStr">
         <is>
@@ -1678,10 +1678,10 @@
         </is>
       </c>
       <c r="C28" t="n">
-        <v>2152</v>
+        <v>2161</v>
       </c>
       <c r="D28" t="n">
-        <v>2994783</v>
+        <v>3007409</v>
       </c>
       <c r="E28" t="inlineStr">
         <is>
@@ -1726,10 +1726,10 @@
         </is>
       </c>
       <c r="C29" t="n">
-        <v>3187</v>
+        <v>3189</v>
       </c>
       <c r="D29" t="n">
-        <v>4609185</v>
+        <v>4610514</v>
       </c>
       <c r="E29" t="inlineStr">
         <is>
@@ -1774,10 +1774,10 @@
         </is>
       </c>
       <c r="C30" t="n">
-        <v>6428</v>
+        <v>6430</v>
       </c>
       <c r="D30" t="n">
-        <v>9406358</v>
+        <v>9409358</v>
       </c>
       <c r="E30" t="inlineStr">
         <is>
@@ -1822,10 +1822,10 @@
         </is>
       </c>
       <c r="C31" t="n">
-        <v>1988</v>
+        <v>1989</v>
       </c>
       <c r="D31" t="n">
-        <v>2945383</v>
+        <v>2946883</v>
       </c>
       <c r="E31" t="inlineStr">
         <is>
@@ -2014,10 +2014,10 @@
         </is>
       </c>
       <c r="C35" t="n">
-        <v>2510</v>
+        <v>2511</v>
       </c>
       <c r="D35" t="n">
-        <v>3214290</v>
+        <v>3215790</v>
       </c>
       <c r="E35" t="inlineStr">
         <is>
@@ -2446,10 +2446,10 @@
         </is>
       </c>
       <c r="C44" t="n">
-        <v>8949</v>
+        <v>8951</v>
       </c>
       <c r="D44" t="n">
-        <v>13116663</v>
+        <v>13119663</v>
       </c>
       <c r="E44" t="inlineStr">
         <is>
@@ -2542,10 +2542,10 @@
         </is>
       </c>
       <c r="C46" t="n">
-        <v>1137</v>
+        <v>1138</v>
       </c>
       <c r="D46" t="n">
-        <v>1696285</v>
+        <v>1697785</v>
       </c>
       <c r="E46" t="inlineStr">
         <is>
@@ -2686,10 +2686,10 @@
         </is>
       </c>
       <c r="C49" t="n">
-        <v>4998</v>
+        <v>5000</v>
       </c>
       <c r="D49" t="n">
-        <v>6838820</v>
+        <v>6841820</v>
       </c>
       <c r="E49" t="inlineStr">
         <is>
@@ -2734,10 +2734,10 @@
         </is>
       </c>
       <c r="C50" t="n">
-        <v>5836</v>
+        <v>5843</v>
       </c>
       <c r="D50" t="n">
-        <v>8446610</v>
+        <v>8457110</v>
       </c>
       <c r="E50" t="inlineStr">
         <is>
@@ -2782,10 +2782,10 @@
         </is>
       </c>
       <c r="C51" t="n">
-        <v>13628</v>
+        <v>13635</v>
       </c>
       <c r="D51" t="n">
-        <v>20037749</v>
+        <v>20047843</v>
       </c>
       <c r="E51" t="inlineStr">
         <is>
@@ -2830,10 +2830,10 @@
         </is>
       </c>
       <c r="C52" t="n">
-        <v>4622</v>
+        <v>4625</v>
       </c>
       <c r="D52" t="n">
-        <v>6844750</v>
+        <v>6849250</v>
       </c>
       <c r="E52" t="inlineStr">
         <is>
@@ -2878,10 +2878,10 @@
         </is>
       </c>
       <c r="C53" t="n">
-        <v>1249</v>
+        <v>1252</v>
       </c>
       <c r="D53" t="n">
-        <v>1855497</v>
+        <v>1859997</v>
       </c>
       <c r="E53" t="inlineStr">
         <is>
@@ -3070,10 +3070,10 @@
         </is>
       </c>
       <c r="C57" t="n">
-        <v>5624</v>
+        <v>5628</v>
       </c>
       <c r="D57" t="n">
-        <v>7702199</v>
+        <v>7706697</v>
       </c>
       <c r="E57" t="inlineStr">
         <is>
@@ -3118,10 +3118,10 @@
         </is>
       </c>
       <c r="C58" t="n">
-        <v>3172</v>
+        <v>3173</v>
       </c>
       <c r="D58" t="n">
-        <v>4578739</v>
+        <v>4580239</v>
       </c>
       <c r="E58" t="inlineStr">
         <is>
@@ -3166,10 +3166,10 @@
         </is>
       </c>
       <c r="C59" t="n">
-        <v>7832</v>
+        <v>7834</v>
       </c>
       <c r="D59" t="n">
-        <v>11480705</v>
+        <v>11483705</v>
       </c>
       <c r="E59" t="inlineStr">
         <is>
@@ -3214,10 +3214,10 @@
         </is>
       </c>
       <c r="C60" t="n">
-        <v>2491</v>
+        <v>2492</v>
       </c>
       <c r="D60" t="n">
-        <v>3671532</v>
+        <v>3673032</v>
       </c>
       <c r="E60" t="inlineStr">
         <is>
@@ -3262,10 +3262,10 @@
         </is>
       </c>
       <c r="C61" t="n">
-        <v>635</v>
+        <v>636</v>
       </c>
       <c r="D61" t="n">
-        <v>940087</v>
+        <v>941587</v>
       </c>
       <c r="E61" t="inlineStr">
         <is>
@@ -3406,10 +3406,10 @@
         </is>
       </c>
       <c r="C64" t="n">
-        <v>3383</v>
+        <v>3384</v>
       </c>
       <c r="D64" t="n">
-        <v>4410514</v>
+        <v>4412014</v>
       </c>
       <c r="E64" t="inlineStr">
         <is>
@@ -3454,10 +3454,10 @@
         </is>
       </c>
       <c r="C65" t="n">
-        <v>2688</v>
+        <v>2690</v>
       </c>
       <c r="D65" t="n">
-        <v>3862237</v>
+        <v>3865237</v>
       </c>
       <c r="E65" t="inlineStr">
         <is>
@@ -3502,10 +3502,10 @@
         </is>
       </c>
       <c r="C66" t="n">
-        <v>7028</v>
+        <v>7031</v>
       </c>
       <c r="D66" t="n">
-        <v>10281810</v>
+        <v>10286310</v>
       </c>
       <c r="E66" t="inlineStr">
         <is>
@@ -3742,10 +3742,10 @@
         </is>
       </c>
       <c r="C71" t="n">
-        <v>3007</v>
+        <v>3009</v>
       </c>
       <c r="D71" t="n">
-        <v>3971701</v>
+        <v>3973723</v>
       </c>
       <c r="E71" t="inlineStr">
         <is>
@@ -3790,10 +3790,10 @@
         </is>
       </c>
       <c r="C72" t="n">
-        <v>9157</v>
+        <v>9169</v>
       </c>
       <c r="D72" t="n">
-        <v>13280220</v>
+        <v>13298056</v>
       </c>
       <c r="E72" t="inlineStr">
         <is>
@@ -3838,10 +3838,10 @@
         </is>
       </c>
       <c r="C73" t="n">
-        <v>22483</v>
+        <v>22497</v>
       </c>
       <c r="D73" t="n">
-        <v>33030016</v>
+        <v>33049583</v>
       </c>
       <c r="E73" t="inlineStr">
         <is>
@@ -3886,10 +3886,10 @@
         </is>
       </c>
       <c r="C74" t="n">
-        <v>7744</v>
+        <v>7747</v>
       </c>
       <c r="D74" t="n">
-        <v>11495901</v>
+        <v>11500401</v>
       </c>
       <c r="E74" t="inlineStr">
         <is>
@@ -3934,10 +3934,10 @@
         </is>
       </c>
       <c r="C75" t="n">
-        <v>2172</v>
+        <v>2175</v>
       </c>
       <c r="D75" t="n">
-        <v>3232872</v>
+        <v>3237372</v>
       </c>
       <c r="E75" t="inlineStr">
         <is>
@@ -4222,10 +4222,10 @@
         </is>
       </c>
       <c r="C81" t="n">
-        <v>7465</v>
+        <v>7470</v>
       </c>
       <c r="D81" t="n">
-        <v>10264324</v>
+        <v>10269815</v>
       </c>
       <c r="E81" t="inlineStr">
         <is>
@@ -4270,10 +4270,10 @@
         </is>
       </c>
       <c r="C82" t="n">
-        <v>2763</v>
+        <v>2766</v>
       </c>
       <c r="D82" t="n">
-        <v>4006357</v>
+        <v>4010857</v>
       </c>
       <c r="E82" t="inlineStr">
         <is>
@@ -4318,10 +4318,10 @@
         </is>
       </c>
       <c r="C83" t="n">
-        <v>6439</v>
+        <v>6441</v>
       </c>
       <c r="D83" t="n">
-        <v>9424239</v>
+        <v>9427239</v>
       </c>
       <c r="E83" t="inlineStr">
         <is>
@@ -4366,10 +4366,10 @@
         </is>
       </c>
       <c r="C84" t="n">
-        <v>2873</v>
+        <v>2874</v>
       </c>
       <c r="D84" t="n">
-        <v>4257644</v>
+        <v>4259144</v>
       </c>
       <c r="E84" t="inlineStr">
         <is>
@@ -4462,10 +4462,10 @@
         </is>
       </c>
       <c r="C86" t="n">
-        <v>310</v>
+        <v>312</v>
       </c>
       <c r="D86" t="n">
-        <v>460775</v>
+        <v>463775</v>
       </c>
       <c r="E86" t="inlineStr">
         <is>
@@ -4558,10 +4558,10 @@
         </is>
       </c>
       <c r="C88" t="n">
-        <v>6461</v>
+        <v>6462</v>
       </c>
       <c r="D88" t="n">
-        <v>9069498</v>
+        <v>9070998</v>
       </c>
       <c r="E88" t="inlineStr">
         <is>
@@ -4606,10 +4606,10 @@
         </is>
       </c>
       <c r="C89" t="n">
-        <v>1924</v>
+        <v>1927</v>
       </c>
       <c r="D89" t="n">
-        <v>2795960</v>
+        <v>2800445</v>
       </c>
       <c r="E89" t="inlineStr">
         <is>
@@ -4654,10 +4654,10 @@
         </is>
       </c>
       <c r="C90" t="n">
-        <v>4921</v>
+        <v>4923</v>
       </c>
       <c r="D90" t="n">
-        <v>7226534</v>
+        <v>7228709</v>
       </c>
       <c r="E90" t="inlineStr">
         <is>
@@ -4942,10 +4942,10 @@
         </is>
       </c>
       <c r="C96" t="n">
-        <v>1704</v>
+        <v>1705</v>
       </c>
       <c r="D96" t="n">
-        <v>2463284</v>
+        <v>2464784</v>
       </c>
       <c r="E96" t="inlineStr">
         <is>
@@ -4990,10 +4990,10 @@
         </is>
       </c>
       <c r="C97" t="n">
-        <v>4545</v>
+        <v>4548</v>
       </c>
       <c r="D97" t="n">
-        <v>6669046</v>
+        <v>6673139</v>
       </c>
       <c r="E97" t="inlineStr">
         <is>
@@ -5278,10 +5278,10 @@
         </is>
       </c>
       <c r="C103" t="n">
-        <v>1547</v>
+        <v>1549</v>
       </c>
       <c r="D103" t="n">
-        <v>2088805</v>
+        <v>2090801</v>
       </c>
       <c r="E103" t="inlineStr">
         <is>
@@ -5614,10 +5614,10 @@
         </is>
       </c>
       <c r="C110" t="n">
-        <v>1110</v>
+        <v>1112</v>
       </c>
       <c r="D110" t="n">
-        <v>1606975</v>
+        <v>1609975</v>
       </c>
       <c r="E110" t="inlineStr">
         <is>
@@ -6238,10 +6238,10 @@
         </is>
       </c>
       <c r="C123" t="n">
-        <v>1966</v>
+        <v>1968</v>
       </c>
       <c r="D123" t="n">
-        <v>2842213</v>
+        <v>2845213</v>
       </c>
       <c r="E123" t="inlineStr">
         <is>
@@ -6334,10 +6334,10 @@
         </is>
       </c>
       <c r="C125" t="n">
-        <v>1735</v>
+        <v>1736</v>
       </c>
       <c r="D125" t="n">
-        <v>2584519</v>
+        <v>2586019</v>
       </c>
       <c r="E125" t="inlineStr">
         <is>
@@ -6478,10 +6478,10 @@
         </is>
       </c>
       <c r="C128" t="n">
-        <v>2465</v>
+        <v>2467</v>
       </c>
       <c r="D128" t="n">
-        <v>3319362</v>
+        <v>3321087</v>
       </c>
       <c r="E128" t="inlineStr">
         <is>
@@ -6574,10 +6574,10 @@
         </is>
       </c>
       <c r="C130" t="n">
-        <v>1126</v>
+        <v>1128</v>
       </c>
       <c r="D130" t="n">
-        <v>1649390</v>
+        <v>1652390</v>
       </c>
       <c r="E130" t="inlineStr">
         <is>
@@ -6766,10 +6766,10 @@
         </is>
       </c>
       <c r="C134" t="n">
-        <v>349</v>
+        <v>350</v>
       </c>
       <c r="D134" t="n">
-        <v>458704</v>
+        <v>460204</v>
       </c>
       <c r="E134" t="inlineStr">
         <is>
@@ -7006,10 +7006,10 @@
         </is>
       </c>
       <c r="C139" t="n">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="D139" t="n">
-        <v>45180</v>
+        <v>46680</v>
       </c>
       <c r="E139" t="inlineStr">
         <is>
@@ -7102,10 +7102,10 @@
         </is>
       </c>
       <c r="C141" t="n">
-        <v>1138</v>
+        <v>1139</v>
       </c>
       <c r="D141" t="n">
-        <v>1492041</v>
+        <v>1492903</v>
       </c>
       <c r="E141" t="inlineStr">
         <is>
@@ -7150,10 +7150,10 @@
         </is>
       </c>
       <c r="C142" t="n">
-        <v>2647</v>
+        <v>2649</v>
       </c>
       <c r="D142" t="n">
-        <v>3826741</v>
+        <v>3829741</v>
       </c>
       <c r="E142" t="inlineStr">
         <is>
@@ -7198,10 +7198,10 @@
         </is>
       </c>
       <c r="C143" t="n">
-        <v>6089</v>
+        <v>6091</v>
       </c>
       <c r="D143" t="n">
-        <v>8913451</v>
+        <v>8916451</v>
       </c>
       <c r="E143" t="inlineStr">
         <is>
@@ -7246,10 +7246,10 @@
         </is>
       </c>
       <c r="C144" t="n">
-        <v>1677</v>
+        <v>1678</v>
       </c>
       <c r="D144" t="n">
-        <v>2492755</v>
+        <v>2493568</v>
       </c>
       <c r="E144" t="inlineStr">
         <is>
@@ -7438,10 +7438,10 @@
         </is>
       </c>
       <c r="C148" t="n">
-        <v>2399</v>
+        <v>2400</v>
       </c>
       <c r="D148" t="n">
-        <v>3147191</v>
+        <v>3147791</v>
       </c>
       <c r="E148" t="inlineStr">
         <is>
@@ -7486,10 +7486,10 @@
         </is>
       </c>
       <c r="C149" t="n">
-        <v>3611</v>
+        <v>3612</v>
       </c>
       <c r="D149" t="n">
-        <v>5203913</v>
+        <v>5205413</v>
       </c>
       <c r="E149" t="inlineStr">
         <is>
@@ -7534,10 +7534,10 @@
         </is>
       </c>
       <c r="C150" t="n">
-        <v>8232</v>
+        <v>8233</v>
       </c>
       <c r="D150" t="n">
-        <v>12046135</v>
+        <v>12047210</v>
       </c>
       <c r="E150" t="inlineStr">
         <is>
@@ -7774,10 +7774,10 @@
         </is>
       </c>
       <c r="C155" t="n">
-        <v>3133</v>
+        <v>3134</v>
       </c>
       <c r="D155" t="n">
-        <v>4182602</v>
+        <v>4183714</v>
       </c>
       <c r="E155" t="inlineStr">
         <is>
@@ -7822,10 +7822,10 @@
         </is>
       </c>
       <c r="C156" t="n">
-        <v>3393</v>
+        <v>3397</v>
       </c>
       <c r="D156" t="n">
-        <v>4919082</v>
+        <v>4924227</v>
       </c>
       <c r="E156" t="inlineStr">
         <is>
@@ -7918,10 +7918,10 @@
         </is>
       </c>
       <c r="C158" t="n">
-        <v>3110</v>
+        <v>3112</v>
       </c>
       <c r="D158" t="n">
-        <v>4629622</v>
+        <v>4632622</v>
       </c>
       <c r="E158" t="inlineStr">
         <is>
@@ -8110,10 +8110,10 @@
         </is>
       </c>
       <c r="C162" t="n">
-        <v>3164</v>
+        <v>3167</v>
       </c>
       <c r="D162" t="n">
-        <v>4263721</v>
+        <v>4267715</v>
       </c>
       <c r="E162" t="inlineStr">
         <is>
@@ -8158,10 +8158,10 @@
         </is>
       </c>
       <c r="C163" t="n">
-        <v>3728</v>
+        <v>3730</v>
       </c>
       <c r="D163" t="n">
-        <v>5368756</v>
+        <v>5371756</v>
       </c>
       <c r="E163" t="inlineStr">
         <is>
@@ -8206,10 +8206,10 @@
         </is>
       </c>
       <c r="C164" t="n">
-        <v>7892</v>
+        <v>7893</v>
       </c>
       <c r="D164" t="n">
-        <v>11569176</v>
+        <v>11570676</v>
       </c>
       <c r="E164" t="inlineStr">
         <is>
@@ -8254,10 +8254,10 @@
         </is>
       </c>
       <c r="C165" t="n">
-        <v>2555</v>
+        <v>2556</v>
       </c>
       <c r="D165" t="n">
-        <v>3799225</v>
+        <v>3800725</v>
       </c>
       <c r="E165" t="inlineStr">
         <is>
@@ -8446,10 +8446,10 @@
         </is>
       </c>
       <c r="C169" t="n">
-        <v>2990</v>
+        <v>2992</v>
       </c>
       <c r="D169" t="n">
-        <v>4016039</v>
+        <v>4019039</v>
       </c>
       <c r="E169" t="inlineStr">
         <is>
@@ -8782,10 +8782,10 @@
         </is>
       </c>
       <c r="C176" t="n">
-        <v>1196</v>
+        <v>1197</v>
       </c>
       <c r="D176" t="n">
-        <v>1551091</v>
+        <v>1552591</v>
       </c>
       <c r="E176" t="inlineStr">
         <is>
@@ -8878,10 +8878,10 @@
         </is>
       </c>
       <c r="C178" t="n">
-        <v>3501</v>
+        <v>3502</v>
       </c>
       <c r="D178" t="n">
-        <v>5161215</v>
+        <v>5162715</v>
       </c>
       <c r="E178" t="inlineStr">
         <is>
@@ -8974,10 +8974,10 @@
         </is>
       </c>
       <c r="C180" t="n">
-        <v>299</v>
+        <v>300</v>
       </c>
       <c r="D180" t="n">
-        <v>445376</v>
+        <v>446876</v>
       </c>
       <c r="E180" t="inlineStr">
         <is>
@@ -9406,10 +9406,10 @@
         </is>
       </c>
       <c r="C189" t="n">
-        <v>848</v>
+        <v>849</v>
       </c>
       <c r="D189" t="n">
-        <v>1076670</v>
+        <v>1078170</v>
       </c>
       <c r="E189" t="inlineStr">
         <is>
@@ -9502,10 +9502,10 @@
         </is>
       </c>
       <c r="C191" t="n">
-        <v>5745</v>
+        <v>5747</v>
       </c>
       <c r="D191" t="n">
-        <v>8415319</v>
+        <v>8418319</v>
       </c>
       <c r="E191" t="inlineStr">
         <is>
@@ -9790,10 +9790,10 @@
         </is>
       </c>
       <c r="C197" t="n">
-        <v>1870</v>
+        <v>1871</v>
       </c>
       <c r="D197" t="n">
-        <v>2723721</v>
+        <v>2725221</v>
       </c>
       <c r="E197" t="inlineStr">
         <is>
@@ -9838,10 +9838,10 @@
         </is>
       </c>
       <c r="C198" t="n">
-        <v>5637</v>
+        <v>5640</v>
       </c>
       <c r="D198" t="n">
-        <v>8292989</v>
+        <v>8296979</v>
       </c>
       <c r="E198" t="inlineStr">
         <is>
@@ -10414,10 +10414,10 @@
         </is>
       </c>
       <c r="C210" t="n">
-        <v>1112</v>
+        <v>1113</v>
       </c>
       <c r="D210" t="n">
-        <v>1496344</v>
+        <v>1496789</v>
       </c>
       <c r="E210" t="inlineStr">
         <is>
@@ -10510,10 +10510,10 @@
         </is>
       </c>
       <c r="C212" t="n">
-        <v>3719</v>
+        <v>3723</v>
       </c>
       <c r="D212" t="n">
-        <v>5432219</v>
+        <v>5438219</v>
       </c>
       <c r="E212" t="inlineStr">
         <is>
@@ -10750,10 +10750,10 @@
         </is>
       </c>
       <c r="C217" t="n">
-        <v>2286</v>
+        <v>2288</v>
       </c>
       <c r="D217" t="n">
-        <v>3308708</v>
+        <v>3311708</v>
       </c>
       <c r="E217" t="inlineStr">
         <is>
@@ -10798,10 +10798,10 @@
         </is>
       </c>
       <c r="C218" t="n">
-        <v>4109</v>
+        <v>4113</v>
       </c>
       <c r="D218" t="n">
-        <v>5999715</v>
+        <v>6005715</v>
       </c>
       <c r="E218" t="inlineStr">
         <is>
@@ -10990,10 +10990,10 @@
         </is>
       </c>
       <c r="C222" t="n">
-        <v>1692</v>
+        <v>1693</v>
       </c>
       <c r="D222" t="n">
-        <v>2301026</v>
+        <v>2302526</v>
       </c>
       <c r="E222" t="inlineStr">
         <is>
@@ -11086,10 +11086,10 @@
         </is>
       </c>
       <c r="C224" t="n">
-        <v>2286</v>
+        <v>2287</v>
       </c>
       <c r="D224" t="n">
-        <v>3325121</v>
+        <v>3326621</v>
       </c>
       <c r="E224" t="inlineStr">
         <is>
@@ -11278,10 +11278,10 @@
         </is>
       </c>
       <c r="C228" t="n">
-        <v>945</v>
+        <v>947</v>
       </c>
       <c r="D228" t="n">
-        <v>1217370</v>
+        <v>1219905</v>
       </c>
       <c r="E228" t="inlineStr">
         <is>
@@ -11326,10 +11326,10 @@
         </is>
       </c>
       <c r="C229" t="n">
-        <v>941</v>
+        <v>943</v>
       </c>
       <c r="D229" t="n">
-        <v>1359318</v>
+        <v>1362318</v>
       </c>
       <c r="E229" t="inlineStr">
         <is>
@@ -11614,10 +11614,10 @@
         </is>
       </c>
       <c r="C235" t="n">
-        <v>3970</v>
+        <v>3975</v>
       </c>
       <c r="D235" t="n">
-        <v>5743730</v>
+        <v>5751230</v>
       </c>
       <c r="E235" t="inlineStr">
         <is>
@@ -11662,10 +11662,10 @@
         </is>
       </c>
       <c r="C236" t="n">
-        <v>12419</v>
+        <v>12430</v>
       </c>
       <c r="D236" t="n">
-        <v>18216772</v>
+        <v>18232320</v>
       </c>
       <c r="E236" t="inlineStr">
         <is>
@@ -11710,10 +11710,10 @@
         </is>
       </c>
       <c r="C237" t="n">
-        <v>4807</v>
+        <v>4808</v>
       </c>
       <c r="D237" t="n">
-        <v>7133375</v>
+        <v>7134875</v>
       </c>
       <c r="E237" t="inlineStr">
         <is>
@@ -11758,10 +11758,10 @@
         </is>
       </c>
       <c r="C238" t="n">
-        <v>1487</v>
+        <v>1488</v>
       </c>
       <c r="D238" t="n">
-        <v>2207818</v>
+        <v>2209318</v>
       </c>
       <c r="E238" t="inlineStr">
         <is>
@@ -11902,10 +11902,10 @@
         </is>
       </c>
       <c r="C241" t="n">
-        <v>3437</v>
+        <v>3438</v>
       </c>
       <c r="D241" t="n">
-        <v>4658218</v>
+        <v>4658722</v>
       </c>
       <c r="E241" t="inlineStr">
         <is>
@@ -11998,10 +11998,10 @@
         </is>
       </c>
       <c r="C243" t="n">
-        <v>1378</v>
+        <v>1379</v>
       </c>
       <c r="D243" t="n">
-        <v>2007196</v>
+        <v>2008696</v>
       </c>
       <c r="E243" t="inlineStr">
         <is>
@@ -12094,10 +12094,10 @@
         </is>
       </c>
       <c r="C245" t="n">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="D245" t="n">
-        <v>209528</v>
+        <v>211028</v>
       </c>
       <c r="E245" t="inlineStr">
         <is>
@@ -12286,10 +12286,10 @@
         </is>
       </c>
       <c r="C249" t="n">
-        <v>2688</v>
+        <v>2691</v>
       </c>
       <c r="D249" t="n">
-        <v>3885626</v>
+        <v>3890126</v>
       </c>
       <c r="E249" t="inlineStr">
         <is>
@@ -12334,10 +12334,10 @@
         </is>
       </c>
       <c r="C250" t="n">
-        <v>7920</v>
+        <v>7929</v>
       </c>
       <c r="D250" t="n">
-        <v>11620340</v>
+        <v>11633171</v>
       </c>
       <c r="E250" t="inlineStr">
         <is>
@@ -12382,10 +12382,10 @@
         </is>
       </c>
       <c r="C251" t="n">
-        <v>3213</v>
+        <v>3218</v>
       </c>
       <c r="D251" t="n">
-        <v>4772482</v>
+        <v>4779982</v>
       </c>
       <c r="E251" t="inlineStr">
         <is>
@@ -12430,10 +12430,10 @@
         </is>
       </c>
       <c r="C252" t="n">
-        <v>874</v>
+        <v>875</v>
       </c>
       <c r="D252" t="n">
-        <v>1304392</v>
+        <v>1305892</v>
       </c>
       <c r="E252" t="inlineStr">
         <is>
@@ -12766,10 +12766,10 @@
         </is>
       </c>
       <c r="C259" t="n">
-        <v>4951</v>
+        <v>4952</v>
       </c>
       <c r="D259" t="n">
-        <v>7288119</v>
+        <v>7289619</v>
       </c>
       <c r="E259" t="inlineStr">
         <is>
@@ -12862,10 +12862,10 @@
         </is>
       </c>
       <c r="C261" t="n">
-        <v>541</v>
+        <v>542</v>
       </c>
       <c r="D261" t="n">
-        <v>805039</v>
+        <v>806539</v>
       </c>
       <c r="E261" t="inlineStr">
         <is>
@@ -13006,10 +13006,10 @@
         </is>
       </c>
       <c r="C264" t="n">
-        <v>1935</v>
+        <v>1936</v>
       </c>
       <c r="D264" t="n">
-        <v>2536183</v>
+        <v>2536453</v>
       </c>
       <c r="E264" t="inlineStr">
         <is>
@@ -13054,10 +13054,10 @@
         </is>
       </c>
       <c r="C265" t="n">
-        <v>1852</v>
+        <v>1853</v>
       </c>
       <c r="D265" t="n">
-        <v>2705365</v>
+        <v>2706865</v>
       </c>
       <c r="E265" t="inlineStr">
         <is>
@@ -13102,10 +13102,10 @@
         </is>
       </c>
       <c r="C266" t="n">
-        <v>5552</v>
+        <v>5553</v>
       </c>
       <c r="D266" t="n">
-        <v>8161344</v>
+        <v>8162844</v>
       </c>
       <c r="E266" t="inlineStr">
         <is>
@@ -13150,10 +13150,10 @@
         </is>
       </c>
       <c r="C267" t="n">
-        <v>1927</v>
+        <v>1928</v>
       </c>
       <c r="D267" t="n">
-        <v>2860392</v>
+        <v>2861892</v>
       </c>
       <c r="E267" t="inlineStr">
         <is>
@@ -13342,10 +13342,10 @@
         </is>
       </c>
       <c r="C271" t="n">
-        <v>2178</v>
+        <v>2179</v>
       </c>
       <c r="D271" t="n">
-        <v>2931186</v>
+        <v>2931436</v>
       </c>
       <c r="E271" t="inlineStr">
         <is>
@@ -13678,10 +13678,10 @@
         </is>
       </c>
       <c r="C278" t="n">
-        <v>2641</v>
+        <v>2642</v>
       </c>
       <c r="D278" t="n">
-        <v>3824200</v>
+        <v>3825700</v>
       </c>
       <c r="E278" t="inlineStr">
         <is>
@@ -13726,10 +13726,10 @@
         </is>
       </c>
       <c r="C279" t="n">
-        <v>8584</v>
+        <v>8586</v>
       </c>
       <c r="D279" t="n">
-        <v>12581868</v>
+        <v>12584868</v>
       </c>
       <c r="E279" t="inlineStr">
         <is>
@@ -13774,10 +13774,10 @@
         </is>
       </c>
       <c r="C280" t="n">
-        <v>3547</v>
+        <v>3548</v>
       </c>
       <c r="D280" t="n">
-        <v>5275258</v>
+        <v>5276758</v>
       </c>
       <c r="E280" t="inlineStr">
         <is>
@@ -13822,10 +13822,10 @@
         </is>
       </c>
       <c r="C281" t="n">
-        <v>1107</v>
+        <v>1108</v>
       </c>
       <c r="D281" t="n">
-        <v>1656862</v>
+        <v>1658362</v>
       </c>
       <c r="E281" t="inlineStr">
         <is>
@@ -13966,10 +13966,10 @@
         </is>
       </c>
       <c r="C284" t="n">
-        <v>2416</v>
+        <v>2417</v>
       </c>
       <c r="D284" t="n">
-        <v>3223847</v>
+        <v>3223967</v>
       </c>
       <c r="E284" t="inlineStr">
         <is>
@@ -14014,10 +14014,10 @@
         </is>
       </c>
       <c r="C285" t="n">
-        <v>1597</v>
+        <v>1598</v>
       </c>
       <c r="D285" t="n">
-        <v>2292495</v>
+        <v>2293995</v>
       </c>
       <c r="E285" t="inlineStr">
         <is>
@@ -14062,10 +14062,10 @@
         </is>
       </c>
       <c r="C286" t="n">
-        <v>3959</v>
+        <v>3961</v>
       </c>
       <c r="D286" t="n">
-        <v>5810805</v>
+        <v>5813805</v>
       </c>
       <c r="E286" t="inlineStr">
         <is>
@@ -14302,10 +14302,10 @@
         </is>
       </c>
       <c r="C291" t="n">
-        <v>1645</v>
+        <v>1646</v>
       </c>
       <c r="D291" t="n">
-        <v>2171129</v>
+        <v>2171509</v>
       </c>
       <c r="E291" t="inlineStr">
         <is>
@@ -14398,10 +14398,10 @@
         </is>
       </c>
       <c r="C293" t="n">
-        <v>6901</v>
+        <v>6906</v>
       </c>
       <c r="D293" t="n">
-        <v>10144579</v>
+        <v>10152079</v>
       </c>
       <c r="E293" t="inlineStr">
         <is>
@@ -14446,10 +14446,10 @@
         </is>
       </c>
       <c r="C294" t="n">
-        <v>2348</v>
+        <v>2350</v>
       </c>
       <c r="D294" t="n">
-        <v>3506918</v>
+        <v>3509918</v>
       </c>
       <c r="E294" t="inlineStr">
         <is>
@@ -14638,10 +14638,10 @@
         </is>
       </c>
       <c r="C298" t="n">
-        <v>6985</v>
+        <v>6993</v>
       </c>
       <c r="D298" t="n">
-        <v>9601687</v>
+        <v>9611817</v>
       </c>
       <c r="E298" t="inlineStr">
         <is>
@@ -14686,10 +14686,10 @@
         </is>
       </c>
       <c r="C299" t="n">
-        <v>946</v>
+        <v>951</v>
       </c>
       <c r="D299" t="n">
-        <v>1388579</v>
+        <v>1396079</v>
       </c>
       <c r="E299" t="inlineStr">
         <is>
@@ -14734,10 +14734,10 @@
         </is>
       </c>
       <c r="C300" t="n">
-        <v>2381</v>
+        <v>2386</v>
       </c>
       <c r="D300" t="n">
-        <v>3530337</v>
+        <v>3537837</v>
       </c>
       <c r="E300" t="inlineStr">
         <is>
@@ -14782,10 +14782,10 @@
         </is>
       </c>
       <c r="C301" t="n">
-        <v>945</v>
+        <v>948</v>
       </c>
       <c r="D301" t="n">
-        <v>1407001</v>
+        <v>1411501</v>
       </c>
       <c r="E301" t="inlineStr">
         <is>
@@ -14830,10 +14830,10 @@
         </is>
       </c>
       <c r="C302" t="n">
-        <v>322</v>
+        <v>323</v>
       </c>
       <c r="D302" t="n">
-        <v>482758</v>
+        <v>484258</v>
       </c>
       <c r="E302" t="inlineStr">
         <is>
@@ -14926,10 +14926,10 @@
         </is>
       </c>
       <c r="C304" t="n">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D304" t="n">
-        <v>25500</v>
+        <v>27000</v>
       </c>
       <c r="E304" t="inlineStr">
         <is>
@@ -14974,10 +14974,10 @@
         </is>
       </c>
       <c r="C305" t="n">
-        <v>1393</v>
+        <v>1400</v>
       </c>
       <c r="D305" t="n">
-        <v>1960706</v>
+        <v>1970306</v>
       </c>
       <c r="E305" t="inlineStr">
         <is>
@@ -15070,10 +15070,10 @@
         </is>
       </c>
       <c r="C307" t="n">
-        <v>3567</v>
+        <v>3569</v>
       </c>
       <c r="D307" t="n">
-        <v>5232523</v>
+        <v>5235523</v>
       </c>
       <c r="E307" t="inlineStr">
         <is>
@@ -15118,10 +15118,10 @@
         </is>
       </c>
       <c r="C308" t="n">
-        <v>1343</v>
+        <v>1345</v>
       </c>
       <c r="D308" t="n">
-        <v>1988253</v>
+        <v>1991253</v>
       </c>
       <c r="E308" t="inlineStr">
         <is>
@@ -15406,10 +15406,10 @@
         </is>
       </c>
       <c r="C314" t="n">
-        <v>6997</v>
+        <v>7003</v>
       </c>
       <c r="D314" t="n">
-        <v>10094951</v>
+        <v>10103951</v>
       </c>
       <c r="E314" t="inlineStr">
         <is>
@@ -15454,10 +15454,10 @@
         </is>
       </c>
       <c r="C315" t="n">
-        <v>19589</v>
+        <v>19597</v>
       </c>
       <c r="D315" t="n">
-        <v>28656684</v>
+        <v>28668056</v>
       </c>
       <c r="E315" t="inlineStr">
         <is>
@@ -15502,10 +15502,10 @@
         </is>
       </c>
       <c r="C316" t="n">
-        <v>6947</v>
+        <v>6949</v>
       </c>
       <c r="D316" t="n">
-        <v>10339162</v>
+        <v>10342077</v>
       </c>
       <c r="E316" t="inlineStr">
         <is>
@@ -15598,10 +15598,10 @@
         </is>
       </c>
       <c r="C318" t="n">
-        <v>454</v>
+        <v>455</v>
       </c>
       <c r="D318" t="n">
-        <v>676042</v>
+        <v>677542</v>
       </c>
       <c r="E318" t="inlineStr">
         <is>
@@ -15742,10 +15742,10 @@
         </is>
       </c>
       <c r="C321" t="n">
-        <v>6210</v>
+        <v>6216</v>
       </c>
       <c r="D321" t="n">
-        <v>8166090</v>
+        <v>8173225</v>
       </c>
       <c r="E321" t="inlineStr">
         <is>
@@ -15790,10 +15790,10 @@
         </is>
       </c>
       <c r="C322" t="n">
-        <v>2092</v>
+        <v>2093</v>
       </c>
       <c r="D322" t="n">
-        <v>3063892</v>
+        <v>3065392</v>
       </c>
       <c r="E322" t="inlineStr">
         <is>
@@ -15838,10 +15838,10 @@
         </is>
       </c>
       <c r="C323" t="n">
-        <v>6500</v>
+        <v>6501</v>
       </c>
       <c r="D323" t="n">
-        <v>9543281</v>
+        <v>9544781</v>
       </c>
       <c r="E323" t="inlineStr">
         <is>
@@ -15886,10 +15886,10 @@
         </is>
       </c>
       <c r="C324" t="n">
-        <v>2289</v>
+        <v>2290</v>
       </c>
       <c r="D324" t="n">
-        <v>3405530</v>
+        <v>3407030</v>
       </c>
       <c r="E324" t="inlineStr">
         <is>
@@ -16078,10 +16078,10 @@
         </is>
       </c>
       <c r="C328" t="n">
-        <v>1981</v>
+        <v>1982</v>
       </c>
       <c r="D328" t="n">
-        <v>2690989</v>
+        <v>2692489</v>
       </c>
       <c r="E328" t="inlineStr">
         <is>
@@ -16126,10 +16126,10 @@
         </is>
       </c>
       <c r="C329" t="n">
-        <v>3584</v>
+        <v>3585</v>
       </c>
       <c r="D329" t="n">
-        <v>5152751</v>
+        <v>5154251</v>
       </c>
       <c r="E329" t="inlineStr">
         <is>
@@ -16174,10 +16174,10 @@
         </is>
       </c>
       <c r="C330" t="n">
-        <v>10782</v>
+        <v>10784</v>
       </c>
       <c r="D330" t="n">
-        <v>15754207</v>
+        <v>15757207</v>
       </c>
       <c r="E330" t="inlineStr">
         <is>
@@ -16270,10 +16270,10 @@
         </is>
       </c>
       <c r="C332" t="n">
-        <v>1091</v>
+        <v>1092</v>
       </c>
       <c r="D332" t="n">
-        <v>1621873</v>
+        <v>1622284</v>
       </c>
       <c r="E332" t="inlineStr">
         <is>
@@ -16462,10 +16462,10 @@
         </is>
       </c>
       <c r="C336" t="n">
-        <v>3795</v>
+        <v>3797</v>
       </c>
       <c r="D336" t="n">
-        <v>4955069</v>
+        <v>4958069</v>
       </c>
       <c r="E336" t="inlineStr">
         <is>
@@ -16510,10 +16510,10 @@
         </is>
       </c>
       <c r="C337" t="n">
-        <v>1514</v>
+        <v>1515</v>
       </c>
       <c r="D337" t="n">
-        <v>2190837</v>
+        <v>2192337</v>
       </c>
       <c r="E337" t="inlineStr">
         <is>
@@ -16558,10 +16558,10 @@
         </is>
       </c>
       <c r="C338" t="n">
-        <v>4235</v>
+        <v>4236</v>
       </c>
       <c r="D338" t="n">
-        <v>6186458</v>
+        <v>6187958</v>
       </c>
       <c r="E338" t="inlineStr">
         <is>
@@ -16846,10 +16846,10 @@
         </is>
       </c>
       <c r="C344" t="n">
-        <v>3613</v>
+        <v>3614</v>
       </c>
       <c r="D344" t="n">
-        <v>5275560</v>
+        <v>5277060</v>
       </c>
       <c r="E344" t="inlineStr">
         <is>
@@ -16894,10 +16894,10 @@
         </is>
       </c>
       <c r="C345" t="n">
-        <v>10402</v>
+        <v>10406</v>
       </c>
       <c r="D345" t="n">
-        <v>15348602</v>
+        <v>15354602</v>
       </c>
       <c r="E345" t="inlineStr">
         <is>
@@ -17278,10 +17278,10 @@
         </is>
       </c>
       <c r="C353" t="n">
-        <v>6459</v>
+        <v>6464</v>
       </c>
       <c r="D353" t="n">
-        <v>9407370</v>
+        <v>9414870</v>
       </c>
       <c r="E353" t="inlineStr">
         <is>
@@ -17326,10 +17326,10 @@
         </is>
       </c>
       <c r="C354" t="n">
-        <v>15631</v>
+        <v>15638</v>
       </c>
       <c r="D354" t="n">
-        <v>23019813</v>
+        <v>23029813</v>
       </c>
       <c r="E354" t="inlineStr">
         <is>
@@ -17374,10 +17374,10 @@
         </is>
       </c>
       <c r="C355" t="n">
-        <v>6936</v>
+        <v>6939</v>
       </c>
       <c r="D355" t="n">
-        <v>10337390</v>
+        <v>10341890</v>
       </c>
       <c r="E355" t="inlineStr">
         <is>
@@ -17422,10 +17422,10 @@
         </is>
       </c>
       <c r="C356" t="n">
-        <v>2114</v>
+        <v>2115</v>
       </c>
       <c r="D356" t="n">
-        <v>3155651</v>
+        <v>3157151</v>
       </c>
       <c r="E356" t="inlineStr">
         <is>
@@ -17566,10 +17566,10 @@
         </is>
       </c>
       <c r="C359" t="n">
-        <v>5731</v>
+        <v>5738</v>
       </c>
       <c r="D359" t="n">
-        <v>7820408</v>
+        <v>7829243</v>
       </c>
       <c r="E359" t="inlineStr">
         <is>
@@ -17614,10 +17614,10 @@
         </is>
       </c>
       <c r="C360" t="n">
-        <v>18869</v>
+        <v>18885</v>
       </c>
       <c r="D360" t="n">
-        <v>27391648</v>
+        <v>27413334</v>
       </c>
       <c r="E360" t="inlineStr">
         <is>
@@ -17662,10 +17662,10 @@
         </is>
       </c>
       <c r="C361" t="n">
-        <v>51711</v>
+        <v>51743</v>
       </c>
       <c r="D361" t="n">
-        <v>76198388</v>
+        <v>76244823</v>
       </c>
       <c r="E361" t="inlineStr">
         <is>
@@ -17710,10 +17710,10 @@
         </is>
       </c>
       <c r="C362" t="n">
-        <v>24160</v>
+        <v>24168</v>
       </c>
       <c r="D362" t="n">
-        <v>36045300</v>
+        <v>36057300</v>
       </c>
       <c r="E362" t="inlineStr">
         <is>
@@ -17758,10 +17758,10 @@
         </is>
       </c>
       <c r="C363" t="n">
-        <v>8692</v>
+        <v>8698</v>
       </c>
       <c r="D363" t="n">
-        <v>12998704</v>
+        <v>13007704</v>
       </c>
       <c r="E363" t="inlineStr">
         <is>
@@ -17806,10 +17806,10 @@
         </is>
       </c>
       <c r="C364" t="n">
-        <v>2215</v>
+        <v>2217</v>
       </c>
       <c r="D364" t="n">
-        <v>3310459</v>
+        <v>3313459</v>
       </c>
       <c r="E364" t="inlineStr">
         <is>
@@ -18046,10 +18046,10 @@
         </is>
       </c>
       <c r="C369" t="n">
-        <v>18562</v>
+        <v>18581</v>
       </c>
       <c r="D369" t="n">
-        <v>25167693</v>
+        <v>25190708</v>
       </c>
       <c r="E369" t="inlineStr">
         <is>
@@ -18094,10 +18094,10 @@
         </is>
       </c>
       <c r="C370" t="n">
-        <v>4336</v>
+        <v>4339</v>
       </c>
       <c r="D370" t="n">
-        <v>6312694</v>
+        <v>6317194</v>
       </c>
       <c r="E370" t="inlineStr">
         <is>
@@ -18142,10 +18142,10 @@
         </is>
       </c>
       <c r="C371" t="n">
-        <v>12348</v>
+        <v>12355</v>
       </c>
       <c r="D371" t="n">
-        <v>18155250</v>
+        <v>18165750</v>
       </c>
       <c r="E371" t="inlineStr">
         <is>
@@ -18190,10 +18190,10 @@
         </is>
       </c>
       <c r="C372" t="n">
-        <v>4664</v>
+        <v>4665</v>
       </c>
       <c r="D372" t="n">
-        <v>6924788</v>
+        <v>6926288</v>
       </c>
       <c r="E372" t="inlineStr">
         <is>
@@ -18238,10 +18238,10 @@
         </is>
       </c>
       <c r="C373" t="n">
-        <v>1432</v>
+        <v>1433</v>
       </c>
       <c r="D373" t="n">
-        <v>2137981</v>
+        <v>2139481</v>
       </c>
       <c r="E373" t="inlineStr">
         <is>
@@ -18382,10 +18382,10 @@
         </is>
       </c>
       <c r="C376" t="n">
-        <v>4356</v>
+        <v>4361</v>
       </c>
       <c r="D376" t="n">
-        <v>5950124</v>
+        <v>5957624</v>
       </c>
       <c r="E376" t="inlineStr">
         <is>
@@ -18430,10 +18430,10 @@
         </is>
       </c>
       <c r="C377" t="n">
-        <v>5425</v>
+        <v>5431</v>
       </c>
       <c r="D377" t="n">
-        <v>7895771</v>
+        <v>7904771</v>
       </c>
       <c r="E377" t="inlineStr">
         <is>
@@ -18478,10 +18478,10 @@
         </is>
       </c>
       <c r="C378" t="n">
-        <v>19207</v>
+        <v>19221</v>
       </c>
       <c r="D378" t="n">
-        <v>28294727</v>
+        <v>28314743</v>
       </c>
       <c r="E378" t="inlineStr">
         <is>
@@ -18526,10 +18526,10 @@
         </is>
       </c>
       <c r="C379" t="n">
-        <v>8954</v>
+        <v>8959</v>
       </c>
       <c r="D379" t="n">
-        <v>13352034</v>
+        <v>13359534</v>
       </c>
       <c r="E379" t="inlineStr">
         <is>
@@ -18622,10 +18622,10 @@
         </is>
       </c>
       <c r="C381" t="n">
-        <v>629</v>
+        <v>630</v>
       </c>
       <c r="D381" t="n">
-        <v>940595</v>
+        <v>942095</v>
       </c>
       <c r="E381" t="inlineStr">
         <is>
@@ -18718,10 +18718,10 @@
         </is>
       </c>
       <c r="C383" t="n">
-        <v>5613</v>
+        <v>5617</v>
       </c>
       <c r="D383" t="n">
-        <v>7566306</v>
+        <v>7572306</v>
       </c>
       <c r="E383" t="inlineStr">
         <is>
@@ -18766,10 +18766,10 @@
         </is>
       </c>
       <c r="C384" t="n">
-        <v>4855</v>
+        <v>4856</v>
       </c>
       <c r="D384" t="n">
-        <v>7076666</v>
+        <v>7078166</v>
       </c>
       <c r="E384" t="inlineStr">
         <is>
@@ -18814,10 +18814,10 @@
         </is>
       </c>
       <c r="C385" t="n">
-        <v>13927</v>
+        <v>13932</v>
       </c>
       <c r="D385" t="n">
-        <v>20501724</v>
+        <v>20509224</v>
       </c>
       <c r="E385" t="inlineStr">
         <is>
@@ -18862,10 +18862,10 @@
         </is>
       </c>
       <c r="C386" t="n">
-        <v>5742</v>
+        <v>5743</v>
       </c>
       <c r="D386" t="n">
-        <v>8552239</v>
+        <v>8553739</v>
       </c>
       <c r="E386" t="inlineStr">
         <is>
@@ -18910,10 +18910,10 @@
         </is>
       </c>
       <c r="C387" t="n">
-        <v>1647</v>
+        <v>1648</v>
       </c>
       <c r="D387" t="n">
-        <v>2457622</v>
+        <v>2459122</v>
       </c>
       <c r="E387" t="inlineStr">
         <is>
@@ -18958,10 +18958,10 @@
         </is>
       </c>
       <c r="C388" t="n">
-        <v>399</v>
+        <v>400</v>
       </c>
       <c r="D388" t="n">
-        <v>595606</v>
+        <v>597106</v>
       </c>
       <c r="E388" t="inlineStr">
         <is>
@@ -19102,10 +19102,10 @@
         </is>
       </c>
       <c r="C391" t="n">
-        <v>5024</v>
+        <v>5028</v>
       </c>
       <c r="D391" t="n">
-        <v>6852145</v>
+        <v>6857410</v>
       </c>
       <c r="E391" t="inlineStr">
         <is>
@@ -19150,10 +19150,10 @@
         </is>
       </c>
       <c r="C392" t="n">
-        <v>3662</v>
+        <v>3663</v>
       </c>
       <c r="D392" t="n">
-        <v>5342700</v>
+        <v>5344200</v>
       </c>
       <c r="E392" t="inlineStr">
         <is>
@@ -19198,10 +19198,10 @@
         </is>
       </c>
       <c r="C393" t="n">
-        <v>11547</v>
+        <v>11551</v>
       </c>
       <c r="D393" t="n">
-        <v>17032584</v>
+        <v>17038584</v>
       </c>
       <c r="E393" t="inlineStr">
         <is>
@@ -19246,10 +19246,10 @@
         </is>
       </c>
       <c r="C394" t="n">
-        <v>4838</v>
+        <v>4839</v>
       </c>
       <c r="D394" t="n">
-        <v>7198559</v>
+        <v>7200059</v>
       </c>
       <c r="E394" t="inlineStr">
         <is>
@@ -19294,10 +19294,10 @@
         </is>
       </c>
       <c r="C395" t="n">
-        <v>1406</v>
+        <v>1407</v>
       </c>
       <c r="D395" t="n">
-        <v>2095422</v>
+        <v>2096922</v>
       </c>
       <c r="E395" t="inlineStr">
         <is>
@@ -19486,10 +19486,10 @@
         </is>
       </c>
       <c r="C399" t="n">
-        <v>3924</v>
+        <v>3926</v>
       </c>
       <c r="D399" t="n">
-        <v>5298876</v>
+        <v>5301876</v>
       </c>
       <c r="E399" t="inlineStr">
         <is>
@@ -19534,10 +19534,10 @@
         </is>
       </c>
       <c r="C400" t="n">
-        <v>4163</v>
+        <v>4165</v>
       </c>
       <c r="D400" t="n">
-        <v>6068083</v>
+        <v>6069883</v>
       </c>
       <c r="E400" t="inlineStr">
         <is>
@@ -19582,10 +19582,10 @@
         </is>
       </c>
       <c r="C401" t="n">
-        <v>11263</v>
+        <v>11267</v>
       </c>
       <c r="D401" t="n">
-        <v>16591995</v>
+        <v>16597995</v>
       </c>
       <c r="E401" t="inlineStr">
         <is>
@@ -19630,10 +19630,10 @@
         </is>
       </c>
       <c r="C402" t="n">
-        <v>4332</v>
+        <v>4333</v>
       </c>
       <c r="D402" t="n">
-        <v>6445892</v>
+        <v>6447392</v>
       </c>
       <c r="E402" t="inlineStr">
         <is>
@@ -19678,10 +19678,10 @@
         </is>
       </c>
       <c r="C403" t="n">
-        <v>1362</v>
+        <v>1363</v>
       </c>
       <c r="D403" t="n">
-        <v>2035820</v>
+        <v>2037320</v>
       </c>
       <c r="E403" t="inlineStr">
         <is>
@@ -19870,10 +19870,10 @@
         </is>
       </c>
       <c r="C407" t="n">
-        <v>4602</v>
+        <v>4606</v>
       </c>
       <c r="D407" t="n">
-        <v>6667513</v>
+        <v>6673050</v>
       </c>
       <c r="E407" t="inlineStr">
         <is>
@@ -19918,10 +19918,10 @@
         </is>
       </c>
       <c r="C408" t="n">
-        <v>11563</v>
+        <v>11569</v>
       </c>
       <c r="D408" t="n">
-        <v>16987319</v>
+        <v>16996319</v>
       </c>
       <c r="E408" t="inlineStr">
         <is>
@@ -19966,10 +19966,10 @@
         </is>
       </c>
       <c r="C409" t="n">
-        <v>3883</v>
+        <v>3884</v>
       </c>
       <c r="D409" t="n">
-        <v>5787083</v>
+        <v>5788583</v>
       </c>
       <c r="E409" t="inlineStr">
         <is>
@@ -20206,10 +20206,10 @@
         </is>
       </c>
       <c r="C414" t="n">
-        <v>5411</v>
+        <v>5416</v>
       </c>
       <c r="D414" t="n">
-        <v>7274275</v>
+        <v>7281775</v>
       </c>
       <c r="E414" t="inlineStr">
         <is>
@@ -20302,10 +20302,10 @@
         </is>
       </c>
       <c r="C416" t="n">
-        <v>5164</v>
+        <v>5166</v>
       </c>
       <c r="D416" t="n">
-        <v>7604743</v>
+        <v>7607743</v>
       </c>
       <c r="E416" t="inlineStr">
         <is>
@@ -20350,10 +20350,10 @@
         </is>
       </c>
       <c r="C417" t="n">
-        <v>1939</v>
+        <v>1940</v>
       </c>
       <c r="D417" t="n">
-        <v>2888437</v>
+        <v>2889937</v>
       </c>
       <c r="E417" t="inlineStr">
         <is>
@@ -20446,10 +20446,10 @@
         </is>
       </c>
       <c r="C419" t="n">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="D419" t="n">
-        <v>275113</v>
+        <v>276613</v>
       </c>
       <c r="E419" t="inlineStr">
         <is>
@@ -20494,10 +20494,10 @@
         </is>
       </c>
       <c r="C420" t="n">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D420" t="n">
-        <v>27000</v>
+        <v>28500</v>
       </c>
       <c r="E420" t="inlineStr">
         <is>
@@ -20590,10 +20590,10 @@
         </is>
       </c>
       <c r="C422" t="n">
-        <v>3562</v>
+        <v>3566</v>
       </c>
       <c r="D422" t="n">
-        <v>4715264</v>
+        <v>4719108</v>
       </c>
       <c r="E422" t="inlineStr">
         <is>
@@ -20638,10 +20638,10 @@
         </is>
       </c>
       <c r="C423" t="n">
-        <v>602</v>
+        <v>604</v>
       </c>
       <c r="D423" t="n">
-        <v>896664</v>
+        <v>899664</v>
       </c>
       <c r="E423" t="inlineStr">
         <is>
@@ -20734,10 +20734,10 @@
         </is>
       </c>
       <c r="C425" t="n">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="D425" t="n">
-        <v>193500</v>
+        <v>195000</v>
       </c>
       <c r="E425" t="inlineStr">
         <is>
@@ -20878,10 +20878,10 @@
         </is>
       </c>
       <c r="C428" t="n">
-        <v>3083</v>
+        <v>3084</v>
       </c>
       <c r="D428" t="n">
-        <v>4465172</v>
+        <v>4466672</v>
       </c>
       <c r="E428" t="inlineStr">
         <is>
@@ -20926,10 +20926,10 @@
         </is>
       </c>
       <c r="C429" t="n">
-        <v>7377</v>
+        <v>7379</v>
       </c>
       <c r="D429" t="n">
-        <v>10825048</v>
+        <v>10828048</v>
       </c>
       <c r="E429" t="inlineStr">
         <is>
@@ -21166,10 +21166,10 @@
         </is>
       </c>
       <c r="C434" t="n">
-        <v>2423</v>
+        <v>2424</v>
       </c>
       <c r="D434" t="n">
-        <v>3234899</v>
+        <v>3236399</v>
       </c>
       <c r="E434" t="inlineStr">
         <is>
@@ -21214,10 +21214,10 @@
         </is>
       </c>
       <c r="C435" t="n">
-        <v>1736</v>
+        <v>1737</v>
       </c>
       <c r="D435" t="n">
-        <v>2521809</v>
+        <v>2522555</v>
       </c>
       <c r="E435" t="inlineStr">
         <is>
@@ -21262,10 +21262,10 @@
         </is>
       </c>
       <c r="C436" t="n">
-        <v>4900</v>
+        <v>4901</v>
       </c>
       <c r="D436" t="n">
-        <v>7192355</v>
+        <v>7193855</v>
       </c>
       <c r="E436" t="inlineStr">
         <is>
@@ -21310,10 +21310,10 @@
         </is>
       </c>
       <c r="C437" t="n">
-        <v>1608</v>
+        <v>1609</v>
       </c>
       <c r="D437" t="n">
-        <v>2395227</v>
+        <v>2396727</v>
       </c>
       <c r="E437" t="inlineStr">
         <is>
@@ -21502,10 +21502,10 @@
         </is>
       </c>
       <c r="C441" t="n">
-        <v>1688</v>
+        <v>1689</v>
       </c>
       <c r="D441" t="n">
-        <v>2214929</v>
+        <v>2216210</v>
       </c>
       <c r="E441" t="inlineStr">
         <is>
@@ -21598,10 +21598,10 @@
         </is>
       </c>
       <c r="C443" t="n">
-        <v>4877</v>
+        <v>4878</v>
       </c>
       <c r="D443" t="n">
-        <v>7164381</v>
+        <v>7165176</v>
       </c>
       <c r="E443" t="inlineStr">
         <is>
@@ -21646,10 +21646,10 @@
         </is>
       </c>
       <c r="C444" t="n">
-        <v>1543</v>
+        <v>1544</v>
       </c>
       <c r="D444" t="n">
-        <v>2288297</v>
+        <v>2289059</v>
       </c>
       <c r="E444" t="inlineStr">
         <is>
@@ -21886,10 +21886,10 @@
         </is>
       </c>
       <c r="C449" t="n">
-        <v>2666</v>
+        <v>2667</v>
       </c>
       <c r="D449" t="n">
-        <v>3910031</v>
+        <v>3911531</v>
       </c>
       <c r="E449" t="inlineStr">
         <is>
@@ -22126,10 +22126,10 @@
         </is>
       </c>
       <c r="C454" t="n">
-        <v>3041</v>
+        <v>3048</v>
       </c>
       <c r="D454" t="n">
-        <v>4426211</v>
+        <v>4436401</v>
       </c>
       <c r="E454" t="inlineStr">
         <is>
@@ -22174,10 +22174,10 @@
         </is>
       </c>
       <c r="C455" t="n">
-        <v>9380</v>
+        <v>9383</v>
       </c>
       <c r="D455" t="n">
-        <v>13810000</v>
+        <v>13813200</v>
       </c>
       <c r="E455" t="inlineStr">
         <is>
@@ -22222,10 +22222,10 @@
         </is>
       </c>
       <c r="C456" t="n">
-        <v>3407</v>
+        <v>3410</v>
       </c>
       <c r="D456" t="n">
-        <v>5064394</v>
+        <v>5068894</v>
       </c>
       <c r="E456" t="inlineStr">
         <is>
@@ -22270,10 +22270,10 @@
         </is>
       </c>
       <c r="C457" t="n">
-        <v>935</v>
+        <v>936</v>
       </c>
       <c r="D457" t="n">
-        <v>1395237</v>
+        <v>1396737</v>
       </c>
       <c r="E457" t="inlineStr">
         <is>
@@ -22318,10 +22318,10 @@
         </is>
       </c>
       <c r="C458" t="n">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="D458" t="n">
-        <v>306060</v>
+        <v>307560</v>
       </c>
       <c r="E458" t="inlineStr">
         <is>
@@ -22462,10 +22462,10 @@
         </is>
       </c>
       <c r="C461" t="n">
-        <v>1217</v>
+        <v>1218</v>
       </c>
       <c r="D461" t="n">
-        <v>1747259</v>
+        <v>1748759</v>
       </c>
       <c r="E461" t="inlineStr">
         <is>
@@ -22510,10 +22510,10 @@
         </is>
       </c>
       <c r="C462" t="n">
-        <v>3242</v>
+        <v>3243</v>
       </c>
       <c r="D462" t="n">
-        <v>4738368</v>
+        <v>4739868</v>
       </c>
       <c r="E462" t="inlineStr">
         <is>
@@ -22798,10 +22798,10 @@
         </is>
       </c>
       <c r="C468" t="n">
-        <v>4426</v>
+        <v>4429</v>
       </c>
       <c r="D468" t="n">
-        <v>6406866</v>
+        <v>6411366</v>
       </c>
       <c r="E468" t="inlineStr">
         <is>
@@ -22846,10 +22846,10 @@
         </is>
       </c>
       <c r="C469" t="n">
-        <v>8239</v>
+        <v>8242</v>
       </c>
       <c r="D469" t="n">
-        <v>12081575</v>
+        <v>12086075</v>
       </c>
       <c r="E469" t="inlineStr">
         <is>
@@ -23086,10 +23086,10 @@
         </is>
       </c>
       <c r="C474" t="n">
-        <v>2784</v>
+        <v>2785</v>
       </c>
       <c r="D474" t="n">
-        <v>3714502</v>
+        <v>3716002</v>
       </c>
       <c r="E474" t="inlineStr">
         <is>
@@ -23182,10 +23182,10 @@
         </is>
       </c>
       <c r="C476" t="n">
-        <v>2610</v>
+        <v>2611</v>
       </c>
       <c r="D476" t="n">
-        <v>3819006</v>
+        <v>3820506</v>
       </c>
       <c r="E476" t="inlineStr">
         <is>
@@ -23374,10 +23374,10 @@
         </is>
       </c>
       <c r="C480" t="n">
-        <v>1394</v>
+        <v>1395</v>
       </c>
       <c r="D480" t="n">
-        <v>1860742</v>
+        <v>1861364</v>
       </c>
       <c r="E480" t="inlineStr">
         <is>
@@ -23710,10 +23710,10 @@
         </is>
       </c>
       <c r="C487" t="n">
-        <v>928</v>
+        <v>931</v>
       </c>
       <c r="D487" t="n">
-        <v>1346908</v>
+        <v>1351408</v>
       </c>
       <c r="E487" t="inlineStr">
         <is>
@@ -23758,10 +23758,10 @@
         </is>
       </c>
       <c r="C488" t="n">
-        <v>2862</v>
+        <v>2865</v>
       </c>
       <c r="D488" t="n">
-        <v>4217748</v>
+        <v>4222248</v>
       </c>
       <c r="E488" t="inlineStr">
         <is>
@@ -24046,10 +24046,10 @@
         </is>
       </c>
       <c r="C494" t="n">
-        <v>5322</v>
+        <v>5325</v>
       </c>
       <c r="D494" t="n">
-        <v>7792062</v>
+        <v>7796321</v>
       </c>
       <c r="E494" t="inlineStr">
         <is>
@@ -24286,10 +24286,10 @@
         </is>
       </c>
       <c r="C499" t="n">
-        <v>2403</v>
+        <v>2405</v>
       </c>
       <c r="D499" t="n">
-        <v>3143794</v>
+        <v>3146794</v>
       </c>
       <c r="E499" t="inlineStr">
         <is>
@@ -24334,10 +24334,10 @@
         </is>
       </c>
       <c r="C500" t="n">
-        <v>8846</v>
+        <v>8849</v>
       </c>
       <c r="D500" t="n">
-        <v>12813582</v>
+        <v>12817768</v>
       </c>
       <c r="E500" t="inlineStr">
         <is>
@@ -24382,10 +24382,10 @@
         </is>
       </c>
       <c r="C501" t="n">
-        <v>18424</v>
+        <v>18438</v>
       </c>
       <c r="D501" t="n">
-        <v>26971978</v>
+        <v>26989272</v>
       </c>
       <c r="E501" t="inlineStr">
         <is>
@@ -24430,10 +24430,10 @@
         </is>
       </c>
       <c r="C502" t="n">
-        <v>6257</v>
+        <v>6259</v>
       </c>
       <c r="D502" t="n">
-        <v>9308427</v>
+        <v>9311427</v>
       </c>
       <c r="E502" t="inlineStr">
         <is>
@@ -24526,10 +24526,10 @@
         </is>
       </c>
       <c r="C504" t="n">
-        <v>399</v>
+        <v>400</v>
       </c>
       <c r="D504" t="n">
-        <v>598115</v>
+        <v>599615</v>
       </c>
       <c r="E504" t="inlineStr">
         <is>
@@ -24622,10 +24622,10 @@
         </is>
       </c>
       <c r="C506" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D506" t="n">
-        <v>7500</v>
+        <v>9000</v>
       </c>
       <c r="E506" t="inlineStr">
         <is>
@@ -24718,10 +24718,10 @@
         </is>
       </c>
       <c r="C508" t="n">
-        <v>6639</v>
+        <v>6641</v>
       </c>
       <c r="D508" t="n">
-        <v>8988831</v>
+        <v>8991623</v>
       </c>
       <c r="E508" t="inlineStr">
         <is>
@@ -24766,10 +24766,10 @@
         </is>
       </c>
       <c r="C509" t="n">
-        <v>1284</v>
+        <v>1285</v>
       </c>
       <c r="D509" t="n">
-        <v>1848615</v>
+        <v>1850115</v>
       </c>
       <c r="E509" t="inlineStr">
         <is>
@@ -24862,10 +24862,10 @@
         </is>
       </c>
       <c r="C511" t="n">
-        <v>1056</v>
+        <v>1057</v>
       </c>
       <c r="D511" t="n">
-        <v>1570169</v>
+        <v>1571669</v>
       </c>
       <c r="E511" t="inlineStr">
         <is>
@@ -25102,10 +25102,10 @@
         </is>
       </c>
       <c r="C516" t="n">
-        <v>2918</v>
+        <v>2919</v>
       </c>
       <c r="D516" t="n">
-        <v>4185278</v>
+        <v>4186778</v>
       </c>
       <c r="E516" t="inlineStr">
         <is>
@@ -25150,10 +25150,10 @@
         </is>
       </c>
       <c r="C517" t="n">
-        <v>4985</v>
+        <v>4986</v>
       </c>
       <c r="D517" t="n">
-        <v>7293997</v>
+        <v>7295497</v>
       </c>
       <c r="E517" t="inlineStr">
         <is>
@@ -25198,10 +25198,10 @@
         </is>
       </c>
       <c r="C518" t="n">
-        <v>1524</v>
+        <v>1525</v>
       </c>
       <c r="D518" t="n">
-        <v>2266290</v>
+        <v>2267790</v>
       </c>
       <c r="E518" t="inlineStr">
         <is>
@@ -25390,10 +25390,10 @@
         </is>
       </c>
       <c r="C522" t="n">
-        <v>1656</v>
+        <v>1657</v>
       </c>
       <c r="D522" t="n">
-        <v>2193178</v>
+        <v>2194678</v>
       </c>
       <c r="E522" t="inlineStr">
         <is>
@@ -25486,10 +25486,10 @@
         </is>
       </c>
       <c r="C524" t="n">
-        <v>3447</v>
+        <v>3448</v>
       </c>
       <c r="D524" t="n">
-        <v>5036466</v>
+        <v>5037966</v>
       </c>
       <c r="E524" t="inlineStr">
         <is>
@@ -25774,10 +25774,10 @@
         </is>
       </c>
       <c r="C530" t="n">
-        <v>3788</v>
+        <v>3789</v>
       </c>
       <c r="D530" t="n">
-        <v>5445670</v>
+        <v>5447170</v>
       </c>
       <c r="E530" t="inlineStr">
         <is>
@@ -25822,10 +25822,10 @@
         </is>
       </c>
       <c r="C531" t="n">
-        <v>9254</v>
+        <v>9255</v>
       </c>
       <c r="D531" t="n">
-        <v>13526619</v>
+        <v>13528119</v>
       </c>
       <c r="E531" t="inlineStr">
         <is>
@@ -26110,10 +26110,10 @@
         </is>
       </c>
       <c r="C537" t="n">
-        <v>3664</v>
+        <v>3665</v>
       </c>
       <c r="D537" t="n">
-        <v>4931419</v>
+        <v>4932919</v>
       </c>
       <c r="E537" t="inlineStr">
         <is>
@@ -26158,10 +26158,10 @@
         </is>
       </c>
       <c r="C538" t="n">
-        <v>1175</v>
+        <v>1176</v>
       </c>
       <c r="D538" t="n">
-        <v>1683765</v>
+        <v>1685265</v>
       </c>
       <c r="E538" t="inlineStr">
         <is>
@@ -26206,10 +26206,10 @@
         </is>
       </c>
       <c r="C539" t="n">
-        <v>3438</v>
+        <v>3440</v>
       </c>
       <c r="D539" t="n">
-        <v>5013441</v>
+        <v>5016441</v>
       </c>
       <c r="E539" t="inlineStr">
         <is>
@@ -26446,10 +26446,10 @@
         </is>
       </c>
       <c r="C544" t="n">
-        <v>1261</v>
+        <v>1263</v>
       </c>
       <c r="D544" t="n">
-        <v>1695406</v>
+        <v>1697906</v>
       </c>
       <c r="E544" t="inlineStr">
         <is>
@@ -26782,10 +26782,10 @@
         </is>
       </c>
       <c r="C551" t="n">
-        <v>876</v>
+        <v>877</v>
       </c>
       <c r="D551" t="n">
-        <v>1108031</v>
+        <v>1108297</v>
       </c>
       <c r="E551" t="inlineStr">
         <is>
@@ -26830,10 +26830,10 @@
         </is>
       </c>
       <c r="C552" t="n">
-        <v>2845</v>
+        <v>2846</v>
       </c>
       <c r="D552" t="n">
-        <v>4081048</v>
+        <v>4082548</v>
       </c>
       <c r="E552" t="inlineStr">
         <is>
@@ -27214,10 +27214,10 @@
         </is>
       </c>
       <c r="C560" t="n">
-        <v>3653</v>
+        <v>3655</v>
       </c>
       <c r="D560" t="n">
-        <v>5340724</v>
+        <v>5342684</v>
       </c>
       <c r="E560" t="inlineStr">
         <is>
@@ -27502,10 +27502,10 @@
         </is>
       </c>
       <c r="C566" t="n">
-        <v>4434</v>
+        <v>4439</v>
       </c>
       <c r="D566" t="n">
-        <v>6403887</v>
+        <v>6411387</v>
       </c>
       <c r="E566" t="inlineStr">
         <is>
@@ -27550,10 +27550,10 @@
         </is>
       </c>
       <c r="C567" t="n">
-        <v>10338</v>
+        <v>10345</v>
       </c>
       <c r="D567" t="n">
-        <v>15119962</v>
+        <v>15130361</v>
       </c>
       <c r="E567" t="inlineStr">
         <is>
@@ -27790,10 +27790,10 @@
         </is>
       </c>
       <c r="C572" t="n">
-        <v>4056</v>
+        <v>4059</v>
       </c>
       <c r="D572" t="n">
-        <v>5371129</v>
+        <v>5375629</v>
       </c>
       <c r="E572" t="inlineStr">
         <is>
@@ -27838,10 +27838,10 @@
         </is>
       </c>
       <c r="C573" t="n">
-        <v>1012</v>
+        <v>1013</v>
       </c>
       <c r="D573" t="n">
-        <v>1467706</v>
+        <v>1469206</v>
       </c>
       <c r="E573" t="inlineStr">
         <is>
@@ -28078,10 +28078,10 @@
         </is>
       </c>
       <c r="C578" t="n">
-        <v>1256</v>
+        <v>1257</v>
       </c>
       <c r="D578" t="n">
-        <v>1649719</v>
+        <v>1651219</v>
       </c>
       <c r="E578" t="inlineStr">
         <is>
@@ -28126,10 +28126,10 @@
         </is>
       </c>
       <c r="C579" t="n">
-        <v>6293</v>
+        <v>6295</v>
       </c>
       <c r="D579" t="n">
-        <v>9087861</v>
+        <v>9089869</v>
       </c>
       <c r="E579" t="inlineStr">
         <is>
@@ -28174,10 +28174,10 @@
         </is>
       </c>
       <c r="C580" t="n">
-        <v>15076</v>
+        <v>15080</v>
       </c>
       <c r="D580" t="n">
-        <v>22099740</v>
+        <v>22105740</v>
       </c>
       <c r="E580" t="inlineStr">
         <is>
@@ -28222,10 +28222,10 @@
         </is>
       </c>
       <c r="C581" t="n">
-        <v>5300</v>
+        <v>5306</v>
       </c>
       <c r="D581" t="n">
-        <v>7876678</v>
+        <v>7885678</v>
       </c>
       <c r="E581" t="inlineStr">
         <is>
@@ -28270,10 +28270,10 @@
         </is>
       </c>
       <c r="C582" t="n">
-        <v>1620</v>
+        <v>1622</v>
       </c>
       <c r="D582" t="n">
-        <v>2413678</v>
+        <v>2416678</v>
       </c>
       <c r="E582" t="inlineStr">
         <is>
@@ -28318,10 +28318,10 @@
         </is>
       </c>
       <c r="C583" t="n">
-        <v>321</v>
+        <v>322</v>
       </c>
       <c r="D583" t="n">
-        <v>476727</v>
+        <v>478227</v>
       </c>
       <c r="E583" t="inlineStr">
         <is>
@@ -28462,10 +28462,10 @@
         </is>
       </c>
       <c r="C586" t="n">
-        <v>6144</v>
+        <v>6145</v>
       </c>
       <c r="D586" t="n">
-        <v>8204033</v>
+        <v>8205533</v>
       </c>
       <c r="E586" t="inlineStr">
         <is>
@@ -28558,10 +28558,10 @@
         </is>
       </c>
       <c r="C588" t="n">
-        <v>3286</v>
+        <v>3287</v>
       </c>
       <c r="D588" t="n">
-        <v>4751061</v>
+        <v>4752411</v>
       </c>
       <c r="E588" t="inlineStr">
         <is>
@@ -28606,10 +28606,10 @@
         </is>
       </c>
       <c r="C589" t="n">
-        <v>1074</v>
+        <v>1075</v>
       </c>
       <c r="D589" t="n">
-        <v>1591297</v>
+        <v>1592797</v>
       </c>
       <c r="E589" t="inlineStr">
         <is>
@@ -28750,10 +28750,10 @@
         </is>
       </c>
       <c r="C592" t="n">
-        <v>1813</v>
+        <v>1814</v>
       </c>
       <c r="D592" t="n">
-        <v>2430498</v>
+        <v>2431998</v>
       </c>
       <c r="E592" t="inlineStr">
         <is>
@@ -28798,10 +28798,10 @@
         </is>
       </c>
       <c r="C593" t="n">
-        <v>8696</v>
+        <v>8700</v>
       </c>
       <c r="D593" t="n">
-        <v>12608026</v>
+        <v>12614026</v>
       </c>
       <c r="E593" t="inlineStr">
         <is>
@@ -28846,10 +28846,10 @@
         </is>
       </c>
       <c r="C594" t="n">
-        <v>18323</v>
+        <v>18329</v>
       </c>
       <c r="D594" t="n">
-        <v>26841535</v>
+        <v>26850535</v>
       </c>
       <c r="E594" t="inlineStr">
         <is>
@@ -28894,10 +28894,10 @@
         </is>
       </c>
       <c r="C595" t="n">
-        <v>5511</v>
+        <v>5513</v>
       </c>
       <c r="D595" t="n">
-        <v>8194715</v>
+        <v>8197715</v>
       </c>
       <c r="E595" t="inlineStr">
         <is>
@@ -28942,10 +28942,10 @@
         </is>
       </c>
       <c r="C596" t="n">
-        <v>1419</v>
+        <v>1420</v>
       </c>
       <c r="D596" t="n">
-        <v>2107236</v>
+        <v>2108736</v>
       </c>
       <c r="E596" t="inlineStr">
         <is>
@@ -29086,10 +29086,10 @@
         </is>
       </c>
       <c r="C599" t="n">
-        <v>6037</v>
+        <v>6040</v>
       </c>
       <c r="D599" t="n">
-        <v>8051686</v>
+        <v>8053857</v>
       </c>
       <c r="E599" t="inlineStr">
         <is>
@@ -29134,10 +29134,10 @@
         </is>
       </c>
       <c r="C600" t="n">
-        <v>1306</v>
+        <v>1308</v>
       </c>
       <c r="D600" t="n">
-        <v>1880289</v>
+        <v>1883289</v>
       </c>
       <c r="E600" t="inlineStr">
         <is>
@@ -29182,10 +29182,10 @@
         </is>
       </c>
       <c r="C601" t="n">
-        <v>2289</v>
+        <v>2290</v>
       </c>
       <c r="D601" t="n">
-        <v>3353154</v>
+        <v>3353756</v>
       </c>
       <c r="E601" t="inlineStr">
         <is>
@@ -29710,10 +29710,10 @@
         </is>
       </c>
       <c r="C612" t="n">
-        <v>911</v>
+        <v>913</v>
       </c>
       <c r="D612" t="n">
-        <v>1263599</v>
+        <v>1266599</v>
       </c>
       <c r="E612" t="inlineStr">
         <is>
@@ -29758,10 +29758,10 @@
         </is>
       </c>
       <c r="C613" t="n">
-        <v>4080</v>
+        <v>4082</v>
       </c>
       <c r="D613" t="n">
-        <v>5923102</v>
+        <v>5926102</v>
       </c>
       <c r="E613" t="inlineStr">
         <is>
@@ -29806,10 +29806,10 @@
         </is>
       </c>
       <c r="C614" t="n">
-        <v>6666</v>
+        <v>6667</v>
       </c>
       <c r="D614" t="n">
-        <v>9699516</v>
+        <v>9701016</v>
       </c>
       <c r="E614" t="inlineStr">
         <is>
@@ -30046,10 +30046,10 @@
         </is>
       </c>
       <c r="C619" t="n">
-        <v>2616</v>
+        <v>2617</v>
       </c>
       <c r="D619" t="n">
-        <v>3478262</v>
+        <v>3479762</v>
       </c>
       <c r="E619" t="inlineStr">
         <is>
@@ -30094,10 +30094,10 @@
         </is>
       </c>
       <c r="C620" t="n">
-        <v>1691</v>
+        <v>1692</v>
       </c>
       <c r="D620" t="n">
-        <v>2444785</v>
+        <v>2446285</v>
       </c>
       <c r="E620" t="inlineStr">
         <is>
@@ -30190,10 +30190,10 @@
         </is>
       </c>
       <c r="C622" t="n">
-        <v>1259</v>
+        <v>1260</v>
       </c>
       <c r="D622" t="n">
-        <v>1860060</v>
+        <v>1861560</v>
       </c>
       <c r="E622" t="inlineStr">
         <is>
@@ -30478,10 +30478,10 @@
         </is>
       </c>
       <c r="C628" t="n">
-        <v>2679</v>
+        <v>2680</v>
       </c>
       <c r="D628" t="n">
-        <v>3920302</v>
+        <v>3921802</v>
       </c>
       <c r="E628" t="inlineStr">
         <is>
@@ -30718,10 +30718,10 @@
         </is>
       </c>
       <c r="C633" t="n">
-        <v>1233</v>
+        <v>1234</v>
       </c>
       <c r="D633" t="n">
-        <v>1620011</v>
+        <v>1620445</v>
       </c>
       <c r="E633" t="inlineStr">
         <is>
@@ -30766,10 +30766,10 @@
         </is>
       </c>
       <c r="C634" t="n">
-        <v>5229</v>
+        <v>5230</v>
       </c>
       <c r="D634" t="n">
-        <v>7579073</v>
+        <v>7580573</v>
       </c>
       <c r="E634" t="inlineStr">
         <is>
@@ -30814,10 +30814,10 @@
         </is>
       </c>
       <c r="C635" t="n">
-        <v>12339</v>
+        <v>12342</v>
       </c>
       <c r="D635" t="n">
-        <v>18155526</v>
+        <v>18160026</v>
       </c>
       <c r="E635" t="inlineStr">
         <is>
@@ -30862,10 +30862,10 @@
         </is>
       </c>
       <c r="C636" t="n">
-        <v>4635</v>
+        <v>4636</v>
       </c>
       <c r="D636" t="n">
-        <v>6878528</v>
+        <v>6879278</v>
       </c>
       <c r="E636" t="inlineStr">
         <is>
@@ -31054,10 +31054,10 @@
         </is>
       </c>
       <c r="C640" t="n">
-        <v>4235</v>
+        <v>4238</v>
       </c>
       <c r="D640" t="n">
-        <v>5651081</v>
+        <v>5655481</v>
       </c>
       <c r="E640" t="inlineStr">
         <is>
@@ -31102,10 +31102,10 @@
         </is>
       </c>
       <c r="C641" t="n">
-        <v>2273</v>
+        <v>2274</v>
       </c>
       <c r="D641" t="n">
-        <v>3277523</v>
+        <v>3279023</v>
       </c>
       <c r="E641" t="inlineStr">
         <is>
@@ -31438,10 +31438,10 @@
         </is>
       </c>
       <c r="C648" t="n">
-        <v>2281</v>
+        <v>2283</v>
       </c>
       <c r="D648" t="n">
-        <v>3081316</v>
+        <v>3083974</v>
       </c>
       <c r="E648" t="inlineStr">
         <is>
@@ -32110,10 +32110,10 @@
         </is>
       </c>
       <c r="C662" t="n">
-        <v>1376</v>
+        <v>1377</v>
       </c>
       <c r="D662" t="n">
-        <v>1791512</v>
+        <v>1793012</v>
       </c>
       <c r="E662" t="inlineStr">
         <is>
@@ -32158,10 +32158,10 @@
         </is>
       </c>
       <c r="C663" t="n">
-        <v>3245</v>
+        <v>3250</v>
       </c>
       <c r="D663" t="n">
-        <v>4711596</v>
+        <v>4719096</v>
       </c>
       <c r="E663" t="inlineStr">
         <is>
@@ -32206,10 +32206,10 @@
         </is>
       </c>
       <c r="C664" t="n">
-        <v>6416</v>
+        <v>6419</v>
       </c>
       <c r="D664" t="n">
-        <v>9391151</v>
+        <v>9395651</v>
       </c>
       <c r="E664" t="inlineStr">
         <is>
@@ -32254,10 +32254,10 @@
         </is>
       </c>
       <c r="C665" t="n">
-        <v>2351</v>
+        <v>2352</v>
       </c>
       <c r="D665" t="n">
-        <v>3500537</v>
+        <v>3502037</v>
       </c>
       <c r="E665" t="inlineStr">
         <is>
@@ -32494,10 +32494,10 @@
         </is>
       </c>
       <c r="C670" t="n">
-        <v>2063</v>
+        <v>2067</v>
       </c>
       <c r="D670" t="n">
-        <v>2761554</v>
+        <v>2767341</v>
       </c>
       <c r="E670" t="inlineStr">
         <is>
@@ -32878,10 +32878,10 @@
         </is>
       </c>
       <c r="C678" t="n">
-        <v>8660</v>
+        <v>8666</v>
       </c>
       <c r="D678" t="n">
-        <v>12535707</v>
+        <v>12544707</v>
       </c>
       <c r="E678" t="inlineStr">
         <is>
@@ -32926,10 +32926,10 @@
         </is>
       </c>
       <c r="C679" t="n">
-        <v>20690</v>
+        <v>20697</v>
       </c>
       <c r="D679" t="n">
-        <v>30356830</v>
+        <v>30366597</v>
       </c>
       <c r="E679" t="inlineStr">
         <is>
@@ -32974,10 +32974,10 @@
         </is>
       </c>
       <c r="C680" t="n">
-        <v>6170</v>
+        <v>6172</v>
       </c>
       <c r="D680" t="n">
-        <v>9173548</v>
+        <v>9176548</v>
       </c>
       <c r="E680" t="inlineStr">
         <is>
@@ -33022,10 +33022,10 @@
         </is>
       </c>
       <c r="C681" t="n">
-        <v>1779</v>
+        <v>1780</v>
       </c>
       <c r="D681" t="n">
-        <v>2656874</v>
+        <v>2658374</v>
       </c>
       <c r="E681" t="inlineStr">
         <is>
@@ -33070,10 +33070,10 @@
         </is>
       </c>
       <c r="C682" t="n">
-        <v>420</v>
+        <v>421</v>
       </c>
       <c r="D682" t="n">
-        <v>621960</v>
+        <v>623460</v>
       </c>
       <c r="E682" t="inlineStr">
         <is>
@@ -33166,10 +33166,10 @@
         </is>
       </c>
       <c r="C684" t="n">
-        <v>7500</v>
+        <v>7505</v>
       </c>
       <c r="D684" t="n">
-        <v>10196518</v>
+        <v>10200579</v>
       </c>
       <c r="E684" t="inlineStr">
         <is>
@@ -33214,10 +33214,10 @@
         </is>
       </c>
       <c r="C685" t="n">
-        <v>10600</v>
+        <v>10606</v>
       </c>
       <c r="D685" t="n">
-        <v>15389322</v>
+        <v>15398322</v>
       </c>
       <c r="E685" t="inlineStr">
         <is>
@@ -33262,10 +33262,10 @@
         </is>
       </c>
       <c r="C686" t="n">
-        <v>28337</v>
+        <v>28340</v>
       </c>
       <c r="D686" t="n">
-        <v>41604168</v>
+        <v>41608668</v>
       </c>
       <c r="E686" t="inlineStr">
         <is>
@@ -33310,10 +33310,10 @@
         </is>
       </c>
       <c r="C687" t="n">
-        <v>8919</v>
+        <v>8922</v>
       </c>
       <c r="D687" t="n">
-        <v>13277653</v>
+        <v>13282153</v>
       </c>
       <c r="E687" t="inlineStr">
         <is>
@@ -33406,10 +33406,10 @@
         </is>
       </c>
       <c r="C689" t="n">
-        <v>551</v>
+        <v>552</v>
       </c>
       <c r="D689" t="n">
-        <v>820998</v>
+        <v>822498</v>
       </c>
       <c r="E689" t="inlineStr">
         <is>
@@ -33550,10 +33550,10 @@
         </is>
       </c>
       <c r="C692" t="n">
-        <v>9499</v>
+        <v>9507</v>
       </c>
       <c r="D692" t="n">
-        <v>12812583</v>
+        <v>12823028</v>
       </c>
       <c r="E692" t="inlineStr">
         <is>
@@ -33598,10 +33598,10 @@
         </is>
       </c>
       <c r="C693" t="n">
-        <v>1300</v>
+        <v>1301</v>
       </c>
       <c r="D693" t="n">
-        <v>1871940</v>
+        <v>1873440</v>
       </c>
       <c r="E693" t="inlineStr">
         <is>
@@ -33646,10 +33646,10 @@
         </is>
       </c>
       <c r="C694" t="n">
-        <v>2698</v>
+        <v>2699</v>
       </c>
       <c r="D694" t="n">
-        <v>3939073</v>
+        <v>3940573</v>
       </c>
       <c r="E694" t="inlineStr">
         <is>
@@ -33934,10 +33934,10 @@
         </is>
       </c>
       <c r="C700" t="n">
-        <v>9074</v>
+        <v>9077</v>
       </c>
       <c r="D700" t="n">
-        <v>12994862</v>
+        <v>12999362</v>
       </c>
       <c r="E700" t="inlineStr">
         <is>
@@ -33982,10 +33982,10 @@
         </is>
       </c>
       <c r="C701" t="n">
-        <v>16969</v>
+        <v>16972</v>
       </c>
       <c r="D701" t="n">
-        <v>24758728</v>
+        <v>24763228</v>
       </c>
       <c r="E701" t="inlineStr">
         <is>
@@ -34030,10 +34030,10 @@
         </is>
       </c>
       <c r="C702" t="n">
-        <v>4708</v>
+        <v>4709</v>
       </c>
       <c r="D702" t="n">
-        <v>6993367</v>
+        <v>6994867</v>
       </c>
       <c r="E702" t="inlineStr">
         <is>
@@ -34318,10 +34318,10 @@
         </is>
       </c>
       <c r="C708" t="n">
-        <v>3831</v>
+        <v>3832</v>
       </c>
       <c r="D708" t="n">
-        <v>5532620</v>
+        <v>5534120</v>
       </c>
       <c r="E708" t="inlineStr">
         <is>
@@ -34366,10 +34366,10 @@
         </is>
       </c>
       <c r="C709" t="n">
-        <v>9614</v>
+        <v>9617</v>
       </c>
       <c r="D709" t="n">
-        <v>14090899</v>
+        <v>14095399</v>
       </c>
       <c r="E709" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
[Fonds de solidarite] Add 2020-11-10 data
</commit_message>
<xml_diff>
--- a/published-data/fonds-solidarite-volet-1-departemental-classe-effectif-latest.xlsx
+++ b/published-data/fonds-solidarite-volet-1-departemental-classe-effectif-latest.xlsx
@@ -430,10 +430,10 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>1393</v>
+        <v>1395</v>
       </c>
       <c r="D2" t="n">
-        <v>2012502</v>
+        <v>2015252</v>
       </c>
       <c r="E2" t="inlineStr">
         <is>
@@ -478,10 +478,10 @@
         </is>
       </c>
       <c r="C3" t="n">
-        <v>6182</v>
+        <v>6184</v>
       </c>
       <c r="D3" t="n">
-        <v>9071105</v>
+        <v>9074105</v>
       </c>
       <c r="E3" t="inlineStr">
         <is>
@@ -526,10 +526,10 @@
         </is>
       </c>
       <c r="C4" t="n">
-        <v>2194</v>
+        <v>2196</v>
       </c>
       <c r="D4" t="n">
-        <v>3260632</v>
+        <v>3264130</v>
       </c>
       <c r="E4" t="inlineStr">
         <is>
@@ -718,10 +718,10 @@
         </is>
       </c>
       <c r="C8" t="n">
-        <v>755</v>
+        <v>756</v>
       </c>
       <c r="D8" t="n">
-        <v>991293</v>
+        <v>992793</v>
       </c>
       <c r="E8" t="inlineStr">
         <is>
@@ -1150,10 +1150,10 @@
         </is>
       </c>
       <c r="C17" t="n">
-        <v>4545</v>
+        <v>4546</v>
       </c>
       <c r="D17" t="n">
-        <v>6619536</v>
+        <v>6620840</v>
       </c>
       <c r="E17" t="inlineStr">
         <is>
@@ -1486,10 +1486,10 @@
         </is>
       </c>
       <c r="C24" t="n">
-        <v>2050</v>
+        <v>2051</v>
       </c>
       <c r="D24" t="n">
-        <v>2974196</v>
+        <v>2975696</v>
       </c>
       <c r="E24" t="inlineStr">
         <is>
@@ -1870,10 +1870,10 @@
         </is>
       </c>
       <c r="C32" t="n">
-        <v>2105</v>
+        <v>2106</v>
       </c>
       <c r="D32" t="n">
-        <v>3119922</v>
+        <v>3121422</v>
       </c>
       <c r="E32" t="inlineStr">
         <is>
@@ -1966,10 +1966,10 @@
         </is>
       </c>
       <c r="C34" t="n">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="D34" t="n">
-        <v>183049</v>
+        <v>186049</v>
       </c>
       <c r="E34" t="inlineStr">
         <is>
@@ -2110,10 +2110,10 @@
         </is>
       </c>
       <c r="C37" t="n">
-        <v>1352</v>
+        <v>1354</v>
       </c>
       <c r="D37" t="n">
-        <v>1932516</v>
+        <v>1935516</v>
       </c>
       <c r="E37" t="inlineStr">
         <is>
@@ -2206,10 +2206,10 @@
         </is>
       </c>
       <c r="C39" t="n">
-        <v>837</v>
+        <v>839</v>
       </c>
       <c r="D39" t="n">
-        <v>1232743</v>
+        <v>1235743</v>
       </c>
       <c r="E39" t="inlineStr">
         <is>
@@ -2446,10 +2446,10 @@
         </is>
       </c>
       <c r="C44" t="n">
-        <v>4404</v>
+        <v>4406</v>
       </c>
       <c r="D44" t="n">
-        <v>6396973</v>
+        <v>6399973</v>
       </c>
       <c r="E44" t="inlineStr">
         <is>
@@ -2494,10 +2494,10 @@
         </is>
       </c>
       <c r="C45" t="n">
-        <v>9713</v>
+        <v>9719</v>
       </c>
       <c r="D45" t="n">
-        <v>14234468</v>
+        <v>14243468</v>
       </c>
       <c r="E45" t="inlineStr">
         <is>
@@ -2542,10 +2542,10 @@
         </is>
       </c>
       <c r="C46" t="n">
-        <v>3897</v>
+        <v>3898</v>
       </c>
       <c r="D46" t="n">
-        <v>5759181</v>
+        <v>5760681</v>
       </c>
       <c r="E46" t="inlineStr">
         <is>
@@ -2590,10 +2590,10 @@
         </is>
       </c>
       <c r="C47" t="n">
-        <v>1266</v>
+        <v>1267</v>
       </c>
       <c r="D47" t="n">
-        <v>1887211</v>
+        <v>1888711</v>
       </c>
       <c r="E47" t="inlineStr">
         <is>
@@ -2638,10 +2638,10 @@
         </is>
       </c>
       <c r="C48" t="n">
-        <v>398</v>
+        <v>399</v>
       </c>
       <c r="D48" t="n">
-        <v>592950</v>
+        <v>594450</v>
       </c>
       <c r="E48" t="inlineStr">
         <is>
@@ -2734,10 +2734,10 @@
         </is>
       </c>
       <c r="C50" t="n">
-        <v>5411</v>
+        <v>5414</v>
       </c>
       <c r="D50" t="n">
-        <v>7399088</v>
+        <v>7402044</v>
       </c>
       <c r="E50" t="inlineStr">
         <is>
@@ -2782,10 +2782,10 @@
         </is>
       </c>
       <c r="C51" t="n">
-        <v>6452</v>
+        <v>6458</v>
       </c>
       <c r="D51" t="n">
-        <v>9324874</v>
+        <v>9333874</v>
       </c>
       <c r="E51" t="inlineStr">
         <is>
@@ -2830,10 +2830,10 @@
         </is>
       </c>
       <c r="C52" t="n">
-        <v>14800</v>
+        <v>14810</v>
       </c>
       <c r="D52" t="n">
-        <v>21761049</v>
+        <v>21776877</v>
       </c>
       <c r="E52" t="inlineStr">
         <is>
@@ -2878,10 +2878,10 @@
         </is>
       </c>
       <c r="C53" t="n">
-        <v>4971</v>
+        <v>4973</v>
       </c>
       <c r="D53" t="n">
-        <v>7356496</v>
+        <v>7358262</v>
       </c>
       <c r="E53" t="inlineStr">
         <is>
@@ -2926,10 +2926,10 @@
         </is>
       </c>
       <c r="C54" t="n">
-        <v>1390</v>
+        <v>1391</v>
       </c>
       <c r="D54" t="n">
-        <v>2061181</v>
+        <v>2062681</v>
       </c>
       <c r="E54" t="inlineStr">
         <is>
@@ -3022,10 +3022,10 @@
         </is>
       </c>
       <c r="C56" t="n">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="D56" t="n">
-        <v>48500</v>
+        <v>50000</v>
       </c>
       <c r="E56" t="inlineStr">
         <is>
@@ -3118,10 +3118,10 @@
         </is>
       </c>
       <c r="C58" t="n">
-        <v>6068</v>
+        <v>6070</v>
       </c>
       <c r="D58" t="n">
-        <v>8261204</v>
+        <v>8264204</v>
       </c>
       <c r="E58" t="inlineStr">
         <is>
@@ -3166,10 +3166,10 @@
         </is>
       </c>
       <c r="C59" t="n">
-        <v>3482</v>
+        <v>3486</v>
       </c>
       <c r="D59" t="n">
-        <v>5022067</v>
+        <v>5025633</v>
       </c>
       <c r="E59" t="inlineStr">
         <is>
@@ -3214,10 +3214,10 @@
         </is>
       </c>
       <c r="C60" t="n">
-        <v>8460</v>
+        <v>8466</v>
       </c>
       <c r="D60" t="n">
-        <v>12387467</v>
+        <v>12396965</v>
       </c>
       <c r="E60" t="inlineStr">
         <is>
@@ -3262,10 +3262,10 @@
         </is>
       </c>
       <c r="C61" t="n">
-        <v>2659</v>
+        <v>2661</v>
       </c>
       <c r="D61" t="n">
-        <v>3919662</v>
+        <v>3921426</v>
       </c>
       <c r="E61" t="inlineStr">
         <is>
@@ -3454,10 +3454,10 @@
         </is>
       </c>
       <c r="C65" t="n">
-        <v>3591</v>
+        <v>3594</v>
       </c>
       <c r="D65" t="n">
-        <v>4667438</v>
+        <v>4669672</v>
       </c>
       <c r="E65" t="inlineStr">
         <is>
@@ -3502,10 +3502,10 @@
         </is>
       </c>
       <c r="C66" t="n">
-        <v>2921</v>
+        <v>2924</v>
       </c>
       <c r="D66" t="n">
-        <v>4188542</v>
+        <v>4192642</v>
       </c>
       <c r="E66" t="inlineStr">
         <is>
@@ -3550,10 +3550,10 @@
         </is>
       </c>
       <c r="C67" t="n">
-        <v>7584</v>
+        <v>7587</v>
       </c>
       <c r="D67" t="n">
-        <v>11080864</v>
+        <v>11085364</v>
       </c>
       <c r="E67" t="inlineStr">
         <is>
@@ -3598,10 +3598,10 @@
         </is>
       </c>
       <c r="C68" t="n">
-        <v>2542</v>
+        <v>2543</v>
       </c>
       <c r="D68" t="n">
-        <v>3755534</v>
+        <v>3757034</v>
       </c>
       <c r="E68" t="inlineStr">
         <is>
@@ -3790,10 +3790,10 @@
         </is>
       </c>
       <c r="C72" t="n">
-        <v>3233</v>
+        <v>3236</v>
       </c>
       <c r="D72" t="n">
-        <v>4261127</v>
+        <v>4264585</v>
       </c>
       <c r="E72" t="inlineStr">
         <is>
@@ -3838,10 +3838,10 @@
         </is>
       </c>
       <c r="C73" t="n">
-        <v>10244</v>
+        <v>10254</v>
       </c>
       <c r="D73" t="n">
-        <v>14824194</v>
+        <v>14839194</v>
       </c>
       <c r="E73" t="inlineStr">
         <is>
@@ -3886,10 +3886,10 @@
         </is>
       </c>
       <c r="C74" t="n">
-        <v>24727</v>
+        <v>24749</v>
       </c>
       <c r="D74" t="n">
-        <v>36289253</v>
+        <v>36320882</v>
       </c>
       <c r="E74" t="inlineStr">
         <is>
@@ -3934,10 +3934,10 @@
         </is>
       </c>
       <c r="C75" t="n">
-        <v>8468</v>
+        <v>8478</v>
       </c>
       <c r="D75" t="n">
-        <v>12559419</v>
+        <v>12572999</v>
       </c>
       <c r="E75" t="inlineStr">
         <is>
@@ -3982,10 +3982,10 @@
         </is>
       </c>
       <c r="C76" t="n">
-        <v>2438</v>
+        <v>2439</v>
       </c>
       <c r="D76" t="n">
-        <v>3631872</v>
+        <v>3633372</v>
       </c>
       <c r="E76" t="inlineStr">
         <is>
@@ -4030,10 +4030,10 @@
         </is>
       </c>
       <c r="C77" t="n">
-        <v>530</v>
+        <v>531</v>
       </c>
       <c r="D77" t="n">
-        <v>791555</v>
+        <v>793055</v>
       </c>
       <c r="E77" t="inlineStr">
         <is>
@@ -4270,10 +4270,10 @@
         </is>
       </c>
       <c r="C82" t="n">
-        <v>8262</v>
+        <v>8268</v>
       </c>
       <c r="D82" t="n">
-        <v>11315787</v>
+        <v>11320085</v>
       </c>
       <c r="E82" t="inlineStr">
         <is>
@@ -4318,10 +4318,10 @@
         </is>
       </c>
       <c r="C83" t="n">
-        <v>3041</v>
+        <v>3043</v>
       </c>
       <c r="D83" t="n">
-        <v>4404366</v>
+        <v>4407366</v>
       </c>
       <c r="E83" t="inlineStr">
         <is>
@@ -4366,10 +4366,10 @@
         </is>
       </c>
       <c r="C84" t="n">
-        <v>7090</v>
+        <v>7100</v>
       </c>
       <c r="D84" t="n">
-        <v>10372096</v>
+        <v>10386992</v>
       </c>
       <c r="E84" t="inlineStr">
         <is>
@@ -4414,10 +4414,10 @@
         </is>
       </c>
       <c r="C85" t="n">
-        <v>3218</v>
+        <v>3221</v>
       </c>
       <c r="D85" t="n">
-        <v>4766406</v>
+        <v>4770906</v>
       </c>
       <c r="E85" t="inlineStr">
         <is>
@@ -4462,10 +4462,10 @@
         </is>
       </c>
       <c r="C86" t="n">
-        <v>1162</v>
+        <v>1164</v>
       </c>
       <c r="D86" t="n">
-        <v>1718573</v>
+        <v>1721573</v>
       </c>
       <c r="E86" t="inlineStr">
         <is>
@@ -4510,10 +4510,10 @@
         </is>
       </c>
       <c r="C87" t="n">
-        <v>382</v>
+        <v>383</v>
       </c>
       <c r="D87" t="n">
-        <v>569273</v>
+        <v>570773</v>
       </c>
       <c r="E87" t="inlineStr">
         <is>
@@ -4606,10 +4606,10 @@
         </is>
       </c>
       <c r="C89" t="n">
-        <v>7016</v>
+        <v>7021</v>
       </c>
       <c r="D89" t="n">
-        <v>9847517</v>
+        <v>9853171</v>
       </c>
       <c r="E89" t="inlineStr">
         <is>
@@ -4702,10 +4702,10 @@
         </is>
       </c>
       <c r="C91" t="n">
-        <v>5327</v>
+        <v>5331</v>
       </c>
       <c r="D91" t="n">
-        <v>7814475</v>
+        <v>7819803</v>
       </c>
       <c r="E91" t="inlineStr">
         <is>
@@ -4750,10 +4750,10 @@
         </is>
       </c>
       <c r="C92" t="n">
-        <v>1877</v>
+        <v>1878</v>
       </c>
       <c r="D92" t="n">
-        <v>2789151</v>
+        <v>2790651</v>
       </c>
       <c r="E92" t="inlineStr">
         <is>
@@ -4798,10 +4798,10 @@
         </is>
       </c>
       <c r="C93" t="n">
-        <v>533</v>
+        <v>534</v>
       </c>
       <c r="D93" t="n">
-        <v>793805</v>
+        <v>795305</v>
       </c>
       <c r="E93" t="inlineStr">
         <is>
@@ -4846,10 +4846,10 @@
         </is>
       </c>
       <c r="C94" t="n">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="D94" t="n">
-        <v>149175</v>
+        <v>152175</v>
       </c>
       <c r="E94" t="inlineStr">
         <is>
@@ -4990,10 +4990,10 @@
         </is>
       </c>
       <c r="C97" t="n">
-        <v>1860</v>
+        <v>1861</v>
       </c>
       <c r="D97" t="n">
-        <v>2682137</v>
+        <v>2683637</v>
       </c>
       <c r="E97" t="inlineStr">
         <is>
@@ -5038,10 +5038,10 @@
         </is>
       </c>
       <c r="C98" t="n">
-        <v>4854</v>
+        <v>4855</v>
       </c>
       <c r="D98" t="n">
-        <v>7113289</v>
+        <v>7114789</v>
       </c>
       <c r="E98" t="inlineStr">
         <is>
@@ -5086,10 +5086,10 @@
         </is>
       </c>
       <c r="C99" t="n">
-        <v>1666</v>
+        <v>1667</v>
       </c>
       <c r="D99" t="n">
-        <v>2469990</v>
+        <v>2471490</v>
       </c>
       <c r="E99" t="inlineStr">
         <is>
@@ -5422,10 +5422,10 @@
         </is>
       </c>
       <c r="C106" t="n">
-        <v>1857</v>
+        <v>1861</v>
       </c>
       <c r="D106" t="n">
-        <v>2729488</v>
+        <v>2735488</v>
       </c>
       <c r="E106" t="inlineStr">
         <is>
@@ -5614,10 +5614,10 @@
         </is>
       </c>
       <c r="C110" t="n">
-        <v>926</v>
+        <v>927</v>
       </c>
       <c r="D110" t="n">
-        <v>1164738</v>
+        <v>1165738</v>
       </c>
       <c r="E110" t="inlineStr">
         <is>
@@ -5710,10 +5710,10 @@
         </is>
       </c>
       <c r="C112" t="n">
-        <v>2846</v>
+        <v>2849</v>
       </c>
       <c r="D112" t="n">
-        <v>4174307</v>
+        <v>4178238</v>
       </c>
       <c r="E112" t="inlineStr">
         <is>
@@ -5998,10 +5998,10 @@
         </is>
       </c>
       <c r="C118" t="n">
-        <v>791</v>
+        <v>792</v>
       </c>
       <c r="D118" t="n">
-        <v>1127359</v>
+        <v>1128859</v>
       </c>
       <c r="E118" t="inlineStr">
         <is>
@@ -6286,10 +6286,10 @@
         </is>
       </c>
       <c r="C124" t="n">
-        <v>2171</v>
+        <v>2174</v>
       </c>
       <c r="D124" t="n">
-        <v>3135694</v>
+        <v>3140194</v>
       </c>
       <c r="E124" t="inlineStr">
         <is>
@@ -6334,10 +6334,10 @@
         </is>
       </c>
       <c r="C125" t="n">
-        <v>6143</v>
+        <v>6145</v>
       </c>
       <c r="D125" t="n">
-        <v>9006259</v>
+        <v>9009259</v>
       </c>
       <c r="E125" t="inlineStr">
         <is>
@@ -6574,10 +6574,10 @@
         </is>
       </c>
       <c r="C130" t="n">
-        <v>2661</v>
+        <v>2662</v>
       </c>
       <c r="D130" t="n">
-        <v>3567095</v>
+        <v>3568595</v>
       </c>
       <c r="E130" t="inlineStr">
         <is>
@@ -6670,10 +6670,10 @@
         </is>
       </c>
       <c r="C132" t="n">
-        <v>1223</v>
+        <v>1224</v>
       </c>
       <c r="D132" t="n">
-        <v>1788251</v>
+        <v>1789751</v>
       </c>
       <c r="E132" t="inlineStr">
         <is>
@@ -6910,10 +6910,10 @@
         </is>
       </c>
       <c r="C137" t="n">
-        <v>1208</v>
+        <v>1210</v>
       </c>
       <c r="D137" t="n">
-        <v>1751071</v>
+        <v>1754071</v>
       </c>
       <c r="E137" t="inlineStr">
         <is>
@@ -6958,10 +6958,10 @@
         </is>
       </c>
       <c r="C138" t="n">
-        <v>3516</v>
+        <v>3518</v>
       </c>
       <c r="D138" t="n">
-        <v>5151999</v>
+        <v>5154999</v>
       </c>
       <c r="E138" t="inlineStr">
         <is>
@@ -7006,10 +7006,10 @@
         </is>
       </c>
       <c r="C139" t="n">
-        <v>1007</v>
+        <v>1009</v>
       </c>
       <c r="D139" t="n">
-        <v>1498524</v>
+        <v>1501524</v>
       </c>
       <c r="E139" t="inlineStr">
         <is>
@@ -7198,10 +7198,10 @@
         </is>
       </c>
       <c r="C143" t="n">
-        <v>1229</v>
+        <v>1232</v>
       </c>
       <c r="D143" t="n">
-        <v>1608015</v>
+        <v>1609809</v>
       </c>
       <c r="E143" t="inlineStr">
         <is>
@@ -7246,10 +7246,10 @@
         </is>
       </c>
       <c r="C144" t="n">
-        <v>2833</v>
+        <v>2835</v>
       </c>
       <c r="D144" t="n">
-        <v>4088614</v>
+        <v>4092242</v>
       </c>
       <c r="E144" t="inlineStr">
         <is>
@@ -7294,10 +7294,10 @@
         </is>
       </c>
       <c r="C145" t="n">
-        <v>6425</v>
+        <v>6428</v>
       </c>
       <c r="D145" t="n">
-        <v>9395842</v>
+        <v>9400342</v>
       </c>
       <c r="E145" t="inlineStr">
         <is>
@@ -7582,10 +7582,10 @@
         </is>
       </c>
       <c r="C151" t="n">
-        <v>3857</v>
+        <v>3859</v>
       </c>
       <c r="D151" t="n">
-        <v>5552682</v>
+        <v>5555682</v>
       </c>
       <c r="E151" t="inlineStr">
         <is>
@@ -7678,10 +7678,10 @@
         </is>
       </c>
       <c r="C153" t="n">
-        <v>3019</v>
+        <v>3021</v>
       </c>
       <c r="D153" t="n">
-        <v>4480446</v>
+        <v>4483446</v>
       </c>
       <c r="E153" t="inlineStr">
         <is>
@@ -7726,10 +7726,10 @@
         </is>
       </c>
       <c r="C154" t="n">
-        <v>763</v>
+        <v>765</v>
       </c>
       <c r="D154" t="n">
-        <v>1128032</v>
+        <v>1131032</v>
       </c>
       <c r="E154" t="inlineStr">
         <is>
@@ -7870,10 +7870,10 @@
         </is>
       </c>
       <c r="C157" t="n">
-        <v>3316</v>
+        <v>3321</v>
       </c>
       <c r="D157" t="n">
-        <v>4408064</v>
+        <v>4413229</v>
       </c>
       <c r="E157" t="inlineStr">
         <is>
@@ -7918,10 +7918,10 @@
         </is>
       </c>
       <c r="C158" t="n">
-        <v>3746</v>
+        <v>3747</v>
       </c>
       <c r="D158" t="n">
-        <v>5417031</v>
+        <v>5418531</v>
       </c>
       <c r="E158" t="inlineStr">
         <is>
@@ -7966,10 +7966,10 @@
         </is>
       </c>
       <c r="C159" t="n">
-        <v>10219</v>
+        <v>10225</v>
       </c>
       <c r="D159" t="n">
-        <v>15061346</v>
+        <v>15070124</v>
       </c>
       <c r="E159" t="inlineStr">
         <is>
@@ -8014,10 +8014,10 @@
         </is>
       </c>
       <c r="C160" t="n">
-        <v>3319</v>
+        <v>3326</v>
       </c>
       <c r="D160" t="n">
-        <v>4938560</v>
+        <v>4949406</v>
       </c>
       <c r="E160" t="inlineStr">
         <is>
@@ -8254,10 +8254,10 @@
         </is>
       </c>
       <c r="C165" t="n">
-        <v>4043</v>
+        <v>4047</v>
       </c>
       <c r="D165" t="n">
-        <v>5807423</v>
+        <v>5812363</v>
       </c>
       <c r="E165" t="inlineStr">
         <is>
@@ -8302,10 +8302,10 @@
         </is>
       </c>
       <c r="C166" t="n">
-        <v>8334</v>
+        <v>8335</v>
       </c>
       <c r="D166" t="n">
-        <v>12203597</v>
+        <v>12205097</v>
       </c>
       <c r="E166" t="inlineStr">
         <is>
@@ -8542,10 +8542,10 @@
         </is>
       </c>
       <c r="C171" t="n">
-        <v>3212</v>
+        <v>3213</v>
       </c>
       <c r="D171" t="n">
-        <v>4299946</v>
+        <v>4300099</v>
       </c>
       <c r="E171" t="inlineStr">
         <is>
@@ -8638,10 +8638,10 @@
         </is>
       </c>
       <c r="C173" t="n">
-        <v>2692</v>
+        <v>2693</v>
       </c>
       <c r="D173" t="n">
-        <v>3944304</v>
+        <v>3945804</v>
       </c>
       <c r="E173" t="inlineStr">
         <is>
@@ -8878,10 +8878,10 @@
         </is>
       </c>
       <c r="C178" t="n">
-        <v>1259</v>
+        <v>1261</v>
       </c>
       <c r="D178" t="n">
-        <v>1629646</v>
+        <v>1632646</v>
       </c>
       <c r="E178" t="inlineStr">
         <is>
@@ -8926,10 +8926,10 @@
         </is>
       </c>
       <c r="C179" t="n">
-        <v>1278</v>
+        <v>1279</v>
       </c>
       <c r="D179" t="n">
-        <v>1866396</v>
+        <v>1867752</v>
       </c>
       <c r="E179" t="inlineStr">
         <is>
@@ -8974,10 +8974,10 @@
         </is>
       </c>
       <c r="C180" t="n">
-        <v>3790</v>
+        <v>3794</v>
       </c>
       <c r="D180" t="n">
-        <v>5588664</v>
+        <v>5594664</v>
       </c>
       <c r="E180" t="inlineStr">
         <is>
@@ -9022,10 +9022,10 @@
         </is>
       </c>
       <c r="C181" t="n">
-        <v>1231</v>
+        <v>1232</v>
       </c>
       <c r="D181" t="n">
-        <v>1832307</v>
+        <v>1833807</v>
       </c>
       <c r="E181" t="inlineStr">
         <is>
@@ -9502,10 +9502,10 @@
         </is>
       </c>
       <c r="C191" t="n">
-        <v>943</v>
+        <v>944</v>
       </c>
       <c r="D191" t="n">
-        <v>1188100</v>
+        <v>1189600</v>
       </c>
       <c r="E191" t="inlineStr">
         <is>
@@ -9598,10 +9598,10 @@
         </is>
       </c>
       <c r="C193" t="n">
-        <v>6222</v>
+        <v>6226</v>
       </c>
       <c r="D193" t="n">
-        <v>9111631</v>
+        <v>9117631</v>
       </c>
       <c r="E193" t="inlineStr">
         <is>
@@ -9838,10 +9838,10 @@
         </is>
       </c>
       <c r="C198" t="n">
-        <v>2329</v>
+        <v>2331</v>
       </c>
       <c r="D198" t="n">
-        <v>3119575</v>
+        <v>3120262</v>
       </c>
       <c r="E198" t="inlineStr">
         <is>
@@ -9934,10 +9934,10 @@
         </is>
       </c>
       <c r="C200" t="n">
-        <v>6076</v>
+        <v>6080</v>
       </c>
       <c r="D200" t="n">
-        <v>8928406</v>
+        <v>8934039</v>
       </c>
       <c r="E200" t="inlineStr">
         <is>
@@ -10078,10 +10078,10 @@
         </is>
       </c>
       <c r="C203" t="n">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="D203" t="n">
-        <v>165000</v>
+        <v>166500</v>
       </c>
       <c r="E203" t="inlineStr">
         <is>
@@ -10174,10 +10174,10 @@
         </is>
       </c>
       <c r="C205" t="n">
-        <v>2048</v>
+        <v>2054</v>
       </c>
       <c r="D205" t="n">
-        <v>2680346</v>
+        <v>2687881</v>
       </c>
       <c r="E205" t="inlineStr">
         <is>
@@ -10222,10 +10222,10 @@
         </is>
       </c>
       <c r="C206" t="n">
-        <v>1111</v>
+        <v>1112</v>
       </c>
       <c r="D206" t="n">
-        <v>1600324</v>
+        <v>1601824</v>
       </c>
       <c r="E206" t="inlineStr">
         <is>
@@ -10270,10 +10270,10 @@
         </is>
       </c>
       <c r="C207" t="n">
-        <v>3379</v>
+        <v>3380</v>
       </c>
       <c r="D207" t="n">
-        <v>4958058</v>
+        <v>4959558</v>
       </c>
       <c r="E207" t="inlineStr">
         <is>
@@ -10510,10 +10510,10 @@
         </is>
       </c>
       <c r="C212" t="n">
-        <v>1193</v>
+        <v>1194</v>
       </c>
       <c r="D212" t="n">
-        <v>1592506</v>
+        <v>1592943</v>
       </c>
       <c r="E212" t="inlineStr">
         <is>
@@ -10558,10 +10558,10 @@
         </is>
       </c>
       <c r="C213" t="n">
-        <v>1108</v>
+        <v>1110</v>
       </c>
       <c r="D213" t="n">
-        <v>1585152</v>
+        <v>1587652</v>
       </c>
       <c r="E213" t="inlineStr">
         <is>
@@ -10606,10 +10606,10 @@
         </is>
       </c>
       <c r="C214" t="n">
-        <v>4079</v>
+        <v>4082</v>
       </c>
       <c r="D214" t="n">
-        <v>5961756</v>
+        <v>5964956</v>
       </c>
       <c r="E214" t="inlineStr">
         <is>
@@ -10702,10 +10702,10 @@
         </is>
       </c>
       <c r="C216" t="n">
-        <v>544</v>
+        <v>546</v>
       </c>
       <c r="D216" t="n">
-        <v>809809</v>
+        <v>812809</v>
       </c>
       <c r="E216" t="inlineStr">
         <is>
@@ -10942,10 +10942,10 @@
         </is>
       </c>
       <c r="C221" t="n">
-        <v>4552</v>
+        <v>4558</v>
       </c>
       <c r="D221" t="n">
-        <v>6649289</v>
+        <v>6658289</v>
       </c>
       <c r="E221" t="inlineStr">
         <is>
@@ -11134,10 +11134,10 @@
         </is>
       </c>
       <c r="C225" t="n">
-        <v>1879</v>
+        <v>1882</v>
       </c>
       <c r="D225" t="n">
-        <v>2546866</v>
+        <v>2550991</v>
       </c>
       <c r="E225" t="inlineStr">
         <is>
@@ -11230,10 +11230,10 @@
         </is>
       </c>
       <c r="C227" t="n">
-        <v>2429</v>
+        <v>2430</v>
       </c>
       <c r="D227" t="n">
-        <v>3533761</v>
+        <v>3535261</v>
       </c>
       <c r="E227" t="inlineStr">
         <is>
@@ -11614,10 +11614,10 @@
         </is>
       </c>
       <c r="C235" t="n">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="D235" t="n">
-        <v>364639</v>
+        <v>366139</v>
       </c>
       <c r="E235" t="inlineStr">
         <is>
@@ -11758,10 +11758,10 @@
         </is>
       </c>
       <c r="C238" t="n">
-        <v>4411</v>
+        <v>4413</v>
       </c>
       <c r="D238" t="n">
-        <v>6367816</v>
+        <v>6370816</v>
       </c>
       <c r="E238" t="inlineStr">
         <is>
@@ -11806,10 +11806,10 @@
         </is>
       </c>
       <c r="C239" t="n">
-        <v>13394</v>
+        <v>13403</v>
       </c>
       <c r="D239" t="n">
-        <v>19631457</v>
+        <v>19644957</v>
       </c>
       <c r="E239" t="inlineStr">
         <is>
@@ -11854,10 +11854,10 @@
         </is>
       </c>
       <c r="C240" t="n">
-        <v>5112</v>
+        <v>5113</v>
       </c>
       <c r="D240" t="n">
-        <v>7578924</v>
+        <v>7580424</v>
       </c>
       <c r="E240" t="inlineStr">
         <is>
@@ -11950,10 +11950,10 @@
         </is>
       </c>
       <c r="C242" t="n">
-        <v>401</v>
+        <v>402</v>
       </c>
       <c r="D242" t="n">
-        <v>598262</v>
+        <v>599762</v>
       </c>
       <c r="E242" t="inlineStr">
         <is>
@@ -12046,10 +12046,10 @@
         </is>
       </c>
       <c r="C244" t="n">
-        <v>3824</v>
+        <v>3827</v>
       </c>
       <c r="D244" t="n">
-        <v>5169186</v>
+        <v>5172386</v>
       </c>
       <c r="E244" t="inlineStr">
         <is>
@@ -12478,10 +12478,10 @@
         </is>
       </c>
       <c r="C253" t="n">
-        <v>8472</v>
+        <v>8476</v>
       </c>
       <c r="D253" t="n">
-        <v>12428242</v>
+        <v>12433042</v>
       </c>
       <c r="E253" t="inlineStr">
         <is>
@@ -12574,10 +12574,10 @@
         </is>
       </c>
       <c r="C255" t="n">
-        <v>944</v>
+        <v>945</v>
       </c>
       <c r="D255" t="n">
-        <v>1408775</v>
+        <v>1410275</v>
       </c>
       <c r="E255" t="inlineStr">
         <is>
@@ -12814,10 +12814,10 @@
         </is>
       </c>
       <c r="C260" t="n">
-        <v>2246</v>
+        <v>2248</v>
       </c>
       <c r="D260" t="n">
-        <v>2921824</v>
+        <v>2924566</v>
       </c>
       <c r="E260" t="inlineStr">
         <is>
@@ -12862,10 +12862,10 @@
         </is>
       </c>
       <c r="C261" t="n">
-        <v>1927</v>
+        <v>1929</v>
       </c>
       <c r="D261" t="n">
-        <v>2797924</v>
+        <v>2800924</v>
       </c>
       <c r="E261" t="inlineStr">
         <is>
@@ -12910,10 +12910,10 @@
         </is>
       </c>
       <c r="C262" t="n">
-        <v>5405</v>
+        <v>5412</v>
       </c>
       <c r="D262" t="n">
-        <v>7949873</v>
+        <v>7960373</v>
       </c>
       <c r="E262" t="inlineStr">
         <is>
@@ -12958,10 +12958,10 @@
         </is>
       </c>
       <c r="C263" t="n">
-        <v>1931</v>
+        <v>1932</v>
       </c>
       <c r="D263" t="n">
-        <v>2870105</v>
+        <v>2871605</v>
       </c>
       <c r="E263" t="inlineStr">
         <is>
@@ -13150,10 +13150,10 @@
         </is>
       </c>
       <c r="C267" t="n">
-        <v>2182</v>
+        <v>2185</v>
       </c>
       <c r="D267" t="n">
-        <v>2847149</v>
+        <v>2851649</v>
       </c>
       <c r="E267" t="inlineStr">
         <is>
@@ -13198,10 +13198,10 @@
         </is>
       </c>
       <c r="C268" t="n">
-        <v>2006</v>
+        <v>2008</v>
       </c>
       <c r="D268" t="n">
-        <v>2930031</v>
+        <v>2932458</v>
       </c>
       <c r="E268" t="inlineStr">
         <is>
@@ -13246,10 +13246,10 @@
         </is>
       </c>
       <c r="C269" t="n">
-        <v>5952</v>
+        <v>5953</v>
       </c>
       <c r="D269" t="n">
-        <v>8744492</v>
+        <v>8745992</v>
       </c>
       <c r="E269" t="inlineStr">
         <is>
@@ -13390,10 +13390,10 @@
         </is>
       </c>
       <c r="C272" t="n">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="D272" t="n">
-        <v>267682</v>
+        <v>269182</v>
       </c>
       <c r="E272" t="inlineStr">
         <is>
@@ -13774,10 +13774,10 @@
         </is>
       </c>
       <c r="C280" t="n">
-        <v>645</v>
+        <v>647</v>
       </c>
       <c r="D280" t="n">
-        <v>851381</v>
+        <v>852097</v>
       </c>
       <c r="E280" t="inlineStr">
         <is>
@@ -13822,10 +13822,10 @@
         </is>
       </c>
       <c r="C281" t="n">
-        <v>2861</v>
+        <v>2862</v>
       </c>
       <c r="D281" t="n">
-        <v>4127775</v>
+        <v>4129225</v>
       </c>
       <c r="E281" t="inlineStr">
         <is>
@@ -13870,10 +13870,10 @@
         </is>
       </c>
       <c r="C282" t="n">
-        <v>9120</v>
+        <v>9123</v>
       </c>
       <c r="D282" t="n">
-        <v>13357888</v>
+        <v>13360842</v>
       </c>
       <c r="E282" t="inlineStr">
         <is>
@@ -14158,10 +14158,10 @@
         </is>
       </c>
       <c r="C288" t="n">
-        <v>2576</v>
+        <v>2578</v>
       </c>
       <c r="D288" t="n">
-        <v>3424004</v>
+        <v>3426304</v>
       </c>
       <c r="E288" t="inlineStr">
         <is>
@@ -14254,10 +14254,10 @@
         </is>
       </c>
       <c r="C290" t="n">
-        <v>4227</v>
+        <v>4228</v>
       </c>
       <c r="D290" t="n">
-        <v>6186986</v>
+        <v>6187614</v>
       </c>
       <c r="E290" t="inlineStr">
         <is>
@@ -14494,10 +14494,10 @@
         </is>
       </c>
       <c r="C295" t="n">
-        <v>1760</v>
+        <v>1761</v>
       </c>
       <c r="D295" t="n">
-        <v>2313030</v>
+        <v>2314530</v>
       </c>
       <c r="E295" t="inlineStr">
         <is>
@@ -14590,10 +14590,10 @@
         </is>
       </c>
       <c r="C297" t="n">
-        <v>7981</v>
+        <v>7987</v>
       </c>
       <c r="D297" t="n">
-        <v>11723028</v>
+        <v>11732028</v>
       </c>
       <c r="E297" t="inlineStr">
         <is>
@@ -14638,10 +14638,10 @@
         </is>
       </c>
       <c r="C298" t="n">
-        <v>2675</v>
+        <v>2677</v>
       </c>
       <c r="D298" t="n">
-        <v>3992633</v>
+        <v>3995633</v>
       </c>
       <c r="E298" t="inlineStr">
         <is>
@@ -14686,10 +14686,10 @@
         </is>
       </c>
       <c r="C299" t="n">
-        <v>843</v>
+        <v>845</v>
       </c>
       <c r="D299" t="n">
-        <v>1259414</v>
+        <v>1262414</v>
       </c>
       <c r="E299" t="inlineStr">
         <is>
@@ -14830,10 +14830,10 @@
         </is>
       </c>
       <c r="C302" t="n">
-        <v>7953</v>
+        <v>7957</v>
       </c>
       <c r="D302" t="n">
-        <v>10941837</v>
+        <v>10947304</v>
       </c>
       <c r="E302" t="inlineStr">
         <is>
@@ -14878,10 +14878,10 @@
         </is>
       </c>
       <c r="C303" t="n">
-        <v>1650</v>
+        <v>1654</v>
       </c>
       <c r="D303" t="n">
-        <v>3316440</v>
+        <v>3326816</v>
       </c>
       <c r="E303" t="inlineStr">
         <is>
@@ -14926,10 +14926,10 @@
         </is>
       </c>
       <c r="C304" t="n">
-        <v>3939</v>
+        <v>3944</v>
       </c>
       <c r="D304" t="n">
-        <v>7882312</v>
+        <v>7897312</v>
       </c>
       <c r="E304" t="inlineStr">
         <is>
@@ -14974,10 +14974,10 @@
         </is>
       </c>
       <c r="C305" t="n">
-        <v>1557</v>
+        <v>1560</v>
       </c>
       <c r="D305" t="n">
-        <v>3121294</v>
+        <v>3130126</v>
       </c>
       <c r="E305" t="inlineStr">
         <is>
@@ -15022,10 +15022,10 @@
         </is>
       </c>
       <c r="C306" t="n">
-        <v>528</v>
+        <v>531</v>
       </c>
       <c r="D306" t="n">
-        <v>1053083</v>
+        <v>1059083</v>
       </c>
       <c r="E306" t="inlineStr">
         <is>
@@ -15070,10 +15070,10 @@
         </is>
       </c>
       <c r="C307" t="n">
-        <v>191</v>
+        <v>193</v>
       </c>
       <c r="D307" t="n">
-        <v>394487</v>
+        <v>397487</v>
       </c>
       <c r="E307" t="inlineStr">
         <is>
@@ -15166,10 +15166,10 @@
         </is>
       </c>
       <c r="C309" t="n">
-        <v>2561</v>
+        <v>2568</v>
       </c>
       <c r="D309" t="n">
-        <v>4752864</v>
+        <v>4769464</v>
       </c>
       <c r="E309" t="inlineStr">
         <is>
@@ -15262,10 +15262,10 @@
         </is>
       </c>
       <c r="C311" t="n">
-        <v>3851</v>
+        <v>3852</v>
       </c>
       <c r="D311" t="n">
-        <v>5638250</v>
+        <v>5639750</v>
       </c>
       <c r="E311" t="inlineStr">
         <is>
@@ -15598,10 +15598,10 @@
         </is>
       </c>
       <c r="C318" t="n">
-        <v>7850</v>
+        <v>7861</v>
       </c>
       <c r="D318" t="n">
-        <v>11318907</v>
+        <v>11335905</v>
       </c>
       <c r="E318" t="inlineStr">
         <is>
@@ -15646,10 +15646,10 @@
         </is>
       </c>
       <c r="C319" t="n">
-        <v>21389</v>
+        <v>21414</v>
       </c>
       <c r="D319" t="n">
-        <v>31254764</v>
+        <v>31291001</v>
       </c>
       <c r="E319" t="inlineStr">
         <is>
@@ -15694,10 +15694,10 @@
         </is>
       </c>
       <c r="C320" t="n">
-        <v>7600</v>
+        <v>7604</v>
       </c>
       <c r="D320" t="n">
-        <v>11308850</v>
+        <v>11315348</v>
       </c>
       <c r="E320" t="inlineStr">
         <is>
@@ -15742,10 +15742,10 @@
         </is>
       </c>
       <c r="C321" t="n">
-        <v>2323</v>
+        <v>2325</v>
       </c>
       <c r="D321" t="n">
-        <v>3466362</v>
+        <v>3469362</v>
       </c>
       <c r="E321" t="inlineStr">
         <is>
@@ -15790,10 +15790,10 @@
         </is>
       </c>
       <c r="C322" t="n">
-        <v>563</v>
+        <v>564</v>
       </c>
       <c r="D322" t="n">
-        <v>838439</v>
+        <v>839939</v>
       </c>
       <c r="E322" t="inlineStr">
         <is>
@@ -15934,10 +15934,10 @@
         </is>
       </c>
       <c r="C325" t="n">
-        <v>6669</v>
+        <v>6673</v>
       </c>
       <c r="D325" t="n">
-        <v>8742465</v>
+        <v>8748465</v>
       </c>
       <c r="E325" t="inlineStr">
         <is>
@@ -15982,10 +15982,10 @@
         </is>
       </c>
       <c r="C326" t="n">
-        <v>2301</v>
+        <v>2303</v>
       </c>
       <c r="D326" t="n">
-        <v>3368843</v>
+        <v>3371843</v>
       </c>
       <c r="E326" t="inlineStr">
         <is>
@@ -16030,10 +16030,10 @@
         </is>
       </c>
       <c r="C327" t="n">
-        <v>7106</v>
+        <v>7110</v>
       </c>
       <c r="D327" t="n">
-        <v>10433922</v>
+        <v>10439922</v>
       </c>
       <c r="E327" t="inlineStr">
         <is>
@@ -16078,10 +16078,10 @@
         </is>
       </c>
       <c r="C328" t="n">
-        <v>2440</v>
+        <v>2442</v>
       </c>
       <c r="D328" t="n">
-        <v>3628902</v>
+        <v>3631892</v>
       </c>
       <c r="E328" t="inlineStr">
         <is>
@@ -16270,10 +16270,10 @@
         </is>
       </c>
       <c r="C332" t="n">
-        <v>2110</v>
+        <v>2111</v>
       </c>
       <c r="D332" t="n">
-        <v>2856294</v>
+        <v>2856572</v>
       </c>
       <c r="E332" t="inlineStr">
         <is>
@@ -16366,10 +16366,10 @@
         </is>
       </c>
       <c r="C334" t="n">
-        <v>11411</v>
+        <v>11415</v>
       </c>
       <c r="D334" t="n">
-        <v>16653376</v>
+        <v>16658710</v>
       </c>
       <c r="E334" t="inlineStr">
         <is>
@@ -16414,10 +16414,10 @@
         </is>
       </c>
       <c r="C335" t="n">
-        <v>3671</v>
+        <v>3672</v>
       </c>
       <c r="D335" t="n">
-        <v>5446521</v>
+        <v>5448021</v>
       </c>
       <c r="E335" t="inlineStr">
         <is>
@@ -16462,10 +16462,10 @@
         </is>
       </c>
       <c r="C336" t="n">
-        <v>1162</v>
+        <v>1164</v>
       </c>
       <c r="D336" t="n">
-        <v>1727284</v>
+        <v>1730284</v>
       </c>
       <c r="E336" t="inlineStr">
         <is>
@@ -16510,10 +16510,10 @@
         </is>
       </c>
       <c r="C337" t="n">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="D337" t="n">
-        <v>315849</v>
+        <v>317349</v>
       </c>
       <c r="E337" t="inlineStr">
         <is>
@@ -16654,10 +16654,10 @@
         </is>
       </c>
       <c r="C340" t="n">
-        <v>4034</v>
+        <v>4035</v>
       </c>
       <c r="D340" t="n">
-        <v>5236255</v>
+        <v>5237024</v>
       </c>
       <c r="E340" t="inlineStr">
         <is>
@@ -16750,10 +16750,10 @@
         </is>
       </c>
       <c r="C342" t="n">
-        <v>4552</v>
+        <v>4557</v>
       </c>
       <c r="D342" t="n">
-        <v>6636689</v>
+        <v>6643089</v>
       </c>
       <c r="E342" t="inlineStr">
         <is>
@@ -16798,10 +16798,10 @@
         </is>
       </c>
       <c r="C343" t="n">
-        <v>1724</v>
+        <v>1725</v>
       </c>
       <c r="D343" t="n">
-        <v>2562528</v>
+        <v>2564028</v>
       </c>
       <c r="E343" t="inlineStr">
         <is>
@@ -16846,10 +16846,10 @@
         </is>
       </c>
       <c r="C344" t="n">
-        <v>423</v>
+        <v>425</v>
       </c>
       <c r="D344" t="n">
-        <v>621589</v>
+        <v>624589</v>
       </c>
       <c r="E344" t="inlineStr">
         <is>
@@ -17086,10 +17086,10 @@
         </is>
       </c>
       <c r="C349" t="n">
-        <v>11701</v>
+        <v>11708</v>
       </c>
       <c r="D349" t="n">
-        <v>17251572</v>
+        <v>17260335</v>
       </c>
       <c r="E349" t="inlineStr">
         <is>
@@ -17134,10 +17134,10 @@
         </is>
       </c>
       <c r="C350" t="n">
-        <v>4343</v>
+        <v>4344</v>
       </c>
       <c r="D350" t="n">
-        <v>6463857</v>
+        <v>6465357</v>
       </c>
       <c r="E350" t="inlineStr">
         <is>
@@ -17182,10 +17182,10 @@
         </is>
       </c>
       <c r="C351" t="n">
-        <v>1296</v>
+        <v>1297</v>
       </c>
       <c r="D351" t="n">
-        <v>1935679</v>
+        <v>1937179</v>
       </c>
       <c r="E351" t="inlineStr">
         <is>
@@ -17422,10 +17422,10 @@
         </is>
       </c>
       <c r="C356" t="n">
-        <v>4013</v>
+        <v>4021</v>
       </c>
       <c r="D356" t="n">
-        <v>5521468</v>
+        <v>5531134</v>
       </c>
       <c r="E356" t="inlineStr">
         <is>
@@ -17470,10 +17470,10 @@
         </is>
       </c>
       <c r="C357" t="n">
-        <v>8105</v>
+        <v>8111</v>
       </c>
       <c r="D357" t="n">
-        <v>11787671</v>
+        <v>11795076</v>
       </c>
       <c r="E357" t="inlineStr">
         <is>
@@ -17518,10 +17518,10 @@
         </is>
       </c>
       <c r="C358" t="n">
-        <v>18695</v>
+        <v>18710</v>
       </c>
       <c r="D358" t="n">
-        <v>27513532</v>
+        <v>27536351</v>
       </c>
       <c r="E358" t="inlineStr">
         <is>
@@ -17566,10 +17566,10 @@
         </is>
       </c>
       <c r="C359" t="n">
-        <v>7990</v>
+        <v>7998</v>
       </c>
       <c r="D359" t="n">
-        <v>11909753</v>
+        <v>11921341</v>
       </c>
       <c r="E359" t="inlineStr">
         <is>
@@ -17614,10 +17614,10 @@
         </is>
       </c>
       <c r="C360" t="n">
-        <v>2413</v>
+        <v>2416</v>
       </c>
       <c r="D360" t="n">
-        <v>3602739</v>
+        <v>3607239</v>
       </c>
       <c r="E360" t="inlineStr">
         <is>
@@ -17662,10 +17662,10 @@
         </is>
       </c>
       <c r="C361" t="n">
-        <v>579</v>
+        <v>580</v>
       </c>
       <c r="D361" t="n">
-        <v>861211</v>
+        <v>862711</v>
       </c>
       <c r="E361" t="inlineStr">
         <is>
@@ -17710,10 +17710,10 @@
         </is>
       </c>
       <c r="C362" t="n">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="D362" t="n">
-        <v>62803</v>
+        <v>64801</v>
       </c>
       <c r="E362" t="inlineStr">
         <is>
@@ -17758,10 +17758,10 @@
         </is>
       </c>
       <c r="C363" t="n">
-        <v>6955</v>
+        <v>6965</v>
       </c>
       <c r="D363" t="n">
-        <v>9422524</v>
+        <v>9437018</v>
       </c>
       <c r="E363" t="inlineStr">
         <is>
@@ -17806,10 +17806,10 @@
         </is>
       </c>
       <c r="C364" t="n">
-        <v>23061</v>
+        <v>23089</v>
       </c>
       <c r="D364" t="n">
-        <v>33439477</v>
+        <v>33480824</v>
       </c>
       <c r="E364" t="inlineStr">
         <is>
@@ -17854,10 +17854,10 @@
         </is>
       </c>
       <c r="C365" t="n">
-        <v>61401</v>
+        <v>61472</v>
       </c>
       <c r="D365" t="n">
-        <v>90356842</v>
+        <v>90461362</v>
       </c>
       <c r="E365" t="inlineStr">
         <is>
@@ -17902,10 +17902,10 @@
         </is>
       </c>
       <c r="C366" t="n">
-        <v>29046</v>
+        <v>29089</v>
       </c>
       <c r="D366" t="n">
-        <v>43300534</v>
+        <v>43364478</v>
       </c>
       <c r="E366" t="inlineStr">
         <is>
@@ -17950,10 +17950,10 @@
         </is>
       </c>
       <c r="C367" t="n">
-        <v>10881</v>
+        <v>10905</v>
       </c>
       <c r="D367" t="n">
-        <v>16258687</v>
+        <v>16294687</v>
       </c>
       <c r="E367" t="inlineStr">
         <is>
@@ -17998,10 +17998,10 @@
         </is>
       </c>
       <c r="C368" t="n">
-        <v>3111</v>
+        <v>3126</v>
       </c>
       <c r="D368" t="n">
-        <v>4643473</v>
+        <v>4665973</v>
       </c>
       <c r="E368" t="inlineStr">
         <is>
@@ -18046,10 +18046,10 @@
         </is>
       </c>
       <c r="C369" t="n">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="D369" t="n">
-        <v>344488</v>
+        <v>345988</v>
       </c>
       <c r="E369" t="inlineStr">
         <is>
@@ -18286,10 +18286,10 @@
         </is>
       </c>
       <c r="C374" t="n">
-        <v>22566</v>
+        <v>22599</v>
       </c>
       <c r="D374" t="n">
-        <v>30288489</v>
+        <v>30333320</v>
       </c>
       <c r="E374" t="inlineStr">
         <is>
@@ -18334,10 +18334,10 @@
         </is>
       </c>
       <c r="C375" t="n">
-        <v>5135</v>
+        <v>5138</v>
       </c>
       <c r="D375" t="n">
-        <v>7467429</v>
+        <v>7471929</v>
       </c>
       <c r="E375" t="inlineStr">
         <is>
@@ -18382,10 +18382,10 @@
         </is>
       </c>
       <c r="C376" t="n">
-        <v>13718</v>
+        <v>13730</v>
       </c>
       <c r="D376" t="n">
-        <v>20146005</v>
+        <v>20162519</v>
       </c>
       <c r="E376" t="inlineStr">
         <is>
@@ -18430,10 +18430,10 @@
         </is>
       </c>
       <c r="C377" t="n">
-        <v>5070</v>
+        <v>5076</v>
       </c>
       <c r="D377" t="n">
-        <v>7529454</v>
+        <v>7538454</v>
       </c>
       <c r="E377" t="inlineStr">
         <is>
@@ -18478,10 +18478,10 @@
         </is>
       </c>
       <c r="C378" t="n">
-        <v>1559</v>
+        <v>1560</v>
       </c>
       <c r="D378" t="n">
-        <v>2328481</v>
+        <v>2329981</v>
       </c>
       <c r="E378" t="inlineStr">
         <is>
@@ -18526,10 +18526,10 @@
         </is>
       </c>
       <c r="C379" t="n">
-        <v>330</v>
+        <v>331</v>
       </c>
       <c r="D379" t="n">
-        <v>493020</v>
+        <v>494520</v>
       </c>
       <c r="E379" t="inlineStr">
         <is>
@@ -18622,10 +18622,10 @@
         </is>
       </c>
       <c r="C381" t="n">
-        <v>5292</v>
+        <v>5297</v>
       </c>
       <c r="D381" t="n">
-        <v>7169952</v>
+        <v>7176302</v>
       </c>
       <c r="E381" t="inlineStr">
         <is>
@@ -18670,10 +18670,10 @@
         </is>
       </c>
       <c r="C382" t="n">
-        <v>6892</v>
+        <v>6896</v>
       </c>
       <c r="D382" t="n">
-        <v>9999755</v>
+        <v>10005755</v>
       </c>
       <c r="E382" t="inlineStr">
         <is>
@@ -18718,10 +18718,10 @@
         </is>
       </c>
       <c r="C383" t="n">
-        <v>22733</v>
+        <v>22748</v>
       </c>
       <c r="D383" t="n">
-        <v>33452213</v>
+        <v>33474436</v>
       </c>
       <c r="E383" t="inlineStr">
         <is>
@@ -18766,10 +18766,10 @@
         </is>
       </c>
       <c r="C384" t="n">
-        <v>9917</v>
+        <v>9928</v>
       </c>
       <c r="D384" t="n">
-        <v>14767413</v>
+        <v>14783913</v>
       </c>
       <c r="E384" t="inlineStr">
         <is>
@@ -18814,10 +18814,10 @@
         </is>
       </c>
       <c r="C385" t="n">
-        <v>2747</v>
+        <v>2753</v>
       </c>
       <c r="D385" t="n">
-        <v>4105466</v>
+        <v>4114466</v>
       </c>
       <c r="E385" t="inlineStr">
         <is>
@@ -18958,10 +18958,10 @@
         </is>
       </c>
       <c r="C388" t="n">
-        <v>7129</v>
+        <v>7138</v>
       </c>
       <c r="D388" t="n">
-        <v>9561489</v>
+        <v>9572634</v>
       </c>
       <c r="E388" t="inlineStr">
         <is>
@@ -19006,10 +19006,10 @@
         </is>
       </c>
       <c r="C389" t="n">
-        <v>5928</v>
+        <v>5934</v>
       </c>
       <c r="D389" t="n">
-        <v>8640721</v>
+        <v>8649721</v>
       </c>
       <c r="E389" t="inlineStr">
         <is>
@@ -19054,10 +19054,10 @@
         </is>
       </c>
       <c r="C390" t="n">
-        <v>16300</v>
+        <v>16315</v>
       </c>
       <c r="D390" t="n">
-        <v>23964429</v>
+        <v>23982807</v>
       </c>
       <c r="E390" t="inlineStr">
         <is>
@@ -19102,10 +19102,10 @@
         </is>
       </c>
       <c r="C391" t="n">
-        <v>6403</v>
+        <v>6408</v>
       </c>
       <c r="D391" t="n">
-        <v>9528745</v>
+        <v>9536245</v>
       </c>
       <c r="E391" t="inlineStr">
         <is>
@@ -19198,10 +19198,10 @@
         </is>
       </c>
       <c r="C393" t="n">
-        <v>474</v>
+        <v>475</v>
       </c>
       <c r="D393" t="n">
-        <v>707282</v>
+        <v>708782</v>
       </c>
       <c r="E393" t="inlineStr">
         <is>
@@ -19342,10 +19342,10 @@
         </is>
       </c>
       <c r="C396" t="n">
-        <v>6238</v>
+        <v>6251</v>
       </c>
       <c r="D396" t="n">
-        <v>8397202</v>
+        <v>8411043</v>
       </c>
       <c r="E396" t="inlineStr">
         <is>
@@ -19390,10 +19390,10 @@
         </is>
       </c>
       <c r="C397" t="n">
-        <v>4447</v>
+        <v>4451</v>
       </c>
       <c r="D397" t="n">
-        <v>6476594</v>
+        <v>6482594</v>
       </c>
       <c r="E397" t="inlineStr">
         <is>
@@ -19438,10 +19438,10 @@
         </is>
       </c>
       <c r="C398" t="n">
-        <v>13340</v>
+        <v>13344</v>
       </c>
       <c r="D398" t="n">
-        <v>19653604</v>
+        <v>19659604</v>
       </c>
       <c r="E398" t="inlineStr">
         <is>
@@ -19486,10 +19486,10 @@
         </is>
       </c>
       <c r="C399" t="n">
-        <v>5297</v>
+        <v>5302</v>
       </c>
       <c r="D399" t="n">
-        <v>7876310</v>
+        <v>7883810</v>
       </c>
       <c r="E399" t="inlineStr">
         <is>
@@ -19582,10 +19582,10 @@
         </is>
       </c>
       <c r="C401" t="n">
-        <v>360</v>
+        <v>361</v>
       </c>
       <c r="D401" t="n">
-        <v>537053</v>
+        <v>538553</v>
       </c>
       <c r="E401" t="inlineStr">
         <is>
@@ -19726,10 +19726,10 @@
         </is>
       </c>
       <c r="C404" t="n">
-        <v>4691</v>
+        <v>4696</v>
       </c>
       <c r="D404" t="n">
-        <v>6263066</v>
+        <v>6268306</v>
       </c>
       <c r="E404" t="inlineStr">
         <is>
@@ -19774,10 +19774,10 @@
         </is>
       </c>
       <c r="C405" t="n">
-        <v>4750</v>
+        <v>4752</v>
       </c>
       <c r="D405" t="n">
-        <v>6922726</v>
+        <v>6925891</v>
       </c>
       <c r="E405" t="inlineStr">
         <is>
@@ -19822,10 +19822,10 @@
         </is>
       </c>
       <c r="C406" t="n">
-        <v>12432</v>
+        <v>12437</v>
       </c>
       <c r="D406" t="n">
-        <v>18305241</v>
+        <v>18312573</v>
       </c>
       <c r="E406" t="inlineStr">
         <is>
@@ -19870,10 +19870,10 @@
         </is>
       </c>
       <c r="C407" t="n">
-        <v>4706</v>
+        <v>4711</v>
       </c>
       <c r="D407" t="n">
-        <v>7000466</v>
+        <v>7007966</v>
       </c>
       <c r="E407" t="inlineStr">
         <is>
@@ -19918,10 +19918,10 @@
         </is>
       </c>
       <c r="C408" t="n">
-        <v>1524</v>
+        <v>1527</v>
       </c>
       <c r="D408" t="n">
-        <v>2278086</v>
+        <v>2282586</v>
       </c>
       <c r="E408" t="inlineStr">
         <is>
@@ -20062,10 +20062,10 @@
         </is>
       </c>
       <c r="C411" t="n">
-        <v>4678</v>
+        <v>4681</v>
       </c>
       <c r="D411" t="n">
-        <v>6379321</v>
+        <v>6383821</v>
       </c>
       <c r="E411" t="inlineStr">
         <is>
@@ -20110,10 +20110,10 @@
         </is>
       </c>
       <c r="C412" t="n">
-        <v>5133</v>
+        <v>5134</v>
       </c>
       <c r="D412" t="n">
-        <v>7435873</v>
+        <v>7437373</v>
       </c>
       <c r="E412" t="inlineStr">
         <is>
@@ -20158,10 +20158,10 @@
         </is>
       </c>
       <c r="C413" t="n">
-        <v>12616</v>
+        <v>12619</v>
       </c>
       <c r="D413" t="n">
-        <v>18525814</v>
+        <v>18530221</v>
       </c>
       <c r="E413" t="inlineStr">
         <is>
@@ -20206,10 +20206,10 @@
         </is>
       </c>
       <c r="C414" t="n">
-        <v>4136</v>
+        <v>4137</v>
       </c>
       <c r="D414" t="n">
-        <v>6163126</v>
+        <v>6164626</v>
       </c>
       <c r="E414" t="inlineStr">
         <is>
@@ -20254,10 +20254,10 @@
         </is>
       </c>
       <c r="C415" t="n">
-        <v>1455</v>
+        <v>1456</v>
       </c>
       <c r="D415" t="n">
-        <v>2173611</v>
+        <v>2175111</v>
       </c>
       <c r="E415" t="inlineStr">
         <is>
@@ -20302,10 +20302,10 @@
         </is>
       </c>
       <c r="C416" t="n">
-        <v>349</v>
+        <v>350</v>
       </c>
       <c r="D416" t="n">
-        <v>520012</v>
+        <v>521512</v>
       </c>
       <c r="E416" t="inlineStr">
         <is>
@@ -20350,10 +20350,10 @@
         </is>
       </c>
       <c r="C417" t="n">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D417" t="n">
-        <v>47902</v>
+        <v>49402</v>
       </c>
       <c r="E417" t="inlineStr">
         <is>
@@ -20446,10 +20446,10 @@
         </is>
       </c>
       <c r="C419" t="n">
-        <v>5874</v>
+        <v>5879</v>
       </c>
       <c r="D419" t="n">
-        <v>7877874</v>
+        <v>7885374</v>
       </c>
       <c r="E419" t="inlineStr">
         <is>
@@ -20494,10 +20494,10 @@
         </is>
       </c>
       <c r="C420" t="n">
-        <v>1849</v>
+        <v>1851</v>
       </c>
       <c r="D420" t="n">
-        <v>2661993</v>
+        <v>2664993</v>
       </c>
       <c r="E420" t="inlineStr">
         <is>
@@ -20542,10 +20542,10 @@
         </is>
       </c>
       <c r="C421" t="n">
-        <v>5865</v>
+        <v>5876</v>
       </c>
       <c r="D421" t="n">
-        <v>8642757</v>
+        <v>8658589</v>
       </c>
       <c r="E421" t="inlineStr">
         <is>
@@ -20830,10 +20830,10 @@
         </is>
       </c>
       <c r="C427" t="n">
-        <v>3984</v>
+        <v>3989</v>
       </c>
       <c r="D427" t="n">
-        <v>5280363</v>
+        <v>5286563</v>
       </c>
       <c r="E427" t="inlineStr">
         <is>
@@ -21118,10 +21118,10 @@
         </is>
       </c>
       <c r="C433" t="n">
-        <v>3397</v>
+        <v>3398</v>
       </c>
       <c r="D433" t="n">
-        <v>4919082</v>
+        <v>4920582</v>
       </c>
       <c r="E433" t="inlineStr">
         <is>
@@ -21166,10 +21166,10 @@
         </is>
       </c>
       <c r="C434" t="n">
-        <v>7826</v>
+        <v>7828</v>
       </c>
       <c r="D434" t="n">
-        <v>11464610</v>
+        <v>11467610</v>
       </c>
       <c r="E434" t="inlineStr">
         <is>
@@ -21214,10 +21214,10 @@
         </is>
       </c>
       <c r="C435" t="n">
-        <v>2627</v>
+        <v>2628</v>
       </c>
       <c r="D435" t="n">
-        <v>3916892</v>
+        <v>3918392</v>
       </c>
       <c r="E435" t="inlineStr">
         <is>
@@ -21358,10 +21358,10 @@
         </is>
       </c>
       <c r="C438" t="n">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D438" t="n">
-        <v>28500</v>
+        <v>30000</v>
       </c>
       <c r="E438" t="inlineStr">
         <is>
@@ -21406,10 +21406,10 @@
         </is>
       </c>
       <c r="C439" t="n">
-        <v>2580</v>
+        <v>2582</v>
       </c>
       <c r="D439" t="n">
-        <v>3429701</v>
+        <v>3432701</v>
       </c>
       <c r="E439" t="inlineStr">
         <is>
@@ -21454,10 +21454,10 @@
         </is>
       </c>
       <c r="C440" t="n">
-        <v>1952</v>
+        <v>1954</v>
       </c>
       <c r="D440" t="n">
-        <v>2830282</v>
+        <v>2833582</v>
       </c>
       <c r="E440" t="inlineStr">
         <is>
@@ -21502,10 +21502,10 @@
         </is>
       </c>
       <c r="C441" t="n">
-        <v>5239</v>
+        <v>5240</v>
       </c>
       <c r="D441" t="n">
-        <v>7688113</v>
+        <v>7689613</v>
       </c>
       <c r="E441" t="inlineStr">
         <is>
@@ -21550,10 +21550,10 @@
         </is>
       </c>
       <c r="C442" t="n">
-        <v>1715</v>
+        <v>1717</v>
       </c>
       <c r="D442" t="n">
-        <v>2552660</v>
+        <v>2555660</v>
       </c>
       <c r="E442" t="inlineStr">
         <is>
@@ -21790,10 +21790,10 @@
         </is>
       </c>
       <c r="C447" t="n">
-        <v>1810</v>
+        <v>1811</v>
       </c>
       <c r="D447" t="n">
-        <v>2367486</v>
+        <v>2368986</v>
       </c>
       <c r="E447" t="inlineStr">
         <is>
@@ -21838,10 +21838,10 @@
         </is>
       </c>
       <c r="C448" t="n">
-        <v>2172</v>
+        <v>2176</v>
       </c>
       <c r="D448" t="n">
-        <v>3129551</v>
+        <v>3134095</v>
       </c>
       <c r="E448" t="inlineStr">
         <is>
@@ -21886,10 +21886,10 @@
         </is>
       </c>
       <c r="C449" t="n">
-        <v>5152</v>
+        <v>5154</v>
       </c>
       <c r="D449" t="n">
-        <v>7560488</v>
+        <v>7563181</v>
       </c>
       <c r="E449" t="inlineStr">
         <is>
@@ -22510,10 +22510,10 @@
         </is>
       </c>
       <c r="C462" t="n">
-        <v>10077</v>
+        <v>10085</v>
       </c>
       <c r="D462" t="n">
-        <v>14817372</v>
+        <v>14829372</v>
       </c>
       <c r="E462" t="inlineStr">
         <is>
@@ -22558,10 +22558,10 @@
         </is>
       </c>
       <c r="C463" t="n">
-        <v>3641</v>
+        <v>3645</v>
       </c>
       <c r="D463" t="n">
-        <v>5410665</v>
+        <v>5416665</v>
       </c>
       <c r="E463" t="inlineStr">
         <is>
@@ -22606,10 +22606,10 @@
         </is>
       </c>
       <c r="C464" t="n">
-        <v>1013</v>
+        <v>1017</v>
       </c>
       <c r="D464" t="n">
-        <v>1512042</v>
+        <v>1518042</v>
       </c>
       <c r="E464" t="inlineStr">
         <is>
@@ -22750,10 +22750,10 @@
         </is>
       </c>
       <c r="C467" t="n">
-        <v>3215</v>
+        <v>3216</v>
       </c>
       <c r="D467" t="n">
-        <v>4184164</v>
+        <v>4185387</v>
       </c>
       <c r="E467" t="inlineStr">
         <is>
@@ -23134,10 +23134,10 @@
         </is>
       </c>
       <c r="C475" t="n">
-        <v>4736</v>
+        <v>4738</v>
       </c>
       <c r="D475" t="n">
-        <v>6849775</v>
+        <v>6852775</v>
       </c>
       <c r="E475" t="inlineStr">
         <is>
@@ -23182,10 +23182,10 @@
         </is>
       </c>
       <c r="C476" t="n">
-        <v>8627</v>
+        <v>8630</v>
       </c>
       <c r="D476" t="n">
-        <v>12637536</v>
+        <v>12641018</v>
       </c>
       <c r="E476" t="inlineStr">
         <is>
@@ -23230,10 +23230,10 @@
         </is>
       </c>
       <c r="C477" t="n">
-        <v>2504</v>
+        <v>2505</v>
       </c>
       <c r="D477" t="n">
-        <v>3724648</v>
+        <v>3726148</v>
       </c>
       <c r="E477" t="inlineStr">
         <is>
@@ -23470,10 +23470,10 @@
         </is>
       </c>
       <c r="C482" t="n">
-        <v>1145</v>
+        <v>1148</v>
       </c>
       <c r="D482" t="n">
-        <v>1653210</v>
+        <v>1657710</v>
       </c>
       <c r="E482" t="inlineStr">
         <is>
@@ -23710,10 +23710,10 @@
         </is>
       </c>
       <c r="C487" t="n">
-        <v>1488</v>
+        <v>1490</v>
       </c>
       <c r="D487" t="n">
-        <v>1977831</v>
+        <v>1980067</v>
       </c>
       <c r="E487" t="inlineStr">
         <is>
@@ -23806,10 +23806,10 @@
         </is>
       </c>
       <c r="C489" t="n">
-        <v>1154</v>
+        <v>1156</v>
       </c>
       <c r="D489" t="n">
-        <v>1662792</v>
+        <v>1665792</v>
       </c>
       <c r="E489" t="inlineStr">
         <is>
@@ -24094,10 +24094,10 @@
         </is>
       </c>
       <c r="C495" t="n">
-        <v>3052</v>
+        <v>3053</v>
       </c>
       <c r="D495" t="n">
-        <v>4499780</v>
+        <v>4501280</v>
       </c>
       <c r="E495" t="inlineStr">
         <is>
@@ -24286,10 +24286,10 @@
         </is>
       </c>
       <c r="C499" t="n">
-        <v>1122</v>
+        <v>1125</v>
       </c>
       <c r="D499" t="n">
-        <v>1517991</v>
+        <v>1522065</v>
       </c>
       <c r="E499" t="inlineStr">
         <is>
@@ -24334,10 +24334,10 @@
         </is>
       </c>
       <c r="C500" t="n">
-        <v>3086</v>
+        <v>3089</v>
       </c>
       <c r="D500" t="n">
-        <v>4406057</v>
+        <v>4410557</v>
       </c>
       <c r="E500" t="inlineStr">
         <is>
@@ -24382,10 +24382,10 @@
         </is>
       </c>
       <c r="C501" t="n">
-        <v>5653</v>
+        <v>5655</v>
       </c>
       <c r="D501" t="n">
-        <v>8271965</v>
+        <v>8274965</v>
       </c>
       <c r="E501" t="inlineStr">
         <is>
@@ -24430,10 +24430,10 @@
         </is>
       </c>
       <c r="C502" t="n">
-        <v>1602</v>
+        <v>1603</v>
       </c>
       <c r="D502" t="n">
-        <v>2373409</v>
+        <v>2374909</v>
       </c>
       <c r="E502" t="inlineStr">
         <is>
@@ -24622,10 +24622,10 @@
         </is>
       </c>
       <c r="C506" t="n">
-        <v>2542</v>
+        <v>2545</v>
       </c>
       <c r="D506" t="n">
-        <v>3327652</v>
+        <v>3331452</v>
       </c>
       <c r="E506" t="inlineStr">
         <is>
@@ -24670,10 +24670,10 @@
         </is>
       </c>
       <c r="C507" t="n">
-        <v>9824</v>
+        <v>9838</v>
       </c>
       <c r="D507" t="n">
-        <v>14224983</v>
+        <v>14243632</v>
       </c>
       <c r="E507" t="inlineStr">
         <is>
@@ -24718,10 +24718,10 @@
         </is>
       </c>
       <c r="C508" t="n">
-        <v>20204</v>
+        <v>20215</v>
       </c>
       <c r="D508" t="n">
-        <v>29550119</v>
+        <v>29564255</v>
       </c>
       <c r="E508" t="inlineStr">
         <is>
@@ -24766,10 +24766,10 @@
         </is>
       </c>
       <c r="C509" t="n">
-        <v>6831</v>
+        <v>6835</v>
       </c>
       <c r="D509" t="n">
-        <v>10148783</v>
+        <v>10153335</v>
       </c>
       <c r="E509" t="inlineStr">
         <is>
@@ -24814,10 +24814,10 @@
         </is>
       </c>
       <c r="C510" t="n">
-        <v>2168</v>
+        <v>2169</v>
       </c>
       <c r="D510" t="n">
-        <v>3227857</v>
+        <v>3229357</v>
       </c>
       <c r="E510" t="inlineStr">
         <is>
@@ -24862,10 +24862,10 @@
         </is>
       </c>
       <c r="C511" t="n">
-        <v>487</v>
+        <v>488</v>
       </c>
       <c r="D511" t="n">
-        <v>729818</v>
+        <v>731318</v>
       </c>
       <c r="E511" t="inlineStr">
         <is>
@@ -25054,10 +25054,10 @@
         </is>
       </c>
       <c r="C515" t="n">
-        <v>7262</v>
+        <v>7269</v>
       </c>
       <c r="D515" t="n">
-        <v>9785670</v>
+        <v>9793176</v>
       </c>
       <c r="E515" t="inlineStr">
         <is>
@@ -25102,10 +25102,10 @@
         </is>
       </c>
       <c r="C516" t="n">
-        <v>1413</v>
+        <v>1415</v>
       </c>
       <c r="D516" t="n">
-        <v>2031810</v>
+        <v>2034810</v>
       </c>
       <c r="E516" t="inlineStr">
         <is>
@@ -25150,10 +25150,10 @@
         </is>
       </c>
       <c r="C517" t="n">
-        <v>3433</v>
+        <v>3436</v>
       </c>
       <c r="D517" t="n">
-        <v>5027928</v>
+        <v>5031848</v>
       </c>
       <c r="E517" t="inlineStr">
         <is>
@@ -25486,10 +25486,10 @@
         </is>
       </c>
       <c r="C524" t="n">
-        <v>5358</v>
+        <v>5362</v>
       </c>
       <c r="D524" t="n">
-        <v>7840358</v>
+        <v>7846113</v>
       </c>
       <c r="E524" t="inlineStr">
         <is>
@@ -25582,10 +25582,10 @@
         </is>
       </c>
       <c r="C526" t="n">
-        <v>436</v>
+        <v>437</v>
       </c>
       <c r="D526" t="n">
-        <v>648379</v>
+        <v>649879</v>
       </c>
       <c r="E526" t="inlineStr">
         <is>
@@ -25678,10 +25678,10 @@
         </is>
       </c>
       <c r="C528" t="n">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="D528" t="n">
-        <v>21000</v>
+        <v>25500</v>
       </c>
       <c r="E528" t="inlineStr">
         <is>
@@ -25726,10 +25726,10 @@
         </is>
       </c>
       <c r="C529" t="n">
-        <v>1772</v>
+        <v>1773</v>
       </c>
       <c r="D529" t="n">
-        <v>2339509</v>
+        <v>2340214</v>
       </c>
       <c r="E529" t="inlineStr">
         <is>
@@ -25918,10 +25918,10 @@
         </is>
       </c>
       <c r="C533" t="n">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="D533" t="n">
-        <v>428675</v>
+        <v>430175</v>
       </c>
       <c r="E533" t="inlineStr">
         <is>
@@ -26062,10 +26062,10 @@
         </is>
       </c>
       <c r="C536" t="n">
-        <v>1588</v>
+        <v>1589</v>
       </c>
       <c r="D536" t="n">
-        <v>2141839</v>
+        <v>2143339</v>
       </c>
       <c r="E536" t="inlineStr">
         <is>
@@ -26110,10 +26110,10 @@
         </is>
       </c>
       <c r="C537" t="n">
-        <v>4170</v>
+        <v>4176</v>
       </c>
       <c r="D537" t="n">
-        <v>5995985</v>
+        <v>6004985</v>
       </c>
       <c r="E537" t="inlineStr">
         <is>
@@ -26158,10 +26158,10 @@
         </is>
       </c>
       <c r="C538" t="n">
-        <v>9893</v>
+        <v>9897</v>
       </c>
       <c r="D538" t="n">
-        <v>14458064</v>
+        <v>14464064</v>
       </c>
       <c r="E538" t="inlineStr">
         <is>
@@ -26206,10 +26206,10 @@
         </is>
       </c>
       <c r="C539" t="n">
-        <v>3284</v>
+        <v>3285</v>
       </c>
       <c r="D539" t="n">
-        <v>4870537</v>
+        <v>4872037</v>
       </c>
       <c r="E539" t="inlineStr">
         <is>
@@ -26446,10 +26446,10 @@
         </is>
       </c>
       <c r="C544" t="n">
-        <v>3863</v>
+        <v>3867</v>
       </c>
       <c r="D544" t="n">
-        <v>5197945</v>
+        <v>5203945</v>
       </c>
       <c r="E544" t="inlineStr">
         <is>
@@ -26494,10 +26494,10 @@
         </is>
       </c>
       <c r="C545" t="n">
-        <v>1295</v>
+        <v>1298</v>
       </c>
       <c r="D545" t="n">
-        <v>1848776</v>
+        <v>1853276</v>
       </c>
       <c r="E545" t="inlineStr">
         <is>
@@ -26638,10 +26638,10 @@
         </is>
       </c>
       <c r="C548" t="n">
-        <v>374</v>
+        <v>377</v>
       </c>
       <c r="D548" t="n">
-        <v>554420</v>
+        <v>558920</v>
       </c>
       <c r="E548" t="inlineStr">
         <is>
@@ -26686,10 +26686,10 @@
         </is>
       </c>
       <c r="C549" t="n">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="D549" t="n">
-        <v>85073</v>
+        <v>86573</v>
       </c>
       <c r="E549" t="inlineStr">
         <is>
@@ -26926,10 +26926,10 @@
         </is>
       </c>
       <c r="C554" t="n">
-        <v>677</v>
+        <v>679</v>
       </c>
       <c r="D554" t="n">
-        <v>1010906</v>
+        <v>1013906</v>
       </c>
       <c r="E554" t="inlineStr">
         <is>
@@ -27166,10 +27166,10 @@
         </is>
       </c>
       <c r="C559" t="n">
-        <v>3170</v>
+        <v>3172</v>
       </c>
       <c r="D559" t="n">
-        <v>4550568</v>
+        <v>4553568</v>
       </c>
       <c r="E559" t="inlineStr">
         <is>
@@ -27214,10 +27214,10 @@
         </is>
       </c>
       <c r="C560" t="n">
-        <v>5538</v>
+        <v>5539</v>
       </c>
       <c r="D560" t="n">
-        <v>8101971</v>
+        <v>8102783</v>
       </c>
       <c r="E560" t="inlineStr">
         <is>
@@ -27262,10 +27262,10 @@
         </is>
       </c>
       <c r="C561" t="n">
-        <v>1639</v>
+        <v>1640</v>
       </c>
       <c r="D561" t="n">
-        <v>2434325</v>
+        <v>2435825</v>
       </c>
       <c r="E561" t="inlineStr">
         <is>
@@ -27454,10 +27454,10 @@
         </is>
       </c>
       <c r="C565" t="n">
-        <v>2017</v>
+        <v>2019</v>
       </c>
       <c r="D565" t="n">
-        <v>2641881</v>
+        <v>2644881</v>
       </c>
       <c r="E565" t="inlineStr">
         <is>
@@ -27502,10 +27502,10 @@
         </is>
       </c>
       <c r="C566" t="n">
-        <v>1966</v>
+        <v>1974</v>
       </c>
       <c r="D566" t="n">
-        <v>2810852</v>
+        <v>2822794</v>
       </c>
       <c r="E566" t="inlineStr">
         <is>
@@ -27550,10 +27550,10 @@
         </is>
       </c>
       <c r="C567" t="n">
-        <v>3918</v>
+        <v>3921</v>
       </c>
       <c r="D567" t="n">
-        <v>5727577</v>
+        <v>5732077</v>
       </c>
       <c r="E567" t="inlineStr">
         <is>
@@ -27694,10 +27694,10 @@
         </is>
       </c>
       <c r="C570" t="n">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="D570" t="n">
-        <v>123000</v>
+        <v>124500</v>
       </c>
       <c r="E570" t="inlineStr">
         <is>
@@ -27838,10 +27838,10 @@
         </is>
       </c>
       <c r="C573" t="n">
-        <v>4883</v>
+        <v>4885</v>
       </c>
       <c r="D573" t="n">
-        <v>7044939</v>
+        <v>7047939</v>
       </c>
       <c r="E573" t="inlineStr">
         <is>
@@ -27886,10 +27886,10 @@
         </is>
       </c>
       <c r="C574" t="n">
-        <v>11164</v>
+        <v>11170</v>
       </c>
       <c r="D574" t="n">
-        <v>16300481</v>
+        <v>16308219</v>
       </c>
       <c r="E574" t="inlineStr">
         <is>
@@ -27934,10 +27934,10 @@
         </is>
       </c>
       <c r="C575" t="n">
-        <v>3040</v>
+        <v>3043</v>
       </c>
       <c r="D575" t="n">
-        <v>4503570</v>
+        <v>4508070</v>
       </c>
       <c r="E575" t="inlineStr">
         <is>
@@ -28126,10 +28126,10 @@
         </is>
       </c>
       <c r="C579" t="n">
-        <v>4365</v>
+        <v>4367</v>
       </c>
       <c r="D579" t="n">
-        <v>5773737</v>
+        <v>5776057</v>
       </c>
       <c r="E579" t="inlineStr">
         <is>
@@ -28414,10 +28414,10 @@
         </is>
       </c>
       <c r="C585" t="n">
-        <v>1374</v>
+        <v>1377</v>
       </c>
       <c r="D585" t="n">
-        <v>1796111</v>
+        <v>1800611</v>
       </c>
       <c r="E585" t="inlineStr">
         <is>
@@ -28462,10 +28462,10 @@
         </is>
       </c>
       <c r="C586" t="n">
-        <v>7017</v>
+        <v>7019</v>
       </c>
       <c r="D586" t="n">
-        <v>10117715</v>
+        <v>10120715</v>
       </c>
       <c r="E586" t="inlineStr">
         <is>
@@ -28510,10 +28510,10 @@
         </is>
       </c>
       <c r="C587" t="n">
-        <v>16605</v>
+        <v>16616</v>
       </c>
       <c r="D587" t="n">
-        <v>24317394</v>
+        <v>24332374</v>
       </c>
       <c r="E587" t="inlineStr">
         <is>
@@ -28558,10 +28558,10 @@
         </is>
       </c>
       <c r="C588" t="n">
-        <v>5818</v>
+        <v>5821</v>
       </c>
       <c r="D588" t="n">
-        <v>8642641</v>
+        <v>8646515</v>
       </c>
       <c r="E588" t="inlineStr">
         <is>
@@ -28798,10 +28798,10 @@
         </is>
       </c>
       <c r="C593" t="n">
-        <v>6646</v>
+        <v>6651</v>
       </c>
       <c r="D593" t="n">
-        <v>8841300</v>
+        <v>8846877</v>
       </c>
       <c r="E593" t="inlineStr">
         <is>
@@ -28846,10 +28846,10 @@
         </is>
       </c>
       <c r="C594" t="n">
-        <v>1871</v>
+        <v>1872</v>
       </c>
       <c r="D594" t="n">
-        <v>2637730</v>
+        <v>2639230</v>
       </c>
       <c r="E594" t="inlineStr">
         <is>
@@ -28942,10 +28942,10 @@
         </is>
       </c>
       <c r="C596" t="n">
-        <v>1172</v>
+        <v>1174</v>
       </c>
       <c r="D596" t="n">
-        <v>1732753</v>
+        <v>1735753</v>
       </c>
       <c r="E596" t="inlineStr">
         <is>
@@ -28990,10 +28990,10 @@
         </is>
       </c>
       <c r="C597" t="n">
-        <v>313</v>
+        <v>314</v>
       </c>
       <c r="D597" t="n">
-        <v>461922</v>
+        <v>463422</v>
       </c>
       <c r="E597" t="inlineStr">
         <is>
@@ -29038,10 +29038,10 @@
         </is>
       </c>
       <c r="C598" t="n">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="D598" t="n">
-        <v>137318</v>
+        <v>140318</v>
       </c>
       <c r="E598" t="inlineStr">
         <is>
@@ -29182,10 +29182,10 @@
         </is>
       </c>
       <c r="C601" t="n">
-        <v>9609</v>
+        <v>9619</v>
       </c>
       <c r="D601" t="n">
-        <v>13926156</v>
+        <v>13940264</v>
       </c>
       <c r="E601" t="inlineStr">
         <is>
@@ -29230,10 +29230,10 @@
         </is>
       </c>
       <c r="C602" t="n">
-        <v>20008</v>
+        <v>20027</v>
       </c>
       <c r="D602" t="n">
-        <v>29286158</v>
+        <v>29314393</v>
       </c>
       <c r="E602" t="inlineStr">
         <is>
@@ -29278,10 +29278,10 @@
         </is>
       </c>
       <c r="C603" t="n">
-        <v>5893</v>
+        <v>5899</v>
       </c>
       <c r="D603" t="n">
-        <v>8763071</v>
+        <v>8770385</v>
       </c>
       <c r="E603" t="inlineStr">
         <is>
@@ -29326,10 +29326,10 @@
         </is>
       </c>
       <c r="C604" t="n">
-        <v>1530</v>
+        <v>1531</v>
       </c>
       <c r="D604" t="n">
-        <v>2272609</v>
+        <v>2274109</v>
       </c>
       <c r="E604" t="inlineStr">
         <is>
@@ -29470,10 +29470,10 @@
         </is>
       </c>
       <c r="C607" t="n">
-        <v>6524</v>
+        <v>6528</v>
       </c>
       <c r="D607" t="n">
-        <v>8658001</v>
+        <v>8663424</v>
       </c>
       <c r="E607" t="inlineStr">
         <is>
@@ -29518,10 +29518,10 @@
         </is>
       </c>
       <c r="C608" t="n">
-        <v>1408</v>
+        <v>1409</v>
       </c>
       <c r="D608" t="n">
-        <v>2022605</v>
+        <v>2024105</v>
       </c>
       <c r="E608" t="inlineStr">
         <is>
@@ -29806,10 +29806,10 @@
         </is>
       </c>
       <c r="C614" t="n">
-        <v>1294</v>
+        <v>1297</v>
       </c>
       <c r="D614" t="n">
-        <v>1703000</v>
+        <v>1706176</v>
       </c>
       <c r="E614" t="inlineStr">
         <is>
@@ -29854,10 +29854,10 @@
         </is>
       </c>
       <c r="C615" t="n">
-        <v>749</v>
+        <v>751</v>
       </c>
       <c r="D615" t="n">
-        <v>1071879</v>
+        <v>1073829</v>
       </c>
       <c r="E615" t="inlineStr">
         <is>
@@ -30142,10 +30142,10 @@
         </is>
       </c>
       <c r="C621" t="n">
-        <v>4443</v>
+        <v>4448</v>
       </c>
       <c r="D621" t="n">
-        <v>6447509</v>
+        <v>6455009</v>
       </c>
       <c r="E621" t="inlineStr">
         <is>
@@ -30190,10 +30190,10 @@
         </is>
       </c>
       <c r="C622" t="n">
-        <v>7169</v>
+        <v>7173</v>
       </c>
       <c r="D622" t="n">
-        <v>10420956</v>
+        <v>10426956</v>
       </c>
       <c r="E622" t="inlineStr">
         <is>
@@ -30238,10 +30238,10 @@
         </is>
       </c>
       <c r="C623" t="n">
-        <v>2222</v>
+        <v>2224</v>
       </c>
       <c r="D623" t="n">
-        <v>3300961</v>
+        <v>3303961</v>
       </c>
       <c r="E623" t="inlineStr">
         <is>
@@ -30430,10 +30430,10 @@
         </is>
       </c>
       <c r="C627" t="n">
-        <v>2773</v>
+        <v>2774</v>
       </c>
       <c r="D627" t="n">
-        <v>3677794</v>
+        <v>3678518</v>
       </c>
       <c r="E627" t="inlineStr">
         <is>
@@ -30478,10 +30478,10 @@
         </is>
       </c>
       <c r="C628" t="n">
-        <v>1876</v>
+        <v>1879</v>
       </c>
       <c r="D628" t="n">
-        <v>2703917</v>
+        <v>2708417</v>
       </c>
       <c r="E628" t="inlineStr">
         <is>
@@ -30526,10 +30526,10 @@
         </is>
       </c>
       <c r="C629" t="n">
-        <v>4469</v>
+        <v>4470</v>
       </c>
       <c r="D629" t="n">
-        <v>6558674</v>
+        <v>6560174</v>
       </c>
       <c r="E629" t="inlineStr">
         <is>
@@ -30574,10 +30574,10 @@
         </is>
       </c>
       <c r="C630" t="n">
-        <v>1333</v>
+        <v>1334</v>
       </c>
       <c r="D630" t="n">
-        <v>1970380</v>
+        <v>1971880</v>
       </c>
       <c r="E630" t="inlineStr">
         <is>
@@ -31150,10 +31150,10 @@
         </is>
       </c>
       <c r="C642" t="n">
-        <v>5870</v>
+        <v>5873</v>
       </c>
       <c r="D642" t="n">
-        <v>8509031</v>
+        <v>8512582</v>
       </c>
       <c r="E642" t="inlineStr">
         <is>
@@ -31198,10 +31198,10 @@
         </is>
       </c>
       <c r="C643" t="n">
-        <v>13306</v>
+        <v>13310</v>
       </c>
       <c r="D643" t="n">
-        <v>19551079</v>
+        <v>19556366</v>
       </c>
       <c r="E643" t="inlineStr">
         <is>
@@ -31246,10 +31246,10 @@
         </is>
       </c>
       <c r="C644" t="n">
-        <v>4951</v>
+        <v>4952</v>
       </c>
       <c r="D644" t="n">
-        <v>7344343</v>
+        <v>7345843</v>
       </c>
       <c r="E644" t="inlineStr">
         <is>
@@ -31294,10 +31294,10 @@
         </is>
       </c>
       <c r="C645" t="n">
-        <v>1353</v>
+        <v>1354</v>
       </c>
       <c r="D645" t="n">
-        <v>2019293</v>
+        <v>2020793</v>
       </c>
       <c r="E645" t="inlineStr">
         <is>
@@ -31486,10 +31486,10 @@
         </is>
       </c>
       <c r="C649" t="n">
-        <v>4583</v>
+        <v>4585</v>
       </c>
       <c r="D649" t="n">
-        <v>6109128</v>
+        <v>6111598</v>
       </c>
       <c r="E649" t="inlineStr">
         <is>
@@ -31534,10 +31534,10 @@
         </is>
       </c>
       <c r="C650" t="n">
-        <v>2485</v>
+        <v>2488</v>
       </c>
       <c r="D650" t="n">
-        <v>3578342</v>
+        <v>3582842</v>
       </c>
       <c r="E650" t="inlineStr">
         <is>
@@ -31582,10 +31582,10 @@
         </is>
       </c>
       <c r="C651" t="n">
-        <v>7391</v>
+        <v>7392</v>
       </c>
       <c r="D651" t="n">
-        <v>10860378</v>
+        <v>10861878</v>
       </c>
       <c r="E651" t="inlineStr">
         <is>
@@ -31630,10 +31630,10 @@
         </is>
       </c>
       <c r="C652" t="n">
-        <v>2424</v>
+        <v>2425</v>
       </c>
       <c r="D652" t="n">
-        <v>3598896</v>
+        <v>3600396</v>
       </c>
       <c r="E652" t="inlineStr">
         <is>
@@ -31966,10 +31966,10 @@
         </is>
       </c>
       <c r="C659" t="n">
-        <v>2675</v>
+        <v>2678</v>
       </c>
       <c r="D659" t="n">
-        <v>3918743</v>
+        <v>3923043</v>
       </c>
       <c r="E659" t="inlineStr">
         <is>
@@ -32302,10 +32302,10 @@
         </is>
       </c>
       <c r="C666" t="n">
-        <v>4482</v>
+        <v>4487</v>
       </c>
       <c r="D666" t="n">
-        <v>6579459</v>
+        <v>6586959</v>
       </c>
       <c r="E666" t="inlineStr">
         <is>
@@ -32350,10 +32350,10 @@
         </is>
       </c>
       <c r="C667" t="n">
-        <v>1477</v>
+        <v>1480</v>
       </c>
       <c r="D667" t="n">
-        <v>2195747</v>
+        <v>2200247</v>
       </c>
       <c r="E667" t="inlineStr">
         <is>
@@ -32542,10 +32542,10 @@
         </is>
       </c>
       <c r="C671" t="n">
-        <v>1467</v>
+        <v>1468</v>
       </c>
       <c r="D671" t="n">
-        <v>1898057</v>
+        <v>1898990</v>
       </c>
       <c r="E671" t="inlineStr">
         <is>
@@ -32638,10 +32638,10 @@
         </is>
       </c>
       <c r="C673" t="n">
-        <v>6764</v>
+        <v>6767</v>
       </c>
       <c r="D673" t="n">
-        <v>9896085</v>
+        <v>9899604</v>
       </c>
       <c r="E673" t="inlineStr">
         <is>
@@ -32782,10 +32782,10 @@
         </is>
       </c>
       <c r="C676" t="n">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="D676" t="n">
-        <v>117954</v>
+        <v>119454</v>
       </c>
       <c r="E676" t="inlineStr">
         <is>
@@ -32926,10 +32926,10 @@
         </is>
       </c>
       <c r="C679" t="n">
-        <v>2207</v>
+        <v>2209</v>
       </c>
       <c r="D679" t="n">
-        <v>2931649</v>
+        <v>2934649</v>
       </c>
       <c r="E679" t="inlineStr">
         <is>
@@ -32974,10 +32974,10 @@
         </is>
       </c>
       <c r="C680" t="n">
-        <v>1693</v>
+        <v>1696</v>
       </c>
       <c r="D680" t="n">
-        <v>2447263</v>
+        <v>2451763</v>
       </c>
       <c r="E680" t="inlineStr">
         <is>
@@ -33310,10 +33310,10 @@
         </is>
       </c>
       <c r="C687" t="n">
-        <v>10042</v>
+        <v>10046</v>
       </c>
       <c r="D687" t="n">
-        <v>14537069</v>
+        <v>14541949</v>
       </c>
       <c r="E687" t="inlineStr">
         <is>
@@ -33358,10 +33358,10 @@
         </is>
       </c>
       <c r="C688" t="n">
-        <v>23184</v>
+        <v>23211</v>
       </c>
       <c r="D688" t="n">
-        <v>33996899</v>
+        <v>34036541</v>
       </c>
       <c r="E688" t="inlineStr">
         <is>
@@ -33406,10 +33406,10 @@
         </is>
       </c>
       <c r="C689" t="n">
-        <v>6877</v>
+        <v>6886</v>
       </c>
       <c r="D689" t="n">
-        <v>10222485</v>
+        <v>10235985</v>
       </c>
       <c r="E689" t="inlineStr">
         <is>
@@ -33454,10 +33454,10 @@
         </is>
       </c>
       <c r="C690" t="n">
-        <v>1999</v>
+        <v>2002</v>
       </c>
       <c r="D690" t="n">
-        <v>2986296</v>
+        <v>2990796</v>
       </c>
       <c r="E690" t="inlineStr">
         <is>
@@ -33550,10 +33550,10 @@
         </is>
       </c>
       <c r="C692" t="n">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="D692" t="n">
-        <v>51000</v>
+        <v>52500</v>
       </c>
       <c r="E692" t="inlineStr">
         <is>
@@ -33646,10 +33646,10 @@
         </is>
       </c>
       <c r="C694" t="n">
-        <v>8346</v>
+        <v>8356</v>
       </c>
       <c r="D694" t="n">
-        <v>11314890</v>
+        <v>11328614</v>
       </c>
       <c r="E694" t="inlineStr">
         <is>
@@ -33694,10 +33694,10 @@
         </is>
       </c>
       <c r="C695" t="n">
-        <v>11943</v>
+        <v>11951</v>
       </c>
       <c r="D695" t="n">
-        <v>17318153</v>
+        <v>17329106</v>
       </c>
       <c r="E695" t="inlineStr">
         <is>
@@ -33742,10 +33742,10 @@
         </is>
       </c>
       <c r="C696" t="n">
-        <v>31887</v>
+        <v>31932</v>
       </c>
       <c r="D696" t="n">
-        <v>46752663</v>
+        <v>46816986</v>
       </c>
       <c r="E696" t="inlineStr">
         <is>
@@ -33790,10 +33790,10 @@
         </is>
       </c>
       <c r="C697" t="n">
-        <v>10087</v>
+        <v>10115</v>
       </c>
       <c r="D697" t="n">
-        <v>15017932</v>
+        <v>15063201</v>
       </c>
       <c r="E697" t="inlineStr">
         <is>
@@ -33838,10 +33838,10 @@
         </is>
       </c>
       <c r="C698" t="n">
-        <v>2735</v>
+        <v>2741</v>
       </c>
       <c r="D698" t="n">
-        <v>4076737</v>
+        <v>4085896</v>
       </c>
       <c r="E698" t="inlineStr">
         <is>
@@ -33886,10 +33886,10 @@
         </is>
       </c>
       <c r="C699" t="n">
-        <v>723</v>
+        <v>733</v>
       </c>
       <c r="D699" t="n">
-        <v>1074359</v>
+        <v>1093673</v>
       </c>
       <c r="E699" t="inlineStr">
         <is>
@@ -33934,10 +33934,10 @@
         </is>
       </c>
       <c r="C700" t="n">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="D700" t="n">
-        <v>58500</v>
+        <v>60000</v>
       </c>
       <c r="E700" t="inlineStr">
         <is>
@@ -34030,10 +34030,10 @@
         </is>
       </c>
       <c r="C702" t="n">
-        <v>10350</v>
+        <v>10354</v>
       </c>
       <c r="D702" t="n">
-        <v>13877009</v>
+        <v>13879972</v>
       </c>
       <c r="E702" t="inlineStr">
         <is>
@@ -34126,10 +34126,10 @@
         </is>
       </c>
       <c r="C704" t="n">
-        <v>2932</v>
+        <v>2933</v>
       </c>
       <c r="D704" t="n">
-        <v>4280742</v>
+        <v>4282242</v>
       </c>
       <c r="E704" t="inlineStr">
         <is>
@@ -34270,10 +34270,10 @@
         </is>
       </c>
       <c r="C707" t="n">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="D707" t="n">
-        <v>149121</v>
+        <v>150621</v>
       </c>
       <c r="E707" t="inlineStr">
         <is>
@@ -34366,10 +34366,10 @@
         </is>
       </c>
       <c r="C709" t="n">
-        <v>2231</v>
+        <v>2235</v>
       </c>
       <c r="D709" t="n">
-        <v>3068537</v>
+        <v>3072539</v>
       </c>
       <c r="E709" t="inlineStr">
         <is>
@@ -34414,10 +34414,10 @@
         </is>
       </c>
       <c r="C710" t="n">
-        <v>9822</v>
+        <v>9831</v>
       </c>
       <c r="D710" t="n">
-        <v>14064794</v>
+        <v>14077661</v>
       </c>
       <c r="E710" t="inlineStr">
         <is>
@@ -34462,10 +34462,10 @@
         </is>
       </c>
       <c r="C711" t="n">
-        <v>18111</v>
+        <v>18118</v>
       </c>
       <c r="D711" t="n">
-        <v>26412582</v>
+        <v>26421987</v>
       </c>
       <c r="E711" t="inlineStr">
         <is>
@@ -34558,10 +34558,10 @@
         </is>
       </c>
       <c r="C713" t="n">
-        <v>1220</v>
+        <v>1221</v>
       </c>
       <c r="D713" t="n">
-        <v>1822081</v>
+        <v>1823581</v>
       </c>
       <c r="E713" t="inlineStr">
         <is>
@@ -34750,10 +34750,10 @@
         </is>
       </c>
       <c r="C717" t="n">
-        <v>6013</v>
+        <v>6014</v>
       </c>
       <c r="D717" t="n">
-        <v>8089266</v>
+        <v>8090666</v>
       </c>
       <c r="E717" t="inlineStr">
         <is>
@@ -34798,10 +34798,10 @@
         </is>
       </c>
       <c r="C718" t="n">
-        <v>4285</v>
+        <v>4289</v>
       </c>
       <c r="D718" t="n">
-        <v>6185689</v>
+        <v>6192187</v>
       </c>
       <c r="E718" t="inlineStr">
         <is>
@@ -34846,10 +34846,10 @@
         </is>
       </c>
       <c r="C719" t="n">
-        <v>10599</v>
+        <v>10601</v>
       </c>
       <c r="D719" t="n">
-        <v>15516632</v>
+        <v>15519632</v>
       </c>
       <c r="E719" t="inlineStr">
         <is>
@@ -34894,10 +34894,10 @@
         </is>
       </c>
       <c r="C720" t="n">
-        <v>2884</v>
+        <v>2885</v>
       </c>
       <c r="D720" t="n">
-        <v>4274172</v>
+        <v>4275672</v>
       </c>
       <c r="E720" t="inlineStr">
         <is>
@@ -34942,10 +34942,10 @@
         </is>
       </c>
       <c r="C721" t="n">
-        <v>674</v>
+        <v>675</v>
       </c>
       <c r="D721" t="n">
-        <v>994993</v>
+        <v>996991</v>
       </c>
       <c r="E721" t="inlineStr">
         <is>
@@ -34990,10 +34990,10 @@
         </is>
       </c>
       <c r="C722" t="n">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="D722" t="n">
-        <v>264498</v>
+        <v>266496</v>
       </c>
       <c r="E722" t="inlineStr">
         <is>
@@ -35086,10 +35086,10 @@
         </is>
       </c>
       <c r="C724" t="n">
-        <v>3461</v>
+        <v>3463</v>
       </c>
       <c r="D724" t="n">
-        <v>4537036</v>
+        <v>4540036</v>
       </c>
       <c r="E724" t="inlineStr">
         <is>

</xml_diff>